<commit_message>
add function for KeckLFC
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\astrocomb\KeckLFC-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBBD0B8-6187-4A15-8FB2-17390A92C1F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9998D7B-C097-44CA-939A-413240C0E695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="957" uniqueCount="442">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="479">
   <si>
     <t>Keyword</t>
   </si>
@@ -1405,6 +1405,117 @@
   </si>
   <si>
     <t>Pritel output power</t>
+  </si>
+  <si>
+    <t>mw</t>
+  </si>
+  <si>
+    <t>apc mode:450mw</t>
+  </si>
+  <si>
+    <t>LFC_EDFA27_AUTO_ON</t>
+  </si>
+  <si>
+    <t>acc' or 'apc' or none</t>
+  </si>
+  <si>
+    <t>auto set power or current and turn on</t>
+  </si>
+  <si>
+    <t>LFC_RFOSCI_ONOFF</t>
+  </si>
+  <si>
+    <t>1 or 0</t>
+  </si>
+  <si>
+    <t>set on or off of rfosc powersup</t>
+  </si>
+  <si>
+    <t>LFC_RFAMP_ONOFF</t>
+  </si>
+  <si>
+    <t>set on or off of rfamp powersup</t>
+  </si>
+  <si>
+    <t>LFC_EDFA23_AUTO_ON</t>
+  </si>
+  <si>
+    <t>acc'or none</t>
+  </si>
+  <si>
+    <t>ma</t>
+  </si>
+  <si>
+    <t>acc:80mA</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>reset arduino</t>
+  </si>
+  <si>
+    <t>LFC_YJ_SHUTTER</t>
+  </si>
+  <si>
+    <t>set YJ shutter 1 or 0</t>
+  </si>
+  <si>
+    <t>1:pass light/0:shut light</t>
+  </si>
+  <si>
+    <t>LFC_2BY2_SWITCH</t>
+  </si>
+  <si>
+    <t>1 or 0 or none</t>
+  </si>
+  <si>
+    <t>set 2 by 2 switch</t>
+  </si>
+  <si>
+    <t>1 or 2 or none</t>
+  </si>
+  <si>
+    <t>1:YJ/2:HK</t>
+  </si>
+  <si>
+    <t>LFC_HK_SHUTTER</t>
+  </si>
+  <si>
+    <t>set hk shutter</t>
+  </si>
+  <si>
+    <t>1 or open:pass light/0 or close:shut light</t>
+  </si>
+  <si>
+    <t>LFC_VOA1550_ATTEN</t>
+  </si>
+  <si>
+    <t>db number</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t xml:space="preserve">set attenuation db </t>
+  </si>
+  <si>
+    <t>0-60db</t>
+  </si>
+  <si>
+    <t>LFC_VOA1310_ATTEN</t>
+  </si>
+  <si>
+    <t>LFC_VOA2000_ATTEN</t>
+  </si>
+  <si>
+    <t>LFC_IM_LOCK_MODE</t>
+  </si>
+  <si>
+    <t>pid' or 'man'</t>
+  </si>
+  <si>
+    <t>set lock mode</t>
   </si>
 </sst>
 </file>
@@ -1887,6 +1998,18 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1895,12 +2018,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1914,11 +2031,56 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -1933,57 +2095,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -2340,7 +2451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S193"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2362,68 +2473,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="44"/>
-      <c r="B1" s="45" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="40"/>
-      <c r="L1" s="42" t="s">
+      <c r="K1" s="44"/>
+      <c r="L1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="40"/>
-      <c r="O1" s="42" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="41" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="47"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="49"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="43"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="43"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="42"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
@@ -2576,10 +2687,10 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="48" t="s">
+      <c r="J7" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="48"/>
+      <c r="K7" s="40"/>
       <c r="M7">
         <v>0</v>
       </c>
@@ -2606,10 +2717,10 @@
       <c r="H8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="48" t="s">
+      <c r="J8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="48"/>
+      <c r="K8" s="40"/>
       <c r="M8">
         <v>0</v>
       </c>
@@ -2673,7 +2784,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="39" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
@@ -2697,13 +2808,13 @@
       <c r="H11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="48" t="s">
+      <c r="J11" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="48"/>
+      <c r="K11" s="40"/>
     </row>
     <row r="12" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A12" s="49"/>
+      <c r="A12" s="39"/>
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -2725,10 +2836,10 @@
       <c r="H12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="48" t="s">
+      <c r="J12" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="48"/>
+      <c r="K12" s="40"/>
     </row>
     <row r="13" spans="1:19" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A13" s="31"/>
@@ -3593,7 +3704,7 @@
       <c r="H54" s="11"/>
     </row>
     <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="43" t="s">
         <v>153</v>
       </c>
       <c r="B55" t="s">
@@ -3603,7 +3714,7 @@
       <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A56" s="39"/>
+      <c r="A56" s="43"/>
       <c r="B56" t="s">
         <v>155</v>
       </c>
@@ -3611,7 +3722,7 @@
       <c r="H56" s="11"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A57" s="39"/>
+      <c r="A57" s="43"/>
       <c r="B57" t="s">
         <v>156</v>
       </c>
@@ -3619,7 +3730,7 @@
       <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A58" s="39"/>
+      <c r="A58" s="43"/>
       <c r="B58" t="s">
         <v>157</v>
       </c>
@@ -3627,7 +3738,7 @@
       <c r="H58" s="11"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A59" s="39"/>
+      <c r="A59" s="43"/>
       <c r="B59" t="s">
         <v>158</v>
       </c>
@@ -3635,7 +3746,7 @@
       <c r="H59" s="11"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A60" s="39"/>
+      <c r="A60" s="43"/>
       <c r="B60" t="s">
         <v>159</v>
       </c>
@@ -3643,7 +3754,7 @@
       <c r="H60" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A61" s="39"/>
+      <c r="A61" s="43"/>
       <c r="B61" t="s">
         <v>160</v>
       </c>
@@ -3656,7 +3767,7 @@
       <c r="H62" s="11"/>
     </row>
     <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="39" t="s">
+      <c r="A63" s="43" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
@@ -3666,7 +3777,7 @@
       <c r="H63" s="11"/>
     </row>
     <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A64" s="39"/>
+      <c r="A64" s="43"/>
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -3674,7 +3785,7 @@
       <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A65" s="39"/>
+      <c r="A65" s="43"/>
       <c r="B65" t="s">
         <v>164</v>
       </c>
@@ -3682,7 +3793,7 @@
       <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A66" s="39"/>
+      <c r="A66" s="43"/>
       <c r="B66" t="s">
         <v>165</v>
       </c>
@@ -3690,7 +3801,7 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A67" s="39"/>
+      <c r="A67" s="43"/>
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -3698,7 +3809,7 @@
       <c r="H67" s="11"/>
     </row>
     <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A68" s="39"/>
+      <c r="A68" s="43"/>
       <c r="B68" t="s">
         <v>167</v>
       </c>
@@ -3706,7 +3817,7 @@
       <c r="H68" s="11"/>
     </row>
     <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A69" s="39"/>
+      <c r="A69" s="43"/>
       <c r="B69" t="s">
         <v>168</v>
       </c>
@@ -5395,11 +5506,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A55:A61"/>
     <mergeCell ref="A63:A69"/>
     <mergeCell ref="M1:M2"/>
@@ -5416,6 +5522,11 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5429,15 +5540,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60079DE2-3043-422E-90F3-3EEEEA14A1EF}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
-    <col min="2" max="2" width="13.3984375" customWidth="1"/>
+    <col min="1" max="1" width="4.3984375" customWidth="1"/>
+    <col min="2" max="2" width="21.3984375" customWidth="1"/>
     <col min="3" max="3" width="13.296875" customWidth="1"/>
     <col min="4" max="4" width="20.94921875" customWidth="1"/>
     <col min="5" max="5" width="17.546875" customWidth="1"/>
@@ -5449,66 +5561,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="44"/>
-      <c r="B1" s="45" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="40"/>
-      <c r="L1" s="42" t="s">
+      <c r="K1" s="44"/>
+      <c r="L1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="40"/>
-      <c r="O1" s="42" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="41" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.6">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="47"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="49"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="43"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="43"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="42"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A3" s="17" t="s">
@@ -5529,8 +5641,245 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B5" t="s">
+        <v>452</v>
+      </c>
+      <c r="C5" t="s">
+        <v>453</v>
+      </c>
+      <c r="E5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>446</v>
+      </c>
+      <c r="I5" t="s">
+        <v>454</v>
+      </c>
+      <c r="M5" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B6" t="s">
+        <v>444</v>
+      </c>
+      <c r="C6" s="33" t="s">
+        <v>445</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" t="s">
+        <v>446</v>
+      </c>
+      <c r="I6" t="s">
+        <v>442</v>
+      </c>
+      <c r="M6" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B7" t="s">
+        <v>447</v>
+      </c>
+      <c r="C7" t="s">
+        <v>448</v>
+      </c>
+      <c r="E7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" t="s">
+        <v>377</v>
+      </c>
+      <c r="G7" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B8" t="s">
+        <v>450</v>
+      </c>
+      <c r="C8" t="s">
+        <v>448</v>
+      </c>
+      <c r="E8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" t="s">
+        <v>377</v>
+      </c>
+      <c r="G8" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C9" t="s">
+        <v>456</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
+        <v>377</v>
+      </c>
+      <c r="G9" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B10" t="s">
+        <v>458</v>
+      </c>
+      <c r="C10" t="s">
+        <v>448</v>
+      </c>
+      <c r="E10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F10" t="s">
+        <v>377</v>
+      </c>
+      <c r="G10" t="s">
+        <v>459</v>
+      </c>
+      <c r="H10" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B11" t="s">
+        <v>461</v>
+      </c>
+      <c r="C11" t="s">
+        <v>464</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>377</v>
+      </c>
+      <c r="G11" t="s">
+        <v>463</v>
+      </c>
+      <c r="H11" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B12" t="s">
+        <v>466</v>
+      </c>
+      <c r="C12" t="s">
+        <v>462</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>377</v>
+      </c>
+      <c r="G12" t="s">
+        <v>467</v>
+      </c>
+      <c r="H12" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B13" t="s">
+        <v>469</v>
+      </c>
+      <c r="C13" t="s">
+        <v>470</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>471</v>
+      </c>
+      <c r="G13" t="s">
+        <v>472</v>
+      </c>
+      <c r="H13" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B14" t="s">
+        <v>474</v>
+      </c>
+      <c r="C14" t="s">
+        <v>470</v>
+      </c>
+      <c r="E14" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" t="s">
+        <v>471</v>
+      </c>
+      <c r="G14" t="s">
+        <v>472</v>
+      </c>
+      <c r="H14" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B15" t="s">
+        <v>475</v>
+      </c>
+      <c r="C15" t="s">
+        <v>470</v>
+      </c>
+      <c r="E15" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" t="s">
+        <v>471</v>
+      </c>
+      <c r="G15" t="s">
+        <v>472</v>
+      </c>
+      <c r="H15" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B16" t="s">
+        <v>476</v>
+      </c>
+      <c r="C16" s="33" t="s">
+        <v>477</v>
+      </c>
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>478</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="G1:G2"/>
@@ -5539,12 +5888,6 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5813,38 +6156,38 @@
       <c r="D1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="67" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="50" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="51"/>
+      <c r="H1" s="68"/>
     </row>
     <row r="2" spans="1:8" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="69" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="54"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="3"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="50" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
     </row>
     <row r="4" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="4">
@@ -5854,12 +6197,12 @@
         <v>370</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60" t="s">
+      <c r="D4" s="59"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="61"/>
+      <c r="G4" s="58"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -5870,12 +6213,12 @@
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="62" t="s">
+      <c r="D5" s="55"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="53" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="63"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -5886,12 +6229,12 @@
         <v>372</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60" t="s">
+      <c r="D6" s="59"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="61"/>
+      <c r="G6" s="58"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -5902,12 +6245,12 @@
         <v>373</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="62" t="s">
+      <c r="D7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="53" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="63"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -5918,12 +6261,12 @@
         <v>53</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60" t="s">
+      <c r="D8" s="59"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="61"/>
+      <c r="G8" s="58"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -5934,25 +6277,25 @@
         <v>374</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="65"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="6" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="5"/>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="64" t="s">
         <v>376</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="66"/>
     </row>
     <row r="11" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A11" s="6">
@@ -5964,12 +6307,12 @@
       <c r="C11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E11" s="63"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="65"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -5982,12 +6325,12 @@
       <c r="C12" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E12" s="61"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="59"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -6000,12 +6343,12 @@
       <c r="C13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="62" t="s">
+      <c r="D13" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="65"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="56"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -6016,12 +6359,12 @@
         <v>380</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="59"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -6034,12 +6377,12 @@
       <c r="C15" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="65"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -6052,12 +6395,12 @@
       <c r="C16" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="61"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="59"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -6070,12 +6413,12 @@
       <c r="C17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -6088,12 +6431,12 @@
       <c r="C18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="61"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="59"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="60"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -6106,12 +6449,12 @@
       <c r="C19" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="65"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -6124,12 +6467,12 @@
       <c r="C20" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="59"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="60"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="117.3" thickBot="1" x14ac:dyDescent="0.65">
@@ -6142,12 +6485,12 @@
       <c r="C21" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="62" t="s">
+      <c r="D21" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="65"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
       <c r="H21" s="6" t="s">
         <v>389</v>
       </c>
@@ -6162,12 +6505,12 @@
       <c r="C22" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E22" s="61"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="59"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="60"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -6192,13 +6535,13 @@
     </row>
     <row r="24" spans="1:8" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A24" s="7"/>
-      <c r="B24" s="69" t="s">
+      <c r="B24" s="61" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="71"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="63"/>
     </row>
     <row r="25" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A25" s="6">
@@ -6266,13 +6609,13 @@
     </row>
     <row r="29" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A29" s="3"/>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="50" t="s">
         <v>396</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="57"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="52"/>
     </row>
     <row r="30" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A30" s="4">
@@ -6430,13 +6773,13 @@
     </row>
     <row r="41" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A41" s="3"/>
-      <c r="B41" s="55" t="s">
+      <c r="B41" s="50" t="s">
         <v>408</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="57"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="52"/>
     </row>
     <row r="42" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A42" s="4">
@@ -6510,31 +6853,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="D5:E5"/>
@@ -6548,12 +6872,31 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -6861,6 +7204,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EEDE7DDB808AF47B14A37A2563255CF" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="17d65d9f425ad811f92dcb994434cebd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8efcafe-ecab-455b-a9ec-2441266f5451" xmlns:ns3="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35cb6db38e7d3d9001b7e6afffee4001" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
@@ -7171,15 +7523,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
   <ds:schemaRefs>
@@ -7193,6 +7536,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3366D879-DBBC-469C-98D7-600868252265}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7210,12 +7561,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
clarity pyhton code, keckLFC change, #hardware init for test, lab clarity test, keyword list update
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\astrocomb\KeckLFC-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31ADFC1C-9901-4466-8569-77A1D2A89B06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C7022B0-C30C-445D-B6CB-B439FA3098FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5838" yWindow="810" windowWidth="17280" windowHeight="10620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSF EO Comb" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1273" uniqueCount="517">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="533">
   <si>
     <t>Keyword</t>
   </si>
@@ -1494,9 +1494,6 @@
     <t>db number</t>
   </si>
   <si>
-    <t>int</t>
-  </si>
-  <si>
     <t xml:space="preserve">set attenuation db </t>
   </si>
   <si>
@@ -1551,15 +1548,9 @@
     <t>Small  EDFA (500 mW) 1 auto turn on</t>
   </si>
   <si>
-    <t>apc mode 450mw</t>
-  </si>
-  <si>
     <t>Use constant power mode (APC mode) ; Read is monitored, write is setpoint. Value='default':acc mode 80mw</t>
   </si>
   <si>
-    <t>acc mode 80mw</t>
-  </si>
-  <si>
     <t>Small EDFA (200 mW) 3 auto trun on</t>
   </si>
   <si>
@@ -1575,9 +1566,6 @@
     <t>default set:I=3A</t>
   </si>
   <si>
-    <t>default:3v</t>
-  </si>
-  <si>
     <t xml:space="preserve">set RF osci on/off state </t>
   </si>
   <si>
@@ -1620,9 +1608,6 @@
     <t>voa1310 db set. Default:60db</t>
   </si>
   <si>
-    <t>same as LFC_2BY2_SWITCH. Input value:'YJ' or 'HK'</t>
-  </si>
-  <si>
     <t>LFC_RB_AUTO_LOCK</t>
   </si>
   <si>
@@ -1630,6 +1615,69 @@
   </si>
   <si>
     <t>LFC_WSP_OPTIMIZE</t>
+  </si>
+  <si>
+    <t>LFC_EDFA27_P_DEFAULT</t>
+  </si>
+  <si>
+    <t>value==none:read power/value!=none,set 'apc'mode, 450mw</t>
+  </si>
+  <si>
+    <t>value==none:read power/value !=none, set apc mode 450mw and turn on edfa27</t>
+  </si>
+  <si>
+    <t>LFC_EDFA23_P_DEFAULT</t>
+  </si>
+  <si>
+    <t>value==none:read power/value!=none,set 'acc'mode, 80mA</t>
+  </si>
+  <si>
+    <t>value==none, read emission status/value!=none,set acc mode 80mw and turn on power</t>
+  </si>
+  <si>
+    <t>LFC_RFAMP_DEFAULT</t>
+  </si>
+  <si>
+    <t>read/set RF amp default value</t>
+  </si>
+  <si>
+    <t>value==none, read  voltage and current/value!=none,set v1=30v I1=5A</t>
+  </si>
+  <si>
+    <t>LFC_RFOSCI_DEFAULT</t>
+  </si>
+  <si>
+    <t>read RF Oscillator v and I/set default v and I</t>
+  </si>
+  <si>
+    <t>default:15v</t>
+  </si>
+  <si>
+    <t>Value==none, read V and I/value!=none, set V=15v I =3A</t>
+  </si>
+  <si>
+    <t>LFC_PTAMP_PRE_P_DEFAULT</t>
+  </si>
+  <si>
+    <t>High-power EDFA pre-amp current</t>
+  </si>
+  <si>
+    <t>value=none, read pre amp current/value!=none, set to 600mA</t>
+  </si>
+  <si>
+    <t>LFC_PTAMP_I_DEFAULT</t>
+  </si>
+  <si>
+    <t>High Power EDFA output Power/current set</t>
+  </si>
+  <si>
+    <t>value=none, read out amp current/value!=none, set to 4.1A</t>
+  </si>
+  <si>
+    <t>value==none, read input power voltage/value==1, reset latch circuit/value else, do nothing</t>
+  </si>
+  <si>
+    <t>same as LFC_2BY2_SWITCH. Input value:1(represent YJ) or 2(represent HK) (input number only)</t>
   </si>
 </sst>
 </file>
@@ -2022,7 +2070,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2112,6 +2160,18 @@
     <xf numFmtId="0" fontId="14" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2120,12 +2180,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2139,11 +2193,56 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2160,57 +2259,8 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="25">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2565,8 +2615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S193"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:M10"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -2587,68 +2637,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="44"/>
-      <c r="B1" s="45" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="40"/>
-      <c r="L1" s="42" t="s">
+      <c r="K1" s="44"/>
+      <c r="L1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="40"/>
-      <c r="O1" s="42" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="41" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="47"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="49"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="43"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="43"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="42"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
@@ -2801,10 +2851,10 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="48" t="s">
+      <c r="J7" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="48"/>
+      <c r="K7" s="40"/>
       <c r="M7">
         <v>0</v>
       </c>
@@ -2831,10 +2881,10 @@
       <c r="H8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="48" t="s">
+      <c r="J8" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="48"/>
+      <c r="K8" s="40"/>
       <c r="M8">
         <v>0</v>
       </c>
@@ -2898,7 +2948,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="39" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
@@ -2922,13 +2972,13 @@
       <c r="H11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="48" t="s">
+      <c r="J11" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="48"/>
+      <c r="K11" s="40"/>
     </row>
     <row r="12" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A12" s="49"/>
+      <c r="A12" s="39"/>
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -2950,10 +3000,10 @@
       <c r="H12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="48" t="s">
+      <c r="J12" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="48"/>
+      <c r="K12" s="40"/>
     </row>
     <row r="13" spans="1:19" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A13" s="31"/>
@@ -3818,7 +3868,7 @@
       <c r="H54" s="11"/>
     </row>
     <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A55" s="39" t="s">
+      <c r="A55" s="43" t="s">
         <v>153</v>
       </c>
       <c r="B55" t="s">
@@ -3828,7 +3878,7 @@
       <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A56" s="39"/>
+      <c r="A56" s="43"/>
       <c r="B56" t="s">
         <v>155</v>
       </c>
@@ -3836,7 +3886,7 @@
       <c r="H56" s="11"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A57" s="39"/>
+      <c r="A57" s="43"/>
       <c r="B57" t="s">
         <v>156</v>
       </c>
@@ -3844,7 +3894,7 @@
       <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A58" s="39"/>
+      <c r="A58" s="43"/>
       <c r="B58" t="s">
         <v>157</v>
       </c>
@@ -3852,7 +3902,7 @@
       <c r="H58" s="11"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A59" s="39"/>
+      <c r="A59" s="43"/>
       <c r="B59" t="s">
         <v>158</v>
       </c>
@@ -3860,7 +3910,7 @@
       <c r="H59" s="11"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A60" s="39"/>
+      <c r="A60" s="43"/>
       <c r="B60" t="s">
         <v>159</v>
       </c>
@@ -3868,7 +3918,7 @@
       <c r="H60" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A61" s="39"/>
+      <c r="A61" s="43"/>
       <c r="B61" t="s">
         <v>160</v>
       </c>
@@ -3881,7 +3931,7 @@
       <c r="H62" s="11"/>
     </row>
     <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="39" t="s">
+      <c r="A63" s="43" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
@@ -3891,7 +3941,7 @@
       <c r="H63" s="11"/>
     </row>
     <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A64" s="39"/>
+      <c r="A64" s="43"/>
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -3899,7 +3949,7 @@
       <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A65" s="39"/>
+      <c r="A65" s="43"/>
       <c r="B65" t="s">
         <v>164</v>
       </c>
@@ -3907,7 +3957,7 @@
       <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A66" s="39"/>
+      <c r="A66" s="43"/>
       <c r="B66" t="s">
         <v>165</v>
       </c>
@@ -3915,7 +3965,7 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A67" s="39"/>
+      <c r="A67" s="43"/>
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -3923,7 +3973,7 @@
       <c r="H67" s="11"/>
     </row>
     <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A68" s="39"/>
+      <c r="A68" s="43"/>
       <c r="B68" t="s">
         <v>167</v>
       </c>
@@ -3931,7 +3981,7 @@
       <c r="H68" s="11"/>
     </row>
     <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A69" s="39"/>
+      <c r="A69" s="43"/>
       <c r="B69" t="s">
         <v>168</v>
       </c>
@@ -5620,11 +5670,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A55:A61"/>
     <mergeCell ref="A63:A69"/>
     <mergeCell ref="M1:M2"/>
@@ -5641,6 +5686,11 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5654,10 +5704,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60079DE2-3043-422E-90F3-3EEEEA14A1EF}">
-  <dimension ref="A1:O70"/>
+  <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -5676,66 +5726,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="44"/>
-      <c r="B1" s="45" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="46" t="s">
+      <c r="D1" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="45" t="s">
+      <c r="F1" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="46" t="s">
+      <c r="G1" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="46" t="s">
+      <c r="H1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="47" t="s">
+      <c r="I1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="J1" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="40"/>
-      <c r="L1" s="42" t="s">
+      <c r="K1" s="44"/>
+      <c r="L1" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="40" t="s">
+      <c r="M1" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="40"/>
-      <c r="O1" s="42" t="s">
+      <c r="N1" s="44"/>
+      <c r="O1" s="41" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.6">
-      <c r="A2" s="45"/>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="46"/>
-      <c r="H2" s="46"/>
-      <c r="I2" s="47"/>
+      <c r="A2" s="47"/>
+      <c r="B2" s="47"/>
+      <c r="C2" s="47"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="47"/>
+      <c r="G2" s="48"/>
+      <c r="H2" s="48"/>
+      <c r="I2" s="49"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="43"/>
-      <c r="M2" s="41"/>
-      <c r="N2" s="41"/>
-      <c r="O2" s="43"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="O2" s="42"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A3" s="17" t="s">
@@ -5854,7 +5904,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.6">
-      <c r="B10" t="s">
+      <c r="B10" s="73" t="s">
         <v>458</v>
       </c>
       <c r="C10" t="s">
@@ -5874,7 +5924,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.6">
-      <c r="B11" t="s">
+      <c r="B11" s="72" t="s">
         <v>461</v>
       </c>
       <c r="C11" t="s">
@@ -5892,9 +5942,15 @@
       <c r="H11" t="s">
         <v>465</v>
       </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.6">
-      <c r="B12" t="s">
+      <c r="B12" s="73" t="s">
         <v>466</v>
       </c>
       <c r="C12" t="s">
@@ -5914,7 +5970,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.6">
-      <c r="B13" t="s">
+      <c r="B13" s="72" t="s">
         <v>469</v>
       </c>
       <c r="C13" t="s">
@@ -5924,18 +5980,24 @@
         <v>17</v>
       </c>
       <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" t="s">
         <v>471</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>472</v>
       </c>
-      <c r="H13" t="s">
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="B14" s="73" t="s">
         <v>473</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.6">
-      <c r="B14" t="s">
-        <v>474</v>
       </c>
       <c r="C14" t="s">
         <v>470</v>
@@ -5944,18 +6006,24 @@
         <v>17</v>
       </c>
       <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" t="s">
         <v>471</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>472</v>
       </c>
-      <c r="H14" t="s">
-        <v>473</v>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.6">
-      <c r="B15" t="s">
-        <v>475</v>
+      <c r="B15" s="72" t="s">
+        <v>474</v>
       </c>
       <c r="C15" t="s">
         <v>470</v>
@@ -5964,52 +6032,58 @@
         <v>17</v>
       </c>
       <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" t="s">
         <v>471</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>472</v>
       </c>
-      <c r="H15" t="s">
-        <v>473</v>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B16" t="s">
+        <v>475</v>
+      </c>
+      <c r="C16" s="33" t="s">
         <v>476</v>
       </c>
-      <c r="C16" s="33" t="s">
+      <c r="E16" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" t="s">
+        <v>478</v>
+      </c>
+      <c r="G16" t="s">
         <v>477</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" t="s">
-        <v>479</v>
-      </c>
-      <c r="G16" t="s">
-        <v>478</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B20" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="G20" t="s">
+        <v>479</v>
+      </c>
+      <c r="H20" t="s">
         <v>480</v>
-      </c>
-      <c r="H20" t="s">
-        <v>481</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B21" t="s">
+        <v>482</v>
+      </c>
+      <c r="G21" t="s">
         <v>483</v>
       </c>
-      <c r="G21" t="s">
-        <v>484</v>
-      </c>
       <c r="H21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.6">
@@ -6024,12 +6098,12 @@
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B24" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B25" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.6">
@@ -6128,7 +6202,7 @@
         <v>85</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I32" t="s">
         <v>87</v>
@@ -6143,73 +6217,61 @@
         <v>630</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.6">
+    <row r="33" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B33" t="s">
-        <v>88</v>
-      </c>
-      <c r="C33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D33" t="s">
-        <v>51</v>
+        <v>512</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
       </c>
-      <c r="F33" t="s">
-        <v>33</v>
-      </c>
       <c r="G33" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="H33" s="19"/>
+        <v>85</v>
+      </c>
+      <c r="H33" s="19" t="s">
+        <v>513</v>
+      </c>
+      <c r="I33" t="s">
+        <v>442</v>
+      </c>
     </row>
     <row r="34" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B34" t="s">
-        <v>488</v>
+        <v>88</v>
+      </c>
+      <c r="C34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E34" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" t="s">
+        <v>33</v>
       </c>
       <c r="G34" s="8" t="s">
-        <v>489</v>
-      </c>
-      <c r="H34" s="19" t="s">
-        <v>490</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H34" s="19"/>
     </row>
     <row r="35" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B35" t="s">
+        <v>444</v>
+      </c>
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>488</v>
+      </c>
+      <c r="H35" s="19" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="36" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="B36" t="s">
         <v>90</v>
-      </c>
-      <c r="C35" t="s">
-        <v>50</v>
-      </c>
-      <c r="D35" t="s">
-        <v>51</v>
-      </c>
-      <c r="E35" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H35" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="I35" t="s">
-        <v>87</v>
-      </c>
-      <c r="J35">
-        <v>0</v>
-      </c>
-      <c r="K35" t="s">
-        <v>92</v>
-      </c>
-      <c r="M35">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.6">
-      <c r="B36" t="s">
-        <v>93</v>
       </c>
       <c r="C36" t="s">
         <v>50</v>
@@ -6220,17 +6282,28 @@
       <c r="E36" t="s">
         <v>17</v>
       </c>
-      <c r="F36" t="s">
-        <v>33</v>
-      </c>
       <c r="G36" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H36" s="11"/>
-    </row>
-    <row r="37" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+        <v>91</v>
+      </c>
+      <c r="H36" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="I36" t="s">
+        <v>87</v>
+      </c>
+      <c r="J36">
+        <v>0</v>
+      </c>
+      <c r="K36" t="s">
+        <v>92</v>
+      </c>
+      <c r="M36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B37" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C37" t="s">
         <v>50</v>
@@ -6241,28 +6314,17 @@
       <c r="E37" t="s">
         <v>17</v>
       </c>
+      <c r="F37" t="s">
+        <v>33</v>
+      </c>
       <c r="G37" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="H37" s="20" t="s">
-        <v>491</v>
-      </c>
-      <c r="I37" t="s">
-        <v>87</v>
-      </c>
-      <c r="J37">
-        <v>0</v>
-      </c>
-      <c r="K37" t="s">
-        <v>92</v>
-      </c>
-      <c r="M37">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.6">
+        <v>94</v>
+      </c>
+      <c r="H37" s="11"/>
+    </row>
+    <row r="38" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
         <v>50</v>
@@ -6273,212 +6335,193 @@
       <c r="E38" t="s">
         <v>17</v>
       </c>
-      <c r="F38" t="s">
-        <v>33</v>
-      </c>
       <c r="G38" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H38" s="11"/>
-    </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.6">
+        <v>96</v>
+      </c>
+      <c r="H38" s="20" t="s">
+        <v>489</v>
+      </c>
+      <c r="I38" t="s">
+        <v>87</v>
+      </c>
+      <c r="J38">
+        <v>0</v>
+      </c>
+      <c r="K38" t="s">
+        <v>92</v>
+      </c>
+      <c r="M38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B39" t="s">
-        <v>488</v>
+        <v>515</v>
+      </c>
+      <c r="E39" t="s">
+        <v>17</v>
       </c>
       <c r="G39" s="8" t="s">
-        <v>493</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>492</v>
+        <v>96</v>
+      </c>
+      <c r="H39" s="19" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="40" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B40" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C40" t="s">
         <v>50</v>
       </c>
       <c r="D40" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E40" t="s">
         <v>17</v>
       </c>
+      <c r="F40" t="s">
+        <v>33</v>
+      </c>
       <c r="G40" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="H40" s="19" t="s">
-        <v>494</v>
-      </c>
-      <c r="I40" t="s">
-        <v>102</v>
-      </c>
-      <c r="L40" t="s">
-        <v>103</v>
-      </c>
-      <c r="M40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+        <v>98</v>
+      </c>
+      <c r="H40" s="11"/>
+    </row>
+    <row r="41" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B41" t="s">
-        <v>105</v>
-      </c>
-      <c r="C41" t="s">
-        <v>50</v>
-      </c>
-      <c r="D41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E41" t="s">
-        <v>17</v>
+        <v>487</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="H41" s="19" t="s">
-        <v>495</v>
-      </c>
-      <c r="I41" t="s">
-        <v>108</v>
-      </c>
-      <c r="J41">
-        <v>30</v>
-      </c>
-      <c r="K41">
-        <v>30</v>
-      </c>
-      <c r="M41">
-        <v>30</v>
+        <v>490</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B42" t="s">
-        <v>450</v>
+        <v>99</v>
+      </c>
+      <c r="C42" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" t="s">
+        <v>16</v>
       </c>
       <c r="E42" t="s">
         <v>17</v>
       </c>
       <c r="G42" s="8" t="s">
-        <v>496</v>
-      </c>
-      <c r="H42" s="19"/>
-    </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.6">
+        <v>100</v>
+      </c>
+      <c r="H42" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="I42" t="s">
+        <v>102</v>
+      </c>
+      <c r="L42" t="s">
+        <v>103</v>
+      </c>
+      <c r="M42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B43" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C43" t="s">
         <v>50</v>
       </c>
       <c r="D43" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E43" t="s">
         <v>17</v>
       </c>
-      <c r="G43" s="19" t="s">
-        <v>110</v>
+      <c r="G43" s="8" t="s">
+        <v>106</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="I43" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="J43">
-        <v>0.35</v>
+        <v>30</v>
       </c>
       <c r="K43">
-        <v>0.7</v>
-      </c>
-      <c r="M43" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.6">
+        <v>30</v>
+      </c>
+      <c r="M43">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B44" t="s">
-        <v>112</v>
-      </c>
-      <c r="C44" t="s">
-        <v>50</v>
-      </c>
-      <c r="D44" t="s">
-        <v>51</v>
+        <v>518</v>
       </c>
       <c r="E44" t="s">
         <v>17</v>
       </c>
-      <c r="G44" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>498</v>
-      </c>
-      <c r="I44" t="s">
-        <v>108</v>
-      </c>
-      <c r="J44">
-        <v>15</v>
-      </c>
-      <c r="K44">
-        <v>15</v>
-      </c>
-      <c r="M44">
-        <v>15</v>
+      <c r="G44" s="8" t="s">
+        <v>519</v>
+      </c>
+      <c r="H44" s="19" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B45" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="E45" t="s">
         <v>17</v>
       </c>
-      <c r="G45" s="19" t="s">
-        <v>499</v>
-      </c>
-      <c r="H45" s="11"/>
-    </row>
-    <row r="46" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="G45" s="8" t="s">
+        <v>493</v>
+      </c>
+      <c r="H45" s="19"/>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B46" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C46" t="s">
         <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>51</v>
+        <v>16</v>
       </c>
       <c r="E46" t="s">
         <v>17</v>
       </c>
-      <c r="F46" t="s">
-        <v>18</v>
-      </c>
       <c r="G46" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="H46" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
+      </c>
+      <c r="H46" s="19" t="s">
+        <v>494</v>
       </c>
       <c r="I46" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="J46">
-        <v>-3</v>
+        <v>0.35</v>
       </c>
       <c r="K46">
-        <v>3</v>
-      </c>
-      <c r="L46">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="47" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+        <v>0.7</v>
+      </c>
+      <c r="M46" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B47" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C47" t="s">
         <v>50</v>
@@ -6489,131 +6532,121 @@
       <c r="E47" t="s">
         <v>17</v>
       </c>
-      <c r="F47" t="s">
-        <v>18</v>
-      </c>
       <c r="G47" s="19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="H47" s="11" t="s">
-        <v>500</v>
+        <v>523</v>
       </c>
       <c r="I47" t="s">
         <v>108</v>
       </c>
       <c r="J47">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K47">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+        <v>15</v>
+      </c>
+      <c r="M47">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B48" t="s">
-        <v>120</v>
-      </c>
-      <c r="C48" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" t="s">
-        <v>51</v>
+        <v>521</v>
       </c>
       <c r="E48" t="s">
         <v>17</v>
       </c>
-      <c r="F48" s="8" t="s">
-        <v>121</v>
-      </c>
       <c r="G48" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H48" s="19" t="s">
-        <v>501</v>
-      </c>
-      <c r="I48" t="s">
-        <v>124</v>
-      </c>
-      <c r="M48" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+        <v>522</v>
+      </c>
+      <c r="H48" s="11" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B49" t="s">
-        <v>126</v>
-      </c>
-      <c r="C49" t="s">
-        <v>50</v>
-      </c>
-      <c r="D49" t="s">
-        <v>51</v>
+        <v>447</v>
       </c>
       <c r="E49" t="s">
         <v>17</v>
       </c>
-      <c r="F49" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G49" s="19"/>
-      <c r="H49" s="19"/>
-    </row>
-    <row r="50" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="G49" s="19" t="s">
+        <v>495</v>
+      </c>
+      <c r="H49" s="11"/>
+    </row>
+    <row r="50" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B50" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C50" t="s">
         <v>50</v>
       </c>
       <c r="D50" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E50" t="s">
         <v>17</v>
       </c>
+      <c r="F50" t="s">
+        <v>18</v>
+      </c>
       <c r="G50" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="H50" s="19" t="s">
-        <v>502</v>
+        <v>116</v>
+      </c>
+      <c r="H50" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="I50" t="s">
-        <v>454</v>
-      </c>
-      <c r="M50">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="51" spans="2:13" x14ac:dyDescent="0.6">
+        <v>108</v>
+      </c>
+      <c r="J50">
+        <v>-3</v>
+      </c>
+      <c r="K50">
+        <v>3</v>
+      </c>
+      <c r="L50">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B51" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C51" t="s">
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E51" t="s">
-        <v>59</v>
-      </c>
-      <c r="G51" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="H51" s="19" t="s">
-        <v>101</v>
+        <v>17</v>
+      </c>
+      <c r="F51" t="s">
+        <v>18</v>
+      </c>
+      <c r="G51" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H51" s="11" t="s">
+        <v>496</v>
       </c>
       <c r="I51" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="J51">
         <v>0</v>
       </c>
       <c r="K51">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="2:13" x14ac:dyDescent="0.6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B52" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="C52" t="s">
         <v>50</v>
@@ -6624,28 +6657,25 @@
       <c r="E52" t="s">
         <v>17</v>
       </c>
-      <c r="G52" s="8" t="s">
-        <v>503</v>
-      </c>
-      <c r="H52" s="11" t="s">
-        <v>504</v>
+      <c r="F52" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G52" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="H52" s="19" t="s">
+        <v>497</v>
       </c>
       <c r="I52" t="s">
-        <v>102</v>
-      </c>
-      <c r="J52">
-        <v>0</v>
-      </c>
-      <c r="K52">
-        <v>4.2</v>
-      </c>
-      <c r="M52">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="53" spans="2:13" x14ac:dyDescent="0.6">
+        <v>124</v>
+      </c>
+      <c r="M52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B53" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C53" t="s">
         <v>50</v>
@@ -6656,46 +6686,81 @@
       <c r="E53" t="s">
         <v>17</v>
       </c>
-      <c r="F53" t="s">
-        <v>33</v>
-      </c>
-      <c r="G53" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H53" s="11"/>
-    </row>
-    <row r="54" spans="2:13" x14ac:dyDescent="0.6">
-      <c r="G54" s="8"/>
-      <c r="H54" s="11"/>
-    </row>
-    <row r="55" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="F53" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G53" s="19"/>
+      <c r="H53" s="19"/>
+    </row>
+    <row r="54" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B54" t="s">
+        <v>127</v>
+      </c>
+      <c r="C54" t="s">
+        <v>50</v>
+      </c>
+      <c r="D54" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" t="s">
+        <v>17</v>
+      </c>
+      <c r="G54" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="H54" s="19" t="s">
+        <v>498</v>
+      </c>
+      <c r="I54" t="s">
+        <v>454</v>
+      </c>
+      <c r="M54">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B55" t="s">
-        <v>137</v>
-      </c>
-      <c r="C55" t="s">
+        <v>525</v>
+      </c>
+      <c r="G55" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="H55" s="19" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="56" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="B56" t="s">
+        <v>130</v>
+      </c>
+      <c r="C56" t="s">
         <v>50</v>
       </c>
-      <c r="D55" t="s">
-        <v>51</v>
-      </c>
-      <c r="E55" t="s">
-        <v>17</v>
-      </c>
-      <c r="F55" t="s">
-        <v>33</v>
-      </c>
-      <c r="G55" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H55" s="11"/>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.6">
-      <c r="G56" s="8"/>
-      <c r="H56" s="11"/>
+      <c r="D56" t="s">
+        <v>16</v>
+      </c>
+      <c r="E56" t="s">
+        <v>59</v>
+      </c>
+      <c r="G56" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="H56" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="I56" t="s">
+        <v>132</v>
+      </c>
+      <c r="J56">
+        <v>0</v>
+      </c>
+      <c r="K56">
+        <v>4</v>
+      </c>
     </row>
     <row r="57" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B57" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="C57" t="s">
         <v>50</v>
@@ -6706,283 +6771,396 @@
       <c r="E57" t="s">
         <v>17</v>
       </c>
-      <c r="F57" t="s">
-        <v>18</v>
-      </c>
-      <c r="G57" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="H57" s="11"/>
-    </row>
-    <row r="58" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="G57" s="8" t="s">
+        <v>499</v>
+      </c>
+      <c r="H57" s="11" t="s">
+        <v>500</v>
+      </c>
+      <c r="I57" t="s">
+        <v>102</v>
+      </c>
+      <c r="J57">
+        <v>0</v>
+      </c>
+      <c r="K57">
+        <v>4.2</v>
+      </c>
+      <c r="M57">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="58" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B58" t="s">
-        <v>141</v>
-      </c>
-      <c r="C58" t="s">
+        <v>528</v>
+      </c>
+      <c r="E58" t="s">
+        <v>17</v>
+      </c>
+      <c r="G58" s="8" t="s">
+        <v>529</v>
+      </c>
+      <c r="H58" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="I58" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="59" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="B59" t="s">
+        <v>135</v>
+      </c>
+      <c r="C59" t="s">
         <v>50</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D59" t="s">
         <v>51</v>
       </c>
-      <c r="E58" t="s">
-        <v>17</v>
-      </c>
-      <c r="F58" t="s">
-        <v>18</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="H58" s="11"/>
-    </row>
-    <row r="60" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B60" t="s">
-        <v>15</v>
-      </c>
-      <c r="D60" t="s">
-        <v>16</v>
-      </c>
-      <c r="E60" t="s">
-        <v>17</v>
-      </c>
-      <c r="F60" t="s">
-        <v>18</v>
-      </c>
-      <c r="G60" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H60" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="I60" t="s">
-        <v>21</v>
-      </c>
-      <c r="J60">
-        <v>0.01</v>
-      </c>
-      <c r="K60">
-        <v>60</v>
-      </c>
-      <c r="L60">
-        <v>0.01</v>
-      </c>
-      <c r="M60">
-        <v>60</v>
-      </c>
+      <c r="E59" t="s">
+        <v>17</v>
+      </c>
+      <c r="F59" t="s">
+        <v>33</v>
+      </c>
+      <c r="G59" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="H59" s="11"/>
+    </row>
+    <row r="60" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="G60" s="8"/>
+      <c r="H60" s="11"/>
     </row>
     <row r="61" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B61" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" t="s">
+        <v>50</v>
+      </c>
+      <c r="D61" t="s">
+        <v>51</v>
+      </c>
+      <c r="E61" t="s">
+        <v>17</v>
+      </c>
+      <c r="F61" t="s">
+        <v>33</v>
+      </c>
+      <c r="G61" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H61" s="11" t="s">
+        <v>531</v>
+      </c>
+      <c r="J61">
+        <v>0</v>
+      </c>
+      <c r="K61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="G62" s="8"/>
+      <c r="H62" s="11"/>
+    </row>
+    <row r="63" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="B63" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" t="s">
+        <v>50</v>
+      </c>
+      <c r="D63" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63" t="s">
+        <v>17</v>
+      </c>
+      <c r="F63" t="s">
+        <v>18</v>
+      </c>
+      <c r="G63" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="H63" s="11"/>
+    </row>
+    <row r="64" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="B64" t="s">
+        <v>141</v>
+      </c>
+      <c r="C64" t="s">
+        <v>50</v>
+      </c>
+      <c r="D64" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64" t="s">
+        <v>17</v>
+      </c>
+      <c r="F64" t="s">
+        <v>18</v>
+      </c>
+      <c r="G64" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="H64" s="11"/>
+    </row>
+    <row r="66" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
+        <v>17</v>
+      </c>
+      <c r="F66" t="s">
+        <v>18</v>
+      </c>
+      <c r="G66" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H66" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="I66" t="s">
+        <v>21</v>
+      </c>
+      <c r="J66">
+        <v>0.01</v>
+      </c>
+      <c r="K66">
+        <v>60</v>
+      </c>
+      <c r="L66">
+        <v>0.01</v>
+      </c>
+      <c r="M66">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="B67" t="s">
         <v>22</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D67" t="s">
         <v>16</v>
       </c>
-      <c r="E61" t="s">
-        <v>17</v>
-      </c>
-      <c r="F61" s="8" t="s">
+      <c r="E67" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G61" s="8" t="s">
+      <c r="G67" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H61" s="27" t="s">
-        <v>506</v>
-      </c>
-      <c r="I61" t="s">
+      <c r="H67" s="27" t="s">
+        <v>502</v>
+      </c>
+      <c r="I67" t="s">
         <v>21</v>
       </c>
-      <c r="J61" t="s">
+      <c r="J67" t="s">
         <v>26</v>
       </c>
-      <c r="K61" t="s">
+      <c r="K67" t="s">
         <v>26</v>
       </c>
-      <c r="L61" t="s">
+      <c r="L67" t="s">
         <v>26</v>
       </c>
-      <c r="M61" t="s">
+      <c r="M67" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.6">
-      <c r="B62" t="s">
-        <v>27</v>
-      </c>
-      <c r="D62" t="s">
-        <v>16</v>
-      </c>
-      <c r="E62" t="s">
-        <v>17</v>
-      </c>
-      <c r="F62" t="s">
-        <v>18</v>
-      </c>
-      <c r="G62" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H62" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="I62" t="s">
-        <v>21</v>
-      </c>
-      <c r="J62">
-        <v>0.01</v>
-      </c>
-      <c r="K62">
-        <v>60</v>
-      </c>
-      <c r="L62">
-        <v>0.01</v>
-      </c>
-      <c r="M62">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="63" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B63" t="s">
-        <v>509</v>
-      </c>
-      <c r="D63" t="s">
-        <v>16</v>
-      </c>
-      <c r="E63" t="s">
-        <v>17</v>
-      </c>
-      <c r="F63" t="s">
-        <v>33</v>
-      </c>
-      <c r="G63" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H63" s="8" t="s">
-        <v>510</v>
-      </c>
-      <c r="J63" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="K63" s="48"/>
-      <c r="M63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B64" t="s">
-        <v>508</v>
-      </c>
-      <c r="D64" t="s">
-        <v>16</v>
-      </c>
-      <c r="E64" t="s">
-        <v>17</v>
-      </c>
-      <c r="F64" t="s">
-        <v>33</v>
-      </c>
-      <c r="G64" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H64" s="27" t="s">
-        <v>511</v>
-      </c>
-      <c r="J64" s="48" t="s">
-        <v>36</v>
-      </c>
-      <c r="K64" s="48"/>
-      <c r="M64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B65" t="s">
-        <v>40</v>
-      </c>
-      <c r="D65" t="s">
-        <v>16</v>
-      </c>
-      <c r="E65" t="s">
-        <v>17</v>
-      </c>
-      <c r="F65" t="s">
-        <v>18</v>
-      </c>
-      <c r="G65" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H65" s="8" t="s">
-        <v>512</v>
-      </c>
-      <c r="I65" t="s">
-        <v>21</v>
-      </c>
-      <c r="J65">
-        <v>0.01</v>
-      </c>
-      <c r="K65">
-        <v>60</v>
-      </c>
-      <c r="L65">
-        <v>0.01</v>
-      </c>
-      <c r="M65">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="66" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B66" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C66" s="35"/>
-      <c r="D66" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E66" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="F66" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G66" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="H66" s="36" t="s">
-        <v>513</v>
-      </c>
-      <c r="I66" s="35"/>
-      <c r="J66" s="35"/>
-      <c r="K66" s="35"/>
-      <c r="L66" s="35"/>
-      <c r="M66" s="35"/>
     </row>
     <row r="68" spans="2:13" x14ac:dyDescent="0.6">
       <c r="B68" t="s">
-        <v>514</v>
-      </c>
-      <c r="C68" t="s">
+        <v>27</v>
+      </c>
+      <c r="D68" t="s">
+        <v>16</v>
+      </c>
+      <c r="E68" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" t="s">
+        <v>18</v>
+      </c>
+      <c r="G68" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H68" s="8" t="s">
+        <v>503</v>
+      </c>
+      <c r="I68" t="s">
+        <v>21</v>
+      </c>
+      <c r="J68">
+        <v>0.01</v>
+      </c>
+      <c r="K68">
+        <v>60</v>
+      </c>
+      <c r="L68">
+        <v>0.01</v>
+      </c>
+      <c r="M68">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B69" t="s">
+        <v>505</v>
+      </c>
+      <c r="D69" t="s">
+        <v>16</v>
+      </c>
+      <c r="E69" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" t="s">
+        <v>33</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="J69" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="K69" s="40"/>
+      <c r="M69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B70" t="s">
+        <v>504</v>
+      </c>
+      <c r="D70" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" t="s">
+        <v>33</v>
+      </c>
+      <c r="G70" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H70" s="27" t="s">
+        <v>507</v>
+      </c>
+      <c r="J70" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="K70" s="40"/>
+      <c r="M70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B71" t="s">
+        <v>40</v>
+      </c>
+      <c r="D71" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H71" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="I71" t="s">
+        <v>21</v>
+      </c>
+      <c r="J71">
+        <v>0.01</v>
+      </c>
+      <c r="K71">
+        <v>60</v>
+      </c>
+      <c r="L71">
+        <v>0.01</v>
+      </c>
+      <c r="M71">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="72" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="B72" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C72" s="35"/>
+      <c r="D72" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G72" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="H72" s="36" t="s">
+        <v>532</v>
+      </c>
+      <c r="I72" s="35"/>
+      <c r="J72" s="35"/>
+      <c r="K72" s="35"/>
+      <c r="L72" s="35"/>
+      <c r="M72" s="35"/>
+    </row>
+    <row r="74" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="B74" t="s">
+        <v>509</v>
+      </c>
+      <c r="C74" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="69" spans="2:13" x14ac:dyDescent="0.6">
-      <c r="B69" t="s">
-        <v>515</v>
-      </c>
-      <c r="C69" t="s">
+    <row r="75" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="B75" t="s">
+        <v>510</v>
+      </c>
+      <c r="C75" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="70" spans="2:13" x14ac:dyDescent="0.6">
-      <c r="B70" t="s">
-        <v>516</v>
-      </c>
-      <c r="C70" t="s">
+    <row r="76" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="B76" t="s">
+        <v>511</v>
+      </c>
+      <c r="C76" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J63:K63"/>
-    <mergeCell ref="J64:K64"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="J69:K69"/>
+    <mergeCell ref="J70:K70"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="G1:G2"/>
@@ -6991,12 +7169,6 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7266,38 +7438,38 @@
       <c r="D1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="50" t="s">
+      <c r="E1" s="67" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="51"/>
-      <c r="G1" s="50" t="s">
+      <c r="F1" s="68"/>
+      <c r="G1" s="67" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="51"/>
+      <c r="H1" s="68"/>
     </row>
     <row r="2" spans="1:8" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="69" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="54"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="71"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="3"/>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="50" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="56"/>
-      <c r="D3" s="56"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="56"/>
-      <c r="G3" s="56"/>
-      <c r="H3" s="57"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="52"/>
     </row>
     <row r="4" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="4">
@@ -7307,12 +7479,12 @@
         <v>370</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60" t="s">
+      <c r="D4" s="59"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="61"/>
+      <c r="G4" s="58"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7323,12 +7495,12 @@
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="62" t="s">
+      <c r="D5" s="55"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="53" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="63"/>
+      <c r="G5" s="54"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7339,12 +7511,12 @@
         <v>372</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60" t="s">
+      <c r="D6" s="59"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="61"/>
+      <c r="G6" s="58"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7355,12 +7527,12 @@
         <v>373</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="62" t="s">
+      <c r="D7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="53" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="63"/>
+      <c r="G7" s="54"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7371,12 +7543,12 @@
         <v>53</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60" t="s">
+      <c r="D8" s="59"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="57" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="61"/>
+      <c r="G8" s="58"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -7387,25 +7559,25 @@
         <v>374</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="65"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="56"/>
       <c r="H9" s="6" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="5"/>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="64" t="s">
         <v>376</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="68"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="66"/>
     </row>
     <row r="11" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A11" s="6">
@@ -7417,12 +7589,12 @@
       <c r="C11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="62" t="s">
+      <c r="D11" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E11" s="63"/>
-      <c r="F11" s="64"/>
-      <c r="G11" s="65"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="56"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7435,12 +7607,12 @@
       <c r="C12" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D12" s="60" t="s">
+      <c r="D12" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E12" s="61"/>
-      <c r="F12" s="58"/>
-      <c r="G12" s="59"/>
+      <c r="E12" s="58"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7453,12 +7625,12 @@
       <c r="C13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="62" t="s">
+      <c r="D13" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="63"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="65"/>
+      <c r="E13" s="54"/>
+      <c r="F13" s="55"/>
+      <c r="G13" s="56"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7469,12 +7641,12 @@
         <v>380</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="60" t="s">
+      <c r="D14" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="61"/>
-      <c r="F14" s="58"/>
-      <c r="G14" s="59"/>
+      <c r="E14" s="58"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7487,12 +7659,12 @@
       <c r="C15" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="62" t="s">
+      <c r="D15" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="64"/>
-      <c r="G15" s="65"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7505,12 +7677,12 @@
       <c r="C16" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D16" s="60" t="s">
+      <c r="D16" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="61"/>
-      <c r="F16" s="58"/>
-      <c r="G16" s="59"/>
+      <c r="E16" s="58"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -7523,12 +7695,12 @@
       <c r="C17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D17" s="62" t="s">
+      <c r="D17" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="63"/>
-      <c r="F17" s="64"/>
-      <c r="G17" s="65"/>
+      <c r="E17" s="54"/>
+      <c r="F17" s="55"/>
+      <c r="G17" s="56"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7541,12 +7713,12 @@
       <c r="C18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D18" s="60" t="s">
+      <c r="D18" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="61"/>
-      <c r="F18" s="58"/>
-      <c r="G18" s="59"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="60"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7559,12 +7731,12 @@
       <c r="C19" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="D19" s="62" t="s">
+      <c r="D19" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="64"/>
-      <c r="G19" s="65"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="55"/>
+      <c r="G19" s="56"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7577,12 +7749,12 @@
       <c r="C20" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="60" t="s">
+      <c r="D20" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E20" s="61"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="59"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="60"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="117.3" thickBot="1" x14ac:dyDescent="0.65">
@@ -7595,12 +7767,12 @@
       <c r="C21" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="62" t="s">
+      <c r="D21" s="53" t="s">
         <v>378</v>
       </c>
-      <c r="E21" s="63"/>
-      <c r="F21" s="64"/>
-      <c r="G21" s="65"/>
+      <c r="E21" s="54"/>
+      <c r="F21" s="55"/>
+      <c r="G21" s="56"/>
       <c r="H21" s="6" t="s">
         <v>389</v>
       </c>
@@ -7615,12 +7787,12 @@
       <c r="C22" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="60" t="s">
+      <c r="D22" s="57" t="s">
         <v>378</v>
       </c>
-      <c r="E22" s="61"/>
-      <c r="F22" s="58"/>
-      <c r="G22" s="59"/>
+      <c r="E22" s="58"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="60"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -7645,13 +7817,13 @@
     </row>
     <row r="24" spans="1:8" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A24" s="7"/>
-      <c r="B24" s="69" t="s">
+      <c r="B24" s="61" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="70"/>
-      <c r="D24" s="70"/>
-      <c r="E24" s="70"/>
-      <c r="F24" s="71"/>
+      <c r="C24" s="62"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="62"/>
+      <c r="F24" s="63"/>
     </row>
     <row r="25" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A25" s="6">
@@ -7719,13 +7891,13 @@
     </row>
     <row r="29" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A29" s="3"/>
-      <c r="B29" s="55" t="s">
+      <c r="B29" s="50" t="s">
         <v>396</v>
       </c>
-      <c r="C29" s="56"/>
-      <c r="D29" s="56"/>
-      <c r="E29" s="56"/>
-      <c r="F29" s="57"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="51"/>
+      <c r="F29" s="52"/>
     </row>
     <row r="30" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A30" s="4">
@@ -7883,13 +8055,13 @@
     </row>
     <row r="41" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A41" s="3"/>
-      <c r="B41" s="55" t="s">
+      <c r="B41" s="50" t="s">
         <v>408</v>
       </c>
-      <c r="C41" s="56"/>
-      <c r="D41" s="56"/>
-      <c r="E41" s="56"/>
-      <c r="F41" s="57"/>
+      <c r="C41" s="51"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="52"/>
     </row>
     <row r="42" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A42" s="4">
@@ -7963,31 +8135,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="D5:E5"/>
@@ -8001,12 +8154,31 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -8298,19 +8470,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
-    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8625,22 +8790,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
+    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8666,9 +8834,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
time period for continue reading
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\astrocomb\KeckLFC-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90CFA7A3-CB64-4603-AE83-4AB355E99FC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E04CF5-D0EC-4324-8728-F8FAC89799A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="810" windowWidth="17280" windowHeight="10620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSF EO Comb" sheetId="1" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1302" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="534">
   <si>
     <t>Keyword</t>
   </si>
@@ -1678,6 +1678,9 @@
   </si>
   <si>
     <t>more detail below</t>
+  </si>
+  <si>
+    <t>time period(unit:s)</t>
   </si>
 </sst>
 </file>
@@ -2161,18 +2164,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2181,6 +2172,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2194,6 +2191,27 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2201,6 +2219,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2215,27 +2245,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2245,19 +2254,13 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -2636,68 +2639,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="42" t="s">
+      <c r="K1" s="41"/>
+      <c r="L1" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="42" t="s">
+      <c r="N1" s="41"/>
+      <c r="O1" s="43" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="43"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="43"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="44"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
@@ -2850,10 +2853,10 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="41" t="s">
+      <c r="J7" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="41"/>
+      <c r="K7" s="49"/>
       <c r="M7">
         <v>0</v>
       </c>
@@ -2880,10 +2883,10 @@
       <c r="H8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="41"/>
+      <c r="K8" s="49"/>
       <c r="M8">
         <v>0</v>
       </c>
@@ -2947,7 +2950,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="40" t="s">
+      <c r="A11" s="50" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
@@ -2971,13 +2974,13 @@
       <c r="H11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="41" t="s">
+      <c r="J11" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="41"/>
+      <c r="K11" s="49"/>
     </row>
     <row r="12" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A12" s="40"/>
+      <c r="A12" s="50"/>
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -2999,10 +3002,10 @@
       <c r="H12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="41" t="s">
+      <c r="J12" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="41"/>
+      <c r="K12" s="49"/>
     </row>
     <row r="13" spans="1:19" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A13" s="31"/>
@@ -3867,7 +3870,7 @@
       <c r="H54" s="11"/>
     </row>
     <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A55" s="44" t="s">
+      <c r="A55" s="40" t="s">
         <v>153</v>
       </c>
       <c r="B55" t="s">
@@ -3877,7 +3880,7 @@
       <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A56" s="44"/>
+      <c r="A56" s="40"/>
       <c r="B56" t="s">
         <v>155</v>
       </c>
@@ -3885,7 +3888,7 @@
       <c r="H56" s="11"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A57" s="44"/>
+      <c r="A57" s="40"/>
       <c r="B57" t="s">
         <v>156</v>
       </c>
@@ -3893,7 +3896,7 @@
       <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A58" s="44"/>
+      <c r="A58" s="40"/>
       <c r="B58" t="s">
         <v>157</v>
       </c>
@@ -3901,7 +3904,7 @@
       <c r="H58" s="11"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A59" s="44"/>
+      <c r="A59" s="40"/>
       <c r="B59" t="s">
         <v>158</v>
       </c>
@@ -3909,7 +3912,7 @@
       <c r="H59" s="11"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A60" s="44"/>
+      <c r="A60" s="40"/>
       <c r="B60" t="s">
         <v>159</v>
       </c>
@@ -3917,7 +3920,7 @@
       <c r="H60" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A61" s="44"/>
+      <c r="A61" s="40"/>
       <c r="B61" t="s">
         <v>160</v>
       </c>
@@ -3930,7 +3933,7 @@
       <c r="H62" s="11"/>
     </row>
     <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="44" t="s">
+      <c r="A63" s="40" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
@@ -3940,7 +3943,7 @@
       <c r="H63" s="11"/>
     </row>
     <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A64" s="44"/>
+      <c r="A64" s="40"/>
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -3948,7 +3951,7 @@
       <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A65" s="44"/>
+      <c r="A65" s="40"/>
       <c r="B65" t="s">
         <v>164</v>
       </c>
@@ -3956,7 +3959,7 @@
       <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A66" s="44"/>
+      <c r="A66" s="40"/>
       <c r="B66" t="s">
         <v>165</v>
       </c>
@@ -3964,7 +3967,7 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A67" s="44"/>
+      <c r="A67" s="40"/>
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -3972,7 +3975,7 @@
       <c r="H67" s="11"/>
     </row>
     <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A68" s="44"/>
+      <c r="A68" s="40"/>
       <c r="B68" t="s">
         <v>167</v>
       </c>
@@ -3980,7 +3983,7 @@
       <c r="H68" s="11"/>
     </row>
     <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A69" s="44"/>
+      <c r="A69" s="40"/>
       <c r="B69" t="s">
         <v>168</v>
       </c>
@@ -5669,6 +5672,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A55:A61"/>
     <mergeCell ref="A63:A69"/>
     <mergeCell ref="M1:M2"/>
@@ -5685,11 +5693,6 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5705,8 +5708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60079DE2-3043-422E-90F3-3EEEEA14A1EF}">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="76" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="O75" sqref="O75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -5714,77 +5717,80 @@
     <col min="1" max="1" width="4.3984375" customWidth="1"/>
     <col min="2" max="2" width="21.3984375" customWidth="1"/>
     <col min="3" max="3" width="15.09765625" customWidth="1"/>
-    <col min="4" max="4" width="20.25" customWidth="1"/>
+    <col min="4" max="4" width="11.59765625" customWidth="1"/>
     <col min="5" max="5" width="10.34765625" customWidth="1"/>
-    <col min="7" max="7" width="36.046875" customWidth="1"/>
+    <col min="7" max="7" width="35.34765625" customWidth="1"/>
     <col min="8" max="8" width="28.796875" customWidth="1"/>
     <col min="9" max="9" width="9.09765625" customWidth="1"/>
     <col min="10" max="10" width="6.8984375" customWidth="1"/>
     <col min="11" max="11" width="8.5" customWidth="1"/>
-    <col min="13" max="13" width="18.6484375" customWidth="1"/>
+    <col min="13" max="13" width="26.44921875" customWidth="1"/>
+    <col min="14" max="14" width="15.296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="47"/>
-      <c r="B1" s="48" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="46" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="49" t="s">
+      <c r="G1" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="49" t="s">
+      <c r="H1" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="50" t="s">
+      <c r="I1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="45" t="s">
+      <c r="J1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="45"/>
-      <c r="L1" s="42" t="s">
+      <c r="K1" s="41"/>
+      <c r="L1" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="45" t="s">
+      <c r="M1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="45"/>
-      <c r="O1" s="42" t="s">
+      <c r="N1" s="41" t="s">
+        <v>533</v>
+      </c>
+      <c r="O1" s="43" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.6">
-      <c r="A2" s="48"/>
-      <c r="B2" s="48"/>
-      <c r="C2" s="48"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
+      <c r="A2" s="46"/>
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="47"/>
+      <c r="E2" s="46"/>
+      <c r="F2" s="46"/>
+      <c r="G2" s="47"/>
+      <c r="H2" s="47"/>
+      <c r="I2" s="48"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="43"/>
-      <c r="M2" s="46"/>
-      <c r="N2" s="46"/>
-      <c r="O2" s="43"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="44"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A3" s="17" t="s">
@@ -5805,6 +5811,11 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.6">
+      <c r="N4">
+        <v>120</v>
+      </c>
+    </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B5" t="s">
         <v>452</v>
@@ -5830,6 +5841,9 @@
       <c r="M5" t="s">
         <v>455</v>
       </c>
+      <c r="N5">
+        <v>120</v>
+      </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B6" t="s">
@@ -5856,6 +5870,9 @@
       <c r="M6" t="s">
         <v>443</v>
       </c>
+      <c r="N6">
+        <v>120</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B7" t="s">
@@ -5873,6 +5890,9 @@
       <c r="G7" t="s">
         <v>449</v>
       </c>
+      <c r="N7">
+        <v>120</v>
+      </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B8" t="s">
@@ -5890,6 +5910,9 @@
       <c r="G8" t="s">
         <v>451</v>
       </c>
+      <c r="N8">
+        <v>120</v>
+      </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B9" t="s">
@@ -5907,6 +5930,9 @@
       <c r="G9" t="s">
         <v>457</v>
       </c>
+      <c r="N9">
+        <v>120</v>
+      </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B10" t="s">
@@ -5927,6 +5953,9 @@
       <c r="H10" t="s">
         <v>460</v>
       </c>
+      <c r="N10">
+        <v>120</v>
+      </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B11" s="39" t="s">
@@ -5953,6 +5982,9 @@
       <c r="K11">
         <v>2</v>
       </c>
+      <c r="N11">
+        <v>120</v>
+      </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B12" t="s">
@@ -5973,6 +6005,9 @@
       <c r="H12" t="s">
         <v>468</v>
       </c>
+      <c r="N12">
+        <v>120</v>
+      </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B13" s="39" t="s">
@@ -5999,6 +6034,9 @@
       <c r="K13">
         <v>60</v>
       </c>
+      <c r="N13">
+        <v>120</v>
+      </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B14" t="s">
@@ -6025,6 +6063,9 @@
       <c r="K14">
         <v>60</v>
       </c>
+      <c r="N14">
+        <v>120</v>
+      </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B15" s="39" t="s">
@@ -6051,6 +6092,9 @@
       <c r="K15">
         <v>60</v>
       </c>
+      <c r="N15">
+        <v>120</v>
+      </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.6">
       <c r="B16" t="s">
@@ -6068,8 +6112,16 @@
       <c r="G16" t="s">
         <v>477</v>
       </c>
-    </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" x14ac:dyDescent="0.6">
+      <c r="N19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B20" t="s">
         <v>481</v>
       </c>
@@ -6079,8 +6131,11 @@
       <c r="H20" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B21" t="s">
         <v>482</v>
       </c>
@@ -6090,43 +6145,64 @@
       <c r="H21" t="s">
         <v>480</v>
       </c>
-    </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B22" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="23" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B23" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="24" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B24" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B25" t="s">
         <v>485</v>
       </c>
-    </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B26" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B27" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B28" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="30" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="30" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B30" t="s">
         <v>77</v>
       </c>
@@ -6157,8 +6233,11 @@
       <c r="M30">
         <v>25</v>
       </c>
-    </row>
-    <row r="31" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="N30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B31" t="s">
         <v>81</v>
       </c>
@@ -6189,8 +6268,11 @@
       <c r="M31">
         <v>145</v>
       </c>
-    </row>
-    <row r="32" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="N31">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B32" t="s">
         <v>84</v>
       </c>
@@ -6221,8 +6303,11 @@
       <c r="M32">
         <v>630</v>
       </c>
-    </row>
-    <row r="33" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="N32">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B33" t="s">
         <v>511</v>
       </c>
@@ -6238,8 +6323,11 @@
       <c r="I33" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N33">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B34" t="s">
         <v>88</v>
       </c>
@@ -6259,8 +6347,11 @@
         <v>89</v>
       </c>
       <c r="H34" s="19"/>
-    </row>
-    <row r="35" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="N34">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B35" t="s">
         <v>444</v>
       </c>
@@ -6273,8 +6364,11 @@
       <c r="H35" s="19" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="36" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="N35">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B36" t="s">
         <v>90</v>
       </c>
@@ -6305,8 +6399,11 @@
       <c r="M36">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N36">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B37" t="s">
         <v>93</v>
       </c>
@@ -6326,8 +6423,11 @@
         <v>94</v>
       </c>
       <c r="H37" s="11"/>
-    </row>
-    <row r="38" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="N37">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="38" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B38" t="s">
         <v>95</v>
       </c>
@@ -6358,8 +6458,11 @@
       <c r="M38">
         <v>20</v>
       </c>
-    </row>
-    <row r="39" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="N38">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B39" t="s">
         <v>514</v>
       </c>
@@ -6372,8 +6475,11 @@
       <c r="H39" s="19" t="s">
         <v>515</v>
       </c>
-    </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N39">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B40" t="s">
         <v>97</v>
       </c>
@@ -6393,8 +6499,11 @@
         <v>98</v>
       </c>
       <c r="H40" s="11"/>
-    </row>
-    <row r="41" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="N40">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B41" t="s">
         <v>452</v>
       </c>
@@ -6404,8 +6513,11 @@
       <c r="H41" s="11" t="s">
         <v>516</v>
       </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N41">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B42" t="s">
         <v>99</v>
       </c>
@@ -6433,8 +6545,11 @@
       <c r="M42" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="43" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="N42">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B43" t="s">
         <v>105</v>
       </c>
@@ -6465,8 +6580,11 @@
       <c r="M43">
         <v>30</v>
       </c>
-    </row>
-    <row r="44" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="N43">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B44" t="s">
         <v>517</v>
       </c>
@@ -6479,8 +6597,11 @@
       <c r="H44" s="19" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="45" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N44">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B45" t="s">
         <v>450</v>
       </c>
@@ -6491,8 +6612,11 @@
         <v>492</v>
       </c>
       <c r="H45" s="19"/>
-    </row>
-    <row r="46" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N45">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B46" t="s">
         <v>109</v>
       </c>
@@ -6523,8 +6647,11 @@
       <c r="M46" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N46">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B47" t="s">
         <v>112</v>
       </c>
@@ -6555,8 +6682,11 @@
       <c r="M47">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="N47">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="48" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B48" t="s">
         <v>520</v>
       </c>
@@ -6569,8 +6699,11 @@
       <c r="H48" s="11" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="49" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N48">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B49" t="s">
         <v>447</v>
       </c>
@@ -6581,8 +6714,11 @@
         <v>494</v>
       </c>
       <c r="H49" s="11"/>
-    </row>
-    <row r="50" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="N49">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B50" t="s">
         <v>115</v>
       </c>
@@ -6616,8 +6752,11 @@
       <c r="L50">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="51" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="N50">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B51" t="s">
         <v>118</v>
       </c>
@@ -6648,8 +6787,11 @@
       <c r="K51">
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="N51">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B52" t="s">
         <v>120</v>
       </c>
@@ -6677,8 +6819,11 @@
       <c r="M52" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="53" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="N52">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B53" t="s">
         <v>126</v>
       </c>
@@ -6696,8 +6841,11 @@
       </c>
       <c r="G53" s="19"/>
       <c r="H53" s="19"/>
-    </row>
-    <row r="54" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="N53">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B54" t="s">
         <v>127</v>
       </c>
@@ -6722,8 +6870,11 @@
       <c r="M54">
         <v>135</v>
       </c>
-    </row>
-    <row r="55" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="N54">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B55" t="s">
         <v>524</v>
       </c>
@@ -6733,8 +6884,11 @@
       <c r="H55" s="19" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="56" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N55">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="56" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B56" t="s">
         <v>130</v>
       </c>
@@ -6762,8 +6916,11 @@
       <c r="K56">
         <v>4</v>
       </c>
-    </row>
-    <row r="57" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N56">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B57" t="s">
         <v>133</v>
       </c>
@@ -6794,8 +6951,11 @@
       <c r="M57">
         <v>3.6</v>
       </c>
-    </row>
-    <row r="58" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="N57">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B58" t="s">
         <v>527</v>
       </c>
@@ -6811,8 +6971,11 @@
       <c r="I58" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="59" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N58">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="59" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B59" t="s">
         <v>135</v>
       </c>
@@ -6832,12 +6995,18 @@
         <v>136</v>
       </c>
       <c r="H59" s="11"/>
-    </row>
-    <row r="60" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N59">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="2:14" x14ac:dyDescent="0.6">
       <c r="G60" s="8"/>
       <c r="H60" s="11"/>
-    </row>
-    <row r="61" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="N60">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B61" t="s">
         <v>137</v>
       </c>
@@ -6865,12 +7034,15 @@
       <c r="K61">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N61">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="62" spans="2:14" x14ac:dyDescent="0.6">
       <c r="G62" s="8"/>
       <c r="H62" s="11"/>
     </row>
-    <row r="63" spans="2:13" x14ac:dyDescent="0.6">
+    <row r="63" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B63" t="s">
         <v>139</v>
       </c>
@@ -6890,8 +7062,11 @@
         <v>140</v>
       </c>
       <c r="H63" s="11"/>
-    </row>
-    <row r="64" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B64" t="s">
         <v>141</v>
       </c>
@@ -6911,8 +7086,11 @@
         <v>142</v>
       </c>
       <c r="H64" s="11"/>
-    </row>
-    <row r="66" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="N64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B66" t="s">
         <v>15</v>
       </c>
@@ -6946,8 +7124,11 @@
       <c r="M66">
         <v>60</v>
       </c>
-    </row>
-    <row r="67" spans="2:13" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="N66">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="67" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B67" t="s">
         <v>22</v>
       </c>
@@ -6981,8 +7162,11 @@
       <c r="M67" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="68" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N67">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B68" t="s">
         <v>27</v>
       </c>
@@ -7016,8 +7200,11 @@
       <c r="M68">
         <v>60</v>
       </c>
-    </row>
-    <row r="69" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="N68">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="69" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B69" t="s">
         <v>504</v>
       </c>
@@ -7036,15 +7223,18 @@
       <c r="H69" s="8" t="s">
         <v>505</v>
       </c>
-      <c r="J69" s="41" t="s">
+      <c r="J69" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="K69" s="41"/>
+      <c r="K69" s="49"/>
       <c r="M69">
         <v>0</v>
       </c>
-    </row>
-    <row r="70" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="N69">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B70" t="s">
         <v>503</v>
       </c>
@@ -7063,15 +7253,18 @@
       <c r="H70" s="27" t="s">
         <v>506</v>
       </c>
-      <c r="J70" s="41" t="s">
+      <c r="J70" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="K70" s="41"/>
+      <c r="K70" s="49"/>
       <c r="M70">
         <v>0</v>
       </c>
-    </row>
-    <row r="71" spans="2:13" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="N70">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B71" t="s">
         <v>40</v>
       </c>
@@ -7105,8 +7298,11 @@
       <c r="M71">
         <v>60</v>
       </c>
-    </row>
-    <row r="72" spans="2:13" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="N71">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="72" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B72" s="35" t="s">
         <v>44</v>
       </c>
@@ -7131,8 +7327,11 @@
       <c r="K72" s="35"/>
       <c r="L72" s="35"/>
       <c r="M72" s="35"/>
-    </row>
-    <row r="74" spans="2:13" x14ac:dyDescent="0.6">
+      <c r="N72">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B74" t="s">
         <v>508</v>
       </c>
@@ -7140,7 +7339,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="75" spans="2:13" x14ac:dyDescent="0.6">
+    <row r="75" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B75" t="s">
         <v>509</v>
       </c>
@@ -7148,7 +7347,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="2:13" x14ac:dyDescent="0.6">
+    <row r="76" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B76" t="s">
         <v>510</v>
       </c>
@@ -7158,12 +7357,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
     <mergeCell ref="J69:K69"/>
     <mergeCell ref="J70:K70"/>
     <mergeCell ref="N1:N2"/>
@@ -7174,6 +7367,12 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7443,38 +7642,38 @@
       <c r="D1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="51" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="69"/>
-      <c r="G1" s="68" t="s">
+      <c r="F1" s="52"/>
+      <c r="G1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="69"/>
+      <c r="H1" s="52"/>
     </row>
     <row r="2" spans="1:8" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="70" t="s">
+      <c r="A2" s="53" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="71"/>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="71"/>
-      <c r="G2" s="71"/>
-      <c r="H2" s="72"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="55"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="3"/>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="56" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="52"/>
-      <c r="D3" s="52"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="53"/>
+      <c r="C3" s="57"/>
+      <c r="D3" s="57"/>
+      <c r="E3" s="57"/>
+      <c r="F3" s="57"/>
+      <c r="G3" s="57"/>
+      <c r="H3" s="58"/>
     </row>
     <row r="4" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="4">
@@ -7484,12 +7683,12 @@
         <v>370</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="58" t="s">
+      <c r="D4" s="59"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="59"/>
+      <c r="G4" s="62"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7500,12 +7699,12 @@
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="56"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="54" t="s">
+      <c r="D5" s="65"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="63" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="55"/>
+      <c r="G5" s="64"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7516,12 +7715,12 @@
         <v>372</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="61"/>
-      <c r="F6" s="58" t="s">
+      <c r="D6" s="59"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="59"/>
+      <c r="G6" s="62"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7532,12 +7731,12 @@
         <v>373</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="56"/>
-      <c r="E7" s="57"/>
-      <c r="F7" s="54" t="s">
+      <c r="D7" s="65"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="63" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="55"/>
+      <c r="G7" s="64"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7548,12 +7747,12 @@
         <v>53</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="58" t="s">
+      <c r="D8" s="59"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="61" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="59"/>
+      <c r="G8" s="62"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -7564,25 +7763,25 @@
         <v>374</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="57"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="65"/>
+      <c r="G9" s="66"/>
       <c r="H9" s="6" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="5"/>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="67" t="s">
         <v>376</v>
       </c>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="67"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="69"/>
     </row>
     <row r="11" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A11" s="6">
@@ -7594,12 +7793,12 @@
       <c r="C11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="63" t="s">
         <v>378</v>
       </c>
-      <c r="E11" s="55"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="57"/>
+      <c r="E11" s="64"/>
+      <c r="F11" s="65"/>
+      <c r="G11" s="66"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7612,12 +7811,12 @@
       <c r="C12" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="61" t="s">
         <v>378</v>
       </c>
-      <c r="E12" s="59"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="61"/>
+      <c r="E12" s="62"/>
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7630,12 +7829,12 @@
       <c r="C13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="54" t="s">
+      <c r="D13" s="63" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="55"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="57"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="65"/>
+      <c r="G13" s="66"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7646,12 +7845,12 @@
         <v>380</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="58" t="s">
+      <c r="D14" s="61" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="59"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="61"/>
+      <c r="E14" s="62"/>
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7664,12 +7863,12 @@
       <c r="C15" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="54" t="s">
+      <c r="D15" s="63" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="55"/>
-      <c r="F15" s="56"/>
-      <c r="G15" s="57"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="66"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7682,12 +7881,12 @@
       <c r="C16" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="D16" s="61" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="59"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61"/>
+      <c r="E16" s="62"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -7700,12 +7899,12 @@
       <c r="C17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="D17" s="63" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="55"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
+      <c r="E17" s="64"/>
+      <c r="F17" s="65"/>
+      <c r="G17" s="66"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7718,12 +7917,12 @@
       <c r="C18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D18" s="58" t="s">
+      <c r="D18" s="61" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="59"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="61"/>
+      <c r="E18" s="62"/>
+      <c r="F18" s="59"/>
+      <c r="G18" s="60"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7736,12 +7935,12 @@
       <c r="C19" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="D19" s="54" t="s">
+      <c r="D19" s="63" t="s">
         <v>378</v>
       </c>
-      <c r="E19" s="55"/>
-      <c r="F19" s="56"/>
-      <c r="G19" s="57"/>
+      <c r="E19" s="64"/>
+      <c r="F19" s="65"/>
+      <c r="G19" s="66"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7754,12 +7953,12 @@
       <c r="C20" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="58" t="s">
+      <c r="D20" s="61" t="s">
         <v>378</v>
       </c>
-      <c r="E20" s="59"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="61"/>
+      <c r="E20" s="62"/>
+      <c r="F20" s="59"/>
+      <c r="G20" s="60"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="117.3" thickBot="1" x14ac:dyDescent="0.65">
@@ -7772,12 +7971,12 @@
       <c r="C21" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="54" t="s">
+      <c r="D21" s="63" t="s">
         <v>378</v>
       </c>
-      <c r="E21" s="55"/>
-      <c r="F21" s="56"/>
-      <c r="G21" s="57"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="66"/>
       <c r="H21" s="6" t="s">
         <v>389</v>
       </c>
@@ -7792,12 +7991,12 @@
       <c r="C22" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="58" t="s">
+      <c r="D22" s="61" t="s">
         <v>378</v>
       </c>
-      <c r="E22" s="59"/>
-      <c r="F22" s="60"/>
-      <c r="G22" s="61"/>
+      <c r="E22" s="62"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="60"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -7822,13 +8021,13 @@
     </row>
     <row r="24" spans="1:8" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A24" s="7"/>
-      <c r="B24" s="62" t="s">
+      <c r="B24" s="70" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="64"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="72"/>
     </row>
     <row r="25" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A25" s="6">
@@ -7896,13 +8095,13 @@
     </row>
     <row r="29" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A29" s="3"/>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="56" t="s">
         <v>396</v>
       </c>
-      <c r="C29" s="52"/>
-      <c r="D29" s="52"/>
-      <c r="E29" s="52"/>
-      <c r="F29" s="53"/>
+      <c r="C29" s="57"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="57"/>
+      <c r="F29" s="58"/>
     </row>
     <row r="30" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A30" s="4">
@@ -8060,13 +8259,13 @@
     </row>
     <row r="41" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A41" s="3"/>
-      <c r="B41" s="51" t="s">
+      <c r="B41" s="56" t="s">
         <v>408</v>
       </c>
-      <c r="C41" s="52"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="53"/>
+      <c r="C41" s="57"/>
+      <c r="D41" s="57"/>
+      <c r="E41" s="57"/>
+      <c r="F41" s="58"/>
     </row>
     <row r="42" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A42" s="4">
@@ -8140,12 +8339,31 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="D5:E5"/>
@@ -8159,31 +8377,12 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -8475,12 +8674,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
+    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8795,25 +9001,22 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
-    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8839,13 +9042,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update keyword list for clarity function and close all funtion
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\astrocomb\KeckLFC-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E04CF5-D0EC-4324-8728-F8FAC89799A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF34AB2-3C0A-4F17-A2EF-1871D6274F49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1303" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="540">
   <si>
     <t>Keyword</t>
   </si>
@@ -1681,6 +1681,24 @@
   </si>
   <si>
     <t>time period(unit:s)</t>
+  </si>
+  <si>
+    <t>LFC_TEMP_MONITOR</t>
+  </si>
+  <si>
+    <t>LFC_CLOSE_ALL</t>
+  </si>
+  <si>
+    <t>none or 1</t>
+  </si>
+  <si>
+    <t>close device</t>
+  </si>
+  <si>
+    <t>get temp from all, if temp over threashold, run LFC_CLOSE_ALL</t>
+  </si>
+  <si>
+    <t>if value==1: close device in order: PTAMP, AMONIC23,AMONIC27, RFAMP, RFOSC, CLARITY</t>
   </si>
 </sst>
 </file>
@@ -2164,6 +2182,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2172,12 +2202,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2191,11 +2215,56 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2210,57 +2279,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -2639,68 +2657,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="45"/>
-      <c r="B1" s="46" t="s">
+      <c r="A1" s="47"/>
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="41"/>
-      <c r="L1" s="43" t="s">
+      <c r="K1" s="45"/>
+      <c r="L1" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="41"/>
-      <c r="O1" s="43" t="s">
+      <c r="N1" s="45"/>
+      <c r="O1" s="42" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="44"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="44"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="43"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
@@ -2853,10 +2871,10 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="49" t="s">
+      <c r="J7" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="49"/>
+      <c r="K7" s="41"/>
       <c r="M7">
         <v>0</v>
       </c>
@@ -2883,10 +2901,10 @@
       <c r="H8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="49" t="s">
+      <c r="J8" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="49"/>
+      <c r="K8" s="41"/>
       <c r="M8">
         <v>0</v>
       </c>
@@ -2950,7 +2968,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="40" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
@@ -2974,13 +2992,13 @@
       <c r="H11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="49" t="s">
+      <c r="J11" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="49"/>
+      <c r="K11" s="41"/>
     </row>
     <row r="12" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A12" s="50"/>
+      <c r="A12" s="40"/>
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -3002,10 +3020,10 @@
       <c r="H12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="49" t="s">
+      <c r="J12" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="49"/>
+      <c r="K12" s="41"/>
     </row>
     <row r="13" spans="1:19" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A13" s="31"/>
@@ -3870,7 +3888,7 @@
       <c r="H54" s="11"/>
     </row>
     <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A55" s="40" t="s">
+      <c r="A55" s="44" t="s">
         <v>153</v>
       </c>
       <c r="B55" t="s">
@@ -3880,7 +3898,7 @@
       <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A56" s="40"/>
+      <c r="A56" s="44"/>
       <c r="B56" t="s">
         <v>155</v>
       </c>
@@ -3888,7 +3906,7 @@
       <c r="H56" s="11"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A57" s="40"/>
+      <c r="A57" s="44"/>
       <c r="B57" t="s">
         <v>156</v>
       </c>
@@ -3896,7 +3914,7 @@
       <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A58" s="40"/>
+      <c r="A58" s="44"/>
       <c r="B58" t="s">
         <v>157</v>
       </c>
@@ -3904,7 +3922,7 @@
       <c r="H58" s="11"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A59" s="40"/>
+      <c r="A59" s="44"/>
       <c r="B59" t="s">
         <v>158</v>
       </c>
@@ -3912,7 +3930,7 @@
       <c r="H59" s="11"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A60" s="40"/>
+      <c r="A60" s="44"/>
       <c r="B60" t="s">
         <v>159</v>
       </c>
@@ -3920,7 +3938,7 @@
       <c r="H60" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A61" s="40"/>
+      <c r="A61" s="44"/>
       <c r="B61" t="s">
         <v>160</v>
       </c>
@@ -3933,7 +3951,7 @@
       <c r="H62" s="11"/>
     </row>
     <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="40" t="s">
+      <c r="A63" s="44" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
@@ -3943,7 +3961,7 @@
       <c r="H63" s="11"/>
     </row>
     <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A64" s="40"/>
+      <c r="A64" s="44"/>
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -3951,7 +3969,7 @@
       <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A65" s="40"/>
+      <c r="A65" s="44"/>
       <c r="B65" t="s">
         <v>164</v>
       </c>
@@ -3959,7 +3977,7 @@
       <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A66" s="40"/>
+      <c r="A66" s="44"/>
       <c r="B66" t="s">
         <v>165</v>
       </c>
@@ -3967,7 +3985,7 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A67" s="40"/>
+      <c r="A67" s="44"/>
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -3975,7 +3993,7 @@
       <c r="H67" s="11"/>
     </row>
     <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A68" s="40"/>
+      <c r="A68" s="44"/>
       <c r="B68" t="s">
         <v>167</v>
       </c>
@@ -3983,7 +4001,7 @@
       <c r="H68" s="11"/>
     </row>
     <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A69" s="40"/>
+      <c r="A69" s="44"/>
       <c r="B69" t="s">
         <v>168</v>
       </c>
@@ -5672,11 +5690,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A55:A61"/>
     <mergeCell ref="A63:A69"/>
     <mergeCell ref="M1:M2"/>
@@ -5693,6 +5706,11 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5706,10 +5724,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60079DE2-3043-422E-90F3-3EEEEA14A1EF}">
-  <dimension ref="A1:O76"/>
+  <dimension ref="A1:O78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" zoomScale="76" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O75" sqref="O75"/>
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -5729,68 +5747,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.6" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="45"/>
-      <c r="B1" s="46" t="s">
+      <c r="A1" s="47"/>
+      <c r="B1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="41"/>
-      <c r="L1" s="43" t="s">
+      <c r="K1" s="45"/>
+      <c r="L1" s="42" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="45" t="s">
         <v>533</v>
       </c>
-      <c r="O1" s="43" t="s">
+      <c r="O1" s="42" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.6">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="48"/>
+      <c r="F2" s="48"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="50"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="44"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="44"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="43"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.6">
       <c r="A3" s="17" t="s">
@@ -6116,42 +6134,52 @@
         <v>120</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.6">
+    <row r="19" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B19" t="s">
+        <v>534</v>
+      </c>
+      <c r="C19" t="s">
+        <v>456</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="G19" s="8" t="s">
+        <v>538</v>
+      </c>
       <c r="N19">
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B20" t="s">
-        <v>481</v>
+        <v>535</v>
+      </c>
+      <c r="C20" t="s">
+        <v>536</v>
+      </c>
+      <c r="E20" t="s">
+        <v>132</v>
       </c>
       <c r="G20" t="s">
-        <v>479</v>
-      </c>
-      <c r="H20" t="s">
-        <v>480</v>
+        <v>537</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>539</v>
       </c>
       <c r="N20">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.6">
-      <c r="B21" t="s">
-        <v>482</v>
-      </c>
-      <c r="G21" t="s">
-        <v>483</v>
-      </c>
-      <c r="H21" t="s">
-        <v>480</v>
-      </c>
-      <c r="N21">
-        <v>20</v>
+        <v>120</v>
       </c>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B22" t="s">
-        <v>253</v>
+        <v>481</v>
+      </c>
+      <c r="G22" t="s">
+        <v>479</v>
+      </c>
+      <c r="H22" t="s">
+        <v>480</v>
       </c>
       <c r="N22">
         <v>20</v>
@@ -6159,7 +6187,13 @@
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B23" t="s">
-        <v>255</v>
+        <v>482</v>
+      </c>
+      <c r="G23" t="s">
+        <v>483</v>
+      </c>
+      <c r="H23" t="s">
+        <v>480</v>
       </c>
       <c r="N23">
         <v>20</v>
@@ -6167,7 +6201,7 @@
     </row>
     <row r="24" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B24" t="s">
-        <v>484</v>
+        <v>253</v>
       </c>
       <c r="N24">
         <v>20</v>
@@ -6175,7 +6209,7 @@
     </row>
     <row r="25" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B25" t="s">
-        <v>485</v>
+        <v>255</v>
       </c>
       <c r="N25">
         <v>20</v>
@@ -6183,7 +6217,7 @@
     </row>
     <row r="26" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B26" t="s">
-        <v>273</v>
+        <v>484</v>
       </c>
       <c r="N26">
         <v>20</v>
@@ -6191,7 +6225,7 @@
     </row>
     <row r="27" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B27" t="s">
-        <v>275</v>
+        <v>485</v>
       </c>
       <c r="N27">
         <v>20</v>
@@ -6199,82 +6233,28 @@
     </row>
     <row r="28" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B28" t="s">
+        <v>273</v>
+      </c>
+      <c r="N28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" x14ac:dyDescent="0.6">
+      <c r="B29" t="s">
+        <v>275</v>
+      </c>
+      <c r="N29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" x14ac:dyDescent="0.6">
+      <c r="B30" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="30" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B30" t="s">
+    <row r="32" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B32" t="s">
         <v>77</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="I30" t="s">
-        <v>80</v>
-      </c>
-      <c r="J30">
-        <v>-5</v>
-      </c>
-      <c r="K30">
-        <v>75</v>
-      </c>
-      <c r="M30">
-        <v>25</v>
-      </c>
-      <c r="N30">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B31" t="s">
-        <v>81</v>
-      </c>
-      <c r="C31" t="s">
-        <v>50</v>
-      </c>
-      <c r="D31" t="s">
-        <v>51</v>
-      </c>
-      <c r="E31" t="s">
-        <v>17</v>
-      </c>
-      <c r="G31" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="I31" t="s">
-        <v>83</v>
-      </c>
-      <c r="J31" t="s">
-        <v>26</v>
-      </c>
-      <c r="K31" t="s">
-        <v>26</v>
-      </c>
-      <c r="M31">
-        <v>145</v>
-      </c>
-      <c r="N31">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="B32" t="s">
-        <v>84</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -6286,50 +6266,65 @@
         <v>17</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>486</v>
+        <v>79</v>
       </c>
       <c r="I32" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>-5</v>
       </c>
       <c r="K32">
-        <v>630</v>
+        <v>75</v>
       </c>
       <c r="M32">
-        <v>630</v>
+        <v>25</v>
       </c>
       <c r="N32">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B33" t="s">
-        <v>511</v>
+        <v>81</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
       </c>
       <c r="G33" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>512</v>
+        <v>79</v>
       </c>
       <c r="I33" t="s">
-        <v>442</v>
+        <v>83</v>
+      </c>
+      <c r="J33" t="s">
+        <v>26</v>
+      </c>
+      <c r="K33" t="s">
+        <v>26</v>
+      </c>
+      <c r="M33">
+        <v>145</v>
       </c>
       <c r="N33">
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.6">
+    <row r="34" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B34" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C34" t="s">
         <v>50</v>
@@ -6340,37 +6335,51 @@
       <c r="E34" t="s">
         <v>17</v>
       </c>
-      <c r="F34" t="s">
-        <v>33</v>
-      </c>
       <c r="G34" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="H34" s="19"/>
+        <v>85</v>
+      </c>
+      <c r="H34" s="19" t="s">
+        <v>486</v>
+      </c>
+      <c r="I34" t="s">
+        <v>87</v>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+      <c r="K34">
+        <v>630</v>
+      </c>
+      <c r="M34">
+        <v>630</v>
+      </c>
       <c r="N34">
         <v>120</v>
       </c>
     </row>
     <row r="35" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B35" t="s">
-        <v>444</v>
+        <v>511</v>
       </c>
       <c r="E35" t="s">
         <v>17</v>
       </c>
       <c r="G35" s="8" t="s">
-        <v>487</v>
+        <v>85</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>513</v>
+        <v>512</v>
+      </c>
+      <c r="I35" t="s">
+        <v>442</v>
       </c>
       <c r="N35">
         <v>120</v>
       </c>
     </row>
-    <row r="36" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="36" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B36" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C36" t="s">
         <v>50</v>
@@ -6381,55 +6390,37 @@
       <c r="E36" t="s">
         <v>17</v>
       </c>
+      <c r="F36" t="s">
+        <v>33</v>
+      </c>
       <c r="G36" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H36" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="I36" t="s">
-        <v>87</v>
-      </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36" t="s">
-        <v>92</v>
-      </c>
-      <c r="M36">
-        <v>20</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="H36" s="19"/>
       <c r="N36">
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.6">
+    <row r="37" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B37" t="s">
-        <v>93</v>
-      </c>
-      <c r="C37" t="s">
-        <v>50</v>
-      </c>
-      <c r="D37" t="s">
-        <v>51</v>
+        <v>444</v>
       </c>
       <c r="E37" t="s">
         <v>17</v>
       </c>
-      <c r="F37" t="s">
-        <v>33</v>
-      </c>
       <c r="G37" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H37" s="11"/>
+        <v>487</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>513</v>
+      </c>
       <c r="N37">
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="38" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B38" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C38" t="s">
         <v>50</v>
@@ -6441,10 +6432,10 @@
         <v>17</v>
       </c>
       <c r="G38" s="8" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H38" s="20" t="s">
-        <v>488</v>
+        <v>86</v>
       </c>
       <c r="I38" t="s">
         <v>87</v>
@@ -6462,26 +6453,33 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="39" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B39" t="s">
-        <v>514</v>
+        <v>93</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>51</v>
       </c>
       <c r="E39" t="s">
         <v>17</v>
       </c>
+      <c r="F39" t="s">
+        <v>33</v>
+      </c>
       <c r="G39" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="H39" s="19" t="s">
-        <v>515</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="H39" s="11"/>
       <c r="N39">
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.6">
+    <row r="40" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B40" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C40" t="s">
         <v>50</v>
@@ -6492,26 +6490,40 @@
       <c r="E40" t="s">
         <v>17</v>
       </c>
-      <c r="F40" t="s">
-        <v>33</v>
-      </c>
       <c r="G40" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H40" s="11"/>
+        <v>96</v>
+      </c>
+      <c r="H40" s="20" t="s">
+        <v>488</v>
+      </c>
+      <c r="I40" t="s">
+        <v>87</v>
+      </c>
+      <c r="J40">
+        <v>0</v>
+      </c>
+      <c r="K40" t="s">
+        <v>92</v>
+      </c>
+      <c r="M40">
+        <v>20</v>
+      </c>
       <c r="N40">
         <v>120</v>
       </c>
     </row>
     <row r="41" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B41" t="s">
-        <v>452</v>
+        <v>514</v>
+      </c>
+      <c r="E41" t="s">
+        <v>17</v>
       </c>
       <c r="G41" s="8" t="s">
-        <v>489</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>516</v>
+        <v>96</v>
+      </c>
+      <c r="H41" s="19" t="s">
+        <v>515</v>
       </c>
       <c r="N41">
         <v>120</v>
@@ -6519,133 +6531,121 @@
     </row>
     <row r="42" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B42" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C42" t="s">
         <v>50</v>
       </c>
       <c r="D42" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E42" t="s">
         <v>17</v>
       </c>
+      <c r="F42" t="s">
+        <v>33</v>
+      </c>
       <c r="G42" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="H42" s="19" t="s">
-        <v>490</v>
-      </c>
-      <c r="I42" t="s">
-        <v>102</v>
-      </c>
-      <c r="L42" t="s">
-        <v>103</v>
-      </c>
-      <c r="M42" t="s">
-        <v>104</v>
-      </c>
+        <v>98</v>
+      </c>
+      <c r="H42" s="11"/>
       <c r="N42">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="43" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B43" t="s">
-        <v>105</v>
-      </c>
-      <c r="C43" t="s">
-        <v>50</v>
-      </c>
-      <c r="D43" t="s">
-        <v>51</v>
-      </c>
-      <c r="E43" t="s">
-        <v>17</v>
+        <v>452</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="H43" s="19" t="s">
-        <v>491</v>
-      </c>
-      <c r="I43" t="s">
-        <v>108</v>
-      </c>
-      <c r="J43">
-        <v>30</v>
-      </c>
-      <c r="K43">
-        <v>30</v>
-      </c>
-      <c r="M43">
-        <v>30</v>
+        <v>489</v>
+      </c>
+      <c r="H43" s="11" t="s">
+        <v>516</v>
       </c>
       <c r="N43">
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="44" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B44" t="s">
-        <v>517</v>
+        <v>99</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>16</v>
       </c>
       <c r="E44" t="s">
         <v>17</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>518</v>
+        <v>100</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>519</v>
+        <v>490</v>
+      </c>
+      <c r="I44" t="s">
+        <v>102</v>
+      </c>
+      <c r="L44" t="s">
+        <v>103</v>
+      </c>
+      <c r="M44" t="s">
+        <v>104</v>
       </c>
       <c r="N44">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="2:14" x14ac:dyDescent="0.6">
+    <row r="45" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B45" t="s">
-        <v>450</v>
+        <v>105</v>
+      </c>
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+      <c r="D45" t="s">
+        <v>51</v>
       </c>
       <c r="E45" t="s">
         <v>17</v>
       </c>
       <c r="G45" s="8" t="s">
-        <v>492</v>
-      </c>
-      <c r="H45" s="19"/>
+        <v>106</v>
+      </c>
+      <c r="H45" s="19" t="s">
+        <v>491</v>
+      </c>
+      <c r="I45" t="s">
+        <v>108</v>
+      </c>
+      <c r="J45">
+        <v>30</v>
+      </c>
+      <c r="K45">
+        <v>30</v>
+      </c>
+      <c r="M45">
+        <v>30</v>
+      </c>
       <c r="N45">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.6">
+    <row r="46" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B46" t="s">
-        <v>109</v>
-      </c>
-      <c r="C46" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" t="s">
-        <v>16</v>
+        <v>517</v>
       </c>
       <c r="E46" t="s">
         <v>17</v>
       </c>
-      <c r="G46" s="19" t="s">
-        <v>110</v>
+      <c r="G46" s="8" t="s">
+        <v>518</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>493</v>
-      </c>
-      <c r="I46" t="s">
-        <v>102</v>
-      </c>
-      <c r="J46">
-        <v>0.35</v>
-      </c>
-      <c r="K46">
-        <v>0.7</v>
-      </c>
-      <c r="M46" t="s">
-        <v>111</v>
+        <v>519</v>
       </c>
       <c r="N46">
         <v>120</v>
@@ -6653,51 +6653,49 @@
     </row>
     <row r="47" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B47" t="s">
-        <v>112</v>
-      </c>
-      <c r="C47" t="s">
-        <v>50</v>
-      </c>
-      <c r="D47" t="s">
-        <v>51</v>
+        <v>450</v>
       </c>
       <c r="E47" t="s">
         <v>17</v>
       </c>
-      <c r="G47" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>522</v>
-      </c>
-      <c r="I47" t="s">
-        <v>108</v>
-      </c>
-      <c r="J47">
-        <v>15</v>
-      </c>
-      <c r="K47">
-        <v>15</v>
-      </c>
-      <c r="M47">
-        <v>15</v>
-      </c>
+      <c r="G47" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="H47" s="19"/>
       <c r="N47">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="48" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B48" t="s">
-        <v>520</v>
+        <v>109</v>
+      </c>
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
       </c>
       <c r="E48" t="s">
         <v>17</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>521</v>
-      </c>
-      <c r="H48" s="11" t="s">
-        <v>523</v>
+        <v>110</v>
+      </c>
+      <c r="H48" s="19" t="s">
+        <v>493</v>
+      </c>
+      <c r="I48" t="s">
+        <v>102</v>
+      </c>
+      <c r="J48">
+        <v>0.35</v>
+      </c>
+      <c r="K48">
+        <v>0.7</v>
+      </c>
+      <c r="M48" t="s">
+        <v>111</v>
       </c>
       <c r="N48">
         <v>120</v>
@@ -6705,95 +6703,74 @@
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B49" t="s">
-        <v>447</v>
+        <v>112</v>
+      </c>
+      <c r="C49" t="s">
+        <v>50</v>
+      </c>
+      <c r="D49" t="s">
+        <v>51</v>
       </c>
       <c r="E49" t="s">
         <v>17</v>
       </c>
       <c r="G49" s="19" t="s">
-        <v>494</v>
-      </c>
-      <c r="H49" s="11"/>
+        <v>113</v>
+      </c>
+      <c r="H49" s="11" t="s">
+        <v>522</v>
+      </c>
+      <c r="I49" t="s">
+        <v>108</v>
+      </c>
+      <c r="J49">
+        <v>15</v>
+      </c>
+      <c r="K49">
+        <v>15</v>
+      </c>
+      <c r="M49">
+        <v>15</v>
+      </c>
       <c r="N49">
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="50" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B50" t="s">
-        <v>115</v>
-      </c>
-      <c r="C50" t="s">
-        <v>50</v>
-      </c>
-      <c r="D50" t="s">
-        <v>51</v>
+        <v>520</v>
       </c>
       <c r="E50" t="s">
         <v>17</v>
       </c>
-      <c r="F50" t="s">
-        <v>18</v>
-      </c>
       <c r="G50" s="19" t="s">
-        <v>116</v>
+        <v>521</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="I50" t="s">
-        <v>108</v>
-      </c>
-      <c r="J50">
-        <v>-3</v>
-      </c>
-      <c r="K50">
-        <v>3</v>
-      </c>
-      <c r="L50">
-        <v>1E-3</v>
+        <v>523</v>
       </c>
       <c r="N50">
         <v>120</v>
       </c>
     </row>
-    <row r="51" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="51" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B51" t="s">
-        <v>118</v>
-      </c>
-      <c r="C51" t="s">
-        <v>50</v>
-      </c>
-      <c r="D51" t="s">
-        <v>51</v>
+        <v>447</v>
       </c>
       <c r="E51" t="s">
         <v>17</v>
       </c>
-      <c r="F51" t="s">
-        <v>18</v>
-      </c>
       <c r="G51" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>495</v>
-      </c>
-      <c r="I51" t="s">
-        <v>108</v>
-      </c>
-      <c r="J51">
-        <v>0</v>
-      </c>
-      <c r="K51">
-        <v>10</v>
-      </c>
+        <v>494</v>
+      </c>
+      <c r="H51" s="11"/>
       <c r="N51">
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="52" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B52" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C52" t="s">
         <v>50</v>
@@ -6804,28 +6781,34 @@
       <c r="E52" t="s">
         <v>17</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>121</v>
+      <c r="F52" t="s">
+        <v>18</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H52" s="19" t="s">
-        <v>496</v>
+        <v>116</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>117</v>
       </c>
       <c r="I52" t="s">
-        <v>124</v>
-      </c>
-      <c r="M52" t="s">
-        <v>125</v>
+        <v>108</v>
+      </c>
+      <c r="J52">
+        <v>-3</v>
+      </c>
+      <c r="K52">
+        <v>3</v>
+      </c>
+      <c r="L52">
+        <v>1E-3</v>
       </c>
       <c r="N52">
         <v>120</v>
       </c>
     </row>
-    <row r="53" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="53" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B53" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C53" t="s">
         <v>50</v>
@@ -6836,61 +6819,85 @@
       <c r="E53" t="s">
         <v>17</v>
       </c>
-      <c r="F53" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
+      <c r="F53" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="H53" s="11" t="s">
+        <v>495</v>
+      </c>
+      <c r="I53" t="s">
+        <v>108</v>
+      </c>
+      <c r="J53">
+        <v>0</v>
+      </c>
+      <c r="K53">
+        <v>10</v>
+      </c>
       <c r="N53">
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="54" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B54" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="C54" t="s">
         <v>50</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E54" t="s">
         <v>17</v>
       </c>
+      <c r="F54" s="8" t="s">
+        <v>121</v>
+      </c>
       <c r="G54" s="19" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H54" s="19" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I54" t="s">
-        <v>454</v>
-      </c>
-      <c r="M54">
-        <v>135</v>
+        <v>124</v>
+      </c>
+      <c r="M54" t="s">
+        <v>125</v>
       </c>
       <c r="N54">
         <v>120</v>
       </c>
     </row>
-    <row r="55" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="55" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B55" t="s">
-        <v>524</v>
-      </c>
-      <c r="G55" s="19" t="s">
-        <v>525</v>
-      </c>
-      <c r="H55" s="19" t="s">
-        <v>526</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="C55" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
       <c r="N55">
         <v>120</v>
       </c>
     </row>
-    <row r="56" spans="2:14" x14ac:dyDescent="0.6">
+    <row r="56" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B56" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C56" t="s">
         <v>50</v>
@@ -6899,77 +6906,65 @@
         <v>16</v>
       </c>
       <c r="E56" t="s">
-        <v>59</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>131</v>
+        <v>17</v>
+      </c>
+      <c r="G56" s="19" t="s">
+        <v>128</v>
       </c>
       <c r="H56" s="19" t="s">
-        <v>101</v>
+        <v>497</v>
       </c>
       <c r="I56" t="s">
-        <v>132</v>
-      </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
-      <c r="K56">
-        <v>4</v>
+        <v>454</v>
+      </c>
+      <c r="M56">
+        <v>135</v>
       </c>
       <c r="N56">
         <v>120</v>
       </c>
     </row>
-    <row r="57" spans="2:14" x14ac:dyDescent="0.6">
+    <row r="57" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B57" t="s">
-        <v>133</v>
-      </c>
-      <c r="C57" t="s">
-        <v>50</v>
-      </c>
-      <c r="D57" t="s">
-        <v>51</v>
-      </c>
-      <c r="E57" t="s">
-        <v>17</v>
-      </c>
-      <c r="G57" s="8" t="s">
-        <v>498</v>
-      </c>
-      <c r="H57" s="11" t="s">
-        <v>499</v>
-      </c>
-      <c r="I57" t="s">
-        <v>102</v>
-      </c>
-      <c r="J57">
-        <v>0</v>
-      </c>
-      <c r="K57">
-        <v>4.2</v>
-      </c>
-      <c r="M57">
-        <v>3.6</v>
+        <v>524</v>
+      </c>
+      <c r="G57" s="19" t="s">
+        <v>525</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>526</v>
       </c>
       <c r="N57">
         <v>120</v>
       </c>
     </row>
-    <row r="58" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="58" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B58" t="s">
-        <v>527</v>
+        <v>130</v>
+      </c>
+      <c r="C58" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" t="s">
+        <v>16</v>
       </c>
       <c r="E58" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>528</v>
-      </c>
-      <c r="H58" s="11" t="s">
-        <v>529</v>
+        <v>131</v>
+      </c>
+      <c r="H58" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="I58" t="s">
-        <v>102</v>
+        <v>132</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>4</v>
       </c>
       <c r="N58">
         <v>120</v>
@@ -6977,7 +6972,7 @@
     </row>
     <row r="59" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B59" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C59" t="s">
         <v>50</v>
@@ -6988,27 +6983,51 @@
       <c r="E59" t="s">
         <v>17</v>
       </c>
-      <c r="F59" t="s">
-        <v>33</v>
-      </c>
       <c r="G59" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="H59" s="11"/>
+        <v>498</v>
+      </c>
+      <c r="H59" s="11" t="s">
+        <v>499</v>
+      </c>
+      <c r="I59" t="s">
+        <v>102</v>
+      </c>
+      <c r="J59">
+        <v>0</v>
+      </c>
+      <c r="K59">
+        <v>4.2</v>
+      </c>
+      <c r="M59">
+        <v>3.6</v>
+      </c>
       <c r="N59">
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="2:14" x14ac:dyDescent="0.6">
-      <c r="G60" s="8"/>
-      <c r="H60" s="11"/>
+    <row r="60" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B60" t="s">
+        <v>527</v>
+      </c>
+      <c r="E60" t="s">
+        <v>17</v>
+      </c>
+      <c r="G60" s="8" t="s">
+        <v>528</v>
+      </c>
+      <c r="H60" s="11" t="s">
+        <v>529</v>
+      </c>
+      <c r="I60" t="s">
+        <v>102</v>
+      </c>
       <c r="N60">
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="61" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B61" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C61" t="s">
         <v>50</v>
@@ -7023,17 +7042,9 @@
         <v>33</v>
       </c>
       <c r="G61" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>530</v>
-      </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
-      <c r="K61">
-        <v>1</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="H61" s="11"/>
       <c r="N61">
         <v>120</v>
       </c>
@@ -7041,10 +7052,13 @@
     <row r="62" spans="2:14" x14ac:dyDescent="0.6">
       <c r="G62" s="8"/>
       <c r="H62" s="11"/>
-    </row>
-    <row r="63" spans="2:14" x14ac:dyDescent="0.6">
+      <c r="N62">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B63" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C63" t="s">
         <v>50</v>
@@ -7056,46 +7070,61 @@
         <v>17</v>
       </c>
       <c r="F63" t="s">
+        <v>33</v>
+      </c>
+      <c r="G63" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H63" s="11" t="s">
+        <v>530</v>
+      </c>
+      <c r="J63">
+        <v>0</v>
+      </c>
+      <c r="K63">
+        <v>1</v>
+      </c>
+      <c r="N63">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="64" spans="2:14" x14ac:dyDescent="0.6">
+      <c r="G64" s="8"/>
+      <c r="H64" s="11"/>
+    </row>
+    <row r="65" spans="2:14" x14ac:dyDescent="0.6">
+      <c r="B65" t="s">
+        <v>139</v>
+      </c>
+      <c r="C65" t="s">
+        <v>50</v>
+      </c>
+      <c r="D65" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" t="s">
         <v>18</v>
       </c>
-      <c r="G63" s="19" t="s">
+      <c r="G65" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="H63" s="11"/>
-      <c r="N63">
+      <c r="H65" s="11"/>
+      <c r="N65">
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="2:14" x14ac:dyDescent="0.6">
-      <c r="B64" t="s">
+    <row r="66" spans="2:14" x14ac:dyDescent="0.6">
+      <c r="B66" t="s">
         <v>141</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C66" t="s">
         <v>50</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D66" t="s">
         <v>51</v>
-      </c>
-      <c r="E64" t="s">
-        <v>17</v>
-      </c>
-      <c r="F64" t="s">
-        <v>18</v>
-      </c>
-      <c r="G64" s="19" t="s">
-        <v>142</v>
-      </c>
-      <c r="H64" s="11"/>
-      <c r="N64">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="66" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B66" t="s">
-        <v>15</v>
-      </c>
-      <c r="D66" t="s">
-        <v>16</v>
       </c>
       <c r="E66" t="s">
         <v>17</v>
@@ -7103,72 +7132,17 @@
       <c r="F66" t="s">
         <v>18</v>
       </c>
-      <c r="G66" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H66" s="8" t="s">
-        <v>500</v>
-      </c>
-      <c r="I66" t="s">
-        <v>21</v>
-      </c>
-      <c r="J66">
-        <v>0.01</v>
-      </c>
-      <c r="K66">
-        <v>60</v>
-      </c>
-      <c r="L66">
-        <v>0.01</v>
-      </c>
-      <c r="M66">
-        <v>60</v>
-      </c>
+      <c r="G66" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="H66" s="11"/>
       <c r="N66">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="67" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="B67" t="s">
-        <v>22</v>
-      </c>
-      <c r="D67" t="s">
-        <v>16</v>
-      </c>
-      <c r="E67" t="s">
-        <v>17</v>
-      </c>
-      <c r="F67" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G67" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H67" s="27" t="s">
-        <v>501</v>
-      </c>
-      <c r="I67" t="s">
-        <v>21</v>
-      </c>
-      <c r="J67" t="s">
-        <v>26</v>
-      </c>
-      <c r="K67" t="s">
-        <v>26</v>
-      </c>
-      <c r="L67" t="s">
-        <v>26</v>
-      </c>
-      <c r="M67" t="s">
-        <v>26</v>
-      </c>
-      <c r="N67">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="68" spans="2:14" x14ac:dyDescent="0.6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B68" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="D68" t="s">
         <v>16</v>
@@ -7180,10 +7154,10 @@
         <v>18</v>
       </c>
       <c r="G68" s="8" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H68" s="8" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="I68" t="s">
         <v>21</v>
@@ -7204,9 +7178,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="69" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="69" spans="2:14" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B69" t="s">
-        <v>504</v>
+        <v>22</v>
       </c>
       <c r="D69" t="s">
         <v>16</v>
@@ -7214,29 +7188,37 @@
       <c r="E69" t="s">
         <v>17</v>
       </c>
-      <c r="F69" t="s">
-        <v>33</v>
+      <c r="F69" s="8" t="s">
+        <v>23</v>
       </c>
       <c r="G69" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H69" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="J69" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="K69" s="49"/>
-      <c r="M69">
-        <v>0</v>
+        <v>24</v>
+      </c>
+      <c r="H69" s="27" t="s">
+        <v>501</v>
+      </c>
+      <c r="I69" t="s">
+        <v>21</v>
+      </c>
+      <c r="J69" t="s">
+        <v>26</v>
+      </c>
+      <c r="K69" t="s">
+        <v>26</v>
+      </c>
+      <c r="L69" t="s">
+        <v>26</v>
+      </c>
+      <c r="M69" t="s">
+        <v>26</v>
       </c>
       <c r="N69">
         <v>120</v>
       </c>
     </row>
-    <row r="70" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="70" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B70" t="s">
-        <v>503</v>
+        <v>27</v>
       </c>
       <c r="D70" t="s">
         <v>16</v>
@@ -7245,20 +7227,28 @@
         <v>17</v>
       </c>
       <c r="F70" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="G70" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H70" s="27" t="s">
-        <v>506</v>
-      </c>
-      <c r="J70" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="K70" s="49"/>
+        <v>28</v>
+      </c>
+      <c r="H70" s="8" t="s">
+        <v>502</v>
+      </c>
+      <c r="I70" t="s">
+        <v>21</v>
+      </c>
+      <c r="J70">
+        <v>0.01</v>
+      </c>
+      <c r="K70">
+        <v>60</v>
+      </c>
+      <c r="L70">
+        <v>0.01</v>
+      </c>
       <c r="M70">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="N70">
         <v>120</v>
@@ -7266,7 +7256,7 @@
     </row>
     <row r="71" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B71" t="s">
-        <v>40</v>
+        <v>504</v>
       </c>
       <c r="D71" t="s">
         <v>16</v>
@@ -7275,90 +7265,156 @@
         <v>17</v>
       </c>
       <c r="F71" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="G71" s="8" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="H71" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="I71" t="s">
-        <v>21</v>
-      </c>
-      <c r="J71">
-        <v>0.01</v>
-      </c>
-      <c r="K71">
-        <v>60</v>
-      </c>
-      <c r="L71">
-        <v>0.01</v>
-      </c>
+        <v>505</v>
+      </c>
+      <c r="J71" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="K71" s="41"/>
       <c r="M71">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="N71">
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="B72" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35" t="s">
+    <row r="72" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B72" t="s">
+        <v>503</v>
+      </c>
+      <c r="D72" t="s">
         <v>16</v>
       </c>
-      <c r="E72" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="F72" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G72" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="H72" s="36" t="s">
-        <v>531</v>
-      </c>
-      <c r="I72" s="35"/>
-      <c r="J72" s="35"/>
-      <c r="K72" s="35"/>
-      <c r="L72" s="35"/>
-      <c r="M72" s="35"/>
+      <c r="E72" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" t="s">
+        <v>33</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H72" s="27" t="s">
+        <v>506</v>
+      </c>
+      <c r="J72" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="K72" s="41"/>
+      <c r="M72">
+        <v>0</v>
+      </c>
       <c r="N72">
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="2:14" x14ac:dyDescent="0.6">
-      <c r="B74" t="s">
-        <v>508</v>
-      </c>
-      <c r="C74" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="75" spans="2:14" x14ac:dyDescent="0.6">
-      <c r="B75" t="s">
-        <v>509</v>
-      </c>
-      <c r="C75" t="s">
-        <v>26</v>
+    <row r="73" spans="2:14" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B73" t="s">
+        <v>40</v>
+      </c>
+      <c r="D73" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73" t="s">
+        <v>18</v>
+      </c>
+      <c r="G73" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="H73" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="I73" t="s">
+        <v>21</v>
+      </c>
+      <c r="J73">
+        <v>0.01</v>
+      </c>
+      <c r="K73">
+        <v>60</v>
+      </c>
+      <c r="L73">
+        <v>0.01</v>
+      </c>
+      <c r="M73">
+        <v>60</v>
+      </c>
+      <c r="N73">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="2:14" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="B74" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="C74" s="35"/>
+      <c r="D74" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F74" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="G74" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="H74" s="36" t="s">
+        <v>531</v>
+      </c>
+      <c r="I74" s="35"/>
+      <c r="J74" s="35"/>
+      <c r="K74" s="35"/>
+      <c r="L74" s="35"/>
+      <c r="M74" s="35"/>
+      <c r="N74">
+        <v>120</v>
       </c>
     </row>
     <row r="76" spans="2:14" x14ac:dyDescent="0.6">
       <c r="B76" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="C76" t="s">
         <v>26</v>
       </c>
     </row>
+    <row r="77" spans="2:14" x14ac:dyDescent="0.6">
+      <c r="B77" t="s">
+        <v>509</v>
+      </c>
+      <c r="C77" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="2:14" x14ac:dyDescent="0.6">
+      <c r="B78" t="s">
+        <v>510</v>
+      </c>
+      <c r="C78" t="s">
+        <v>26</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="J69:K69"/>
-    <mergeCell ref="J70:K70"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="J71:K71"/>
+    <mergeCell ref="J72:K72"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="G1:G2"/>
@@ -7367,12 +7423,6 @@
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:L2"/>
     <mergeCell ref="M1:M2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -7642,38 +7692,38 @@
       <c r="D1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="68" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="51" t="s">
+      <c r="F1" s="69"/>
+      <c r="G1" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="52"/>
+      <c r="H1" s="69"/>
     </row>
     <row r="2" spans="1:8" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="70" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="55"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="71"/>
+      <c r="G2" s="71"/>
+      <c r="H2" s="72"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="3"/>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="51" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53"/>
     </row>
     <row r="4" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="4">
@@ -7683,12 +7733,12 @@
         <v>370</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="61" t="s">
+      <c r="D4" s="60"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="58" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="62"/>
+      <c r="G4" s="59"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7699,12 +7749,12 @@
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="63" t="s">
+      <c r="D5" s="56"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="54" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="64"/>
+      <c r="G5" s="55"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7715,12 +7765,12 @@
         <v>372</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="61" t="s">
+      <c r="D6" s="60"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="58" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="62"/>
+      <c r="G6" s="59"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7731,12 +7781,12 @@
         <v>373</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="63" t="s">
+      <c r="D7" s="56"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="54" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="64"/>
+      <c r="G7" s="55"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7747,12 +7797,12 @@
         <v>53</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="61" t="s">
+      <c r="D8" s="60"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="58" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="62"/>
+      <c r="G8" s="59"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -7763,25 +7813,25 @@
         <v>374</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="66"/>
+      <c r="D9" s="56"/>
+      <c r="E9" s="57"/>
+      <c r="F9" s="56"/>
+      <c r="G9" s="57"/>
       <c r="H9" s="6" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="5"/>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="65" t="s">
         <v>376</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="69"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="67"/>
     </row>
     <row r="11" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A11" s="6">
@@ -7793,12 +7843,12 @@
       <c r="C11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="54" t="s">
         <v>378</v>
       </c>
-      <c r="E11" s="64"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="57"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7811,12 +7861,12 @@
       <c r="C12" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="58" t="s">
         <v>378</v>
       </c>
-      <c r="E12" s="62"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="60"/>
+      <c r="E12" s="59"/>
+      <c r="F12" s="60"/>
+      <c r="G12" s="61"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7829,12 +7879,12 @@
       <c r="C13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="54" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="64"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="66"/>
+      <c r="E13" s="55"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="57"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7845,12 +7895,12 @@
         <v>380</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="58" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="62"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="60"/>
+      <c r="E14" s="59"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="61"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -7863,12 +7913,12 @@
       <c r="C15" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="54" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="64"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="66"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="56"/>
+      <c r="G15" s="57"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7881,12 +7931,12 @@
       <c r="C16" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="58" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="62"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="60"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="60"/>
+      <c r="G16" s="61"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -7899,12 +7949,12 @@
       <c r="C17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="54" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="64"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="66"/>
+      <c r="E17" s="55"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7917,12 +7967,12 @@
       <c r="C18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="58" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="62"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="60"/>
+      <c r="E18" s="59"/>
+      <c r="F18" s="60"/>
+      <c r="G18" s="61"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -7935,12 +7985,12 @@
       <c r="C19" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="D19" s="63" t="s">
+      <c r="D19" s="54" t="s">
         <v>378</v>
       </c>
-      <c r="E19" s="64"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="66"/>
+      <c r="E19" s="55"/>
+      <c r="F19" s="56"/>
+      <c r="G19" s="57"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -7953,12 +8003,12 @@
       <c r="C20" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="58" t="s">
         <v>378</v>
       </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="60"/>
+      <c r="E20" s="59"/>
+      <c r="F20" s="60"/>
+      <c r="G20" s="61"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="117.3" thickBot="1" x14ac:dyDescent="0.65">
@@ -7971,12 +8021,12 @@
       <c r="C21" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="63" t="s">
+      <c r="D21" s="54" t="s">
         <v>378</v>
       </c>
-      <c r="E21" s="64"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="66"/>
+      <c r="E21" s="55"/>
+      <c r="F21" s="56"/>
+      <c r="G21" s="57"/>
       <c r="H21" s="6" t="s">
         <v>389</v>
       </c>
@@ -7991,12 +8041,12 @@
       <c r="C22" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="58" t="s">
         <v>378</v>
       </c>
-      <c r="E22" s="62"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="60"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="60"/>
+      <c r="G22" s="61"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -8021,13 +8071,13 @@
     </row>
     <row r="24" spans="1:8" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A24" s="7"/>
-      <c r="B24" s="70" t="s">
+      <c r="B24" s="62" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="72"/>
+      <c r="C24" s="63"/>
+      <c r="D24" s="63"/>
+      <c r="E24" s="63"/>
+      <c r="F24" s="64"/>
     </row>
     <row r="25" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A25" s="6">
@@ -8095,13 +8145,13 @@
     </row>
     <row r="29" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A29" s="3"/>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="51" t="s">
         <v>396</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="58"/>
+      <c r="C29" s="52"/>
+      <c r="D29" s="52"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="53"/>
     </row>
     <row r="30" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A30" s="4">
@@ -8259,13 +8309,13 @@
     </row>
     <row r="41" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A41" s="3"/>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="51" t="s">
         <v>408</v>
       </c>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="58"/>
+      <c r="C41" s="52"/>
+      <c r="D41" s="52"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="53"/>
     </row>
     <row r="42" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A42" s="4">
@@ -8339,31 +8389,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="D5:E5"/>
@@ -8377,12 +8408,31 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -8674,19 +8724,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
-    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9001,22 +9044,25 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
+    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9042,9 +9088,13 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
updated keyword list/status after discussion
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -5,12 +5,12 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjkim/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjkim/Documents/KeckLFC-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F45A5F2-9ED4-A648-AA07-42492F206F08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4F1EF0A4-37F9-A440-9201-C45D3FCECAAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-720" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSF EO Comb" sheetId="1" r:id="rId1"/>
@@ -49,18 +49,35 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={A12C35E2-454A-E044-AA6F-90F49746B87E}</author>
-    <author>tc={8E385BD7-CB1A-6B4B-9A34-FB5994ACFAE5}</author>
-    <author>tc={571BE3E8-65E3-834D-971C-F4F7A8109EE5}</author>
+    <author>tc={D3C2FCEF-3C80-CE41-B2E7-DD6B9F50FECC}</author>
     <author>tc={7CFD64FF-9EC6-294B-9BEF-9777389E8580}</author>
     <author>tc={C35B52B2-9CE8-754E-ABC4-B8F8053DF728}</author>
     <author>tc={34097AA0-B693-B145-BC43-7609B0047A34}</author>
     <author>tc={203D725E-9B82-8244-B953-050D9845AB73}</author>
+    <author>tc={43EE3C90-F8DC-844A-90D6-FE4B195F4D19}</author>
+    <author>tc={734F326A-1433-1D42-B27D-80F6AB5B01F2}</author>
+    <author>tc={65E7EA58-AEBE-9E43-B699-4C2E84AB06AE}</author>
+    <author>tc={9270FBFE-6EFE-1048-9F63-76932967FCB6}</author>
     <author>tc={430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}</author>
     <author>tc={897DD710-C2AF-F348-9BE6-70FC899ABE2C}</author>
+    <author>tc={D3AE0575-FA6E-1242-8525-02B45DC7B747}</author>
     <author>tc={EF222E0F-25E5-D547-9265-DB5E371F9AC7}</author>
+    <author>tc={91A521E9-8C58-AA4E-9DB6-3B7C40324E9D}</author>
     <author>tc={E8CBB725-766B-9540-AD26-3D88E8136C7F}</author>
+    <author>tc={3A13DE3F-FDB4-D54D-8D34-92EEE889D658}</author>
+    <author>tc={A2C7FC53-1505-8A45-99CE-70D3C4FD5518}</author>
+    <author>tc={3FE72732-F7D7-6A44-A781-0E38E560C217}</author>
+    <author>tc={0490C4F1-599B-AB44-B1CC-7E63E4E8065B}</author>
     <author>tc={C82D50AC-F6ED-B841-AC03-1967E28B201E}</author>
     <author>tc={C7739DC9-A5B2-EF49-9CE8-416CEC34862C}</author>
+    <author>tc={3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}</author>
+    <author>tc={B06CDA75-3D09-3A4C-9CA2-5DAFC7D0A49C}</author>
+    <author>tc={6ED25ED1-E5D3-0547-B2AE-B068D8D2FCAB}</author>
+    <author>tc={766C4F7D-809F-8546-936F-F77DAB106C65}</author>
+    <author>tc={BF9BF349-FB0E-2A49-BEAB-473752D32B3F}</author>
+    <author>tc={506BB1FA-65AC-2844-8BBF-2A90D38F6707}</author>
+    <author>tc={1DDB399D-F138-F04F-99C1-98F0475A5FB6}</author>
+    <author>tc={30C5F121-C7F3-DF45-95C8-DA0E6762ECA7}</author>
     <author>tc={E0A4D72A-0143-6945-8315-0EBFC4A9749A}</author>
   </authors>
   <commentList>
@@ -72,25 +89,17 @@
     Please fill these in (used in help message for users, see LFC.xml.sin file)</t>
       </text>
     </comment>
-    <comment ref="C5" authorId="1" shapeId="0" xr:uid="{8E385BD7-CB1A-6B4B-9A34-FB5994ACFAE5}">
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{D3C2FCEF-3C80-CE41-B2E7-DD6B9F50FECC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Needs to be float number
+    Split into two keywords?
 Reply:
-    Or the keyword type needs to be boolean or enumerated</t>
+    How to read after reset?</t>
       </text>
     </comment>
-    <comment ref="C6" authorId="2" shapeId="0" xr:uid="{571BE3E8-65E3-834D-971C-F4F7A8109EE5}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Needs to be float number</t>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="3" shapeId="0" xr:uid="{7CFD64FF-9EC6-294B-9BEF-9777389E8580}">
+    <comment ref="C7" authorId="2" shapeId="0" xr:uid="{7CFD64FF-9EC6-294B-9BEF-9777389E8580}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -98,7 +107,7 @@
     Implemented as 1 or 0, 1=on and 0=off</t>
       </text>
     </comment>
-    <comment ref="F11" authorId="4" shapeId="0" xr:uid="{C35B52B2-9CE8-754E-ABC4-B8F8053DF728}">
+    <comment ref="F9" authorId="3" shapeId="0" xr:uid="{C35B52B2-9CE8-754E-ABC4-B8F8053DF728}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -106,7 +115,7 @@
     I implemented this as enumerated</t>
       </text>
     </comment>
-    <comment ref="F13" authorId="5" shapeId="0" xr:uid="{34097AA0-B693-B145-BC43-7609B0047A34}">
+    <comment ref="F11" authorId="4" shapeId="0" xr:uid="{34097AA0-B693-B145-BC43-7609B0047A34}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -114,23 +123,61 @@
     Please provide formats for float types. For example, float(%.2f)</t>
       </text>
     </comment>
-    <comment ref="C16" authorId="6" shapeId="0" xr:uid="{203D725E-9B82-8244-B953-050D9845AB73}">
+    <comment ref="C14" authorId="5" shapeId="0" xr:uid="{203D725E-9B82-8244-B953-050D9845AB73}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    If this keyword value is going to be either “pid” or “man”, it could be implemented as enumerated type, as in LFC_2BY2_SWITCH</t>
+    If this keyword value is going to be either “pid” or “man”, it could be implemented as enumerated type, as in LFC_2BY2_SWITCH
+Reply:
+    Implementing as boolean</t>
       </text>
     </comment>
-    <comment ref="B20" authorId="7" shapeId="0" xr:uid="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
+    <comment ref="B17" authorId="6" shapeId="0" xr:uid="{43EE3C90-F8DC-844A-90D6-FE4B195F4D19}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Maybe these are okay to remove?</t>
+    Fault or okay - boolean
+Reply:
+    0: Fault, 1: Normal</t>
       </text>
     </comment>
-    <comment ref="F32" authorId="8" shapeId="0" xr:uid="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
+    <comment ref="H17" authorId="7" shapeId="0" xr:uid="{734F326A-1433-1D42-B27D-80F6AB5B01F2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    0:Fault, 1:Normal</t>
+      </text>
+    </comment>
+    <comment ref="N17" authorId="8" shapeId="0" xr:uid="{65E7EA58-AEBE-9E43-B699-4C2E84AB06AE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Please fill in</t>
+      </text>
+    </comment>
+    <comment ref="B19" authorId="9" shapeId="0" xr:uid="{9270FBFE-6EFE-1048-9F63-76932967FCB6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Doesn’t have to be KTL keyword</t>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="10" shapeId="0" xr:uid="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Maybe these are okay to remove?
+Reply:
+    Keep them and change names</t>
+      </text>
+    </comment>
+    <comment ref="F33" authorId="11" shapeId="0" xr:uid="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -138,7 +185,17 @@
     Implementing as float</t>
       </text>
     </comment>
-    <comment ref="F33" authorId="9" shapeId="0" xr:uid="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
+    <comment ref="B34" authorId="12" shapeId="0" xr:uid="{D3AE0575-FA6E-1242-8525-02B45DC7B747}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not exposed to end user?
+Reply:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="13" shapeId="0" xr:uid="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -146,7 +203,15 @@
     Not sure what type it’s supposed to be</t>
       </text>
     </comment>
-    <comment ref="F35" authorId="10" shapeId="0" xr:uid="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
+    <comment ref="B36" authorId="14" shapeId="0" xr:uid="{91A521E9-8C58-AA4E-9DB6-3B7C40324E9D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="F36" authorId="15" shapeId="0" xr:uid="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -154,7 +219,39 @@
     Not sure what type it’s supposed to be</t>
       </text>
     </comment>
-    <comment ref="F52" authorId="11" shapeId="0" xr:uid="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
+    <comment ref="B40" authorId="16" shapeId="0" xr:uid="{3A13DE3F-FDB4-D54D-8D34-92EEE889D658}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="B42" authorId="17" shapeId="0" xr:uid="{A2C7FC53-1505-8A45-99CE-70D3C4FD5518}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="B45" authorId="18" shapeId="0" xr:uid="{3FE72732-F7D7-6A44-A781-0E38E560C217}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="B49" authorId="19" shapeId="0" xr:uid="{0490C4F1-599B-AB44-B1CC-7E63E4E8065B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="F53" authorId="20" shapeId="0" xr:uid="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -162,7 +259,7 @@
     Only 1-dimensional array allowed</t>
       </text>
     </comment>
-    <comment ref="F54" authorId="12" shapeId="0" xr:uid="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
+    <comment ref="F55" authorId="21" shapeId="0" xr:uid="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -170,7 +267,71 @@
     Implemented as float</t>
       </text>
     </comment>
-    <comment ref="H72" authorId="13" shapeId="0" xr:uid="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
+    <comment ref="B56" authorId="22" shapeId="0" xr:uid="{3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="B59" authorId="23" shapeId="0" xr:uid="{B06CDA75-3D09-3A4C-9CA2-5DAFC7D0A49C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="B67" authorId="24" shapeId="0" xr:uid="{6ED25ED1-E5D3-0547-B2AE-B068D8D2FCAB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B69" authorId="25" shapeId="0" xr:uid="{766C4F7D-809F-8546-936F-F77DAB106C65}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B70" authorId="26" shapeId="0" xr:uid="{BF9BF349-FB0E-2A49-BEAB-473752D32B3F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B71" authorId="27" shapeId="0" xr:uid="{506BB1FA-65AC-2844-8BBF-2A90D38F6707}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B72" authorId="28" shapeId="0" xr:uid="{1DDB399D-F138-F04F-99C1-98F0475A5FB6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B73" authorId="29" shapeId="0" xr:uid="{30C5F121-C7F3-DF45-95C8-DA0E6762ECA7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="H73" authorId="30" shapeId="0" xr:uid="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -201,7 +362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1357" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="557">
   <si>
     <t>Keyword</t>
   </si>
@@ -1549,18 +1710,9 @@
     <t>mw</t>
   </si>
   <si>
-    <t>apc mode:450mw</t>
-  </si>
-  <si>
     <t>LFC_EDFA27_AUTO_ON</t>
   </si>
   <si>
-    <t>acc' or 'apc' or none</t>
-  </si>
-  <si>
-    <t>auto set power or current and turn on</t>
-  </si>
-  <si>
     <t>LFC_RFOSCI_ONOFF</t>
   </si>
   <si>
@@ -1579,15 +1731,9 @@
     <t>LFC_EDFA23_AUTO_ON</t>
   </si>
   <si>
-    <t>acc'or none</t>
-  </si>
-  <si>
     <t>ma</t>
   </si>
   <si>
-    <t>acc:80mA</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -1615,9 +1761,6 @@
     <t>1 or 2 or none</t>
   </si>
   <si>
-    <t>1:YJ/2:HK</t>
-  </si>
-  <si>
     <t>LFC_HK_SHUTTER</t>
   </si>
   <si>
@@ -1648,27 +1791,12 @@
     <t>LFC_IM_LOCK_MODE</t>
   </si>
   <si>
-    <t>pid' or 'man'</t>
-  </si>
-  <si>
-    <t>set lock mode</t>
-  </si>
-  <si>
-    <t>str</t>
-  </si>
-  <si>
     <t>get all temp on USBdaq1</t>
   </si>
   <si>
     <t>test</t>
   </si>
   <si>
-    <t>LFC_TEMP1_TEST1</t>
-  </si>
-  <si>
-    <t>LFC_TEMP1_TEST2</t>
-  </si>
-  <si>
     <t>get all temp on USBdaq2</t>
   </si>
   <si>
@@ -1810,15 +1938,9 @@
     <t>value=none, read out amp current/value!=none, set to 4.1A</t>
   </si>
   <si>
-    <t>value==none, read input power voltage/value==1, reset latch circuit/value else, do nothing</t>
-  </si>
-  <si>
     <t>same as LFC_2BY2_SWITCH. Input value:1(represent YJ) or 2(represent HK) (input number only)</t>
   </si>
   <si>
-    <t>more detail below</t>
-  </si>
-  <si>
     <t>time period(unit:s)</t>
   </si>
   <si>
@@ -1844,6 +1966,90 @@
   </si>
   <si>
     <t>verbose</t>
+  </si>
+  <si>
+    <t>none or 1</t>
+  </si>
+  <si>
+    <t>value==none:get voltage//value==1:reset latch</t>
+  </si>
+  <si>
+    <t>enumerate</t>
+  </si>
+  <si>
+    <t>1:YJ/2:HK //none:get status</t>
+  </si>
+  <si>
+    <t>float(%.2f)</t>
+  </si>
+  <si>
+    <t>value==1:pid mode//value==0:manual mode</t>
+  </si>
+  <si>
+    <t>set lock mode//read after write</t>
+  </si>
+  <si>
+    <t>LFC_WSP_PHASE(TBD)</t>
+  </si>
+  <si>
+    <t>LFC_TEMP_MONITOR</t>
+  </si>
+  <si>
+    <t>LFC_CLOSE_ALL</t>
+  </si>
+  <si>
+    <t>1 or none</t>
+  </si>
+  <si>
+    <t>shut up all power device</t>
+  </si>
+  <si>
+    <t>value==1:shut up all output</t>
+  </si>
+  <si>
+    <t>auto temp monitor</t>
+  </si>
+  <si>
+    <t>LFC_EMAIL</t>
+  </si>
+  <si>
+    <t>if temp goes above threshold, trigger LFC_CLOSE_ALL and LFC_EMAIL</t>
+  </si>
+  <si>
+    <t>can test</t>
+  </si>
+  <si>
+    <t>test after comb on</t>
+  </si>
+  <si>
+    <t>float array(%.2f)</t>
+  </si>
+  <si>
+    <t>can test (10-25)</t>
+  </si>
+  <si>
+    <t>can test (145-155)</t>
+  </si>
+  <si>
+    <t>can test if off (check LFC_RFAMP_ONOFF, make sure it's off)</t>
+  </si>
+  <si>
+    <t>can test if off (check LFC_RFOSCI_ONOFF, make sure it's off)</t>
+  </si>
+  <si>
+    <t>Y (lockout)</t>
+  </si>
+  <si>
+    <t>can test (+/- 0.5 degrees)</t>
+  </si>
+  <si>
+    <t>can test (+/- 0.5 degrees from where it is)</t>
+  </si>
+  <si>
+    <t>LFC_TEMP_TEST1</t>
+  </si>
+  <si>
+    <t>LFC_TEMP_TEST2</t>
   </si>
 </sst>
 </file>
@@ -1986,7 +2192,7 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2060,13 +2266,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2242,7 +2449,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2269,9 +2476,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2362,6 +2568,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="25"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2461,12 +2673,22 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="26"/>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="25"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="25" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
-    <cellStyle name="Bad" xfId="26" builtinId="27"/>
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
@@ -2814,46 +3036,109 @@
   <threadedComment ref="U1" dT="2024-05-25T16:13:18.71" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{A12C35E2-454A-E044-AA6F-90F49746B87E}">
     <text>Please fill these in (used in help message for users, see LFC.xml.sin file)</text>
   </threadedComment>
-  <threadedComment ref="C5" dT="2024-05-25T15:46:18.30" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{8E385BD7-CB1A-6B4B-9A34-FB5994ACFAE5}">
-    <text>Needs to be float number</text>
+  <threadedComment ref="B7" dT="2024-06-03T18:22:26.07" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{D3C2FCEF-3C80-CE41-B2E7-DD6B9F50FECC}">
+    <text>Split into two keywords?</text>
   </threadedComment>
-  <threadedComment ref="C5" dT="2024-05-25T15:47:16.72" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{3A85D8C2-1E59-E14F-AED4-0153EC258617}" parentId="{8E385BD7-CB1A-6B4B-9A34-FB5994ACFAE5}">
-    <text>Or the keyword type needs to be boolean or enumerated</text>
+  <threadedComment ref="B7" dT="2024-06-03T18:30:30.74" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{D5106230-4936-3E43-B433-25ED7C9F13BE}" parentId="{D3C2FCEF-3C80-CE41-B2E7-DD6B9F50FECC}">
+    <text>How to read after reset?</text>
   </threadedComment>
-  <threadedComment ref="C6" dT="2024-05-25T15:46:44.69" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{571BE3E8-65E3-834D-971C-F4F7A8109EE5}">
-    <text>Needs to be float number</text>
-  </threadedComment>
-  <threadedComment ref="C9" dT="2024-05-25T15:57:35.22" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{7CFD64FF-9EC6-294B-9BEF-9777389E8580}">
+  <threadedComment ref="C7" dT="2024-05-25T15:57:35.22" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{7CFD64FF-9EC6-294B-9BEF-9777389E8580}">
     <text>Implemented as 1 or 0, 1=on and 0=off</text>
   </threadedComment>
-  <threadedComment ref="F11" dT="2024-05-25T15:48:09.66" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C35B52B2-9CE8-754E-ABC4-B8F8053DF728}">
+  <threadedComment ref="F9" dT="2024-05-25T15:48:09.66" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C35B52B2-9CE8-754E-ABC4-B8F8053DF728}">
     <text>I implemented this as enumerated</text>
   </threadedComment>
-  <threadedComment ref="F13" dT="2024-05-25T16:17:43.67" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{34097AA0-B693-B145-BC43-7609B0047A34}">
+  <threadedComment ref="F11" dT="2024-05-25T16:17:43.67" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{34097AA0-B693-B145-BC43-7609B0047A34}">
     <text>Please provide formats for float types. For example, float(%.2f)</text>
   </threadedComment>
-  <threadedComment ref="C16" dT="2024-05-25T15:49:02.90" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{203D725E-9B82-8244-B953-050D9845AB73}">
+  <threadedComment ref="C14" dT="2024-05-25T15:49:02.90" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{203D725E-9B82-8244-B953-050D9845AB73}">
     <text>If this keyword value is going to be either “pid” or “man”, it could be implemented as enumerated type, as in LFC_2BY2_SWITCH</text>
   </threadedComment>
-  <threadedComment ref="B20" dT="2024-05-25T16:14:22.88" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
+  <threadedComment ref="C14" dT="2024-06-03T20:29:43.17" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{038E729A-82CE-F148-AAB1-60ADED45E6B8}" parentId="{203D725E-9B82-8244-B953-050D9845AB73}">
+    <text>Implementing as boolean</text>
+  </threadedComment>
+  <threadedComment ref="B17" dT="2024-06-03T18:35:54.88" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{43EE3C90-F8DC-844A-90D6-FE4B195F4D19}">
+    <text>Fault or okay - boolean</text>
+  </threadedComment>
+  <threadedComment ref="B17" dT="2024-06-03T20:37:28.72" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{4F472B1F-3735-B649-9078-98AB15E83A44}" parentId="{43EE3C90-F8DC-844A-90D6-FE4B195F4D19}">
+    <text>0: Fault, 1: Normal</text>
+  </threadedComment>
+  <threadedComment ref="H17" dT="2024-06-03T20:37:48.93" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{734F326A-1433-1D42-B27D-80F6AB5B01F2}">
+    <text>0:Fault, 1:Normal</text>
+  </threadedComment>
+  <threadedComment ref="N17" dT="2024-06-03T20:31:30.31" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{65E7EA58-AEBE-9E43-B699-4C2E84AB06AE}">
+    <text>Please fill in</text>
+  </threadedComment>
+  <threadedComment ref="B19" dT="2024-06-03T18:40:46.49" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{9270FBFE-6EFE-1048-9F63-76932967FCB6}">
+    <text>Doesn’t have to be KTL keyword</text>
+  </threadedComment>
+  <threadedComment ref="B21" dT="2024-05-25T16:14:22.88" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
     <text>Maybe these are okay to remove?</text>
   </threadedComment>
-  <threadedComment ref="F32" dT="2024-05-25T16:23:38.53" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
+  <threadedComment ref="B21" dT="2024-06-03T18:43:05.98" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{5296AF8B-E0AA-1846-89CA-ED67E861F12F}" parentId="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
+    <text>Keep them and change names</text>
+  </threadedComment>
+  <threadedComment ref="F33" dT="2024-05-25T16:23:38.53" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
     <text>Implementing as float</text>
   </threadedComment>
-  <threadedComment ref="F33" dT="2024-05-25T16:27:45.79" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
+  <threadedComment ref="B34" dT="2024-06-03T18:54:55.02" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{D3AE0575-FA6E-1242-8525-02B45DC7B747}">
+    <text>Not exposed to end user?</text>
+  </threadedComment>
+  <threadedComment ref="B34" dT="2024-06-03T18:56:33.55" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{50BBA82F-D96D-894B-A5A6-CF02B225EDD9}" parentId="{D3AE0575-FA6E-1242-8525-02B45DC7B747}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="F34" dT="2024-05-25T16:27:45.79" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
     <text>Not sure what type it’s supposed to be</text>
   </threadedComment>
-  <threadedComment ref="F35" dT="2024-05-25T16:28:10.48" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
+  <threadedComment ref="B36" dT="2024-06-03T18:58:56.66" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{91A521E9-8C58-AA4E-9DB6-3B7C40324E9D}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="F36" dT="2024-05-25T16:28:10.48" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
     <text>Not sure what type it’s supposed to be</text>
   </threadedComment>
-  <threadedComment ref="F52" dT="2024-05-25T16:35:00.27" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
+  <threadedComment ref="B40" dT="2024-06-03T18:59:47.18" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{3A13DE3F-FDB4-D54D-8D34-92EEE889D658}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B42" dT="2024-06-03T18:59:56.11" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{A2C7FC53-1505-8A45-99CE-70D3C4FD5518}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B45" dT="2024-06-03T19:01:27.62" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{3FE72732-F7D7-6A44-A781-0E38E560C217}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B49" dT="2024-06-03T19:04:26.19" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{0490C4F1-599B-AB44-B1CC-7E63E4E8065B}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="F53" dT="2024-05-25T16:35:00.27" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
     <text>Only 1-dimensional array allowed</text>
   </threadedComment>
-  <threadedComment ref="F54" dT="2024-05-25T16:42:43.15" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
+  <threadedComment ref="F55" dT="2024-05-25T16:42:43.15" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
     <text>Implemented as float</text>
   </threadedComment>
-  <threadedComment ref="H72" dT="2024-05-25T15:51:08.40" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
+  <threadedComment ref="B56" dT="2024-06-03T19:15:47.42" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B59" dT="2024-06-03T19:15:57.20" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{B06CDA75-3D09-3A4C-9CA2-5DAFC7D0A49C}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B67" dT="2024-06-03T19:24:16.35" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{6ED25ED1-E5D3-0547-B2AE-B068D8D2FCAB}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="B69" dT="2024-06-03T19:24:21.88" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{766C4F7D-809F-8546-936F-F77DAB106C65}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="B70" dT="2024-06-03T19:24:53.91" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{BF9BF349-FB0E-2A49-BEAB-473752D32B3F}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="B71" dT="2024-06-03T19:25:20.88" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{506BB1FA-65AC-2844-8BBF-2A90D38F6707}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="B72" dT="2024-06-03T19:25:16.63" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{1DDB399D-F138-F04F-99C1-98F0475A5FB6}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="B73" dT="2024-06-03T19:25:36.80" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{30C5F121-C7F3-DF45-95C8-DA0E6762ECA7}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="H73" dT="2024-05-25T15:51:08.40" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
     <text>Is this needed, separate from LFC_2BY2_SWITCH?</text>
   </threadedComment>
 </ThreadedComments>
@@ -2893,68 +3178,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="46" t="s">
+      <c r="A1" s="49"/>
+      <c r="B1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="41"/>
-      <c r="L1" s="43" t="s">
+      <c r="K1" s="45"/>
+      <c r="L1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="41"/>
-      <c r="O1" s="43" t="s">
+      <c r="N1" s="45"/>
+      <c r="O1" s="47" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="44"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="44"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="48"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
@@ -3107,10 +3392,10 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="49" t="s">
+      <c r="J7" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="49"/>
+      <c r="K7" s="53"/>
       <c r="M7">
         <v>0</v>
       </c>
@@ -3137,10 +3422,10 @@
       <c r="H8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="49" t="s">
+      <c r="J8" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="49"/>
+      <c r="K8" s="53"/>
       <c r="M8">
         <v>0</v>
       </c>
@@ -3204,7 +3489,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="50" t="s">
+      <c r="A11" s="54" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
@@ -3228,13 +3513,13 @@
       <c r="H11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="49" t="s">
+      <c r="J11" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="49"/>
+      <c r="K11" s="53"/>
     </row>
     <row r="12" spans="1:19" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="50"/>
+      <c r="A12" s="54"/>
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -3256,10 +3541,10 @@
       <c r="H12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="49" t="s">
+      <c r="J12" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="49"/>
+      <c r="K12" s="53"/>
     </row>
     <row r="13" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="31"/>
@@ -4124,7 +4409,7 @@
       <c r="H54" s="11"/>
     </row>
     <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="40" t="s">
+      <c r="A55" s="44" t="s">
         <v>153</v>
       </c>
       <c r="B55" t="s">
@@ -4134,7 +4419,7 @@
       <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="40"/>
+      <c r="A56" s="44"/>
       <c r="B56" t="s">
         <v>155</v>
       </c>
@@ -4142,7 +4427,7 @@
       <c r="H56" s="11"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="40"/>
+      <c r="A57" s="44"/>
       <c r="B57" t="s">
         <v>156</v>
       </c>
@@ -4150,7 +4435,7 @@
       <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="40"/>
+      <c r="A58" s="44"/>
       <c r="B58" t="s">
         <v>157</v>
       </c>
@@ -4158,7 +4443,7 @@
       <c r="H58" s="11"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="40"/>
+      <c r="A59" s="44"/>
       <c r="B59" t="s">
         <v>158</v>
       </c>
@@ -4166,7 +4451,7 @@
       <c r="H59" s="11"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="40"/>
+      <c r="A60" s="44"/>
       <c r="B60" t="s">
         <v>159</v>
       </c>
@@ -4174,7 +4459,7 @@
       <c r="H60" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="40"/>
+      <c r="A61" s="44"/>
       <c r="B61" t="s">
         <v>160</v>
       </c>
@@ -4187,7 +4472,7 @@
       <c r="H62" s="11"/>
     </row>
     <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="40" t="s">
+      <c r="A63" s="44" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
@@ -4197,7 +4482,7 @@
       <c r="H63" s="11"/>
     </row>
     <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="40"/>
+      <c r="A64" s="44"/>
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -4205,7 +4490,7 @@
       <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="40"/>
+      <c r="A65" s="44"/>
       <c r="B65" t="s">
         <v>164</v>
       </c>
@@ -4213,7 +4498,7 @@
       <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="40"/>
+      <c r="A66" s="44"/>
       <c r="B66" t="s">
         <v>165</v>
       </c>
@@ -4221,7 +4506,7 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="40"/>
+      <c r="A67" s="44"/>
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -4229,7 +4514,7 @@
       <c r="H67" s="11"/>
     </row>
     <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="40"/>
+      <c r="A68" s="44"/>
       <c r="B68" t="s">
         <v>167</v>
       </c>
@@ -4237,7 +4522,7 @@
       <c r="H68" s="11"/>
     </row>
     <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="40"/>
+      <c r="A69" s="44"/>
       <c r="B69" t="s">
         <v>168</v>
       </c>
@@ -5960,10 +6245,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60079DE2-3043-422E-90F3-3EEEEA14A1EF}">
-  <dimension ref="A1:V76"/>
+  <dimension ref="A1:V77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="106" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5973,14 +6259,15 @@
     <col min="3" max="3" width="15.1640625" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" customWidth="1"/>
     <col min="5" max="5" width="10.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="35.33203125" customWidth="1"/>
     <col min="8" max="8" width="28.83203125" customWidth="1"/>
     <col min="9" max="9" width="9.1640625" customWidth="1"/>
-    <col min="10" max="10" width="6.83203125" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
     <col min="11" max="11" width="8.5" customWidth="1"/>
     <col min="13" max="13" width="26.5" customWidth="1"/>
     <col min="14" max="14" width="15.33203125" customWidth="1"/>
-    <col min="17" max="17" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
     <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.6640625" customWidth="1"/>
@@ -5988,91 +6275,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45"/>
-      <c r="B1" s="46" t="s">
+      <c r="A1" s="49"/>
+      <c r="B1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="47" t="s">
+      <c r="G1" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="47" t="s">
+      <c r="H1" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="41"/>
-      <c r="L1" s="43" t="s">
+      <c r="K1" s="45"/>
+      <c r="L1" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="41" t="s">
-        <v>533</v>
-      </c>
-      <c r="O1" s="43" t="s">
+      <c r="N1" s="45" t="s">
+        <v>520</v>
+      </c>
+      <c r="O1" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="45" t="s">
-        <v>534</v>
-      </c>
-      <c r="R1" s="45"/>
-      <c r="S1" s="45"/>
-      <c r="U1" s="45" t="s">
-        <v>539</v>
-      </c>
-      <c r="V1" s="45"/>
+      <c r="Q1" s="49" t="s">
+        <v>521</v>
+      </c>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="U1" s="49" t="s">
+        <v>526</v>
+      </c>
+      <c r="V1" s="49"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="46"/>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="47"/>
-      <c r="E2" s="46"/>
-      <c r="F2" s="46"/>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
-      <c r="I2" s="48"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="52"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="44"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="O2" s="44"/>
+      <c r="L2" s="48"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="O2" s="48"/>
       <c r="Q2" s="1" t="s">
-        <v>535</v>
+        <v>522</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>536</v>
+        <v>523</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>537</v>
+        <v>524</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>540</v>
+        <v>527</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>541</v>
+        <v>528</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.2">
@@ -6094,77 +6381,58 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="N4">
-        <v>120</v>
-      </c>
-    </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>452</v>
+        <v>444</v>
       </c>
       <c r="C5" t="s">
-        <v>453</v>
+        <v>445</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>377</v>
       </c>
       <c r="G5" t="s">
         <v>446</v>
       </c>
-      <c r="H5" t="s">
-        <v>532</v>
-      </c>
-      <c r="I5" t="s">
-        <v>454</v>
-      </c>
-      <c r="M5" t="s">
-        <v>455</v>
-      </c>
       <c r="N5">
         <v>120</v>
       </c>
-      <c r="Q5" s="73"/>
+      <c r="Q5" s="40" t="s">
+        <v>525</v>
+      </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>444</v>
-      </c>
-      <c r="C6" s="33" t="s">
+        <v>447</v>
+      </c>
+      <c r="C6" t="s">
         <v>445</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>377</v>
       </c>
       <c r="G6" t="s">
-        <v>446</v>
-      </c>
-      <c r="H6" t="s">
-        <v>532</v>
-      </c>
-      <c r="I6" t="s">
-        <v>442</v>
-      </c>
-      <c r="M6" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="N6">
         <v>120</v>
       </c>
-      <c r="Q6" s="73"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q6" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>447</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>448</v>
+        <v>529</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
@@ -6173,90 +6441,129 @@
         <v>377</v>
       </c>
       <c r="G7" t="s">
-        <v>449</v>
+        <v>452</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>530</v>
       </c>
       <c r="N7">
         <v>120</v>
       </c>
-      <c r="Q7" s="74" t="s">
-        <v>538</v>
+      <c r="Q7" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R7" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="39" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="C8" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="F8" t="s">
         <v>377</v>
       </c>
       <c r="G8" t="s">
-        <v>451</v>
+        <v>454</v>
+      </c>
+      <c r="H8" t="s">
+        <v>455</v>
       </c>
       <c r="N8">
         <v>120</v>
       </c>
-      <c r="Q8" s="74" t="s">
-        <v>538</v>
+      <c r="Q8" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R8" t="s">
+        <v>545</v>
+      </c>
+      <c r="S8" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>137</v>
+      <c r="B9" s="39" t="s">
+        <v>456</v>
       </c>
       <c r="C9" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="E9" t="s">
         <v>17</v>
       </c>
       <c r="F9" t="s">
-        <v>377</v>
+        <v>531</v>
       </c>
       <c r="G9" t="s">
-        <v>457</v>
+        <v>458</v>
+      </c>
+      <c r="H9" t="s">
+        <v>532</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
       </c>
       <c r="N9">
         <v>120</v>
       </c>
-      <c r="Q9" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q9" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R9" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S9" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="C10" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="E10" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
         <v>377</v>
       </c>
       <c r="G10" t="s">
-        <v>459</v>
-      </c>
-      <c r="H10" t="s">
-        <v>460</v>
+        <v>461</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>462</v>
       </c>
       <c r="N10">
         <v>120</v>
       </c>
-      <c r="Q10" s="74" t="s">
-        <v>538</v>
+      <c r="Q10" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R10" t="s">
+        <v>545</v>
+      </c>
+      <c r="S10" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B11" s="39" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C11" t="s">
         <v>464</v>
@@ -6265,77 +6572,89 @@
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>377</v>
+        <v>533</v>
       </c>
       <c r="G11" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="H11" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="N11">
         <v>120</v>
       </c>
-      <c r="Q11" s="74" t="s">
-        <v>538</v>
-      </c>
-      <c r="R11" s="74" t="s">
-        <v>538</v>
-      </c>
-      <c r="S11" s="74" t="s">
-        <v>538</v>
+      <c r="Q11" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R11" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S11" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
+        <v>467</v>
+      </c>
+      <c r="C12" t="s">
+        <v>464</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>533</v>
+      </c>
+      <c r="G12" t="s">
+        <v>465</v>
+      </c>
+      <c r="H12" t="s">
         <v>466</v>
       </c>
-      <c r="C12" t="s">
-        <v>462</v>
-      </c>
-      <c r="E12" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" t="s">
-        <v>377</v>
-      </c>
-      <c r="G12" t="s">
-        <v>467</v>
-      </c>
-      <c r="H12" t="s">
-        <v>468</v>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>60</v>
       </c>
       <c r="N12">
         <v>120</v>
       </c>
-      <c r="Q12" s="74" t="s">
-        <v>538</v>
+      <c r="Q12" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R12" s="34" t="s">
+        <v>545</v>
+      </c>
+      <c r="S12" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B13" s="39" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C13" t="s">
-        <v>470</v>
+        <v>464</v>
       </c>
       <c r="E13" t="s">
         <v>17</v>
       </c>
       <c r="F13" t="s">
-        <v>18</v>
+        <v>533</v>
       </c>
       <c r="G13" t="s">
-        <v>471</v>
+        <v>465</v>
       </c>
       <c r="H13" t="s">
-        <v>472</v>
+        <v>466</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -6346,304 +6665,338 @@
       <c r="N13">
         <v>120</v>
       </c>
-      <c r="Q13" s="74" t="s">
-        <v>538</v>
-      </c>
-      <c r="R13" s="74" t="s">
-        <v>538</v>
-      </c>
-      <c r="S13" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="Q13" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R13" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S13" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>473</v>
-      </c>
-      <c r="C14" t="s">
-        <v>470</v>
+        <v>469</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>445</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>18</v>
+        <v>377</v>
       </c>
       <c r="G14" t="s">
-        <v>471</v>
-      </c>
-      <c r="H14" t="s">
-        <v>472</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>60</v>
+        <v>535</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>534</v>
       </c>
       <c r="N14">
         <v>120</v>
       </c>
-      <c r="Q14" s="74" t="s">
+      <c r="Q14" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R14" s="34" t="s">
+        <v>545</v>
+      </c>
+      <c r="S14" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" ht="51" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>537</v>
+      </c>
+      <c r="C17" t="s">
+        <v>451</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" t="s">
+        <v>377</v>
+      </c>
+      <c r="G17" t="s">
+        <v>542</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>544</v>
+      </c>
+      <c r="Q17" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R17" s="34" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B15" s="39" t="s">
-        <v>474</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
+        <v>539</v>
+      </c>
+      <c r="E18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F18" t="s">
+        <v>377</v>
+      </c>
+      <c r="G18" t="s">
+        <v>540</v>
+      </c>
+      <c r="H18" t="s">
+        <v>541</v>
+      </c>
+      <c r="Q18" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" s="77" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="77" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>555</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" t="s">
+        <v>547</v>
+      </c>
+      <c r="G21" t="s">
         <v>470</v>
       </c>
-      <c r="E15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" t="s">
+      <c r="H21" t="s">
         <v>471</v>
-      </c>
-      <c r="H15" t="s">
-        <v>472</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>60</v>
-      </c>
-      <c r="N15">
-        <v>120</v>
-      </c>
-      <c r="Q15" s="74" t="s">
-        <v>538</v>
-      </c>
-      <c r="R15" s="74" t="s">
-        <v>538</v>
-      </c>
-      <c r="S15" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="B16" t="s">
-        <v>475</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>476</v>
-      </c>
-      <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" t="s">
-        <v>478</v>
-      </c>
-      <c r="G16" t="s">
-        <v>477</v>
-      </c>
-      <c r="N16">
-        <v>120</v>
-      </c>
-      <c r="Q16" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="N19">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20" t="s">
-        <v>481</v>
-      </c>
-      <c r="G20" t="s">
-        <v>479</v>
-      </c>
-      <c r="H20" t="s">
-        <v>480</v>
-      </c>
-      <c r="N20">
-        <v>20</v>
-      </c>
-      <c r="Q20" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" t="s">
-        <v>482</v>
-      </c>
-      <c r="G21" t="s">
-        <v>483</v>
-      </c>
-      <c r="H21" t="s">
-        <v>480</v>
       </c>
       <c r="N21">
         <v>20</v>
       </c>
-      <c r="Q21" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q21" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R21" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>253</v>
+        <v>556</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" t="s">
+        <v>547</v>
+      </c>
+      <c r="G22" t="s">
+        <v>472</v>
+      </c>
+      <c r="H22" t="s">
+        <v>471</v>
       </c>
       <c r="N22">
         <v>20</v>
       </c>
-      <c r="Q22" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q22" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R22" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>255</v>
+        <v>253</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
+        <v>533</v>
       </c>
       <c r="N23">
         <v>20</v>
       </c>
-      <c r="Q23" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q23" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R23" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>484</v>
+        <v>255</v>
+      </c>
+      <c r="E24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" t="s">
+        <v>533</v>
       </c>
       <c r="N24">
         <v>20</v>
       </c>
-      <c r="Q24" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q24" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R24" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>485</v>
+        <v>473</v>
+      </c>
+      <c r="E25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" t="s">
+        <v>533</v>
       </c>
       <c r="N25">
         <v>20</v>
       </c>
-      <c r="Q25" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q25" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R25" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>273</v>
+        <v>474</v>
+      </c>
+      <c r="E26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" t="s">
+        <v>533</v>
       </c>
       <c r="N26">
         <v>20</v>
       </c>
-      <c r="Q26" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q26" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R26" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>275</v>
+        <v>273</v>
+      </c>
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" t="s">
+        <v>533</v>
       </c>
       <c r="N27">
         <v>20</v>
       </c>
-      <c r="Q27" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="Q27" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R27" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
+        <v>275</v>
+      </c>
+      <c r="E28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" t="s">
+        <v>533</v>
+      </c>
+      <c r="N28">
+        <v>20</v>
+      </c>
+      <c r="Q28" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R28" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B29" t="s">
         <v>277</v>
       </c>
-      <c r="Q28" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="30" spans="2:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="B30" t="s">
+      <c r="E29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" t="s">
+        <v>533</v>
+      </c>
+      <c r="Q29" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R29" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>77</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
-      </c>
-      <c r="D30" t="s">
-        <v>51</v>
-      </c>
-      <c r="E30" t="s">
-        <v>17</v>
-      </c>
-      <c r="G30" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="H30" s="19" t="s">
-        <v>79</v>
-      </c>
-      <c r="I30" t="s">
-        <v>80</v>
-      </c>
-      <c r="J30">
-        <v>-5</v>
-      </c>
-      <c r="K30">
-        <v>75</v>
-      </c>
-      <c r="M30">
-        <v>25</v>
-      </c>
-      <c r="N30">
-        <v>20</v>
-      </c>
-      <c r="Q30" s="74" t="s">
-        <v>538</v>
-      </c>
-      <c r="R30" s="75" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="31" spans="2:18" ht="34" x14ac:dyDescent="0.2">
-      <c r="B31" t="s">
-        <v>81</v>
       </c>
       <c r="C31" t="s">
         <v>50</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>552</v>
       </c>
       <c r="E31" t="s">
         <v>17</v>
       </c>
       <c r="G31" s="8" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H31" s="19" t="s">
         <v>79</v>
       </c>
       <c r="I31" t="s">
-        <v>83</v>
-      </c>
-      <c r="J31" t="s">
-        <v>26</v>
-      </c>
-      <c r="K31" t="s">
-        <v>26</v>
+        <v>80</v>
+      </c>
+      <c r="J31">
+        <v>10</v>
+      </c>
+      <c r="K31">
+        <v>25</v>
       </c>
       <c r="M31">
-        <v>145</v>
+        <v>19.181000000000001</v>
       </c>
       <c r="N31">
-        <v>120</v>
-      </c>
-      <c r="Q31" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="32" spans="2:18" ht="68" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="Q31" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R31" s="41" t="s">
+        <v>525</v>
+      </c>
+      <c r="S31" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" ht="34" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C32" t="s">
         <v>50</v>
@@ -6655,135 +7008,159 @@
         <v>17</v>
       </c>
       <c r="G32" s="8" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>486</v>
+        <v>79</v>
       </c>
       <c r="I32" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>145</v>
       </c>
       <c r="K32">
-        <v>630</v>
+        <v>155</v>
       </c>
       <c r="M32">
-        <v>630</v>
+        <v>150</v>
       </c>
       <c r="N32">
         <v>120</v>
       </c>
-      <c r="Q32" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="33" spans="2:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q32" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R32" t="s">
+        <v>545</v>
+      </c>
+      <c r="S32" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" ht="68" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>511</v>
+        <v>84</v>
+      </c>
+      <c r="C33" t="s">
+        <v>50</v>
+      </c>
+      <c r="D33" t="s">
+        <v>51</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>85</v>
       </c>
       <c r="H33" s="19" t="s">
-        <v>512</v>
+        <v>475</v>
       </c>
       <c r="I33" t="s">
-        <v>442</v>
+        <v>87</v>
+      </c>
+      <c r="J33">
+        <v>0</v>
+      </c>
+      <c r="K33">
+        <v>630</v>
+      </c>
+      <c r="M33">
+        <v>630</v>
       </c>
       <c r="N33">
         <v>120</v>
       </c>
-    </row>
-    <row r="34" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
+      <c r="Q33" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R33" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" s="77" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B34" s="77" t="s">
+        <v>500</v>
+      </c>
+      <c r="E34" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="G34" s="78" t="s">
+        <v>85</v>
+      </c>
+      <c r="H34" s="79" t="s">
+        <v>501</v>
+      </c>
+      <c r="I34" s="77" t="s">
+        <v>442</v>
+      </c>
+      <c r="N34" s="77">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
         <v>88</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C35" t="s">
         <v>50</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D35" t="s">
         <v>51</v>
       </c>
-      <c r="E34" t="s">
-        <v>17</v>
-      </c>
-      <c r="F34" t="s">
+      <c r="E35" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" t="s">
         <v>33</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G35" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="H34" s="19"/>
-      <c r="N34">
-        <v>120</v>
-      </c>
-      <c r="Q34" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="35" spans="2:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>444</v>
-      </c>
-      <c r="E35" t="s">
-        <v>17</v>
-      </c>
-      <c r="G35" s="8" t="s">
-        <v>487</v>
-      </c>
-      <c r="H35" s="19" t="s">
-        <v>513</v>
-      </c>
+      <c r="H35" s="19"/>
       <c r="N35">
         <v>120</v>
       </c>
-    </row>
-    <row r="36" spans="2:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
+      <c r="Q35" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R35" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" s="77" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B36" s="77" t="s">
+        <v>443</v>
+      </c>
+      <c r="C36" s="77" t="s">
+        <v>529</v>
+      </c>
+      <c r="E36" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="G36" s="78" t="s">
+        <v>476</v>
+      </c>
+      <c r="H36" s="79" t="s">
+        <v>502</v>
+      </c>
+      <c r="N36" s="77">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19" ht="51" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
         <v>90</v>
-      </c>
-      <c r="C36" t="s">
-        <v>50</v>
-      </c>
-      <c r="D36" t="s">
-        <v>51</v>
-      </c>
-      <c r="E36" t="s">
-        <v>17</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H36" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="I36" t="s">
-        <v>87</v>
-      </c>
-      <c r="J36">
-        <v>0</v>
-      </c>
-      <c r="K36" t="s">
-        <v>92</v>
-      </c>
-      <c r="M36">
-        <v>20</v>
-      </c>
-      <c r="N36">
-        <v>120</v>
-      </c>
-      <c r="Q36" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="37" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>93</v>
       </c>
       <c r="C37" t="s">
         <v>50</v>
@@ -6794,23 +7171,37 @@
       <c r="E37" t="s">
         <v>17</v>
       </c>
-      <c r="F37" t="s">
-        <v>33</v>
-      </c>
       <c r="G37" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="H37" s="11"/>
+        <v>91</v>
+      </c>
+      <c r="H37" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="I37" t="s">
+        <v>87</v>
+      </c>
+      <c r="J37">
+        <v>0</v>
+      </c>
+      <c r="K37" t="s">
+        <v>92</v>
+      </c>
+      <c r="M37">
+        <v>20</v>
+      </c>
       <c r="N37">
         <v>120</v>
       </c>
-      <c r="Q37" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="38" spans="2:17" ht="68" x14ac:dyDescent="0.2">
+      <c r="Q37" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R37" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C38" t="s">
         <v>50</v>
@@ -6821,127 +7212,140 @@
       <c r="E38" t="s">
         <v>17</v>
       </c>
+      <c r="F38" t="s">
+        <v>33</v>
+      </c>
       <c r="G38" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="H38" s="20" t="s">
-        <v>488</v>
-      </c>
-      <c r="I38" t="s">
-        <v>87</v>
-      </c>
-      <c r="J38">
-        <v>0</v>
-      </c>
-      <c r="K38" t="s">
-        <v>92</v>
-      </c>
-      <c r="M38">
-        <v>20</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="H38" s="11"/>
       <c r="N38">
         <v>120</v>
       </c>
-      <c r="Q38" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="39" spans="2:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q38" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R38" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19" ht="68" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>514</v>
+        <v>95</v>
+      </c>
+      <c r="C39" t="s">
+        <v>50</v>
+      </c>
+      <c r="D39" t="s">
+        <v>51</v>
       </c>
       <c r="E39" t="s">
         <v>17</v>
+      </c>
+      <c r="F39" t="s">
+        <v>18</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="H39" s="19" t="s">
-        <v>515</v>
+      <c r="H39" s="20" t="s">
+        <v>477</v>
+      </c>
+      <c r="I39" t="s">
+        <v>87</v>
+      </c>
+      <c r="J39">
+        <v>0</v>
+      </c>
+      <c r="K39" t="s">
+        <v>92</v>
+      </c>
+      <c r="M39">
+        <v>20</v>
       </c>
       <c r="N39">
         <v>120</v>
       </c>
-    </row>
-    <row r="40" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+      <c r="Q39" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R39" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" s="77" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B40" s="77" t="s">
+        <v>503</v>
+      </c>
+      <c r="E40" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F40" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="78" t="s">
+        <v>96</v>
+      </c>
+      <c r="H40" s="79" t="s">
+        <v>504</v>
+      </c>
+      <c r="N40" s="77">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
         <v>97</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>50</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D41" t="s">
         <v>51</v>
       </c>
-      <c r="E40" t="s">
-        <v>17</v>
-      </c>
-      <c r="F40" t="s">
+      <c r="E41" t="s">
+        <v>17</v>
+      </c>
+      <c r="F41" t="s">
         <v>33</v>
       </c>
-      <c r="G40" s="8" t="s">
+      <c r="G41" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H40" s="11"/>
-      <c r="N40">
-        <v>120</v>
-      </c>
-      <c r="Q40" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="41" spans="2:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>452</v>
-      </c>
-      <c r="G41" s="8" t="s">
-        <v>489</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>516</v>
-      </c>
+      <c r="H41" s="11"/>
       <c r="N41">
         <v>120</v>
       </c>
-    </row>
-    <row r="42" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
+      <c r="Q41" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R41" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" s="77" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B42" s="77" t="s">
+        <v>449</v>
+      </c>
+      <c r="C42" s="77" t="s">
+        <v>529</v>
+      </c>
+      <c r="F42" s="77" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="78" t="s">
+        <v>478</v>
+      </c>
+      <c r="H42" s="80" t="s">
+        <v>505</v>
+      </c>
+      <c r="N42" s="77">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
         <v>99</v>
-      </c>
-      <c r="C42" t="s">
-        <v>50</v>
-      </c>
-      <c r="D42" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" t="s">
-        <v>17</v>
-      </c>
-      <c r="G42" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="H42" s="19" t="s">
-        <v>490</v>
-      </c>
-      <c r="I42" t="s">
-        <v>102</v>
-      </c>
-      <c r="L42" t="s">
-        <v>103</v>
-      </c>
-      <c r="M42" t="s">
-        <v>104</v>
-      </c>
-      <c r="N42">
-        <v>120</v>
-      </c>
-      <c r="Q42" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="43" spans="2:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>105</v>
       </c>
       <c r="C43" t="s">
         <v>50</v>
@@ -6953,103 +7357,121 @@
         <v>17</v>
       </c>
       <c r="G43" s="8" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H43" s="19" t="s">
-        <v>491</v>
+        <v>479</v>
       </c>
       <c r="I43" t="s">
-        <v>108</v>
-      </c>
-      <c r="J43">
-        <v>30</v>
-      </c>
-      <c r="K43">
-        <v>30</v>
-      </c>
-      <c r="M43">
-        <v>30</v>
+        <v>102</v>
+      </c>
+      <c r="L43" t="s">
+        <v>103</v>
+      </c>
+      <c r="M43" t="s">
+        <v>104</v>
       </c>
       <c r="N43">
         <v>120</v>
       </c>
-      <c r="Q43" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="44" spans="2:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="Q43" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R43" t="s">
+        <v>545</v>
+      </c>
+      <c r="S43" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" ht="68" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
-        <v>517</v>
+        <v>105</v>
+      </c>
+      <c r="C44" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" t="s">
+        <v>51</v>
       </c>
       <c r="E44" t="s">
         <v>17</v>
       </c>
       <c r="G44" s="8" t="s">
-        <v>518</v>
+        <v>106</v>
       </c>
       <c r="H44" s="19" t="s">
-        <v>519</v>
+        <v>480</v>
+      </c>
+      <c r="I44" t="s">
+        <v>108</v>
+      </c>
+      <c r="J44">
+        <v>30</v>
+      </c>
+      <c r="K44">
+        <v>30</v>
+      </c>
+      <c r="M44">
+        <v>30</v>
       </c>
       <c r="N44">
         <v>120</v>
       </c>
-    </row>
-    <row r="45" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>450</v>
-      </c>
-      <c r="E45" t="s">
-        <v>17</v>
-      </c>
-      <c r="G45" s="8" t="s">
-        <v>492</v>
-      </c>
-      <c r="H45" s="19"/>
-      <c r="N45">
+      <c r="Q44" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R44" t="s">
+        <v>545</v>
+      </c>
+      <c r="S44" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="45" spans="2:19" s="77" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B45" s="77" t="s">
+        <v>506</v>
+      </c>
+      <c r="E45" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="G45" s="78" t="s">
+        <v>507</v>
+      </c>
+      <c r="H45" s="79" t="s">
+        <v>508</v>
+      </c>
+      <c r="N45" s="77">
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="2:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>109</v>
+        <v>447</v>
       </c>
       <c r="C46" t="s">
         <v>50</v>
       </c>
       <c r="D46" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E46" t="s">
         <v>17</v>
       </c>
-      <c r="G46" s="19" t="s">
-        <v>110</v>
-      </c>
-      <c r="H46" s="19" t="s">
-        <v>493</v>
-      </c>
-      <c r="I46" t="s">
-        <v>102</v>
-      </c>
-      <c r="J46">
-        <v>0.35</v>
-      </c>
-      <c r="K46">
-        <v>0.7</v>
-      </c>
-      <c r="M46" t="s">
-        <v>111</v>
-      </c>
+      <c r="G46" s="8" t="s">
+        <v>481</v>
+      </c>
+      <c r="H46" s="19"/>
       <c r="N46">
         <v>120</v>
       </c>
-      <c r="Q46" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="47" spans="2:17" ht="17" x14ac:dyDescent="0.2">
+      <c r="R46" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C47" t="s">
         <v>50</v>
@@ -7061,65 +7483,100 @@
         <v>17</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="H47" s="11" t="s">
-        <v>522</v>
+        <v>110</v>
+      </c>
+      <c r="H47" s="19" t="s">
+        <v>482</v>
       </c>
       <c r="I47" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="J47">
-        <v>15</v>
+        <v>0.35</v>
       </c>
       <c r="K47">
-        <v>15</v>
-      </c>
-      <c r="M47">
-        <v>15</v>
+        <v>0.7</v>
+      </c>
+      <c r="M47" t="s">
+        <v>111</v>
       </c>
       <c r="N47">
         <v>120</v>
       </c>
-      <c r="Q47" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="48" spans="2:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q47" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R47" t="s">
+        <v>545</v>
+      </c>
+      <c r="S47" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
-        <v>520</v>
+        <v>112</v>
+      </c>
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" t="s">
+        <v>51</v>
       </c>
       <c r="E48" t="s">
         <v>17</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>521</v>
+        <v>113</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>523</v>
+        <v>511</v>
+      </c>
+      <c r="I48" t="s">
+        <v>108</v>
+      </c>
+      <c r="J48">
+        <v>15</v>
+      </c>
+      <c r="K48">
+        <v>15</v>
+      </c>
+      <c r="M48">
+        <v>15</v>
       </c>
       <c r="N48">
         <v>120</v>
       </c>
-    </row>
-    <row r="49" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B49" t="s">
-        <v>447</v>
-      </c>
-      <c r="E49" t="s">
-        <v>17</v>
-      </c>
-      <c r="G49" s="19" t="s">
-        <v>494</v>
-      </c>
-      <c r="H49" s="11"/>
-      <c r="N49">
+      <c r="Q48" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R48" t="s">
+        <v>545</v>
+      </c>
+      <c r="S48" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="49" spans="2:19" s="77" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B49" s="77" t="s">
+        <v>509</v>
+      </c>
+      <c r="E49" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="G49" s="79" t="s">
+        <v>510</v>
+      </c>
+      <c r="H49" s="80" t="s">
+        <v>512</v>
+      </c>
+      <c r="N49" s="77">
         <v>120</v>
       </c>
     </row>
-    <row r="50" spans="2:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="50" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
-        <v>115</v>
+        <v>444</v>
       </c>
       <c r="C50" t="s">
         <v>50</v>
@@ -7130,37 +7587,20 @@
       <c r="E50" t="s">
         <v>17</v>
       </c>
-      <c r="F50" t="s">
-        <v>18</v>
-      </c>
       <c r="G50" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="H50" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="I50" t="s">
-        <v>108</v>
-      </c>
-      <c r="J50">
-        <v>-3</v>
-      </c>
-      <c r="K50">
-        <v>3</v>
-      </c>
-      <c r="L50">
-        <v>1E-3</v>
-      </c>
+        <v>483</v>
+      </c>
+      <c r="H50" s="11"/>
       <c r="N50">
         <v>120</v>
       </c>
-      <c r="Q50" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="51" spans="2:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="R50" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="51" spans="2:19" ht="51" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C51" t="s">
         <v>50</v>
@@ -7175,30 +7615,36 @@
         <v>18</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>495</v>
+        <v>117</v>
       </c>
       <c r="I51" t="s">
         <v>108</v>
       </c>
       <c r="J51">
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="K51">
-        <v>10</v>
+        <v>3</v>
+      </c>
+      <c r="L51">
+        <v>1E-3</v>
       </c>
       <c r="N51">
         <v>120</v>
       </c>
-      <c r="Q51" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="52" spans="2:17" ht="68" x14ac:dyDescent="0.2">
+      <c r="Q51" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R51" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="52" spans="2:19" ht="34" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C52" t="s">
         <v>50</v>
@@ -7209,131 +7655,152 @@
       <c r="E52" t="s">
         <v>17</v>
       </c>
-      <c r="F52" s="8" t="s">
-        <v>121</v>
+      <c r="F52" t="s">
+        <v>18</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>122</v>
-      </c>
-      <c r="H52" s="19" t="s">
-        <v>496</v>
+        <v>119</v>
+      </c>
+      <c r="H52" s="11" t="s">
+        <v>484</v>
       </c>
       <c r="I52" t="s">
-        <v>124</v>
-      </c>
-      <c r="M52" t="s">
-        <v>125</v>
+        <v>108</v>
+      </c>
+      <c r="J52">
+        <v>0</v>
+      </c>
+      <c r="K52">
+        <v>10</v>
       </c>
       <c r="N52">
         <v>120</v>
       </c>
-    </row>
-    <row r="53" spans="2:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>126</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="Q52" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R52" s="34" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="53" spans="2:19" ht="51" x14ac:dyDescent="0.2">
+      <c r="B53" s="42" t="s">
+        <v>536</v>
+      </c>
+      <c r="C53" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D53" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E53" t="s">
-        <v>17</v>
-      </c>
-      <c r="F53" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="G53" s="19"/>
-      <c r="H53" s="19"/>
+      <c r="E53" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F53" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="G53" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="H53" s="43" t="s">
+        <v>485</v>
+      </c>
+      <c r="I53" s="42" t="s">
+        <v>124</v>
+      </c>
+      <c r="J53" s="42"/>
+      <c r="K53" s="42"/>
+      <c r="L53" s="42"/>
+      <c r="M53" s="42" t="s">
+        <v>125</v>
+      </c>
       <c r="N53">
         <v>120</v>
       </c>
-    </row>
-    <row r="54" spans="2:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="R53" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="2:19" ht="34" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C54" t="s">
         <v>50</v>
       </c>
       <c r="D54" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E54" t="s">
         <v>17</v>
       </c>
-      <c r="G54" s="19" t="s">
-        <v>128</v>
-      </c>
-      <c r="H54" s="19" t="s">
-        <v>497</v>
-      </c>
-      <c r="I54" t="s">
-        <v>454</v>
-      </c>
-      <c r="M54">
-        <v>135</v>
-      </c>
+      <c r="F54" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
       <c r="N54">
         <v>120</v>
       </c>
-      <c r="Q54" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="55" spans="2:17" ht="51" x14ac:dyDescent="0.2">
+      <c r="R54" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="2:19" ht="34" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>524</v>
+        <v>127</v>
+      </c>
+      <c r="C55" t="s">
+        <v>50</v>
+      </c>
+      <c r="D55" t="s">
+        <v>51</v>
+      </c>
+      <c r="E55" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" t="s">
+        <v>18</v>
       </c>
       <c r="G55" s="19" t="s">
-        <v>525</v>
+        <v>128</v>
       </c>
       <c r="H55" s="19" t="s">
-        <v>526</v>
+        <v>486</v>
+      </c>
+      <c r="I55" t="s">
+        <v>450</v>
+      </c>
+      <c r="M55">
+        <v>135</v>
       </c>
       <c r="N55">
         <v>120</v>
       </c>
-    </row>
-    <row r="56" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
+      <c r="Q55" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R55" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="56" spans="2:19" s="77" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B56" s="77" t="s">
+        <v>513</v>
+      </c>
+      <c r="G56" s="79" t="s">
+        <v>514</v>
+      </c>
+      <c r="H56" s="79" t="s">
+        <v>515</v>
+      </c>
+      <c r="N56" s="77">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="2:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="B57" t="s">
         <v>130</v>
-      </c>
-      <c r="C56" t="s">
-        <v>50</v>
-      </c>
-      <c r="D56" t="s">
-        <v>16</v>
-      </c>
-      <c r="E56" t="s">
-        <v>59</v>
-      </c>
-      <c r="G56" s="8" t="s">
-        <v>131</v>
-      </c>
-      <c r="H56" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="I56" t="s">
-        <v>132</v>
-      </c>
-      <c r="J56">
-        <v>0</v>
-      </c>
-      <c r="K56">
-        <v>4</v>
-      </c>
-      <c r="N56">
-        <v>120</v>
-      </c>
-      <c r="Q56" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="57" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B57" t="s">
-        <v>133</v>
       </c>
       <c r="C57" t="s">
         <v>50</v>
@@ -7342,153 +7809,139 @@
         <v>51</v>
       </c>
       <c r="E57" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="G57" s="8" t="s">
-        <v>498</v>
-      </c>
-      <c r="H57" s="11" t="s">
-        <v>499</v>
+        <v>131</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>101</v>
       </c>
       <c r="I57" t="s">
-        <v>102</v>
+        <v>132</v>
       </c>
       <c r="J57">
         <v>0</v>
       </c>
       <c r="K57">
-        <v>4.2</v>
-      </c>
-      <c r="M57">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="N57">
         <v>120</v>
       </c>
-      <c r="Q57" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="58" spans="2:17" ht="34" x14ac:dyDescent="0.2">
+      <c r="Q57" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R57" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="58" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>527</v>
+        <v>133</v>
+      </c>
+      <c r="C58" t="s">
+        <v>50</v>
+      </c>
+      <c r="D58" t="s">
+        <v>51</v>
       </c>
       <c r="E58" t="s">
         <v>17</v>
       </c>
       <c r="G58" s="8" t="s">
-        <v>528</v>
+        <v>487</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>529</v>
+        <v>488</v>
       </c>
       <c r="I58" t="s">
         <v>102</v>
       </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+      <c r="K58">
+        <v>4.2</v>
+      </c>
+      <c r="M58">
+        <v>3.6</v>
+      </c>
       <c r="N58">
         <v>120</v>
       </c>
-    </row>
-    <row r="59" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
+      <c r="Q58" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R58" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="59" spans="2:19" s="77" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B59" s="77" t="s">
+        <v>516</v>
+      </c>
+      <c r="E59" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="G59" s="78" t="s">
+        <v>517</v>
+      </c>
+      <c r="H59" s="80" t="s">
+        <v>518</v>
+      </c>
+      <c r="I59" s="77" t="s">
+        <v>102</v>
+      </c>
+      <c r="N59" s="77">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="60" spans="2:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="B60" t="s">
         <v>135</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C60" t="s">
         <v>50</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D60" t="s">
         <v>51</v>
       </c>
-      <c r="E59" t="s">
-        <v>17</v>
-      </c>
-      <c r="F59" t="s">
+      <c r="E60" t="s">
+        <v>17</v>
+      </c>
+      <c r="F60" t="s">
         <v>33</v>
       </c>
-      <c r="G59" s="8" t="s">
+      <c r="G60" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="H59" s="11"/>
-      <c r="N59">
-        <v>120</v>
-      </c>
-      <c r="Q59" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="G60" s="8"/>
       <c r="H60" s="11"/>
       <c r="N60">
         <v>120</v>
       </c>
-    </row>
-    <row r="61" spans="2:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="B61" t="s">
-        <v>137</v>
-      </c>
-      <c r="C61" t="s">
-        <v>50</v>
-      </c>
-      <c r="D61" t="s">
-        <v>51</v>
-      </c>
-      <c r="E61" t="s">
-        <v>17</v>
-      </c>
-      <c r="F61" t="s">
-        <v>33</v>
-      </c>
-      <c r="G61" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>530</v>
-      </c>
-      <c r="J61">
-        <v>0</v>
-      </c>
-      <c r="K61">
-        <v>1</v>
-      </c>
-      <c r="N61">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="Q60" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R60" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="61" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="G61" s="8"/>
+      <c r="H61" s="11"/>
+    </row>
+    <row r="62" spans="2:19" x14ac:dyDescent="0.2">
       <c r="G62" s="8"/>
       <c r="H62" s="11"/>
     </row>
-    <row r="63" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B63" t="s">
+    <row r="63" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="G63" s="8"/>
+      <c r="H63" s="11"/>
+    </row>
+    <row r="64" spans="2:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="B64" t="s">
         <v>139</v>
-      </c>
-      <c r="C63" t="s">
-        <v>50</v>
-      </c>
-      <c r="D63" t="s">
-        <v>51</v>
-      </c>
-      <c r="E63" t="s">
-        <v>17</v>
-      </c>
-      <c r="F63" t="s">
-        <v>18</v>
-      </c>
-      <c r="G63" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="H63" s="11"/>
-      <c r="N63">
-        <v>20</v>
-      </c>
-      <c r="Q63" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="64" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B64" t="s">
-        <v>141</v>
       </c>
       <c r="C64" t="s">
         <v>50</v>
@@ -7503,298 +7956,346 @@
         <v>18</v>
       </c>
       <c r="G64" s="19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H64" s="11"/>
+      <c r="I64" t="s">
+        <v>80</v>
+      </c>
+      <c r="J64">
+        <v>22.5</v>
+      </c>
+      <c r="K64">
+        <v>23.5</v>
+      </c>
+      <c r="M64">
+        <v>23</v>
+      </c>
       <c r="N64">
         <v>20</v>
       </c>
-      <c r="Q64" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="66" spans="2:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="B66" t="s">
+      <c r="Q64" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R64" t="s">
+        <v>545</v>
+      </c>
+      <c r="S64" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="65" spans="2:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="B65" t="s">
+        <v>141</v>
+      </c>
+      <c r="C65" t="s">
+        <v>50</v>
+      </c>
+      <c r="D65" t="s">
+        <v>51</v>
+      </c>
+      <c r="E65" t="s">
+        <v>17</v>
+      </c>
+      <c r="F65" t="s">
+        <v>18</v>
+      </c>
+      <c r="G65" s="19" t="s">
+        <v>142</v>
+      </c>
+      <c r="H65" s="11"/>
+      <c r="M65">
+        <v>37</v>
+      </c>
+      <c r="N65">
+        <v>20</v>
+      </c>
+      <c r="Q65" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R65" t="s">
+        <v>545</v>
+      </c>
+      <c r="S65" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="67" spans="2:19" s="77" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B67" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="E66" t="s">
-        <v>17</v>
-      </c>
-      <c r="F66" t="s">
+      <c r="E67" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F67" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="G66" s="8" t="s">
+      <c r="G67" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="H66" s="8" t="s">
-        <v>500</v>
-      </c>
-      <c r="I66" t="s">
+      <c r="H67" s="78" t="s">
+        <v>489</v>
+      </c>
+      <c r="I67" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="J66">
+      <c r="J67" s="77">
         <v>0.01</v>
       </c>
-      <c r="K66">
+      <c r="K67" s="77">
         <v>60</v>
       </c>
-      <c r="L66">
+      <c r="L67" s="77">
         <v>0.01</v>
       </c>
-      <c r="M66">
+      <c r="M67" s="77">
         <v>60</v>
       </c>
-      <c r="N66">
+      <c r="N67" s="77">
         <v>120</v>
       </c>
     </row>
-    <row r="67" spans="2:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="B67" t="s">
+    <row r="68" spans="2:19" s="77" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B68" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D68" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="E67" t="s">
-        <v>17</v>
-      </c>
-      <c r="F67" s="8" t="s">
+      <c r="E68" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F68" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="G67" s="8" t="s">
+      <c r="G68" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="H67" s="27" t="s">
-        <v>501</v>
-      </c>
-      <c r="I67" t="s">
+      <c r="H68" s="78" t="s">
+        <v>490</v>
+      </c>
+      <c r="I68" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="J67" t="s">
+      <c r="J68" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="K67" t="s">
+      <c r="K68" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="L67" t="s">
+      <c r="L68" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="M67" t="s">
+      <c r="M68" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="N67">
+      <c r="N68" s="77">
         <v>120</v>
       </c>
     </row>
-    <row r="68" spans="2:17" ht="17" x14ac:dyDescent="0.2">
-      <c r="B68" t="s">
+    <row r="69" spans="2:19" s="77" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B69" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D69" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="E68" t="s">
-        <v>17</v>
-      </c>
-      <c r="F68" t="s">
+      <c r="E69" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="G68" s="8" t="s">
+      <c r="G69" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="H68" s="8" t="s">
-        <v>502</v>
-      </c>
-      <c r="I68" t="s">
+      <c r="H69" s="78" t="s">
+        <v>491</v>
+      </c>
+      <c r="I69" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="J68">
+      <c r="J69" s="77">
         <v>0.01</v>
       </c>
-      <c r="K68">
+      <c r="K69" s="77">
         <v>60</v>
       </c>
-      <c r="L68">
+      <c r="L69" s="77">
         <v>0.01</v>
       </c>
-      <c r="M68">
+      <c r="M69" s="77">
         <v>60</v>
       </c>
-      <c r="N68">
+      <c r="N69" s="77">
         <v>120</v>
       </c>
-      <c r="Q68" s="74" t="s">
-        <v>538</v>
-      </c>
-    </row>
-    <row r="69" spans="2:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="B69" t="s">
-        <v>504</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="Q69" s="81" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="70" spans="2:19" s="77" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B70" s="77" t="s">
+        <v>493</v>
+      </c>
+      <c r="D70" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="E69" t="s">
-        <v>17</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="E70" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="G69" s="8" t="s">
+      <c r="G70" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="H69" s="8" t="s">
-        <v>505</v>
-      </c>
-      <c r="J69" s="49" t="s">
+      <c r="H70" s="78" t="s">
+        <v>494</v>
+      </c>
+      <c r="J70" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="K69" s="49"/>
-      <c r="M69">
+      <c r="K70" s="82"/>
+      <c r="M70" s="77">
         <v>0</v>
       </c>
-      <c r="N69">
+      <c r="N70" s="77">
         <v>120</v>
       </c>
     </row>
-    <row r="70" spans="2:17" ht="34" x14ac:dyDescent="0.2">
-      <c r="B70" t="s">
-        <v>503</v>
-      </c>
-      <c r="D70" t="s">
+    <row r="71" spans="2:19" s="77" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B71" s="77" t="s">
+        <v>492</v>
+      </c>
+      <c r="D71" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="E70" t="s">
-        <v>17</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E71" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="G70" s="8" t="s">
+      <c r="G71" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="H70" s="27" t="s">
-        <v>506</v>
-      </c>
-      <c r="J70" s="49" t="s">
+      <c r="H71" s="78" t="s">
+        <v>495</v>
+      </c>
+      <c r="J71" s="82" t="s">
         <v>36</v>
       </c>
-      <c r="K70" s="49"/>
-      <c r="M70">
+      <c r="K71" s="82"/>
+      <c r="M71" s="77">
         <v>0</v>
       </c>
-      <c r="N70">
+      <c r="N71" s="77">
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="2:17" ht="51" x14ac:dyDescent="0.2">
-      <c r="B71" t="s">
+    <row r="72" spans="2:19" s="77" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="B72" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D72" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="E71" t="s">
-        <v>17</v>
-      </c>
-      <c r="F71" t="s">
+      <c r="E72" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="77" t="s">
         <v>18</v>
       </c>
-      <c r="G71" s="8" t="s">
+      <c r="G72" s="78" t="s">
         <v>41</v>
       </c>
-      <c r="H71" s="8" t="s">
-        <v>507</v>
-      </c>
-      <c r="I71" t="s">
+      <c r="H72" s="78" t="s">
+        <v>496</v>
+      </c>
+      <c r="I72" s="77" t="s">
         <v>21</v>
       </c>
-      <c r="J71">
+      <c r="J72" s="77">
         <v>0.01</v>
       </c>
-      <c r="K71">
+      <c r="K72" s="77">
         <v>60</v>
       </c>
-      <c r="L71">
+      <c r="L72" s="77">
         <v>0.01</v>
       </c>
-      <c r="M71">
+      <c r="M72" s="77">
         <v>60</v>
       </c>
-      <c r="N71">
+      <c r="N72" s="77">
         <v>120</v>
       </c>
     </row>
-    <row r="72" spans="2:17" ht="68" x14ac:dyDescent="0.2">
-      <c r="B72" s="35" t="s">
+    <row r="73" spans="2:19" s="77" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="B73" s="77" t="s">
         <v>44</v>
       </c>
-      <c r="C72" s="35"/>
-      <c r="D72" s="35" t="s">
+      <c r="D73" s="77" t="s">
         <v>16</v>
       </c>
-      <c r="E72" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="F72" s="35" t="s">
+      <c r="E73" s="77" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73" s="77" t="s">
         <v>45</v>
       </c>
-      <c r="G72" s="36" t="s">
+      <c r="G73" s="78" t="s">
         <v>46</v>
       </c>
-      <c r="H72" s="36" t="s">
-        <v>531</v>
-      </c>
-      <c r="I72" s="35"/>
-      <c r="J72" s="35"/>
-      <c r="K72" s="35"/>
-      <c r="L72" s="35"/>
-      <c r="M72" s="35"/>
-      <c r="N72">
+      <c r="H73" s="78" t="s">
+        <v>519</v>
+      </c>
+      <c r="N73" s="77">
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B74" t="s">
-        <v>508</v>
-      </c>
-      <c r="C74" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="75" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
-        <v>509</v>
+        <v>497</v>
       </c>
       <c r="C75" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="76" spans="2:17" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
-        <v>510</v>
+        <v>498</v>
       </c>
       <c r="C76" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="77" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B77" t="s">
+        <v>499</v>
+      </c>
+      <c r="C77" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="18">
     <mergeCell ref="U1:V1"/>
-    <mergeCell ref="J69:K69"/>
     <mergeCell ref="J70:K70"/>
+    <mergeCell ref="J71:K71"/>
     <mergeCell ref="N1:N2"/>
     <mergeCell ref="O1:O2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="Q1:S1"/>
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -8071,38 +8572,38 @@
       <c r="D1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="55" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="51" t="s">
+      <c r="F1" s="56"/>
+      <c r="G1" s="55" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="52"/>
+      <c r="H1" s="56"/>
     </row>
     <row r="2" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="57" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="55"/>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="60" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="58"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="62"/>
     </row>
     <row r="4" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -8112,12 +8613,12 @@
         <v>370</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="61" t="s">
+      <c r="D4" s="63"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="65" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="62"/>
+      <c r="G4" s="66"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -8128,12 +8629,12 @@
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="65"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="63" t="s">
+      <c r="D5" s="69"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="67" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="64"/>
+      <c r="G5" s="68"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
@@ -8144,12 +8645,12 @@
         <v>372</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="61" t="s">
+      <c r="D6" s="63"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="65" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="62"/>
+      <c r="G6" s="66"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
@@ -8160,12 +8661,12 @@
         <v>373</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="65"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="63" t="s">
+      <c r="D7" s="69"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="67" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="64"/>
+      <c r="G7" s="68"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
@@ -8176,12 +8677,12 @@
         <v>53</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="59"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="61" t="s">
+      <c r="D8" s="63"/>
+      <c r="E8" s="64"/>
+      <c r="F8" s="65" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="62"/>
+      <c r="G8" s="66"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="66" thickBot="1" x14ac:dyDescent="0.25">
@@ -8192,25 +8693,25 @@
         <v>374</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="65"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="65"/>
-      <c r="G9" s="66"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="70"/>
       <c r="H9" s="6" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="71" t="s">
         <v>376</v>
       </c>
-      <c r="C10" s="68"/>
-      <c r="D10" s="68"/>
-      <c r="E10" s="68"/>
-      <c r="F10" s="68"/>
-      <c r="G10" s="68"/>
-      <c r="H10" s="69"/>
+      <c r="C10" s="72"/>
+      <c r="D10" s="72"/>
+      <c r="E10" s="72"/>
+      <c r="F10" s="72"/>
+      <c r="G10" s="72"/>
+      <c r="H10" s="73"/>
     </row>
     <row r="11" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -8222,12 +8723,12 @@
       <c r="C11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="63" t="s">
+      <c r="D11" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E11" s="64"/>
-      <c r="F11" s="65"/>
-      <c r="G11" s="66"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="70"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -8240,12 +8741,12 @@
       <c r="C12" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="65" t="s">
         <v>378</v>
       </c>
-      <c r="E12" s="62"/>
-      <c r="F12" s="59"/>
-      <c r="G12" s="60"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="63"/>
+      <c r="G12" s="64"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -8258,12 +8759,12 @@
       <c r="C13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="63" t="s">
+      <c r="D13" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="64"/>
-      <c r="F13" s="65"/>
-      <c r="G13" s="66"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="70"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -8274,12 +8775,12 @@
         <v>380</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="65" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="62"/>
-      <c r="F14" s="59"/>
-      <c r="G14" s="60"/>
+      <c r="E14" s="66"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="64"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -8292,12 +8793,12 @@
       <c r="C15" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="63" t="s">
+      <c r="D15" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="64"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="66"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="70"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="53" thickBot="1" x14ac:dyDescent="0.25">
@@ -8310,12 +8811,12 @@
       <c r="C16" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="65" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="62"/>
-      <c r="F16" s="59"/>
-      <c r="G16" s="60"/>
+      <c r="E16" s="66"/>
+      <c r="F16" s="63"/>
+      <c r="G16" s="64"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="53" thickBot="1" x14ac:dyDescent="0.25">
@@ -8328,12 +8829,12 @@
       <c r="C17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D17" s="63" t="s">
+      <c r="D17" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="64"/>
-      <c r="F17" s="65"/>
-      <c r="G17" s="66"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -8346,12 +8847,12 @@
       <c r="C18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="65" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="62"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="60"/>
+      <c r="E18" s="66"/>
+      <c r="F18" s="63"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
@@ -8364,12 +8865,12 @@
       <c r="C19" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="D19" s="63" t="s">
+      <c r="D19" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E19" s="64"/>
-      <c r="F19" s="65"/>
-      <c r="G19" s="66"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="70"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -8382,12 +8883,12 @@
       <c r="C20" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="65" t="s">
         <v>378</v>
       </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="59"/>
-      <c r="G20" s="60"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="63"/>
+      <c r="G20" s="64"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="131" thickBot="1" x14ac:dyDescent="0.25">
@@ -8400,12 +8901,12 @@
       <c r="C21" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="63" t="s">
+      <c r="D21" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E21" s="64"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="66"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="70"/>
       <c r="H21" s="6" t="s">
         <v>389</v>
       </c>
@@ -8420,12 +8921,12 @@
       <c r="C22" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="65" t="s">
         <v>378</v>
       </c>
-      <c r="E22" s="62"/>
-      <c r="F22" s="59"/>
-      <c r="G22" s="60"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="63"/>
+      <c r="G22" s="64"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
@@ -8450,13 +8951,13 @@
     </row>
     <row r="24" spans="1:8" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="70" t="s">
+      <c r="B24" s="74" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="71"/>
-      <c r="D24" s="71"/>
-      <c r="E24" s="71"/>
-      <c r="F24" s="72"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="76"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -8524,13 +9025,13 @@
     </row>
     <row r="29" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="60" t="s">
         <v>396</v>
       </c>
-      <c r="C29" s="57"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="57"/>
-      <c r="F29" s="58"/>
+      <c r="C29" s="61"/>
+      <c r="D29" s="61"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="62"/>
     </row>
     <row r="30" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
@@ -8688,13 +9189,13 @@
     </row>
     <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="56" t="s">
+      <c r="B41" s="60" t="s">
         <v>408</v>
       </c>
-      <c r="C41" s="57"/>
-      <c r="D41" s="57"/>
-      <c r="E41" s="57"/>
-      <c r="F41" s="58"/>
+      <c r="C41" s="61"/>
+      <c r="D41" s="61"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="62"/>
     </row>
     <row r="42" spans="1:6" ht="79" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">

</xml_diff>

<commit_message>
auto minicomb setup funtion, auto email sent , arduino latch change, edfa input power measure, keyword list update
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\astrocomb\KeckLFC-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AFFCF8A-71EA-467B-A115-01732778991F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45338A3C-1B30-4106-ACB3-D3E6DCA1985F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,18 +49,35 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={A12C35E2-454A-E044-AA6F-90F49746B87E}</author>
-    <author>tc={8E385BD7-CB1A-6B4B-9A34-FB5994ACFAE5}</author>
-    <author>tc={571BE3E8-65E3-834D-971C-F4F7A8109EE5}</author>
+    <author>tc={D3C2FCEF-3C80-CE41-B2E7-DD6B9F50FECC}</author>
     <author>tc={7CFD64FF-9EC6-294B-9BEF-9777389E8580}</author>
     <author>tc={C35B52B2-9CE8-754E-ABC4-B8F8053DF728}</author>
     <author>tc={34097AA0-B693-B145-BC43-7609B0047A34}</author>
     <author>tc={203D725E-9B82-8244-B953-050D9845AB73}</author>
+    <author>tc={43EE3C90-F8DC-844A-90D6-FE4B195F4D19}</author>
+    <author>tc={734F326A-1433-1D42-B27D-80F6AB5B01F2}</author>
+    <author>tc={65E7EA58-AEBE-9E43-B699-4C2E84AB06AE}</author>
+    <author>tc={9270FBFE-6EFE-1048-9F63-76932967FCB6}</author>
     <author>tc={430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}</author>
     <author>tc={897DD710-C2AF-F348-9BE6-70FC899ABE2C}</author>
+    <author>tc={D3AE0575-FA6E-1242-8525-02B45DC7B747}</author>
     <author>tc={EF222E0F-25E5-D547-9265-DB5E371F9AC7}</author>
+    <author>tc={91A521E9-8C58-AA4E-9DB6-3B7C40324E9D}</author>
     <author>tc={E8CBB725-766B-9540-AD26-3D88E8136C7F}</author>
+    <author>tc={3A13DE3F-FDB4-D54D-8D34-92EEE889D658}</author>
+    <author>tc={A2C7FC53-1505-8A45-99CE-70D3C4FD5518}</author>
+    <author>tc={3FE72732-F7D7-6A44-A781-0E38E560C217}</author>
+    <author>tc={0490C4F1-599B-AB44-B1CC-7E63E4E8065B}</author>
     <author>tc={C82D50AC-F6ED-B841-AC03-1967E28B201E}</author>
     <author>tc={C7739DC9-A5B2-EF49-9CE8-416CEC34862C}</author>
+    <author>tc={3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}</author>
+    <author>tc={B06CDA75-3D09-3A4C-9CA2-5DAFC7D0A49C}</author>
+    <author>tc={6ED25ED1-E5D3-0547-B2AE-B068D8D2FCAB}</author>
+    <author>tc={766C4F7D-809F-8546-936F-F77DAB106C65}</author>
+    <author>tc={BF9BF349-FB0E-2A49-BEAB-473752D32B3F}</author>
+    <author>tc={506BB1FA-65AC-2844-8BBF-2A90D38F6707}</author>
+    <author>tc={1DDB399D-F138-F04F-99C1-98F0475A5FB6}</author>
+    <author>tc={30C5F121-C7F3-DF45-95C8-DA0E6762ECA7}</author>
     <author>tc={E0A4D72A-0143-6945-8315-0EBFC4A9749A}</author>
   </authors>
   <commentList>
@@ -72,25 +89,17 @@
     Please fill these in (used in help message for users, see LFC.xml.sin file)</t>
       </text>
     </comment>
-    <comment ref="C5" authorId="1" shapeId="0" xr:uid="{8E385BD7-CB1A-6B4B-9A34-FB5994ACFAE5}">
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{D3C2FCEF-3C80-CE41-B2E7-DD6B9F50FECC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Needs to be float number
+    Split into two keywords?
 Reply:
-    Or the keyword type needs to be boolean or enumerated</t>
+    How to read after reset?</t>
       </text>
     </comment>
-    <comment ref="C6" authorId="2" shapeId="0" xr:uid="{571BE3E8-65E3-834D-971C-F4F7A8109EE5}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Needs to be float number</t>
-      </text>
-    </comment>
-    <comment ref="C9" authorId="3" shapeId="0" xr:uid="{7CFD64FF-9EC6-294B-9BEF-9777389E8580}">
+    <comment ref="C7" authorId="2" shapeId="0" xr:uid="{7CFD64FF-9EC6-294B-9BEF-9777389E8580}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -98,7 +107,7 @@
     Implemented as 1 or 0, 1=on and 0=off</t>
       </text>
     </comment>
-    <comment ref="F11" authorId="4" shapeId="0" xr:uid="{C35B52B2-9CE8-754E-ABC4-B8F8053DF728}">
+    <comment ref="F9" authorId="3" shapeId="0" xr:uid="{C35B52B2-9CE8-754E-ABC4-B8F8053DF728}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -106,7 +115,7 @@
     I implemented this as enumerated</t>
       </text>
     </comment>
-    <comment ref="F13" authorId="5" shapeId="0" xr:uid="{34097AA0-B693-B145-BC43-7609B0047A34}">
+    <comment ref="F11" authorId="4" shapeId="0" xr:uid="{34097AA0-B693-B145-BC43-7609B0047A34}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -114,23 +123,61 @@
     Please provide formats for float types. For example, float(%.2f)</t>
       </text>
     </comment>
-    <comment ref="C16" authorId="6" shapeId="0" xr:uid="{203D725E-9B82-8244-B953-050D9845AB73}">
+    <comment ref="C14" authorId="5" shapeId="0" xr:uid="{203D725E-9B82-8244-B953-050D9845AB73}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    If this keyword value is going to be either “pid” or “man”, it could be implemented as enumerated type, as in LFC_2BY2_SWITCH</t>
+    If this keyword value is going to be either “pid” or “man”, it could be implemented as enumerated type, as in LFC_2BY2_SWITCH
+Reply:
+    Implementing as boolean</t>
       </text>
     </comment>
-    <comment ref="B23" authorId="7" shapeId="0" xr:uid="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
+    <comment ref="B19" authorId="6" shapeId="0" xr:uid="{43EE3C90-F8DC-844A-90D6-FE4B195F4D19}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Maybe these are okay to remove?</t>
+    Fault or okay - boolean
+Reply:
+    0: Fault, 1: Normal</t>
       </text>
     </comment>
-    <comment ref="F35" authorId="8" shapeId="0" xr:uid="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
+    <comment ref="H19" authorId="7" shapeId="0" xr:uid="{734F326A-1433-1D42-B27D-80F6AB5B01F2}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    0:Fault, 1:Normal</t>
+      </text>
+    </comment>
+    <comment ref="N19" authorId="8" shapeId="0" xr:uid="{65E7EA58-AEBE-9E43-B699-4C2E84AB06AE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Please fill in</t>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="9" shapeId="0" xr:uid="{9270FBFE-6EFE-1048-9F63-76932967FCB6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Doesn’t have to be KTL keyword</t>
+      </text>
+    </comment>
+    <comment ref="B23" authorId="10" shapeId="0" xr:uid="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Maybe these are okay to remove?
+Reply:
+    Keep them and change names</t>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="11" shapeId="0" xr:uid="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -138,7 +185,17 @@
     Implementing as float</t>
       </text>
     </comment>
-    <comment ref="F36" authorId="9" shapeId="0" xr:uid="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
+    <comment ref="B36" authorId="12" shapeId="0" xr:uid="{D3AE0575-FA6E-1242-8525-02B45DC7B747}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not exposed to end user?
+Reply:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="F36" authorId="13" shapeId="0" xr:uid="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -146,7 +203,15 @@
     Not sure what type it’s supposed to be</t>
       </text>
     </comment>
-    <comment ref="F38" authorId="10" shapeId="0" xr:uid="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
+    <comment ref="B38" authorId="14" shapeId="0" xr:uid="{91A521E9-8C58-AA4E-9DB6-3B7C40324E9D}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="F38" authorId="15" shapeId="0" xr:uid="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -154,7 +219,39 @@
     Not sure what type it’s supposed to be</t>
       </text>
     </comment>
-    <comment ref="F55" authorId="11" shapeId="0" xr:uid="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
+    <comment ref="B42" authorId="16" shapeId="0" xr:uid="{3A13DE3F-FDB4-D54D-8D34-92EEE889D658}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="B44" authorId="17" shapeId="0" xr:uid="{A2C7FC53-1505-8A45-99CE-70D3C4FD5518}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="B47" authorId="18" shapeId="0" xr:uid="{3FE72732-F7D7-6A44-A781-0E38E560C217}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="B51" authorId="19" shapeId="0" xr:uid="{0490C4F1-599B-AB44-B1CC-7E63E4E8065B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="F55" authorId="20" shapeId="0" xr:uid="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -162,7 +259,7 @@
     Only 1-dimensional array allowed</t>
       </text>
     </comment>
-    <comment ref="F57" authorId="12" shapeId="0" xr:uid="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
+    <comment ref="F57" authorId="21" shapeId="0" xr:uid="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -170,7 +267,71 @@
     Implemented as float</t>
       </text>
     </comment>
-    <comment ref="H75" authorId="13" shapeId="0" xr:uid="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
+    <comment ref="B58" authorId="22" shapeId="0" xr:uid="{3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="B61" authorId="23" shapeId="0" xr:uid="{B06CDA75-3D09-3A4C-9CA2-5DAFC7D0A49C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Not needed</t>
+      </text>
+    </comment>
+    <comment ref="B69" authorId="24" shapeId="0" xr:uid="{6ED25ED1-E5D3-0547-B2AE-B068D8D2FCAB}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B71" authorId="25" shapeId="0" xr:uid="{766C4F7D-809F-8546-936F-F77DAB106C65}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B72" authorId="26" shapeId="0" xr:uid="{BF9BF349-FB0E-2A49-BEAB-473752D32B3F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B73" authorId="27" shapeId="0" xr:uid="{506BB1FA-65AC-2844-8BBF-2A90D38F6707}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B74" authorId="28" shapeId="0" xr:uid="{1DDB399D-F138-F04F-99C1-98F0475A5FB6}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B75" authorId="29" shapeId="0" xr:uid="{30C5F121-C7F3-DF45-95C8-DA0E6762ECA7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="H75" authorId="30" shapeId="0" xr:uid="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -201,7 +362,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="551">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="563">
   <si>
     <t>Keyword</t>
   </si>
@@ -1549,15 +1710,9 @@
     <t>mw</t>
   </si>
   <si>
-    <t>apc mode:450mw</t>
-  </si>
-  <si>
     <t>LFC_EDFA27_AUTO_ON</t>
   </si>
   <si>
-    <t>auto set power or current and turn on</t>
-  </si>
-  <si>
     <t>LFC_RFOSCI_ONOFF</t>
   </si>
   <si>
@@ -1579,9 +1734,6 @@
     <t>ma</t>
   </si>
   <si>
-    <t>acc:80mA</t>
-  </si>
-  <si>
     <t>none</t>
   </si>
   <si>
@@ -1645,12 +1797,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>LFC_TEMP1_TEST1</t>
-  </si>
-  <si>
-    <t>LFC_TEMP1_TEST2</t>
-  </si>
-  <si>
     <t>get all temp on USBdaq2</t>
   </si>
   <si>
@@ -1792,9 +1938,6 @@
     <t>value=none, read out amp current/value!=none, set to 4.1A</t>
   </si>
   <si>
-    <t>value==none, read input power voltage/value==1, reset latch circuit/value else, do nothing</t>
-  </si>
-  <si>
     <t>same as LFC_2BY2_SWITCH. Input value:1(represent YJ) or 2(represent HK) (input number only)</t>
   </si>
   <si>
@@ -1871,6 +2014,60 @@
   </si>
   <si>
     <t>if temp goes above threshold, trigger LFC_CLOSE_ALL and LFC_EMAIL</t>
+  </si>
+  <si>
+    <t>can test</t>
+  </si>
+  <si>
+    <t>test after comb on</t>
+  </si>
+  <si>
+    <t>float array(%.2f)</t>
+  </si>
+  <si>
+    <t>can test (10-25)</t>
+  </si>
+  <si>
+    <t>can test (145-155)</t>
+  </si>
+  <si>
+    <t>can test if off (check LFC_RFAMP_ONOFF, make sure it's off)</t>
+  </si>
+  <si>
+    <t>can test if off (check LFC_RFOSCI_ONOFF, make sure it's off)</t>
+  </si>
+  <si>
+    <t>Y (lockout)</t>
+  </si>
+  <si>
+    <t>can test (+/- 0.5 degrees)</t>
+  </si>
+  <si>
+    <t>can test (+/- 0.5 degrees from where it is)</t>
+  </si>
+  <si>
+    <t>LFC_TEMP_TEST1</t>
+  </si>
+  <si>
+    <t>LFC_TEMP_TEST2</t>
+  </si>
+  <si>
+    <t>LFC_EDFA27_INPUT_POWER</t>
+  </si>
+  <si>
+    <t>get input power of edfa27</t>
+  </si>
+  <si>
+    <t>LFC_EDFA23_INPUT_POWER</t>
+  </si>
+  <si>
+    <t>get input power of edfa23</t>
+  </si>
+  <si>
+    <t>LFC_MINICOMB_AUTO_SETUP</t>
+  </si>
+  <si>
+    <t>auto setup minicomb, im lock, if wrong, send email</t>
   </si>
 </sst>
 </file>
@@ -2013,14 +2210,13 @@
     </font>
     <font>
       <sz val="12"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF00B0F0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF00B0F0"/>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2088,13 +2284,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor rgb="FF000000"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -2270,7 +2467,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2297,9 +2494,8 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2390,13 +2586,23 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" xfId="26"/>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" xfId="25"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="25" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2429,6 +2635,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2497,8 +2706,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
-    <cellStyle name="Bad" xfId="26" builtinId="27"/>
+  <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
@@ -2846,44 +3054,107 @@
   <threadedComment ref="U1" dT="2024-05-25T16:13:18.71" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{A12C35E2-454A-E044-AA6F-90F49746B87E}">
     <text>Please fill these in (used in help message for users, see LFC.xml.sin file)</text>
   </threadedComment>
-  <threadedComment ref="C5" dT="2024-05-25T15:46:18.30" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{8E385BD7-CB1A-6B4B-9A34-FB5994ACFAE5}">
-    <text>Needs to be float number</text>
+  <threadedComment ref="B7" dT="2024-06-03T18:22:26.07" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{D3C2FCEF-3C80-CE41-B2E7-DD6B9F50FECC}">
+    <text>Split into two keywords?</text>
   </threadedComment>
-  <threadedComment ref="C5" dT="2024-05-25T15:47:16.72" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{3A85D8C2-1E59-E14F-AED4-0153EC258617}" parentId="{8E385BD7-CB1A-6B4B-9A34-FB5994ACFAE5}">
-    <text>Or the keyword type needs to be boolean or enumerated</text>
+  <threadedComment ref="B7" dT="2024-06-03T18:30:30.74" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{D5106230-4936-3E43-B433-25ED7C9F13BE}" parentId="{D3C2FCEF-3C80-CE41-B2E7-DD6B9F50FECC}">
+    <text>How to read after reset?</text>
   </threadedComment>
-  <threadedComment ref="C6" dT="2024-05-25T15:46:44.69" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{571BE3E8-65E3-834D-971C-F4F7A8109EE5}">
-    <text>Needs to be float number</text>
-  </threadedComment>
-  <threadedComment ref="C9" dT="2024-05-25T15:57:35.22" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{7CFD64FF-9EC6-294B-9BEF-9777389E8580}">
+  <threadedComment ref="C7" dT="2024-05-25T15:57:35.22" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{7CFD64FF-9EC6-294B-9BEF-9777389E8580}">
     <text>Implemented as 1 or 0, 1=on and 0=off</text>
   </threadedComment>
-  <threadedComment ref="F11" dT="2024-05-25T15:48:09.66" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C35B52B2-9CE8-754E-ABC4-B8F8053DF728}">
+  <threadedComment ref="F9" dT="2024-05-25T15:48:09.66" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C35B52B2-9CE8-754E-ABC4-B8F8053DF728}">
     <text>I implemented this as enumerated</text>
   </threadedComment>
-  <threadedComment ref="F13" dT="2024-05-25T16:17:43.67" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{34097AA0-B693-B145-BC43-7609B0047A34}">
+  <threadedComment ref="F11" dT="2024-05-25T16:17:43.67" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{34097AA0-B693-B145-BC43-7609B0047A34}">
     <text>Please provide formats for float types. For example, float(%.2f)</text>
   </threadedComment>
-  <threadedComment ref="C16" dT="2024-05-25T15:49:02.90" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{203D725E-9B82-8244-B953-050D9845AB73}">
+  <threadedComment ref="C14" dT="2024-05-25T15:49:02.90" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{203D725E-9B82-8244-B953-050D9845AB73}">
     <text>If this keyword value is going to be either “pid” or “man”, it could be implemented as enumerated type, as in LFC_2BY2_SWITCH</text>
+  </threadedComment>
+  <threadedComment ref="C14" dT="2024-06-03T20:29:43.17" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{038E729A-82CE-F148-AAB1-60ADED45E6B8}" parentId="{203D725E-9B82-8244-B953-050D9845AB73}">
+    <text>Implementing as boolean</text>
+  </threadedComment>
+  <threadedComment ref="B19" dT="2024-06-03T18:35:54.88" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{43EE3C90-F8DC-844A-90D6-FE4B195F4D19}">
+    <text>Fault or okay - boolean</text>
+  </threadedComment>
+  <threadedComment ref="B19" dT="2024-06-03T20:37:28.72" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{4F472B1F-3735-B649-9078-98AB15E83A44}" parentId="{43EE3C90-F8DC-844A-90D6-FE4B195F4D19}">
+    <text>0: Fault, 1: Normal</text>
+  </threadedComment>
+  <threadedComment ref="H19" dT="2024-06-03T20:37:48.93" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{734F326A-1433-1D42-B27D-80F6AB5B01F2}">
+    <text>0:Fault, 1:Normal</text>
+  </threadedComment>
+  <threadedComment ref="N19" dT="2024-06-03T20:31:30.31" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{65E7EA58-AEBE-9E43-B699-4C2E84AB06AE}">
+    <text>Please fill in</text>
+  </threadedComment>
+  <threadedComment ref="B21" dT="2024-06-03T18:40:46.49" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{9270FBFE-6EFE-1048-9F63-76932967FCB6}">
+    <text>Doesn’t have to be KTL keyword</text>
   </threadedComment>
   <threadedComment ref="B23" dT="2024-05-25T16:14:22.88" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
     <text>Maybe these are okay to remove?</text>
   </threadedComment>
+  <threadedComment ref="B23" dT="2024-06-03T18:43:05.98" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{5296AF8B-E0AA-1846-89CA-ED67E861F12F}" parentId="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
+    <text>Keep them and change names</text>
+  </threadedComment>
   <threadedComment ref="F35" dT="2024-05-25T16:23:38.53" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
     <text>Implementing as float</text>
+  </threadedComment>
+  <threadedComment ref="B36" dT="2024-06-03T18:54:55.02" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{D3AE0575-FA6E-1242-8525-02B45DC7B747}">
+    <text>Not exposed to end user?</text>
+  </threadedComment>
+  <threadedComment ref="B36" dT="2024-06-03T18:56:33.55" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{50BBA82F-D96D-894B-A5A6-CF02B225EDD9}" parentId="{D3AE0575-FA6E-1242-8525-02B45DC7B747}">
+    <text>Not needed</text>
   </threadedComment>
   <threadedComment ref="F36" dT="2024-05-25T16:27:45.79" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
     <text>Not sure what type it’s supposed to be</text>
   </threadedComment>
+  <threadedComment ref="B38" dT="2024-06-03T18:58:56.66" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{91A521E9-8C58-AA4E-9DB6-3B7C40324E9D}">
+    <text>Not needed</text>
+  </threadedComment>
   <threadedComment ref="F38" dT="2024-05-25T16:28:10.48" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
     <text>Not sure what type it’s supposed to be</text>
+  </threadedComment>
+  <threadedComment ref="B42" dT="2024-06-03T18:59:47.18" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{3A13DE3F-FDB4-D54D-8D34-92EEE889D658}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B44" dT="2024-06-03T18:59:56.11" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{A2C7FC53-1505-8A45-99CE-70D3C4FD5518}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B47" dT="2024-06-03T19:01:27.62" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{3FE72732-F7D7-6A44-A781-0E38E560C217}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B51" dT="2024-06-03T19:04:26.19" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{0490C4F1-599B-AB44-B1CC-7E63E4E8065B}">
+    <text>Not needed</text>
   </threadedComment>
   <threadedComment ref="F55" dT="2024-05-25T16:35:00.27" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
     <text>Only 1-dimensional array allowed</text>
   </threadedComment>
   <threadedComment ref="F57" dT="2024-05-25T16:42:43.15" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
     <text>Implemented as float</text>
+  </threadedComment>
+  <threadedComment ref="B58" dT="2024-06-03T19:15:47.42" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B61" dT="2024-06-03T19:15:57.20" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{B06CDA75-3D09-3A4C-9CA2-5DAFC7D0A49C}">
+    <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B69" dT="2024-06-03T19:24:16.35" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{6ED25ED1-E5D3-0547-B2AE-B068D8D2FCAB}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="B71" dT="2024-06-03T19:24:21.88" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{766C4F7D-809F-8546-936F-F77DAB106C65}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="B72" dT="2024-06-03T19:24:53.91" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{BF9BF349-FB0E-2A49-BEAB-473752D32B3F}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="B73" dT="2024-06-03T19:25:20.88" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{506BB1FA-65AC-2844-8BBF-2A90D38F6707}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="B74" dT="2024-06-03T19:25:16.63" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{1DDB399D-F138-F04F-99C1-98F0475A5FB6}">
+    <text>Duplicate</text>
+  </threadedComment>
+  <threadedComment ref="B75" dT="2024-06-03T19:25:36.80" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{30C5F121-C7F3-DF45-95C8-DA0E6762ECA7}">
+    <text>Duplicate</text>
   </threadedComment>
   <threadedComment ref="H75" dT="2024-05-25T15:51:08.40" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
     <text>Is this needed, separate from LFC_2BY2_SWITCH?</text>
@@ -2925,68 +3196,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="50"/>
-      <c r="B1" s="51" t="s">
+      <c r="A1" s="54"/>
+      <c r="B1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="48" t="s">
+      <c r="K1" s="50"/>
+      <c r="L1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="46"/>
-      <c r="O1" s="48" t="s">
+      <c r="N1" s="50"/>
+      <c r="O1" s="52" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="53"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="57"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="49"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="49"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="53"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
@@ -3139,10 +3410,10 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="54" t="s">
+      <c r="J7" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="54"/>
+      <c r="K7" s="58"/>
       <c r="M7">
         <v>0</v>
       </c>
@@ -3169,10 +3440,10 @@
       <c r="H8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="54" t="s">
+      <c r="J8" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="54"/>
+      <c r="K8" s="58"/>
       <c r="M8">
         <v>0</v>
       </c>
@@ -3236,7 +3507,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="55" t="s">
+      <c r="A11" s="59" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
@@ -3260,13 +3531,13 @@
       <c r="H11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="54" t="s">
+      <c r="J11" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="54"/>
+      <c r="K11" s="58"/>
     </row>
     <row r="12" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A12" s="55"/>
+      <c r="A12" s="59"/>
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -3288,10 +3559,10 @@
       <c r="H12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="54" t="s">
+      <c r="J12" s="58" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="54"/>
+      <c r="K12" s="58"/>
     </row>
     <row r="13" spans="1:19" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A13" s="31"/>
@@ -4156,7 +4427,7 @@
       <c r="H54" s="11"/>
     </row>
     <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A55" s="45" t="s">
+      <c r="A55" s="49" t="s">
         <v>153</v>
       </c>
       <c r="B55" t="s">
@@ -4166,7 +4437,7 @@
       <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A56" s="45"/>
+      <c r="A56" s="49"/>
       <c r="B56" t="s">
         <v>155</v>
       </c>
@@ -4174,7 +4445,7 @@
       <c r="H56" s="11"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A57" s="45"/>
+      <c r="A57" s="49"/>
       <c r="B57" t="s">
         <v>156</v>
       </c>
@@ -4182,7 +4453,7 @@
       <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A58" s="45"/>
+      <c r="A58" s="49"/>
       <c r="B58" t="s">
         <v>157</v>
       </c>
@@ -4190,7 +4461,7 @@
       <c r="H58" s="11"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A59" s="45"/>
+      <c r="A59" s="49"/>
       <c r="B59" t="s">
         <v>158</v>
       </c>
@@ -4198,7 +4469,7 @@
       <c r="H59" s="11"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A60" s="45"/>
+      <c r="A60" s="49"/>
       <c r="B60" t="s">
         <v>159</v>
       </c>
@@ -4206,7 +4477,7 @@
       <c r="H60" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A61" s="45"/>
+      <c r="A61" s="49"/>
       <c r="B61" t="s">
         <v>160</v>
       </c>
@@ -4219,7 +4490,7 @@
       <c r="H62" s="11"/>
     </row>
     <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="45" t="s">
+      <c r="A63" s="49" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
@@ -4229,7 +4500,7 @@
       <c r="H63" s="11"/>
     </row>
     <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A64" s="45"/>
+      <c r="A64" s="49"/>
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -4237,7 +4508,7 @@
       <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A65" s="45"/>
+      <c r="A65" s="49"/>
       <c r="B65" t="s">
         <v>164</v>
       </c>
@@ -4245,7 +4516,7 @@
       <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A66" s="45"/>
+      <c r="A66" s="49"/>
       <c r="B66" t="s">
         <v>165</v>
       </c>
@@ -4253,7 +4524,7 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A67" s="45"/>
+      <c r="A67" s="49"/>
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -4261,7 +4532,7 @@
       <c r="H67" s="11"/>
     </row>
     <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A68" s="45"/>
+      <c r="A68" s="49"/>
       <c r="B68" t="s">
         <v>167</v>
       </c>
@@ -4269,7 +4540,7 @@
       <c r="H68" s="11"/>
     </row>
     <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A69" s="45"/>
+      <c r="A69" s="49"/>
       <c r="B69" t="s">
         <v>168</v>
       </c>
@@ -5994,26 +6265,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60079DE2-3043-422E-90F3-3EEEEA14A1EF}">
   <dimension ref="A1:V79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H79" sqref="H79"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="4.34765625" customWidth="1"/>
-    <col min="2" max="2" width="21.34765625" customWidth="1"/>
+    <col min="2" max="2" width="24.84765625" customWidth="1"/>
     <col min="3" max="3" width="15.1484375" customWidth="1"/>
     <col min="4" max="4" width="11.6484375" customWidth="1"/>
     <col min="5" max="5" width="10.34765625" customWidth="1"/>
-    <col min="6" max="6" width="13.94921875" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="35.34765625" customWidth="1"/>
     <col min="8" max="8" width="28.84765625" customWidth="1"/>
     <col min="9" max="9" width="9.1484375" customWidth="1"/>
-    <col min="10" max="10" width="6.84765625" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
     <col min="11" max="11" width="8.5" customWidth="1"/>
     <col min="13" max="13" width="26.5" customWidth="1"/>
     <col min="14" max="14" width="15.34765625" customWidth="1"/>
-    <col min="17" max="17" width="18.6484375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" customWidth="1"/>
     <col min="18" max="18" width="11.1484375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.6484375" customWidth="1"/>
@@ -6021,91 +6293,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="50"/>
-      <c r="B1" s="51" t="s">
+      <c r="A1" s="54"/>
+      <c r="B1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="52" t="s">
+      <c r="D1" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="51" t="s">
+      <c r="E1" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="51" t="s">
+      <c r="F1" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="52" t="s">
+      <c r="G1" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="52" t="s">
+      <c r="H1" s="56" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="53" t="s">
+      <c r="I1" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="46" t="s">
+      <c r="J1" s="50" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="46"/>
-      <c r="L1" s="48" t="s">
+      <c r="K1" s="50"/>
+      <c r="L1" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="46" t="s">
+      <c r="M1" s="50" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="46" t="s">
+      <c r="N1" s="50" t="s">
+        <v>520</v>
+      </c>
+      <c r="O1" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="54" t="s">
+        <v>521</v>
+      </c>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="U1" s="54" t="s">
         <v>526</v>
       </c>
-      <c r="O1" s="48" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="50" t="s">
-        <v>527</v>
-      </c>
-      <c r="R1" s="50"/>
-      <c r="S1" s="50"/>
-      <c r="U1" s="50" t="s">
-        <v>532</v>
-      </c>
-      <c r="V1" s="50"/>
+      <c r="V1" s="54"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.6">
-      <c r="A2" s="51"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
-      <c r="I2" s="53"/>
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="57"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="49"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="47"/>
-      <c r="O2" s="49"/>
+      <c r="L2" s="53"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="53"/>
       <c r="Q2" s="1" t="s">
+        <v>522</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>523</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>524</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>528</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>533</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>534</v>
       </c>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.6">
@@ -6127,77 +6399,58 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.6">
-      <c r="N4">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.6">
       <c r="B5" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="C5" t="s">
-        <v>535</v>
+        <v>445</v>
       </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>377</v>
       </c>
       <c r="G5" t="s">
-        <v>445</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>509</v>
-      </c>
-      <c r="I5" t="s">
-        <v>452</v>
-      </c>
-      <c r="M5" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="N5">
         <v>120</v>
       </c>
-      <c r="Q5" s="40"/>
-    </row>
-    <row r="6" spans="1:22" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="Q5" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.6">
       <c r="B6" t="s">
-        <v>444</v>
-      </c>
-      <c r="C6" s="33" t="s">
-        <v>535</v>
+        <v>447</v>
+      </c>
+      <c r="C6" t="s">
+        <v>445</v>
       </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>377</v>
       </c>
       <c r="G6" t="s">
-        <v>445</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>507</v>
-      </c>
-      <c r="I6" t="s">
-        <v>442</v>
-      </c>
-      <c r="M6" t="s">
-        <v>443</v>
+        <v>448</v>
       </c>
       <c r="N6">
         <v>120</v>
       </c>
-      <c r="Q6" s="40"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.6">
+      <c r="Q6" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B7" t="s">
-        <v>446</v>
+        <v>137</v>
       </c>
       <c r="C7" t="s">
-        <v>447</v>
+        <v>529</v>
       </c>
       <c r="E7" t="s">
         <v>17</v>
@@ -6206,172 +6459,220 @@
         <v>377</v>
       </c>
       <c r="G7" t="s">
-        <v>448</v>
+        <v>452</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>530</v>
       </c>
       <c r="N7">
         <v>120</v>
       </c>
-      <c r="Q7" s="41" t="s">
-        <v>531</v>
+      <c r="Q7" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R7" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="S7" s="39" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.6">
       <c r="B8" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="C8" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="E8" t="s">
-        <v>17</v>
+        <v>132</v>
       </c>
       <c r="F8" t="s">
         <v>377</v>
       </c>
       <c r="G8" t="s">
-        <v>450</v>
+        <v>454</v>
+      </c>
+      <c r="H8" t="s">
+        <v>455</v>
       </c>
       <c r="N8">
         <v>120</v>
       </c>
-      <c r="Q8" s="41" t="s">
+      <c r="Q8" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R8" t="s">
+        <v>545</v>
+      </c>
+      <c r="S8" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.6">
+      <c r="B9" s="39" t="s">
+        <v>456</v>
+      </c>
+      <c r="C9" t="s">
+        <v>459</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B9" t="s">
-        <v>137</v>
-      </c>
-      <c r="C9" t="s">
-        <v>535</v>
-      </c>
-      <c r="E9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" t="s">
-        <v>377</v>
-      </c>
       <c r="G9" t="s">
-        <v>455</v>
-      </c>
-      <c r="H9" s="8" t="s">
-        <v>536</v>
+        <v>458</v>
+      </c>
+      <c r="H9" t="s">
+        <v>532</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9">
+        <v>2</v>
       </c>
       <c r="N9">
         <v>120</v>
       </c>
-      <c r="Q9" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.6">
+      <c r="Q9" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R9" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S9" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B10" t="s">
-        <v>456</v>
+        <v>460</v>
       </c>
       <c r="C10" t="s">
-        <v>447</v>
+        <v>457</v>
       </c>
       <c r="E10" t="s">
-        <v>132</v>
+        <v>17</v>
       </c>
       <c r="F10" t="s">
         <v>377</v>
       </c>
       <c r="G10" t="s">
-        <v>457</v>
-      </c>
-      <c r="H10" t="s">
-        <v>458</v>
+        <v>461</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>462</v>
       </c>
       <c r="N10">
         <v>120</v>
       </c>
-      <c r="Q10" s="41" t="s">
-        <v>531</v>
+      <c r="Q10" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R10" t="s">
+        <v>545</v>
+      </c>
+      <c r="S10" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.6">
       <c r="B11" s="39" t="s">
-        <v>459</v>
+        <v>463</v>
       </c>
       <c r="C11" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E11" t="s">
         <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="G11" t="s">
-        <v>461</v>
+        <v>465</v>
       </c>
       <c r="H11" t="s">
-        <v>538</v>
+        <v>466</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="N11">
         <v>120</v>
       </c>
-      <c r="Q11" s="41" t="s">
-        <v>531</v>
-      </c>
-      <c r="R11" s="41" t="s">
-        <v>531</v>
-      </c>
-      <c r="S11" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="12" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="Q11" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R11" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S11" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.6">
       <c r="B12" t="s">
-        <v>463</v>
+        <v>467</v>
       </c>
       <c r="C12" t="s">
-        <v>460</v>
+        <v>464</v>
       </c>
       <c r="E12" t="s">
         <v>17</v>
       </c>
       <c r="F12" t="s">
-        <v>377</v>
+        <v>533</v>
       </c>
       <c r="G12" t="s">
-        <v>464</v>
-      </c>
-      <c r="H12" s="8" t="s">
         <v>465</v>
+      </c>
+      <c r="H12" t="s">
+        <v>466</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>60</v>
       </c>
       <c r="N12">
         <v>120</v>
       </c>
-      <c r="Q12" s="41" t="s">
-        <v>531</v>
+      <c r="Q12" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R12" s="34" t="s">
+        <v>545</v>
+      </c>
+      <c r="S12" t="s">
+        <v>545</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.6">
       <c r="B13" s="39" t="s">
+        <v>468</v>
+      </c>
+      <c r="C13" t="s">
+        <v>464</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>533</v>
+      </c>
+      <c r="G13" t="s">
+        <v>465</v>
+      </c>
+      <c r="H13" t="s">
         <v>466</v>
-      </c>
-      <c r="C13" t="s">
-        <v>467</v>
-      </c>
-      <c r="E13" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" t="s">
-        <v>539</v>
-      </c>
-      <c r="G13" t="s">
-        <v>468</v>
-      </c>
-      <c r="H13" t="s">
-        <v>469</v>
       </c>
       <c r="J13">
         <v>0</v>
@@ -6382,271 +6683,343 @@
       <c r="N13">
         <v>120</v>
       </c>
-      <c r="Q13" s="41" t="s">
-        <v>531</v>
-      </c>
-      <c r="R13" s="41" t="s">
-        <v>531</v>
-      </c>
-      <c r="S13" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.6">
+      <c r="Q13" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R13" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S13" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B14" t="s">
-        <v>470</v>
-      </c>
-      <c r="C14" t="s">
-        <v>467</v>
+        <v>469</v>
+      </c>
+      <c r="C14" s="33" t="s">
+        <v>445</v>
       </c>
       <c r="E14" t="s">
         <v>17</v>
       </c>
       <c r="F14" t="s">
-        <v>539</v>
+        <v>377</v>
       </c>
       <c r="G14" t="s">
-        <v>468</v>
-      </c>
-      <c r="H14" t="s">
-        <v>469</v>
-      </c>
-      <c r="J14">
-        <v>0</v>
-      </c>
-      <c r="K14">
-        <v>60</v>
+        <v>535</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>534</v>
       </c>
       <c r="N14">
         <v>120</v>
       </c>
-      <c r="Q14" s="41" t="s">
-        <v>531</v>
+      <c r="Q14" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R14" s="34" t="s">
+        <v>545</v>
+      </c>
+      <c r="S14" t="s">
+        <v>546</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.6">
       <c r="B15" s="39" t="s">
-        <v>471</v>
+        <v>557</v>
       </c>
       <c r="C15" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="E15" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" t="s">
-        <v>539</v>
+        <v>59</v>
       </c>
       <c r="G15" t="s">
-        <v>468</v>
-      </c>
-      <c r="H15" t="s">
-        <v>469</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>60</v>
+        <v>558</v>
       </c>
       <c r="N15">
         <v>120</v>
       </c>
-      <c r="Q15" s="41" t="s">
-        <v>531</v>
-      </c>
-      <c r="R15" s="41" t="s">
-        <v>531</v>
-      </c>
-      <c r="S15" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B16" t="s">
-        <v>472</v>
-      </c>
-      <c r="C16" s="33" t="s">
-        <v>447</v>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.6">
+      <c r="B16" s="39" t="s">
+        <v>559</v>
+      </c>
+      <c r="C16" t="s">
+        <v>451</v>
       </c>
       <c r="E16" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" t="s">
-        <v>537</v>
+        <v>59</v>
       </c>
       <c r="G16" t="s">
-        <v>541</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>540</v>
+        <v>560</v>
       </c>
       <c r="N16">
         <v>120</v>
       </c>
-      <c r="Q16" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="19" spans="2:17" ht="46.8" x14ac:dyDescent="0.6">
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.6">
+      <c r="B17" s="39"/>
+    </row>
+    <row r="18" spans="2:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B18" s="39" t="s">
+        <v>561</v>
+      </c>
+      <c r="C18" t="s">
+        <v>539</v>
+      </c>
+      <c r="E18" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" s="8" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B19" t="s">
-        <v>543</v>
+        <v>537</v>
       </c>
       <c r="C19" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="E19" t="s">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="F19" t="s">
-        <v>18</v>
+        <v>377</v>
       </c>
       <c r="G19" t="s">
-        <v>548</v>
+        <v>542</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>550</v>
-      </c>
-    </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.6">
+        <v>544</v>
+      </c>
+      <c r="Q19" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R19" s="34" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.6">
       <c r="B20" t="s">
-        <v>544</v>
+        <v>538</v>
       </c>
       <c r="C20" t="s">
-        <v>545</v>
+        <v>539</v>
       </c>
       <c r="E20" t="s">
         <v>132</v>
       </c>
       <c r="F20" t="s">
-        <v>537</v>
+        <v>377</v>
       </c>
       <c r="G20" t="s">
-        <v>546</v>
+        <v>540</v>
       </c>
       <c r="H20" t="s">
+        <v>541</v>
+      </c>
+      <c r="Q20" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" s="44" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="B21" s="44" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.6">
+      <c r="B23" t="s">
+        <v>555</v>
+      </c>
+      <c r="E23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" t="s">
         <v>547</v>
       </c>
-    </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.6">
-      <c r="B21" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.6">
-      <c r="N22">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.6">
-      <c r="B23" t="s">
-        <v>475</v>
-      </c>
       <c r="G23" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="H23" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="N23">
         <v>20</v>
       </c>
-      <c r="Q23" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q23" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R23" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.6">
       <c r="B24" t="s">
-        <v>476</v>
+        <v>556</v>
+      </c>
+      <c r="E24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" t="s">
+        <v>547</v>
       </c>
       <c r="G24" t="s">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="H24" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="N24">
         <v>20</v>
       </c>
-      <c r="Q24" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q24" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R24" s="40" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.6">
       <c r="B25" t="s">
         <v>253</v>
       </c>
+      <c r="E25" t="s">
+        <v>59</v>
+      </c>
+      <c r="F25" t="s">
+        <v>533</v>
+      </c>
       <c r="N25">
         <v>20</v>
       </c>
-      <c r="Q25" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q25" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R25" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.6">
       <c r="B26" t="s">
         <v>255</v>
       </c>
+      <c r="E26" t="s">
+        <v>59</v>
+      </c>
+      <c r="F26" t="s">
+        <v>533</v>
+      </c>
       <c r="N26">
         <v>20</v>
       </c>
-      <c r="Q26" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q26" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R26" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="27" spans="2:18" x14ac:dyDescent="0.6">
       <c r="B27" t="s">
-        <v>478</v>
+        <v>473</v>
+      </c>
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" t="s">
+        <v>533</v>
       </c>
       <c r="N27">
         <v>20</v>
       </c>
-      <c r="Q27" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q27" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R27" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.6">
       <c r="B28" t="s">
-        <v>479</v>
+        <v>474</v>
+      </c>
+      <c r="E28" t="s">
+        <v>59</v>
+      </c>
+      <c r="F28" t="s">
+        <v>533</v>
       </c>
       <c r="N28">
         <v>20</v>
       </c>
-      <c r="Q28" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q28" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R28" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.6">
       <c r="B29" t="s">
         <v>273</v>
       </c>
+      <c r="E29" t="s">
+        <v>59</v>
+      </c>
+      <c r="F29" t="s">
+        <v>533</v>
+      </c>
       <c r="N29">
         <v>20</v>
       </c>
-      <c r="Q29" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q29" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R29" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="30" spans="2:18" x14ac:dyDescent="0.6">
       <c r="B30" t="s">
         <v>275</v>
       </c>
+      <c r="E30" t="s">
+        <v>59</v>
+      </c>
+      <c r="F30" t="s">
+        <v>533</v>
+      </c>
       <c r="N30">
         <v>20</v>
       </c>
-      <c r="Q30" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q30" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R30" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.6">
       <c r="B31" t="s">
         <v>277</v>
       </c>
-      <c r="Q31" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="33" spans="2:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="E31" t="s">
+        <v>59</v>
+      </c>
+      <c r="F31" t="s">
+        <v>533</v>
+      </c>
+      <c r="Q31" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R31" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="33" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B33" t="s">
         <v>77</v>
       </c>
@@ -6654,7 +7027,7 @@
         <v>50</v>
       </c>
       <c r="D33" t="s">
-        <v>51</v>
+        <v>552</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
@@ -6669,25 +7042,28 @@
         <v>80</v>
       </c>
       <c r="J33">
-        <v>-5</v>
+        <v>10</v>
       </c>
       <c r="K33">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="M33">
-        <v>25</v>
+        <v>19.181000000000001</v>
       </c>
       <c r="N33">
         <v>20</v>
       </c>
-      <c r="Q33" s="41" t="s">
-        <v>531</v>
-      </c>
-      <c r="R33" s="42" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="34" spans="2:18" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="Q33" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R33" s="41" t="s">
+        <v>525</v>
+      </c>
+      <c r="S33" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="34" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B34" t="s">
         <v>81</v>
       </c>
@@ -6709,23 +7085,29 @@
       <c r="I34" t="s">
         <v>83</v>
       </c>
-      <c r="J34" t="s">
-        <v>26</v>
-      </c>
-      <c r="K34" t="s">
-        <v>26</v>
+      <c r="J34">
+        <v>145</v>
+      </c>
+      <c r="K34">
+        <v>155</v>
       </c>
       <c r="M34">
-        <v>145</v>
+        <v>150</v>
       </c>
       <c r="N34">
         <v>120</v>
       </c>
-      <c r="Q34" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="35" spans="2:18" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="Q34" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R34" t="s">
+        <v>545</v>
+      </c>
+      <c r="S34" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B35" t="s">
         <v>84</v>
       </c>
@@ -6745,7 +7127,7 @@
         <v>85</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="I35" t="s">
         <v>87</v>
@@ -6762,34 +7144,37 @@
       <c r="N35">
         <v>120</v>
       </c>
-      <c r="Q35" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="36" spans="2:18" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="B36" t="s">
-        <v>505</v>
-      </c>
-      <c r="E36" t="s">
-        <v>17</v>
-      </c>
-      <c r="F36" t="s">
+      <c r="Q35" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R35" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="B36" s="44" t="s">
+        <v>500</v>
+      </c>
+      <c r="E36" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F36" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="H36" s="19" t="s">
-        <v>506</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="H36" s="46" t="s">
+        <v>501</v>
+      </c>
+      <c r="I36" s="44" t="s">
         <v>442</v>
       </c>
-      <c r="N36">
+      <c r="N36" s="44">
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -6812,34 +7197,37 @@
       <c r="N37">
         <v>120</v>
       </c>
-      <c r="Q37" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="38" spans="2:18" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="B38" t="s">
-        <v>444</v>
-      </c>
-      <c r="C38" t="s">
-        <v>535</v>
-      </c>
-      <c r="E38" t="s">
-        <v>17</v>
-      </c>
-      <c r="F38" t="s">
+      <c r="Q37" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R37" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="B38" s="44" t="s">
+        <v>443</v>
+      </c>
+      <c r="C38" s="44" t="s">
+        <v>529</v>
+      </c>
+      <c r="E38" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F38" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="G38" s="8" t="s">
-        <v>481</v>
-      </c>
-      <c r="H38" s="19" t="s">
-        <v>507</v>
-      </c>
-      <c r="N38">
+      <c r="G38" s="45" t="s">
+        <v>476</v>
+      </c>
+      <c r="H38" s="46" t="s">
+        <v>502</v>
+      </c>
+      <c r="N38" s="44">
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="2:18" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="39" spans="2:19" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B39" t="s">
         <v>90</v>
       </c>
@@ -6873,11 +7261,14 @@
       <c r="N39">
         <v>120</v>
       </c>
-      <c r="Q39" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="40" spans="2:18" x14ac:dyDescent="0.6">
+      <c r="Q39" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R39" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B40" t="s">
         <v>93</v>
       </c>
@@ -6900,11 +7291,14 @@
       <c r="N40">
         <v>120</v>
       </c>
-      <c r="Q40" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="41" spans="2:18" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="Q40" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R40" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B41" t="s">
         <v>95</v>
       </c>
@@ -6924,7 +7318,7 @@
         <v>96</v>
       </c>
       <c r="H41" s="20" t="s">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="I41" t="s">
         <v>87</v>
@@ -6941,31 +7335,34 @@
       <c r="N41">
         <v>120</v>
       </c>
-      <c r="Q41" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="42" spans="2:18" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="B42" t="s">
-        <v>508</v>
-      </c>
-      <c r="E42" t="s">
-        <v>17</v>
-      </c>
-      <c r="F42" t="s">
+      <c r="Q41" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R41" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="B42" s="44" t="s">
+        <v>503</v>
+      </c>
+      <c r="E42" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F42" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="G42" s="8" t="s">
+      <c r="G42" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="H42" s="19" t="s">
-        <v>509</v>
-      </c>
-      <c r="N42">
+      <c r="H42" s="46" t="s">
+        <v>504</v>
+      </c>
+      <c r="N42" s="44">
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="43" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B43" t="s">
         <v>97</v>
       </c>
@@ -6988,31 +7385,34 @@
       <c r="N43">
         <v>120</v>
       </c>
-      <c r="Q43" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="44" spans="2:18" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="B44" t="s">
-        <v>451</v>
-      </c>
-      <c r="C44" t="s">
-        <v>535</v>
-      </c>
-      <c r="F44" t="s">
+      <c r="Q43" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R43" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="B44" s="44" t="s">
+        <v>449</v>
+      </c>
+      <c r="C44" s="44" t="s">
+        <v>529</v>
+      </c>
+      <c r="F44" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="G44" s="8" t="s">
-        <v>483</v>
-      </c>
-      <c r="H44" s="11" t="s">
-        <v>510</v>
-      </c>
-      <c r="N44">
+      <c r="G44" s="45" t="s">
+        <v>478</v>
+      </c>
+      <c r="H44" s="47" t="s">
+        <v>505</v>
+      </c>
+      <c r="N44" s="44">
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="45" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B45" t="s">
         <v>99</v>
       </c>
@@ -7020,7 +7420,7 @@
         <v>50</v>
       </c>
       <c r="D45" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E45" t="s">
         <v>17</v>
@@ -7029,7 +7429,7 @@
         <v>100</v>
       </c>
       <c r="H45" s="19" t="s">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="I45" t="s">
         <v>102</v>
@@ -7043,11 +7443,17 @@
       <c r="N45">
         <v>120</v>
       </c>
-      <c r="Q45" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="46" spans="2:18" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="Q45" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R45" t="s">
+        <v>545</v>
+      </c>
+      <c r="S45" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19" ht="62.4" x14ac:dyDescent="0.6">
       <c r="B46" t="s">
         <v>105</v>
       </c>
@@ -7064,7 +7470,7 @@
         <v>106</v>
       </c>
       <c r="H46" s="19" t="s">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="I46" t="s">
         <v>108</v>
@@ -7081,43 +7487,58 @@
       <c r="N46">
         <v>120</v>
       </c>
-      <c r="Q46" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="47" spans="2:18" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="B47" t="s">
-        <v>511</v>
-      </c>
-      <c r="E47" t="s">
-        <v>17</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>512</v>
-      </c>
-      <c r="H47" s="19" t="s">
-        <v>513</v>
-      </c>
-      <c r="N47">
+      <c r="Q46" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R46" t="s">
+        <v>545</v>
+      </c>
+      <c r="S46" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="47" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="B47" s="44" t="s">
+        <v>506</v>
+      </c>
+      <c r="E47" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G47" s="45" t="s">
+        <v>507</v>
+      </c>
+      <c r="H47" s="46" t="s">
+        <v>508</v>
+      </c>
+      <c r="N47" s="44">
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="48" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B48" t="s">
-        <v>449</v>
+        <v>447</v>
+      </c>
+      <c r="C48" t="s">
+        <v>50</v>
+      </c>
+      <c r="D48" t="s">
+        <v>51</v>
       </c>
       <c r="E48" t="s">
         <v>17</v>
       </c>
       <c r="G48" s="8" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="H48" s="19"/>
       <c r="N48">
         <v>120</v>
       </c>
-    </row>
-    <row r="49" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="R48" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="49" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B49" t="s">
         <v>109</v>
       </c>
@@ -7125,7 +7546,7 @@
         <v>50</v>
       </c>
       <c r="D49" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E49" t="s">
         <v>17</v>
@@ -7134,7 +7555,7 @@
         <v>110</v>
       </c>
       <c r="H49" s="19" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="I49" t="s">
         <v>102</v>
@@ -7151,11 +7572,17 @@
       <c r="N49">
         <v>120</v>
       </c>
-      <c r="Q49" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="50" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q49" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R49" t="s">
+        <v>545</v>
+      </c>
+      <c r="S49" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="50" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B50" t="s">
         <v>112</v>
       </c>
@@ -7172,7 +7599,7 @@
         <v>113</v>
       </c>
       <c r="H50" s="11" t="s">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="I50" t="s">
         <v>108</v>
@@ -7189,43 +7616,58 @@
       <c r="N50">
         <v>120</v>
       </c>
-      <c r="Q50" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="51" spans="2:17" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B51" t="s">
-        <v>514</v>
-      </c>
-      <c r="E51" t="s">
-        <v>17</v>
-      </c>
-      <c r="G51" s="19" t="s">
-        <v>515</v>
-      </c>
-      <c r="H51" s="11" t="s">
-        <v>517</v>
-      </c>
-      <c r="N51">
+      <c r="Q50" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R50" t="s">
+        <v>545</v>
+      </c>
+      <c r="S50" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="51" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B51" s="44" t="s">
+        <v>509</v>
+      </c>
+      <c r="E51" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G51" s="46" t="s">
+        <v>510</v>
+      </c>
+      <c r="H51" s="47" t="s">
+        <v>512</v>
+      </c>
+      <c r="N51" s="44">
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="2:17" x14ac:dyDescent="0.6">
+    <row r="52" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B52" t="s">
-        <v>446</v>
+        <v>444</v>
+      </c>
+      <c r="C52" t="s">
+        <v>50</v>
+      </c>
+      <c r="D52" t="s">
+        <v>51</v>
       </c>
       <c r="E52" t="s">
         <v>17</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="H52" s="11"/>
       <c r="N52">
         <v>120</v>
       </c>
-    </row>
-    <row r="53" spans="2:17" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="R52" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="53" spans="2:19" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B53" t="s">
         <v>115</v>
       </c>
@@ -7262,11 +7704,14 @@
       <c r="N53">
         <v>120</v>
       </c>
-      <c r="Q53" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="54" spans="2:17" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="Q53" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R53" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="54" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B54" t="s">
         <v>118</v>
       </c>
@@ -7286,7 +7731,7 @@
         <v>119</v>
       </c>
       <c r="H54" s="11" t="s">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="I54" t="s">
         <v>108</v>
@@ -7300,46 +7745,52 @@
       <c r="N54">
         <v>120</v>
       </c>
-      <c r="Q54" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="55" spans="2:17" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B55" s="43" t="s">
-        <v>542</v>
-      </c>
-      <c r="C55" s="43" t="s">
+      <c r="Q54" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R54" s="34" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="55" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B55" s="42" t="s">
+        <v>536</v>
+      </c>
+      <c r="C55" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="D55" s="43" t="s">
+      <c r="D55" s="42" t="s">
         <v>51</v>
       </c>
-      <c r="E55" s="43" t="s">
-        <v>17</v>
-      </c>
-      <c r="F55" s="44" t="s">
+      <c r="E55" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="F55" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="G55" s="44" t="s">
+      <c r="G55" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="H55" s="44" t="s">
-        <v>490</v>
-      </c>
-      <c r="I55" s="43" t="s">
+      <c r="H55" s="43" t="s">
+        <v>485</v>
+      </c>
+      <c r="I55" s="42" t="s">
         <v>124</v>
       </c>
-      <c r="J55" s="43"/>
-      <c r="K55" s="43"/>
-      <c r="L55" s="43"/>
-      <c r="M55" s="43" t="s">
+      <c r="J55" s="42"/>
+      <c r="K55" s="42"/>
+      <c r="L55" s="42"/>
+      <c r="M55" s="42" t="s">
         <v>125</v>
       </c>
       <c r="N55">
         <v>120</v>
       </c>
-    </row>
-    <row r="56" spans="2:17" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="R55" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="56" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B56" t="s">
         <v>126</v>
       </c>
@@ -7360,8 +7811,11 @@
       <c r="N56">
         <v>120</v>
       </c>
-    </row>
-    <row r="57" spans="2:17" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="R56" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="57" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B57" t="s">
         <v>127</v>
       </c>
@@ -7369,7 +7823,7 @@
         <v>50</v>
       </c>
       <c r="D57" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E57" t="s">
         <v>17</v>
@@ -7381,10 +7835,10 @@
         <v>128</v>
       </c>
       <c r="H57" s="19" t="s">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="I57" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="M57">
         <v>135</v>
@@ -7392,25 +7846,28 @@
       <c r="N57">
         <v>120</v>
       </c>
-      <c r="Q57" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="58" spans="2:17" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="B58" t="s">
-        <v>518</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>519</v>
-      </c>
-      <c r="H58" s="19" t="s">
-        <v>520</v>
-      </c>
-      <c r="N58">
+      <c r="Q57" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R57" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="58" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="B58" s="44" t="s">
+        <v>513</v>
+      </c>
+      <c r="G58" s="46" t="s">
+        <v>514</v>
+      </c>
+      <c r="H58" s="46" t="s">
+        <v>515</v>
+      </c>
+      <c r="N58" s="44">
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="2:17" x14ac:dyDescent="0.6">
+    <row r="59" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B59" t="s">
         <v>130</v>
       </c>
@@ -7418,7 +7875,7 @@
         <v>50</v>
       </c>
       <c r="D59" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="E59" t="s">
         <v>59</v>
@@ -7441,11 +7898,14 @@
       <c r="N59">
         <v>120</v>
       </c>
-      <c r="Q59" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="60" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q59" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R59" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="60" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B60" t="s">
         <v>133</v>
       </c>
@@ -7459,10 +7919,10 @@
         <v>17</v>
       </c>
       <c r="G60" s="8" t="s">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="I60" t="s">
         <v>102</v>
@@ -7479,31 +7939,34 @@
       <c r="N60">
         <v>120</v>
       </c>
-      <c r="Q60" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="61" spans="2:17" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B61" t="s">
-        <v>521</v>
-      </c>
-      <c r="E61" t="s">
-        <v>17</v>
-      </c>
-      <c r="G61" s="8" t="s">
-        <v>522</v>
-      </c>
-      <c r="H61" s="11" t="s">
-        <v>523</v>
-      </c>
-      <c r="I61" t="s">
+      <c r="Q60" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R60" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="61" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B61" s="44" t="s">
+        <v>516</v>
+      </c>
+      <c r="E61" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G61" s="45" t="s">
+        <v>517</v>
+      </c>
+      <c r="H61" s="47" t="s">
+        <v>518</v>
+      </c>
+      <c r="I61" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="N61">
+      <c r="N61" s="44">
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="2:17" x14ac:dyDescent="0.6">
+    <row r="62" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B62" t="s">
         <v>135</v>
       </c>
@@ -7526,54 +7989,26 @@
       <c r="N62">
         <v>120</v>
       </c>
-      <c r="Q62" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="63" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q62" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R62" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="63" spans="2:19" x14ac:dyDescent="0.6">
       <c r="G63" s="8"/>
       <c r="H63" s="11"/>
-      <c r="N63">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="64" spans="2:17" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="B64" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" t="s">
-        <v>50</v>
-      </c>
-      <c r="D64" t="s">
-        <v>51</v>
-      </c>
-      <c r="E64" t="s">
-        <v>17</v>
-      </c>
-      <c r="F64" t="s">
-        <v>33</v>
-      </c>
-      <c r="G64" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="H64" s="11" t="s">
-        <v>524</v>
-      </c>
-      <c r="J64">
-        <v>0</v>
-      </c>
-      <c r="K64">
-        <v>1</v>
-      </c>
-      <c r="N64">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="65" spans="2:17" x14ac:dyDescent="0.6">
+    </row>
+    <row r="64" spans="2:19" x14ac:dyDescent="0.6">
+      <c r="G64" s="8"/>
+      <c r="H64" s="11"/>
+    </row>
+    <row r="65" spans="2:19" x14ac:dyDescent="0.6">
       <c r="G65" s="8"/>
       <c r="H65" s="11"/>
     </row>
-    <row r="66" spans="2:17" x14ac:dyDescent="0.6">
+    <row r="66" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B66" t="s">
         <v>139</v>
       </c>
@@ -7593,14 +8028,32 @@
         <v>140</v>
       </c>
       <c r="H66" s="11"/>
+      <c r="I66" t="s">
+        <v>80</v>
+      </c>
+      <c r="J66">
+        <v>22.5</v>
+      </c>
+      <c r="K66">
+        <v>23.5</v>
+      </c>
+      <c r="M66">
+        <v>23</v>
+      </c>
       <c r="N66">
         <v>20</v>
       </c>
-      <c r="Q66" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="67" spans="2:17" x14ac:dyDescent="0.6">
+      <c r="Q66" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R66" t="s">
+        <v>545</v>
+      </c>
+      <c r="S66" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="67" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B67" t="s">
         <v>141</v>
       </c>
@@ -7620,276 +8073,279 @@
         <v>142</v>
       </c>
       <c r="H67" s="11"/>
+      <c r="M67">
+        <v>37</v>
+      </c>
       <c r="N67">
         <v>20</v>
       </c>
-      <c r="Q67" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="69" spans="2:17" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B69" t="s">
+      <c r="Q67" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="R67" t="s">
+        <v>545</v>
+      </c>
+      <c r="S67" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="69" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B69" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="E69" t="s">
-        <v>17</v>
-      </c>
-      <c r="F69" t="s">
+      <c r="E69" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F69" s="44" t="s">
         <v>18</v>
       </c>
-      <c r="G69" s="8" t="s">
+      <c r="G69" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="H69" s="8" t="s">
+      <c r="H69" s="45" t="s">
+        <v>489</v>
+      </c>
+      <c r="I69" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="J69" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="K69" s="44">
+        <v>60</v>
+      </c>
+      <c r="L69" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="M69" s="44">
+        <v>60</v>
+      </c>
+      <c r="N69" s="44">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="70" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+      <c r="B70" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="D70" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E70" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F70" s="45" t="s">
+        <v>23</v>
+      </c>
+      <c r="G70" s="45" t="s">
+        <v>24</v>
+      </c>
+      <c r="H70" s="45" t="s">
+        <v>490</v>
+      </c>
+      <c r="I70" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="J70" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="K70" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="L70" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="M70" s="44" t="s">
+        <v>26</v>
+      </c>
+      <c r="N70" s="44">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="71" spans="2:19" s="44" customFormat="1" x14ac:dyDescent="0.6">
+      <c r="B71" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D71" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E71" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F71" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="G71" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="H71" s="45" t="s">
+        <v>491</v>
+      </c>
+      <c r="I71" s="44" t="s">
+        <v>21</v>
+      </c>
+      <c r="J71" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="K71" s="44">
+        <v>60</v>
+      </c>
+      <c r="L71" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="M71" s="44">
+        <v>60</v>
+      </c>
+      <c r="N71" s="44">
+        <v>120</v>
+      </c>
+      <c r="Q71" s="48" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="72" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B72" s="44" t="s">
+        <v>493</v>
+      </c>
+      <c r="D72" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E72" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F72" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G72" s="45" t="s">
+        <v>34</v>
+      </c>
+      <c r="H72" s="45" t="s">
         <v>494</v>
       </c>
-      <c r="I69" t="s">
+      <c r="J72" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="K72" s="60"/>
+      <c r="M72" s="44">
+        <v>0</v>
+      </c>
+      <c r="N72" s="44">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B73" s="44" t="s">
+        <v>492</v>
+      </c>
+      <c r="D73" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E73" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F73" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="G73" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="H73" s="45" t="s">
+        <v>495</v>
+      </c>
+      <c r="J73" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="K73" s="60"/>
+      <c r="M73" s="44">
+        <v>0</v>
+      </c>
+      <c r="N73" s="44">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="74" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="B74" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="D74" s="44" t="s">
+        <v>16</v>
+      </c>
+      <c r="E74" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F74" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="G74" s="45" t="s">
+        <v>41</v>
+      </c>
+      <c r="H74" s="45" t="s">
+        <v>496</v>
+      </c>
+      <c r="I74" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="J69">
+      <c r="J74" s="44">
         <v>0.01</v>
       </c>
-      <c r="K69">
+      <c r="K74" s="44">
         <v>60</v>
       </c>
-      <c r="L69">
+      <c r="L74" s="44">
         <v>0.01</v>
       </c>
-      <c r="M69">
+      <c r="M74" s="44">
         <v>60</v>
       </c>
-      <c r="N69">
+      <c r="N74" s="44">
         <v>120</v>
       </c>
     </row>
-    <row r="70" spans="2:17" ht="46.8" x14ac:dyDescent="0.6">
-      <c r="B70" t="s">
-        <v>22</v>
-      </c>
-      <c r="D70" t="s">
+    <row r="75" spans="2:19" s="44" customFormat="1" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="B75" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="D75" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="E70" t="s">
-        <v>17</v>
-      </c>
-      <c r="F70" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="G70" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H70" s="27" t="s">
-        <v>495</v>
-      </c>
-      <c r="I70" t="s">
-        <v>21</v>
-      </c>
-      <c r="J70" t="s">
-        <v>26</v>
-      </c>
-      <c r="K70" t="s">
-        <v>26</v>
-      </c>
-      <c r="L70" t="s">
-        <v>26</v>
-      </c>
-      <c r="M70" t="s">
-        <v>26</v>
-      </c>
-      <c r="N70">
+      <c r="E75" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="F75" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="G75" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="H75" s="45" t="s">
+        <v>519</v>
+      </c>
+      <c r="N75" s="44">
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="2:17" x14ac:dyDescent="0.6">
-      <c r="B71" t="s">
-        <v>27</v>
-      </c>
-      <c r="D71" t="s">
-        <v>16</v>
-      </c>
-      <c r="E71" t="s">
-        <v>17</v>
-      </c>
-      <c r="F71" t="s">
-        <v>18</v>
-      </c>
-      <c r="G71" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="H71" s="8" t="s">
-        <v>496</v>
-      </c>
-      <c r="I71" t="s">
-        <v>21</v>
-      </c>
-      <c r="J71">
-        <v>0.01</v>
-      </c>
-      <c r="K71">
-        <v>60</v>
-      </c>
-      <c r="L71">
-        <v>0.01</v>
-      </c>
-      <c r="M71">
-        <v>60</v>
-      </c>
-      <c r="N71">
-        <v>120</v>
-      </c>
-      <c r="Q71" s="41" t="s">
-        <v>531</v>
-      </c>
-    </row>
-    <row r="72" spans="2:17" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B72" t="s">
-        <v>498</v>
-      </c>
-      <c r="D72" t="s">
-        <v>16</v>
-      </c>
-      <c r="E72" t="s">
-        <v>17</v>
-      </c>
-      <c r="F72" t="s">
-        <v>33</v>
-      </c>
-      <c r="G72" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="H72" s="8" t="s">
-        <v>499</v>
-      </c>
-      <c r="J72" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="K72" s="54"/>
-      <c r="M72">
-        <v>0</v>
-      </c>
-      <c r="N72">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="73" spans="2:17" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B73" t="s">
+    <row r="77" spans="2:19" x14ac:dyDescent="0.6">
+      <c r="B77" t="s">
         <v>497</v>
-      </c>
-      <c r="D73" t="s">
-        <v>16</v>
-      </c>
-      <c r="E73" t="s">
-        <v>17</v>
-      </c>
-      <c r="F73" t="s">
-        <v>33</v>
-      </c>
-      <c r="G73" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H73" s="27" t="s">
-        <v>500</v>
-      </c>
-      <c r="J73" s="54" t="s">
-        <v>36</v>
-      </c>
-      <c r="K73" s="54"/>
-      <c r="M73">
-        <v>0</v>
-      </c>
-      <c r="N73">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="74" spans="2:17" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="B74" t="s">
-        <v>40</v>
-      </c>
-      <c r="D74" t="s">
-        <v>16</v>
-      </c>
-      <c r="E74" t="s">
-        <v>17</v>
-      </c>
-      <c r="F74" t="s">
-        <v>18</v>
-      </c>
-      <c r="G74" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="H74" s="8" t="s">
-        <v>501</v>
-      </c>
-      <c r="I74" t="s">
-        <v>21</v>
-      </c>
-      <c r="J74">
-        <v>0.01</v>
-      </c>
-      <c r="K74">
-        <v>60</v>
-      </c>
-      <c r="L74">
-        <v>0.01</v>
-      </c>
-      <c r="M74">
-        <v>60</v>
-      </c>
-      <c r="N74">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="75" spans="2:17" ht="62.4" x14ac:dyDescent="0.6">
-      <c r="B75" s="35" t="s">
-        <v>44</v>
-      </c>
-      <c r="C75" s="35"/>
-      <c r="D75" s="35" t="s">
-        <v>16</v>
-      </c>
-      <c r="E75" s="35" t="s">
-        <v>17</v>
-      </c>
-      <c r="F75" s="35" t="s">
-        <v>45</v>
-      </c>
-      <c r="G75" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="H75" s="36" t="s">
-        <v>525</v>
-      </c>
-      <c r="I75" s="35"/>
-      <c r="J75" s="35"/>
-      <c r="K75" s="35"/>
-      <c r="L75" s="35"/>
-      <c r="M75" s="35"/>
-      <c r="N75">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="77" spans="2:17" x14ac:dyDescent="0.6">
-      <c r="B77" t="s">
-        <v>502</v>
       </c>
       <c r="C77" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="2:17" x14ac:dyDescent="0.6">
+    <row r="78" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B78" t="s">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="C78" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="2:17" x14ac:dyDescent="0.6">
+    <row r="79" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B79" t="s">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="C79" t="s">
         <v>26</v>
@@ -7916,6 +8372,7 @@
     <mergeCell ref="D1:D2"/>
     <mergeCell ref="E1:E2"/>
   </mergeCells>
+  <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -8185,38 +8642,38 @@
       <c r="D1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="61" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="57"/>
-      <c r="G1" s="56" t="s">
+      <c r="F1" s="62"/>
+      <c r="G1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="57"/>
+      <c r="H1" s="62"/>
     </row>
     <row r="2" spans="1:8" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="58" t="s">
+      <c r="A2" s="63" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="59"/>
-      <c r="C2" s="59"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="60"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="65"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="3"/>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="66" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="68"/>
     </row>
     <row r="4" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="4">
@@ -8226,12 +8683,12 @@
         <v>370</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="66" t="s">
+      <c r="D4" s="69"/>
+      <c r="E4" s="70"/>
+      <c r="F4" s="71" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="67"/>
+      <c r="G4" s="72"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -8242,12 +8699,12 @@
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="68" t="s">
+      <c r="D5" s="75"/>
+      <c r="E5" s="76"/>
+      <c r="F5" s="73" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="69"/>
+      <c r="G5" s="74"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -8258,12 +8715,12 @@
         <v>372</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="66" t="s">
+      <c r="D6" s="69"/>
+      <c r="E6" s="70"/>
+      <c r="F6" s="71" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="67"/>
+      <c r="G6" s="72"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -8274,12 +8731,12 @@
         <v>373</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="70"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="68" t="s">
+      <c r="D7" s="75"/>
+      <c r="E7" s="76"/>
+      <c r="F7" s="73" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="69"/>
+      <c r="G7" s="74"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -8290,12 +8747,12 @@
         <v>53</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="66" t="s">
+      <c r="D8" s="69"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="71" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="67"/>
+      <c r="G8" s="72"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -8306,25 +8763,25 @@
         <v>374</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="71"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="76"/>
       <c r="H9" s="6" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="5"/>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="77" t="s">
         <v>376</v>
       </c>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="73"/>
-      <c r="H10" s="74"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="79"/>
     </row>
     <row r="11" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A11" s="6">
@@ -8336,12 +8793,12 @@
       <c r="C11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="68" t="s">
+      <c r="D11" s="73" t="s">
         <v>378</v>
       </c>
-      <c r="E11" s="69"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="71"/>
+      <c r="E11" s="74"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="76"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -8354,12 +8811,12 @@
       <c r="C12" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E12" s="67"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="65"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="70"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -8372,12 +8829,12 @@
       <c r="C13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="68" t="s">
+      <c r="D13" s="73" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="69"/>
-      <c r="F13" s="70"/>
-      <c r="G13" s="71"/>
+      <c r="E13" s="74"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="76"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -8388,12 +8845,12 @@
         <v>380</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="66" t="s">
+      <c r="D14" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="67"/>
-      <c r="F14" s="64"/>
-      <c r="G14" s="65"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="70"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -8406,12 +8863,12 @@
       <c r="C15" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="68" t="s">
+      <c r="D15" s="73" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="69"/>
-      <c r="F15" s="70"/>
-      <c r="G15" s="71"/>
+      <c r="E15" s="74"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="76"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -8424,12 +8881,12 @@
       <c r="C16" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D16" s="66" t="s">
+      <c r="D16" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="67"/>
-      <c r="F16" s="64"/>
-      <c r="G16" s="65"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="70"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -8442,12 +8899,12 @@
       <c r="C17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D17" s="68" t="s">
+      <c r="D17" s="73" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="69"/>
-      <c r="F17" s="70"/>
-      <c r="G17" s="71"/>
+      <c r="E17" s="74"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="76"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -8460,12 +8917,12 @@
       <c r="C18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D18" s="66" t="s">
+      <c r="D18" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="67"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="65"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="70"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -8478,12 +8935,12 @@
       <c r="C19" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="D19" s="68" t="s">
+      <c r="D19" s="73" t="s">
         <v>378</v>
       </c>
-      <c r="E19" s="69"/>
-      <c r="F19" s="70"/>
-      <c r="G19" s="71"/>
+      <c r="E19" s="74"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="76"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -8496,12 +8953,12 @@
       <c r="C20" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="66" t="s">
+      <c r="D20" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E20" s="67"/>
-      <c r="F20" s="64"/>
-      <c r="G20" s="65"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="70"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="117.3" thickBot="1" x14ac:dyDescent="0.65">
@@ -8514,12 +8971,12 @@
       <c r="C21" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="68" t="s">
+      <c r="D21" s="73" t="s">
         <v>378</v>
       </c>
-      <c r="E21" s="69"/>
-      <c r="F21" s="70"/>
-      <c r="G21" s="71"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="76"/>
       <c r="H21" s="6" t="s">
         <v>389</v>
       </c>
@@ -8534,12 +8991,12 @@
       <c r="C22" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="66" t="s">
+      <c r="D22" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E22" s="67"/>
-      <c r="F22" s="64"/>
-      <c r="G22" s="65"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="70"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -8564,13 +9021,13 @@
     </row>
     <row r="24" spans="1:8" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A24" s="7"/>
-      <c r="B24" s="75" t="s">
+      <c r="B24" s="80" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="76"/>
-      <c r="D24" s="76"/>
-      <c r="E24" s="76"/>
-      <c r="F24" s="77"/>
+      <c r="C24" s="81"/>
+      <c r="D24" s="81"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="82"/>
     </row>
     <row r="25" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A25" s="6">
@@ -8638,13 +9095,13 @@
     </row>
     <row r="29" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A29" s="3"/>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="66" t="s">
         <v>396</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63"/>
+      <c r="C29" s="67"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="67"/>
+      <c r="F29" s="68"/>
     </row>
     <row r="30" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A30" s="4">
@@ -8802,13 +9259,13 @@
     </row>
     <row r="41" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A41" s="3"/>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="66" t="s">
         <v>408</v>
       </c>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="63"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="67"/>
+      <c r="E41" s="67"/>
+      <c r="F41" s="68"/>
     </row>
     <row r="42" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A42" s="4">
@@ -9217,22 +9674,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
-    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EEDE7DDB808AF47B14A37A2563255CF" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="17d65d9f425ad811f92dcb994434cebd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8efcafe-ecab-455b-a9ec-2441266f5451" xmlns:ns3="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35cb6db38e7d3d9001b7e6afffee4001" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
@@ -9543,7 +9984,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -9552,19 +9993,23 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
+    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3366D879-DBBC-469C-98D7-600868252265}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9584,10 +10029,22 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
more KTL keywords implemented
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\astrocomb\KeckLFC-deploy\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjkim/Documents/KeckLFC-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45338A3C-1B30-4106-ACB3-D3E6DCA1985F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12486D21-60BE-9748-81D8-96D2A6A8367E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSF EO Comb" sheetId="1" r:id="rId1"/>
@@ -57,6 +57,7 @@
     <author>tc={43EE3C90-F8DC-844A-90D6-FE4B195F4D19}</author>
     <author>tc={734F326A-1433-1D42-B27D-80F6AB5B01F2}</author>
     <author>tc={65E7EA58-AEBE-9E43-B699-4C2E84AB06AE}</author>
+    <author>tc={6FBD4EDE-C92B-7942-BB7E-96FEA8EF0D1C}</author>
     <author>tc={9270FBFE-6EFE-1048-9F63-76932967FCB6}</author>
     <author>tc={430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}</author>
     <author>tc={897DD710-C2AF-F348-9BE6-70FC899ABE2C}</author>
@@ -67,7 +68,9 @@
     <author>tc={3A13DE3F-FDB4-D54D-8D34-92EEE889D658}</author>
     <author>tc={A2C7FC53-1505-8A45-99CE-70D3C4FD5518}</author>
     <author>tc={3FE72732-F7D7-6A44-A781-0E38E560C217}</author>
+    <author>tc={0D3903E9-918D-E349-9E45-0D2B69F31A28}</author>
     <author>tc={0490C4F1-599B-AB44-B1CC-7E63E4E8065B}</author>
+    <author>tc={0228CFF7-2A46-824A-BD7E-D1163401FED7}</author>
     <author>tc={C82D50AC-F6ED-B841-AC03-1967E28B201E}</author>
     <author>tc={C7739DC9-A5B2-EF49-9CE8-416CEC34862C}</author>
     <author>tc={3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}</author>
@@ -159,7 +162,15 @@
     Please fill in</t>
       </text>
     </comment>
-    <comment ref="B21" authorId="9" shapeId="0" xr:uid="{9270FBFE-6EFE-1048-9F63-76932967FCB6}">
+    <comment ref="H20" authorId="9" shapeId="0" xr:uid="{6FBD4EDE-C92B-7942-BB7E-96FEA8EF0D1C}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    0: running, 1: shut up all output</t>
+      </text>
+    </comment>
+    <comment ref="B21" authorId="10" shapeId="0" xr:uid="{9270FBFE-6EFE-1048-9F63-76932967FCB6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -167,7 +178,7 @@
     Doesn’t have to be KTL keyword</t>
       </text>
     </comment>
-    <comment ref="B23" authorId="10" shapeId="0" xr:uid="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
+    <comment ref="B23" authorId="11" shapeId="0" xr:uid="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -177,7 +188,7 @@
     Keep them and change names</t>
       </text>
     </comment>
-    <comment ref="F35" authorId="11" shapeId="0" xr:uid="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
+    <comment ref="F35" authorId="12" shapeId="0" xr:uid="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -185,7 +196,7 @@
     Implementing as float</t>
       </text>
     </comment>
-    <comment ref="B36" authorId="12" shapeId="0" xr:uid="{D3AE0575-FA6E-1242-8525-02B45DC7B747}">
+    <comment ref="B36" authorId="13" shapeId="0" xr:uid="{D3AE0575-FA6E-1242-8525-02B45DC7B747}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -195,7 +206,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="F36" authorId="13" shapeId="0" xr:uid="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
+    <comment ref="F36" authorId="14" shapeId="0" xr:uid="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -203,7 +214,7 @@
     Not sure what type it’s supposed to be</t>
       </text>
     </comment>
-    <comment ref="B38" authorId="14" shapeId="0" xr:uid="{91A521E9-8C58-AA4E-9DB6-3B7C40324E9D}">
+    <comment ref="B38" authorId="15" shapeId="0" xr:uid="{91A521E9-8C58-AA4E-9DB6-3B7C40324E9D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -211,7 +222,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="F38" authorId="15" shapeId="0" xr:uid="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
+    <comment ref="F38" authorId="16" shapeId="0" xr:uid="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -219,7 +230,7 @@
     Not sure what type it’s supposed to be</t>
       </text>
     </comment>
-    <comment ref="B42" authorId="16" shapeId="0" xr:uid="{3A13DE3F-FDB4-D54D-8D34-92EEE889D658}">
+    <comment ref="B42" authorId="17" shapeId="0" xr:uid="{3A13DE3F-FDB4-D54D-8D34-92EEE889D658}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -227,7 +238,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B44" authorId="17" shapeId="0" xr:uid="{A2C7FC53-1505-8A45-99CE-70D3C4FD5518}">
+    <comment ref="B44" authorId="18" shapeId="0" xr:uid="{A2C7FC53-1505-8A45-99CE-70D3C4FD5518}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -235,7 +246,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B47" authorId="18" shapeId="0" xr:uid="{3FE72732-F7D7-6A44-A781-0E38E560C217}">
+    <comment ref="B47" authorId="19" shapeId="0" xr:uid="{3FE72732-F7D7-6A44-A781-0E38E560C217}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -243,7 +254,15 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B51" authorId="19" shapeId="0" xr:uid="{0490C4F1-599B-AB44-B1CC-7E63E4E8065B}">
+    <comment ref="B48" authorId="20" shapeId="0" xr:uid="{0D3903E9-918D-E349-9E45-0D2B69F31A28}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="B51" authorId="21" shapeId="0" xr:uid="{0490C4F1-599B-AB44-B1CC-7E63E4E8065B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -251,7 +270,15 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="F55" authorId="20" shapeId="0" xr:uid="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
+    <comment ref="B52" authorId="22" shapeId="0" xr:uid="{0228CFF7-2A46-824A-BD7E-D1163401FED7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Duplicate</t>
+      </text>
+    </comment>
+    <comment ref="F55" authorId="23" shapeId="0" xr:uid="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -259,7 +286,7 @@
     Only 1-dimensional array allowed</t>
       </text>
     </comment>
-    <comment ref="F57" authorId="21" shapeId="0" xr:uid="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
+    <comment ref="F57" authorId="24" shapeId="0" xr:uid="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -267,7 +294,7 @@
     Implemented as float</t>
       </text>
     </comment>
-    <comment ref="B58" authorId="22" shapeId="0" xr:uid="{3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}">
+    <comment ref="B58" authorId="25" shapeId="0" xr:uid="{3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -275,7 +302,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B61" authorId="23" shapeId="0" xr:uid="{B06CDA75-3D09-3A4C-9CA2-5DAFC7D0A49C}">
+    <comment ref="B61" authorId="26" shapeId="0" xr:uid="{B06CDA75-3D09-3A4C-9CA2-5DAFC7D0A49C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -283,7 +310,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B69" authorId="24" shapeId="0" xr:uid="{6ED25ED1-E5D3-0547-B2AE-B068D8D2FCAB}">
+    <comment ref="B69" authorId="27" shapeId="0" xr:uid="{6ED25ED1-E5D3-0547-B2AE-B068D8D2FCAB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -291,7 +318,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B71" authorId="25" shapeId="0" xr:uid="{766C4F7D-809F-8546-936F-F77DAB106C65}">
+    <comment ref="B71" authorId="28" shapeId="0" xr:uid="{766C4F7D-809F-8546-936F-F77DAB106C65}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -299,7 +326,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B72" authorId="26" shapeId="0" xr:uid="{BF9BF349-FB0E-2A49-BEAB-473752D32B3F}">
+    <comment ref="B72" authorId="29" shapeId="0" xr:uid="{BF9BF349-FB0E-2A49-BEAB-473752D32B3F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -307,7 +334,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B73" authorId="27" shapeId="0" xr:uid="{506BB1FA-65AC-2844-8BBF-2A90D38F6707}">
+    <comment ref="B73" authorId="30" shapeId="0" xr:uid="{506BB1FA-65AC-2844-8BBF-2A90D38F6707}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -315,7 +342,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B74" authorId="28" shapeId="0" xr:uid="{1DDB399D-F138-F04F-99C1-98F0475A5FB6}">
+    <comment ref="B74" authorId="31" shapeId="0" xr:uid="{1DDB399D-F138-F04F-99C1-98F0475A5FB6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -323,7 +350,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B75" authorId="29" shapeId="0" xr:uid="{30C5F121-C7F3-DF45-95C8-DA0E6762ECA7}">
+    <comment ref="B75" authorId="32" shapeId="0" xr:uid="{30C5F121-C7F3-DF45-95C8-DA0E6762ECA7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -331,7 +358,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="H75" authorId="30" shapeId="0" xr:uid="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
+    <comment ref="H75" authorId="33" shapeId="0" xr:uid="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -362,7 +389,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1444" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="563">
   <si>
     <t>Keyword</t>
   </si>
@@ -2074,7 +2101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2220,6 +2247,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -2495,7 +2528,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2603,6 +2636,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="25" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2611,12 +2656,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2630,14 +2669,59 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2654,57 +2738,7 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="25" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2755,9 +2789,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2795,7 +2829,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2901,7 +2935,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3043,7 +3077,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3087,6 +3121,9 @@
   <threadedComment ref="N19" dT="2024-06-03T20:31:30.31" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{65E7EA58-AEBE-9E43-B699-4C2E84AB06AE}">
     <text>Please fill in</text>
   </threadedComment>
+  <threadedComment ref="H20" dT="2024-06-04T02:44:02.32" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{6FBD4EDE-C92B-7942-BB7E-96FEA8EF0D1C}">
+    <text>0: running, 1: shut up all output</text>
+  </threadedComment>
   <threadedComment ref="B21" dT="2024-06-03T18:40:46.49" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{9270FBFE-6EFE-1048-9F63-76932967FCB6}">
     <text>Doesn’t have to be KTL keyword</text>
   </threadedComment>
@@ -3123,8 +3160,14 @@
   <threadedComment ref="B47" dT="2024-06-03T19:01:27.62" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{3FE72732-F7D7-6A44-A781-0E38E560C217}">
     <text>Not needed</text>
   </threadedComment>
+  <threadedComment ref="B48" dT="2024-06-04T02:52:30.60" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{0D3903E9-918D-E349-9E45-0D2B69F31A28}">
+    <text>Duplicate</text>
+  </threadedComment>
   <threadedComment ref="B51" dT="2024-06-03T19:04:26.19" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{0490C4F1-599B-AB44-B1CC-7E63E4E8065B}">
     <text>Not needed</text>
+  </threadedComment>
+  <threadedComment ref="B52" dT="2024-06-04T02:52:39.98" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{0228CFF7-2A46-824A-BD7E-D1163401FED7}">
+    <text>Duplicate</text>
   </threadedComment>
   <threadedComment ref="F55" dT="2024-05-25T16:35:00.27" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
     <text>Only 1-dimensional array allowed</text>
@@ -3178,90 +3221,90 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16" customWidth="1"/>
-    <col min="2" max="2" width="22.6484375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.5" customWidth="1"/>
-    <col min="4" max="4" width="12.1484375" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="11.6484375" customWidth="1"/>
-    <col min="7" max="7" width="33.6484375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="53.1484375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="53.1640625" style="8" customWidth="1"/>
     <col min="9" max="9" width="12.5" customWidth="1"/>
-    <col min="10" max="10" width="10.34765625" customWidth="1"/>
-    <col min="11" max="11" width="9.6484375" customWidth="1"/>
-    <col min="13" max="13" width="12.1484375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="54"/>
-      <c r="B1" s="55" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="56"/>
+      <c r="B1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="52" t="s">
+      <c r="K1" s="54"/>
+      <c r="L1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="50"/>
-      <c r="O1" s="52" t="s">
+      <c r="N1" s="54"/>
+      <c r="O1" s="51" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="57"/>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="53"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="52"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
@@ -3280,7 +3323,7 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="4" spans="1:19" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>15</v>
       </c>
@@ -3315,7 +3358,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>22</v>
       </c>
@@ -3350,7 +3393,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="78" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>27</v>
       </c>
@@ -3388,7 +3431,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>31</v>
       </c>
@@ -3410,15 +3453,15 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="58" t="s">
+      <c r="J7" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="58"/>
+      <c r="K7" s="50"/>
       <c r="M7">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="78" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:19" ht="85" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>31</v>
       </c>
@@ -3440,15 +3483,15 @@
       <c r="H8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="58" t="s">
+      <c r="J8" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="58"/>
+      <c r="K8" s="50"/>
       <c r="M8">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:19" ht="102" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>40</v>
       </c>
@@ -3483,7 +3526,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="35" customFormat="1" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:19" s="35" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="A10" s="35" t="s">
         <v>43</v>
       </c>
@@ -3506,8 +3549,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="59" t="s">
+    <row r="11" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+      <c r="A11" s="49" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
@@ -3531,13 +3574,13 @@
       <c r="H11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="58" t="s">
+      <c r="J11" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="58"/>
-    </row>
-    <row r="12" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A12" s="59"/>
+      <c r="K11" s="50"/>
+    </row>
+    <row r="12" spans="1:19" ht="51" x14ac:dyDescent="0.2">
+      <c r="A12" s="49"/>
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -3559,12 +3602,12 @@
       <c r="H12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="58" t="s">
+      <c r="J12" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="58"/>
-    </row>
-    <row r="13" spans="1:19" ht="62.4" x14ac:dyDescent="0.6">
+      <c r="K12" s="50"/>
+    </row>
+    <row r="13" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="31"/>
       <c r="B13" t="s">
         <v>58</v>
@@ -3587,7 +3630,7 @@
       <c r="J13" s="28"/>
       <c r="K13" s="28"/>
     </row>
-    <row r="14" spans="1:19" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:19" ht="119" x14ac:dyDescent="0.2">
       <c r="A14" s="30" t="s">
         <v>62</v>
       </c>
@@ -3612,7 +3655,7 @@
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
     </row>
-    <row r="15" spans="1:19" s="9" customFormat="1" ht="78" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:19" s="9" customFormat="1" ht="85" x14ac:dyDescent="0.2">
       <c r="B15" s="9" t="s">
         <v>66</v>
       </c>
@@ -3632,7 +3675,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:19" s="9" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B16" s="9" t="s">
         <v>70</v>
       </c>
@@ -3655,7 +3698,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="17" spans="1:13" s="9" customFormat="1" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="17" spans="1:13" s="9" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A17" s="30" t="s">
         <v>62</v>
       </c>
@@ -3670,7 +3713,7 @@
       </c>
       <c r="H17" s="16"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="17" t="s">
         <v>76</v>
       </c>
@@ -3686,7 +3729,7 @@
       <c r="K18" s="18"/>
       <c r="L18" s="18"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>77</v>
       </c>
@@ -3718,7 +3761,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>81</v>
       </c>
@@ -3750,7 +3793,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="21" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
         <v>84</v>
       </c>
@@ -3782,7 +3825,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="22" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
         <v>88</v>
       </c>
@@ -3803,7 +3846,7 @@
       </c>
       <c r="H22" s="19"/>
     </row>
-    <row r="23" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="23" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>90</v>
       </c>
@@ -3835,7 +3878,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="24" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>93</v>
       </c>
@@ -3856,7 +3899,7 @@
       </c>
       <c r="H24" s="11"/>
     </row>
-    <row r="25" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="25" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>95</v>
       </c>
@@ -3888,7 +3931,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="26" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>97</v>
       </c>
@@ -3909,7 +3952,7 @@
       </c>
       <c r="H26" s="11"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>99</v>
       </c>
@@ -3938,7 +3981,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="28" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>105</v>
       </c>
@@ -3970,7 +4013,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>109</v>
       </c>
@@ -4002,7 +4045,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>112</v>
       </c>
@@ -4034,7 +4077,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="31" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>115</v>
       </c>
@@ -4069,7 +4112,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="32" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>118</v>
       </c>
@@ -4099,7 +4142,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="33" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>120</v>
       </c>
@@ -4128,7 +4171,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="34" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>126</v>
       </c>
@@ -4147,7 +4190,7 @@
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
     </row>
-    <row r="35" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="35" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>127</v>
       </c>
@@ -4179,7 +4222,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>130</v>
       </c>
@@ -4208,7 +4251,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>133</v>
       </c>
@@ -4238,7 +4281,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>135</v>
       </c>
@@ -4259,10 +4302,10 @@
       </c>
       <c r="H38" s="11"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H39" s="11"/>
     </row>
-    <row r="40" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="40" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>137</v>
       </c>
@@ -4283,10 +4326,10 @@
       </c>
       <c r="H40" s="11"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="H41" s="11"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>139</v>
       </c>
@@ -4307,7 +4350,7 @@
       </c>
       <c r="H42" s="11"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>141</v>
       </c>
@@ -4328,11 +4371,11 @@
       </c>
       <c r="H43" s="11"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G44" s="19"/>
       <c r="H44" s="11"/>
     </row>
-    <row r="45" spans="1:13" s="8" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="45" spans="1:13" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="27" t="s">
         <v>143</v>
       </c>
@@ -4342,7 +4385,7 @@
       <c r="G45" s="19"/>
       <c r="H45" s="11"/>
     </row>
-    <row r="46" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="46" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A46" s="27" t="s">
         <v>143</v>
       </c>
@@ -4352,7 +4395,7 @@
       <c r="G46" s="19"/>
       <c r="H46" s="11"/>
     </row>
-    <row r="47" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="47" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A47" s="27" t="s">
         <v>143</v>
       </c>
@@ -4362,7 +4405,7 @@
       <c r="G47" s="19"/>
       <c r="H47" s="11"/>
     </row>
-    <row r="48" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="48" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A48" s="27" t="s">
         <v>143</v>
       </c>
@@ -4372,7 +4415,7 @@
       <c r="G48" s="19"/>
       <c r="H48" s="11"/>
     </row>
-    <row r="49" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="49" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A49" s="27" t="s">
         <v>143</v>
       </c>
@@ -4382,7 +4425,7 @@
       <c r="G49" s="19"/>
       <c r="H49" s="11"/>
     </row>
-    <row r="50" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="50" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A50" s="27" t="s">
         <v>143</v>
       </c>
@@ -4392,7 +4435,7 @@
       <c r="G50" s="19"/>
       <c r="H50" s="11"/>
     </row>
-    <row r="51" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="51" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A51" s="27" t="s">
         <v>143</v>
       </c>
@@ -4402,7 +4445,7 @@
       <c r="G51" s="19"/>
       <c r="H51" s="11"/>
     </row>
-    <row r="52" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="52" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A52" s="27" t="s">
         <v>143</v>
       </c>
@@ -4412,7 +4455,7 @@
       <c r="G52" s="19"/>
       <c r="H52" s="11"/>
     </row>
-    <row r="53" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="53" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A53" s="27" t="s">
         <v>143</v>
       </c>
@@ -4422,12 +4465,12 @@
       <c r="G53" s="19"/>
       <c r="H53" s="11"/>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G54" s="19"/>
       <c r="H54" s="11"/>
     </row>
-    <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A55" s="49" t="s">
+    <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="53" t="s">
         <v>153</v>
       </c>
       <c r="B55" t="s">
@@ -4436,61 +4479,61 @@
       <c r="G55" s="19"/>
       <c r="H55" s="11"/>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A56" s="49"/>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="53"/>
       <c r="B56" t="s">
         <v>155</v>
       </c>
       <c r="G56" s="19"/>
       <c r="H56" s="11"/>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A57" s="49"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="53"/>
       <c r="B57" t="s">
         <v>156</v>
       </c>
       <c r="G57" s="19"/>
       <c r="H57" s="11"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A58" s="49"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="53"/>
       <c r="B58" t="s">
         <v>157</v>
       </c>
       <c r="G58" s="19"/>
       <c r="H58" s="11"/>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A59" s="49"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="53"/>
       <c r="B59" t="s">
         <v>158</v>
       </c>
       <c r="G59" s="19"/>
       <c r="H59" s="11"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A60" s="49"/>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="53"/>
       <c r="B60" t="s">
         <v>159</v>
       </c>
       <c r="G60" s="19"/>
       <c r="H60" s="11"/>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A61" s="49"/>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="53"/>
       <c r="B61" t="s">
         <v>160</v>
       </c>
       <c r="G61" s="19"/>
       <c r="H61" s="11"/>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="8"/>
       <c r="G62" s="19"/>
       <c r="H62" s="11"/>
     </row>
-    <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="49" t="s">
+    <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="53" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
@@ -4499,59 +4542,59 @@
       <c r="G63" s="19"/>
       <c r="H63" s="11"/>
     </row>
-    <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A64" s="49"/>
+    <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="53"/>
       <c r="B64" t="s">
         <v>163</v>
       </c>
       <c r="G64" s="19"/>
       <c r="H64" s="11"/>
     </row>
-    <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A65" s="49"/>
+    <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="53"/>
       <c r="B65" t="s">
         <v>164</v>
       </c>
       <c r="G65" s="19"/>
       <c r="H65" s="11"/>
     </row>
-    <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A66" s="49"/>
+    <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="53"/>
       <c r="B66" t="s">
         <v>165</v>
       </c>
       <c r="G66" s="19"/>
       <c r="H66" s="11"/>
     </row>
-    <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A67" s="49"/>
+    <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="53"/>
       <c r="B67" t="s">
         <v>166</v>
       </c>
       <c r="G67" s="19"/>
       <c r="H67" s="11"/>
     </row>
-    <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A68" s="49"/>
+    <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="53"/>
       <c r="B68" t="s">
         <v>167</v>
       </c>
       <c r="G68" s="19"/>
       <c r="H68" s="11"/>
     </row>
-    <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A69" s="49"/>
+    <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="53"/>
       <c r="B69" t="s">
         <v>168</v>
       </c>
       <c r="G69" s="19"/>
       <c r="H69" s="11"/>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="G70" s="19"/>
       <c r="H70" s="11"/>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
         <v>50</v>
       </c>
@@ -4568,7 +4611,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
         <v>50</v>
       </c>
@@ -4585,7 +4628,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
         <v>50</v>
       </c>
@@ -4602,7 +4645,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
         <v>50</v>
       </c>
@@ -4619,7 +4662,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
         <v>50</v>
       </c>
@@ -4636,7 +4679,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
         <v>50</v>
       </c>
@@ -4653,7 +4696,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
         <v>50</v>
       </c>
@@ -4670,7 +4713,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
         <v>50</v>
       </c>
@@ -4687,7 +4730,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
         <v>50</v>
       </c>
@@ -4704,7 +4747,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
         <v>50</v>
       </c>
@@ -4721,7 +4764,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C81" t="s">
         <v>50</v>
       </c>
@@ -4738,7 +4781,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C82" t="s">
         <v>50</v>
       </c>
@@ -4755,7 +4798,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="83" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="C83" t="s">
         <v>50</v>
       </c>
@@ -4772,7 +4815,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="84" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C84" t="s">
         <v>50</v>
       </c>
@@ -4789,7 +4832,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="85" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A85" s="32" t="s">
         <v>183</v>
       </c>
@@ -4809,7 +4852,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="86" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A86" s="32" t="s">
         <v>183</v>
       </c>
@@ -4829,7 +4872,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="87" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="C87" t="s">
         <v>50</v>
       </c>
@@ -4846,7 +4889,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="88" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A88" s="32" t="s">
         <v>186</v>
       </c>
@@ -4866,7 +4909,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="89" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A89" s="32" t="s">
         <v>186</v>
       </c>
@@ -4886,7 +4929,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="90" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A90" s="32" t="s">
         <v>186</v>
       </c>
@@ -4906,7 +4949,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="91" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A91" s="32" t="s">
         <v>186</v>
       </c>
@@ -4926,7 +4969,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="92" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A92" s="32" t="s">
         <v>186</v>
       </c>
@@ -4946,7 +4989,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="93" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="93" spans="1:8" s="35" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A93" s="35" t="s">
         <v>192</v>
       </c>
@@ -4967,7 +5010,7 @@
       </c>
       <c r="H93" s="36"/>
     </row>
-    <row r="94" spans="1:8" s="35" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="94" spans="1:8" s="35" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="35" t="s">
         <v>192</v>
       </c>
@@ -4988,7 +5031,7 @@
       </c>
       <c r="H94" s="36"/>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="95" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A95" s="27" t="s">
         <v>195</v>
       </c>
@@ -5008,7 +5051,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="96" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A96" s="27" t="s">
         <v>195</v>
       </c>
@@ -5028,7 +5071,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="97" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="97" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A97" s="27" t="s">
         <v>199</v>
       </c>
@@ -5048,7 +5091,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="98" spans="1:13" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="98" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>201</v>
       </c>
@@ -5068,15 +5111,15 @@
         <v>203</v>
       </c>
     </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G99" s="29"/>
       <c r="H99" s="13"/>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G100" s="29"/>
       <c r="H100" s="13"/>
     </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" s="17" t="s">
         <v>204</v>
       </c>
@@ -5092,7 +5135,7 @@
       <c r="K102" s="18"/>
       <c r="L102" s="18"/>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="103" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>205</v>
       </c>
@@ -5112,7 +5155,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="104" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>208</v>
       </c>
@@ -5138,7 +5181,7 @@
         <v>16000000000</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="105" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>212</v>
       </c>
@@ -5158,7 +5201,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="106" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>215</v>
       </c>
@@ -5178,7 +5221,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="107" spans="1:13" ht="187.2" x14ac:dyDescent="0.6">
+    <row r="107" spans="1:13" ht="221" x14ac:dyDescent="0.2">
       <c r="A107" s="27" t="s">
         <v>219</v>
       </c>
@@ -5201,7 +5244,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="108" spans="1:13" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="108" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>223</v>
       </c>
@@ -5221,7 +5264,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="109" spans="1:13" s="24" customFormat="1" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="109" spans="1:13" s="24" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B109" s="24" t="s">
         <v>226</v>
       </c>
@@ -5247,7 +5290,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="110" spans="1:13" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="110" spans="1:13" ht="51" x14ac:dyDescent="0.2">
       <c r="A110" s="32" t="s">
         <v>230</v>
       </c>
@@ -5270,7 +5313,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="111" spans="1:13" ht="124.8" x14ac:dyDescent="0.6">
+    <row r="111" spans="1:13" ht="136" x14ac:dyDescent="0.2">
       <c r="A111" s="27" t="s">
         <v>234</v>
       </c>
@@ -5302,7 +5345,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:13" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="112" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>239</v>
       </c>
@@ -5322,7 +5365,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="113" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="113" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>242</v>
       </c>
@@ -5342,7 +5385,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="114" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>246</v>
       </c>
@@ -5360,7 +5403,7 @@
       </c>
       <c r="H114" s="11"/>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="115" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>248</v>
       </c>
@@ -5378,7 +5421,7 @@
       </c>
       <c r="H115" s="11"/>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="116" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A116" s="32" t="s">
         <v>230</v>
       </c>
@@ -5398,7 +5441,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="117" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="117" spans="1:8" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C117" s="9" t="s">
         <v>251</v>
       </c>
@@ -5408,7 +5451,7 @@
       <c r="G117" s="16"/>
       <c r="H117" s="16"/>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="118" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>253</v>
       </c>
@@ -5426,7 +5469,7 @@
       </c>
       <c r="H118" s="11"/>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="119" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>255</v>
       </c>
@@ -5444,7 +5487,7 @@
       </c>
       <c r="H119" s="11"/>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="120" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>257</v>
       </c>
@@ -5462,7 +5505,7 @@
       </c>
       <c r="H120" s="11"/>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="121" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>259</v>
       </c>
@@ -5480,7 +5523,7 @@
       </c>
       <c r="H121" s="11"/>
     </row>
-    <row r="122" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="122" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>261</v>
       </c>
@@ -5498,7 +5541,7 @@
       </c>
       <c r="H122" s="11"/>
     </row>
-    <row r="123" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="123" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>263</v>
       </c>
@@ -5516,7 +5559,7 @@
       </c>
       <c r="H123" s="11"/>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="124" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>265</v>
       </c>
@@ -5534,7 +5577,7 @@
       </c>
       <c r="H124" s="11"/>
     </row>
-    <row r="125" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="125" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>267</v>
       </c>
@@ -5552,7 +5595,7 @@
       </c>
       <c r="H125" s="11"/>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="126" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>269</v>
       </c>
@@ -5570,7 +5613,7 @@
       </c>
       <c r="H126" s="11"/>
     </row>
-    <row r="127" spans="1:8" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="127" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>271</v>
       </c>
@@ -5588,7 +5631,7 @@
       </c>
       <c r="H127" s="11"/>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="128" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>273</v>
       </c>
@@ -5606,7 +5649,7 @@
       </c>
       <c r="H128" s="11"/>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="129" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>275</v>
       </c>
@@ -5624,7 +5667,7 @@
       </c>
       <c r="H129" s="11"/>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="130" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>277</v>
       </c>
@@ -5642,7 +5685,7 @@
       </c>
       <c r="H130" s="11"/>
     </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="131" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>279</v>
       </c>
@@ -5660,7 +5703,7 @@
       </c>
       <c r="H131" s="11"/>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="132" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>281</v>
       </c>
@@ -5677,15 +5720,15 @@
         <v>282</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G133" s="19"/>
       <c r="H133" s="11"/>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="G134" s="19"/>
       <c r="H134" s="11"/>
     </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" s="17" t="s">
         <v>283</v>
       </c>
@@ -5701,7 +5744,7 @@
       <c r="K135" s="18"/>
       <c r="L135" s="18"/>
     </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="136" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A136" s="32" t="s">
         <v>284</v>
       </c>
@@ -5722,7 +5765,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="137" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A137" s="32" t="s">
         <v>284</v>
       </c>
@@ -5740,7 +5783,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="138" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A138" s="32" t="s">
         <v>284</v>
       </c>
@@ -5758,7 +5801,7 @@
       </c>
       <c r="H138" s="11"/>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="139" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A139" s="32" t="s">
         <v>284</v>
       </c>
@@ -5776,7 +5819,7 @@
       </c>
       <c r="H139" s="11"/>
     </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="140" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A140" s="32" t="s">
         <v>284</v>
       </c>
@@ -5802,7 +5845,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="141" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A141" s="32" t="s">
         <v>284</v>
       </c>
@@ -5813,7 +5856,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="142" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A142" s="32" t="s">
         <v>284</v>
       </c>
@@ -5828,7 +5871,7 @@
       </c>
       <c r="H142" s="11"/>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="143" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A143" s="32" t="s">
         <v>284</v>
       </c>
@@ -5843,7 +5886,7 @@
       </c>
       <c r="H143" s="11"/>
     </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.6">
+    <row r="144" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A144" s="32" t="s">
         <v>284</v>
       </c>
@@ -5860,7 +5903,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="145" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A145" s="32" t="s">
         <v>284</v>
       </c>
@@ -5878,7 +5921,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="146" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A146" s="32" t="s">
         <v>284</v>
       </c>
@@ -5896,7 +5939,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="147" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A147" s="32" t="s">
         <v>284</v>
       </c>
@@ -5914,7 +5957,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="148" spans="1:12" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="148" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A148" s="32" t="s">
         <v>284</v>
       </c>
@@ -5934,7 +5977,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="149" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A149" s="32" t="s">
         <v>284</v>
       </c>
@@ -5952,7 +5995,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A150" s="17" t="s">
         <v>303</v>
       </c>
@@ -5968,7 +6011,7 @@
       <c r="K150" s="18"/>
       <c r="L150" s="18"/>
     </row>
-    <row r="151" spans="1:12" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="151" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="B151" t="s">
         <v>304</v>
       </c>
@@ -5980,13 +6023,13 @@
       <c r="K151" s="8"/>
       <c r="L151" s="8"/>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I152" s="8"/>
       <c r="J152" s="8"/>
       <c r="K152" s="8"/>
       <c r="L152" s="8"/>
     </row>
-    <row r="153" spans="1:12" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="153" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="B153" t="s">
         <v>306</v>
       </c>
@@ -5998,7 +6041,7 @@
       <c r="K153" s="8"/>
       <c r="L153" s="8"/>
     </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="154" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A154" s="17" t="s">
         <v>308</v>
       </c>
@@ -6014,7 +6057,7 @@
       <c r="K154" s="18"/>
       <c r="L154" s="18"/>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B155" t="s">
         <v>309</v>
       </c>
@@ -6023,7 +6066,7 @@
       <c r="K155" s="8"/>
       <c r="L155" s="8"/>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B156" t="s">
         <v>310</v>
       </c>
@@ -6032,7 +6075,7 @@
       <c r="K156" s="8"/>
       <c r="L156" s="8"/>
     </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="157" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B157" t="s">
         <v>311</v>
       </c>
@@ -6041,7 +6084,7 @@
       <c r="K157" s="8"/>
       <c r="L157" s="8"/>
     </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="158" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B158" t="s">
         <v>312</v>
       </c>
@@ -6050,7 +6093,7 @@
       <c r="K158" s="8"/>
       <c r="L158" s="8"/>
     </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="159" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B159" t="s">
         <v>313</v>
       </c>
@@ -6059,7 +6102,7 @@
       <c r="K159" s="8"/>
       <c r="L159" s="8"/>
     </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="160" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B160" t="s">
         <v>314</v>
       </c>
@@ -6068,7 +6111,7 @@
       <c r="K160" s="8"/>
       <c r="L160" s="8"/>
     </row>
-    <row r="161" spans="1:12" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="161" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A161" s="32" t="s">
         <v>284</v>
       </c>
@@ -6083,13 +6126,13 @@
       <c r="K161" s="8"/>
       <c r="L161" s="8"/>
     </row>
-    <row r="162" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="162" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I162" s="8"/>
       <c r="J162" s="8"/>
       <c r="K162" s="8"/>
       <c r="L162" s="8"/>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A163" s="17" t="s">
         <v>317</v>
       </c>
@@ -6105,7 +6148,7 @@
       <c r="K163" s="18"/>
       <c r="L163" s="18"/>
     </row>
-    <row r="164" spans="1:12" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="164" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A164" s="27" t="s">
         <v>318</v>
       </c>
@@ -6120,19 +6163,19 @@
       <c r="K164" s="8"/>
       <c r="L164" s="8"/>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I165" s="8"/>
       <c r="J165" s="8"/>
       <c r="K165" s="8"/>
       <c r="L165" s="8"/>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.2">
       <c r="I166" s="8"/>
       <c r="J166" s="8"/>
       <c r="K166" s="8"/>
       <c r="L166" s="8"/>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="167" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="A167" s="17" t="s">
         <v>321</v>
       </c>
@@ -6150,7 +6193,7 @@
       <c r="K167" s="18"/>
       <c r="L167" s="18"/>
     </row>
-    <row r="168" spans="1:12" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="168" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="G168" s="16" t="s">
         <v>323</v>
       </c>
@@ -6158,7 +6201,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="169" spans="1:12" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="169" spans="1:12" ht="34" x14ac:dyDescent="0.2">
       <c r="A169" s="32" t="s">
         <v>230</v>
       </c>
@@ -6172,7 +6215,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="170" spans="1:12" ht="93.6" x14ac:dyDescent="0.6">
+    <row r="170" spans="1:12" ht="119" x14ac:dyDescent="0.2">
       <c r="A170" s="32" t="s">
         <v>230</v>
       </c>
@@ -6183,7 +6226,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="171" spans="1:12" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="171" spans="1:12" ht="51" x14ac:dyDescent="0.2">
       <c r="A171" s="32" t="s">
         <v>230</v>
       </c>
@@ -6197,7 +6240,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.6">
+    <row r="172" spans="1:12" ht="17" x14ac:dyDescent="0.2">
       <c r="B172" t="s">
         <v>331</v>
       </c>
@@ -6208,7 +6251,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A180" s="12"/>
       <c r="B180" s="12"/>
       <c r="C180" s="12"/>
@@ -6217,23 +6260,18 @@
       <c r="F180" s="12"/>
       <c r="G180" s="13"/>
     </row>
-    <row r="192" spans="1:7" x14ac:dyDescent="0.6">
+    <row r="192" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B192" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="193" spans="2:2" x14ac:dyDescent="0.6">
+    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B193" t="s">
         <v>334</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A55:A61"/>
     <mergeCell ref="A63:A69"/>
     <mergeCell ref="M1:M2"/>
@@ -6250,6 +6288,11 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6266,104 +6309,104 @@
   <dimension ref="A1:V79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <pane ySplit="2" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.34765625" customWidth="1"/>
-    <col min="2" max="2" width="24.84765625" customWidth="1"/>
-    <col min="3" max="3" width="15.1484375" customWidth="1"/>
-    <col min="4" max="4" width="11.6484375" customWidth="1"/>
-    <col min="5" max="5" width="10.34765625" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.33203125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
-    <col min="7" max="7" width="35.34765625" customWidth="1"/>
-    <col min="8" max="8" width="28.84765625" customWidth="1"/>
-    <col min="9" max="9" width="9.1484375" customWidth="1"/>
+    <col min="7" max="7" width="35.33203125" customWidth="1"/>
+    <col min="8" max="8" width="28.83203125" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" customWidth="1"/>
     <col min="10" max="10" width="7" customWidth="1"/>
     <col min="11" max="11" width="8.5" customWidth="1"/>
     <col min="13" max="13" width="26.5" customWidth="1"/>
-    <col min="14" max="14" width="15.34765625" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
-    <col min="18" max="18" width="11.1484375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.6484375" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" customWidth="1"/>
     <col min="22" max="22" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="15.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="54"/>
-      <c r="B1" s="55" t="s">
+    <row r="1" spans="1:22" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="56"/>
+      <c r="B1" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="56" t="s">
+      <c r="D1" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="55" t="s">
+      <c r="E1" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="55" t="s">
+      <c r="F1" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="56" t="s">
+      <c r="G1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="58" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="I1" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="50" t="s">
+      <c r="J1" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="50"/>
-      <c r="L1" s="52" t="s">
+      <c r="K1" s="54"/>
+      <c r="L1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="50" t="s">
+      <c r="M1" s="54" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="50" t="s">
+      <c r="N1" s="54" t="s">
         <v>520</v>
       </c>
-      <c r="O1" s="52" t="s">
+      <c r="O1" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="54" t="s">
+      <c r="Q1" s="56" t="s">
         <v>521</v>
       </c>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="U1" s="54" t="s">
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="U1" s="56" t="s">
         <v>526</v>
       </c>
-      <c r="V1" s="54"/>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.6">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="57"/>
+      <c r="V1" s="56"/>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A2" s="57"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="59"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="53"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="53"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="52"/>
       <c r="Q2" s="1" t="s">
         <v>522</v>
       </c>
@@ -6380,7 +6423,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>14</v>
       </c>
@@ -6399,13 +6442,16 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>444</v>
       </c>
       <c r="C5" t="s">
         <v>445</v>
       </c>
+      <c r="D5" t="s">
+        <v>51</v>
+      </c>
       <c r="E5" t="s">
         <v>17</v>
       </c>
@@ -6421,14 +6467,20 @@
       <c r="Q5" s="40" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.6">
+      <c r="R5" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>447</v>
       </c>
       <c r="C6" t="s">
         <v>445</v>
       </c>
+      <c r="D6" t="s">
+        <v>51</v>
+      </c>
       <c r="E6" t="s">
         <v>17</v>
       </c>
@@ -6444,8 +6496,11 @@
       <c r="Q6" s="40" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
+      <c r="R6" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>137</v>
       </c>
@@ -6477,7 +6532,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>453</v>
       </c>
@@ -6509,7 +6564,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B9" s="39" t="s">
         <v>456</v>
       </c>
@@ -6547,7 +6602,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="10" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>460</v>
       </c>
@@ -6579,7 +6634,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B11" s="39" t="s">
         <v>463</v>
       </c>
@@ -6617,7 +6672,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>467</v>
       </c>
@@ -6655,7 +6710,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B13" s="39" t="s">
         <v>468</v>
       </c>
@@ -6693,7 +6748,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="14" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="14" spans="1:22" ht="34" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>469</v>
       </c>
@@ -6725,7 +6780,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.6">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B15" s="39" t="s">
         <v>557</v>
       </c>
@@ -6742,7 +6797,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.6">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B16" s="39" t="s">
         <v>559</v>
       </c>
@@ -6759,10 +6814,10 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="39"/>
     </row>
-    <row r="18" spans="2:18" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="18" spans="2:18" ht="34" x14ac:dyDescent="0.2">
       <c r="B18" s="39" t="s">
         <v>561</v>
       </c>
@@ -6776,7 +6831,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="19" spans="2:18" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="19" spans="2:18" ht="51" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>537</v>
       </c>
@@ -6802,7 +6857,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="20" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>538</v>
       </c>
@@ -6825,12 +6880,12 @@
         <v>525</v>
       </c>
     </row>
-    <row r="21" spans="2:18" s="44" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="21" spans="2:18" s="44" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B21" s="44" t="s">
         <v>543</v>
       </c>
     </row>
-    <row r="23" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>555</v>
       </c>
@@ -6856,7 +6911,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
         <v>556</v>
       </c>
@@ -6882,7 +6937,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>253</v>
       </c>
@@ -6902,7 +6957,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
         <v>255</v>
       </c>
@@ -6922,7 +6977,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="27" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>473</v>
       </c>
@@ -6942,7 +6997,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>474</v>
       </c>
@@ -6962,7 +7017,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="29" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>273</v>
       </c>
@@ -6982,7 +7037,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="30" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="30" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>275</v>
       </c>
@@ -7002,7 +7057,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="31" spans="2:18" x14ac:dyDescent="0.6">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>277</v>
       </c>
@@ -7019,7 +7074,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="33" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="33" spans="2:19" ht="34" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>77</v>
       </c>
@@ -7063,7 +7118,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="34" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="34" spans="2:19" ht="34" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>81</v>
       </c>
@@ -7107,7 +7162,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="35" spans="2:19" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="35" spans="2:19" ht="68" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>84</v>
       </c>
@@ -7151,7 +7206,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="36" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="36" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B36" s="44" t="s">
         <v>500</v>
       </c>
@@ -7174,7 +7229,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="37" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>88</v>
       </c>
@@ -7204,7 +7259,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="38" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="38" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B38" s="44" t="s">
         <v>443</v>
       </c>
@@ -7227,7 +7282,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="39" spans="2:19" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="39" spans="2:19" ht="51" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>90</v>
       </c>
@@ -7268,7 +7323,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="40" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>93</v>
       </c>
@@ -7298,7 +7353,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="41" spans="2:19" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="41" spans="2:19" ht="68" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>95</v>
       </c>
@@ -7342,7 +7397,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="42" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="42" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B42" s="44" t="s">
         <v>503</v>
       </c>
@@ -7362,7 +7417,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="43" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>97</v>
       </c>
@@ -7392,7 +7447,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="44" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="44" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B44" s="44" t="s">
         <v>449</v>
       </c>
@@ -7412,7 +7467,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="45" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
         <v>99</v>
       </c>
@@ -7453,7 +7508,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="46" spans="2:19" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="46" spans="2:19" ht="68" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
         <v>105</v>
       </c>
@@ -7497,7 +7552,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="47" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="47" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B47" s="44" t="s">
         <v>506</v>
       </c>
@@ -7514,31 +7569,31 @@
         <v>120</v>
       </c>
     </row>
-    <row r="48" spans="2:19" x14ac:dyDescent="0.6">
-      <c r="B48" t="s">
+    <row r="48" spans="2:19" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B48" s="44" t="s">
         <v>447</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E48" t="s">
-        <v>17</v>
-      </c>
-      <c r="G48" s="8" t="s">
+      <c r="E48" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G48" s="45" t="s">
         <v>481</v>
       </c>
-      <c r="H48" s="19"/>
-      <c r="N48">
+      <c r="H48" s="46"/>
+      <c r="N48" s="44">
         <v>120</v>
       </c>
-      <c r="R48" t="s">
+      <c r="R48" s="44" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="49" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="49" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>109</v>
       </c>
@@ -7582,7 +7637,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="50" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="50" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B50" t="s">
         <v>112</v>
       </c>
@@ -7626,7 +7681,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="51" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="51" spans="2:19" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B51" s="44" t="s">
         <v>509</v>
       </c>
@@ -7643,31 +7698,31 @@
         <v>120</v>
       </c>
     </row>
-    <row r="52" spans="2:19" x14ac:dyDescent="0.6">
-      <c r="B52" t="s">
+    <row r="52" spans="2:19" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="B52" s="44" t="s">
         <v>444</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D52" s="44" t="s">
         <v>51</v>
       </c>
-      <c r="E52" t="s">
-        <v>17</v>
-      </c>
-      <c r="G52" s="19" t="s">
+      <c r="E52" s="44" t="s">
+        <v>17</v>
+      </c>
+      <c r="G52" s="46" t="s">
         <v>483</v>
       </c>
-      <c r="H52" s="11"/>
-      <c r="N52">
+      <c r="H52" s="47"/>
+      <c r="N52" s="44">
         <v>120</v>
       </c>
-      <c r="R52" t="s">
+      <c r="R52" s="44" t="s">
         <v>545</v>
       </c>
     </row>
-    <row r="53" spans="2:19" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="53" spans="2:19" ht="51" x14ac:dyDescent="0.2">
       <c r="B53" t="s">
         <v>115</v>
       </c>
@@ -7711,7 +7766,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="54" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="54" spans="2:19" ht="34" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>118</v>
       </c>
@@ -7752,7 +7807,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="55" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="55" spans="2:19" ht="51" x14ac:dyDescent="0.2">
       <c r="B55" s="42" t="s">
         <v>536</v>
       </c>
@@ -7786,11 +7841,14 @@
       <c r="N55">
         <v>120</v>
       </c>
+      <c r="Q55" s="83" t="s">
+        <v>26</v>
+      </c>
       <c r="R55" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="56" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="56" spans="2:19" ht="34" x14ac:dyDescent="0.2">
       <c r="B56" t="s">
         <v>126</v>
       </c>
@@ -7811,11 +7869,14 @@
       <c r="N56">
         <v>120</v>
       </c>
+      <c r="Q56" s="83" t="s">
+        <v>26</v>
+      </c>
       <c r="R56" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="57" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="57" spans="2:19" ht="34" x14ac:dyDescent="0.2">
       <c r="B57" t="s">
         <v>127</v>
       </c>
@@ -7853,7 +7914,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="58" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="58" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B58" s="44" t="s">
         <v>513</v>
       </c>
@@ -7867,7 +7928,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="59" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="59" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B59" t="s">
         <v>130</v>
       </c>
@@ -7905,7 +7966,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="60" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="60" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>133</v>
       </c>
@@ -7946,7 +8007,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="61" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="61" spans="2:19" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B61" s="44" t="s">
         <v>516</v>
       </c>
@@ -7966,7 +8027,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="62" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>135</v>
       </c>
@@ -7996,19 +8057,19 @@
         <v>545</v>
       </c>
     </row>
-    <row r="63" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="63" spans="2:19" x14ac:dyDescent="0.2">
       <c r="G63" s="8"/>
       <c r="H63" s="11"/>
     </row>
-    <row r="64" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="64" spans="2:19" x14ac:dyDescent="0.2">
       <c r="G64" s="8"/>
       <c r="H64" s="11"/>
     </row>
-    <row r="65" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="65" spans="2:19" x14ac:dyDescent="0.2">
       <c r="G65" s="8"/>
       <c r="H65" s="11"/>
     </row>
-    <row r="66" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="66" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>139</v>
       </c>
@@ -8053,7 +8114,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="67" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="67" spans="2:19" ht="17" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>141</v>
       </c>
@@ -8089,7 +8150,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="69" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="69" spans="2:19" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B69" s="44" t="s">
         <v>15</v>
       </c>
@@ -8127,7 +8188,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="70" spans="2:19" s="44" customFormat="1" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="70" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B70" s="44" t="s">
         <v>22</v>
       </c>
@@ -8165,7 +8226,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="71" spans="2:19" s="44" customFormat="1" x14ac:dyDescent="0.6">
+    <row r="71" spans="2:19" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="B71" s="44" t="s">
         <v>27</v>
       </c>
@@ -8206,7 +8267,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="72" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="72" spans="2:19" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B72" s="44" t="s">
         <v>493</v>
       </c>
@@ -8236,7 +8297,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="73" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="73" spans="2:19" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="B73" s="44" t="s">
         <v>492</v>
       </c>
@@ -8266,7 +8327,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="74" spans="2:19" s="44" customFormat="1" ht="31.2" x14ac:dyDescent="0.6">
+    <row r="74" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
       <c r="B74" s="44" t="s">
         <v>40</v>
       </c>
@@ -8304,7 +8365,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="75" spans="2:19" s="44" customFormat="1" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="75" spans="2:19" s="44" customFormat="1" ht="68" x14ac:dyDescent="0.2">
       <c r="B75" s="44" t="s">
         <v>44</v>
       </c>
@@ -8327,7 +8388,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="77" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="77" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>497</v>
       </c>
@@ -8335,7 +8396,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="78" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="78" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>498</v>
       </c>
@@ -8343,7 +8404,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="79" spans="2:19" x14ac:dyDescent="0.6">
+    <row r="79" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>499</v>
       </c>
@@ -8353,6 +8414,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="J72:K72"/>
     <mergeCell ref="J73:K73"/>
@@ -8360,17 +8432,6 @@
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8387,9 +8448,9 @@
       <selection activeCell="E19" sqref="E19:E20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="109.2" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>335</v>
       </c>
@@ -8403,7 +8464,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="12"/>
       <c r="B2" s="12" t="s">
         <v>26</v>
@@ -8419,7 +8480,7 @@
       </c>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>338</v>
       </c>
@@ -8431,7 +8492,7 @@
       <c r="G3" s="12"/>
       <c r="H3" s="8"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="12"/>
       <c r="B4" s="12" t="s">
         <v>339</v>
@@ -8451,7 +8512,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="12"/>
       <c r="B5" s="12" t="s">
         <v>343</v>
@@ -8471,7 +8532,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="62.4" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A6" s="12"/>
       <c r="B6" s="12" t="s">
         <v>346</v>
@@ -8491,7 +8552,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="12"/>
       <c r="B7" s="12" t="s">
         <v>349</v>
@@ -8511,7 +8572,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="140.4" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:8" ht="153" x14ac:dyDescent="0.2">
       <c r="A8" s="12"/>
       <c r="B8" s="12" t="s">
         <v>351</v>
@@ -8531,7 +8592,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="12"/>
       <c r="B9" s="12" t="s">
         <v>354</v>
@@ -8551,7 +8612,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="358.8" x14ac:dyDescent="0.6">
+    <row r="10" spans="1:8" ht="388" x14ac:dyDescent="0.2">
       <c r="A10" s="12"/>
       <c r="B10" s="12" t="s">
         <v>357</v>
@@ -8571,7 +8632,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A11" s="12"/>
       <c r="B11" s="12" t="s">
         <v>360</v>
@@ -8591,7 +8652,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="124.8" x14ac:dyDescent="0.6">
+    <row r="12" spans="1:8" ht="136" x14ac:dyDescent="0.2">
       <c r="A12" s="12"/>
       <c r="B12" s="12" t="s">
         <v>362</v>
@@ -8627,9 +8688,9 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>209</v>
       </c>
@@ -8642,40 +8703,40 @@
       <c r="D1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="61" t="s">
+      <c r="E1" s="78" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="62"/>
-      <c r="G1" s="61" t="s">
+      <c r="F1" s="79"/>
+      <c r="G1" s="78" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="62"/>
-    </row>
-    <row r="2" spans="1:8" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="63" t="s">
+      <c r="H1" s="79"/>
+    </row>
+    <row r="2" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="80" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="65"/>
-    </row>
-    <row r="3" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="82"/>
+    </row>
+    <row r="3" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="61" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="68"/>
-    </row>
-    <row r="4" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="62"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="63"/>
+    </row>
+    <row r="4" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>1</v>
       </c>
@@ -8683,15 +8744,15 @@
         <v>370</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="70"/>
-      <c r="F4" s="71" t="s">
+      <c r="D4" s="70"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="68" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="72"/>
+      <c r="G4" s="69"/>
       <c r="H4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6">
         <v>2</v>
       </c>
@@ -8699,15 +8760,15 @@
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="76"/>
-      <c r="F5" s="73" t="s">
+      <c r="D5" s="66"/>
+      <c r="E5" s="67"/>
+      <c r="F5" s="64" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="74"/>
+      <c r="G5" s="65"/>
       <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>3</v>
       </c>
@@ -8715,15 +8776,15 @@
         <v>372</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="71" t="s">
+      <c r="D6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="68" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="72"/>
+      <c r="G6" s="69"/>
       <c r="H6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>4</v>
       </c>
@@ -8731,15 +8792,15 @@
         <v>373</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="75"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="73" t="s">
+      <c r="D7" s="66"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="64" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="74"/>
+      <c r="G7" s="65"/>
       <c r="H7" s="3"/>
     </row>
-    <row r="8" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>5</v>
       </c>
@@ -8747,15 +8808,15 @@
         <v>53</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="71" t="s">
+      <c r="D8" s="70"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="68" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="72"/>
+      <c r="G8" s="69"/>
       <c r="H8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:8" ht="66" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -8763,27 +8824,27 @@
         <v>374</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="76"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="76"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="67"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="67"/>
       <c r="H9" s="6" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="75" t="s">
         <v>376</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="78"/>
-      <c r="E10" s="78"/>
-      <c r="F10" s="78"/>
-      <c r="G10" s="78"/>
-      <c r="H10" s="79"/>
-    </row>
-    <row r="11" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="77"/>
+    </row>
+    <row r="11" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>7</v>
       </c>
@@ -8793,15 +8854,15 @@
       <c r="C11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="73" t="s">
+      <c r="D11" s="64" t="s">
         <v>378</v>
       </c>
-      <c r="E11" s="74"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="76"/>
+      <c r="E11" s="65"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="67"/>
       <c r="H11" s="3"/>
     </row>
-    <row r="12" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>8</v>
       </c>
@@ -8811,15 +8872,15 @@
       <c r="C12" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D12" s="71" t="s">
+      <c r="D12" s="68" t="s">
         <v>378</v>
       </c>
-      <c r="E12" s="72"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="70"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="70"/>
+      <c r="G12" s="71"/>
       <c r="H12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="13" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>9</v>
       </c>
@@ -8829,15 +8890,15 @@
       <c r="C13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="73" t="s">
+      <c r="D13" s="64" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="74"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="76"/>
+      <c r="E13" s="65"/>
+      <c r="F13" s="66"/>
+      <c r="G13" s="67"/>
       <c r="H13" s="3"/>
     </row>
-    <row r="14" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>10</v>
       </c>
@@ -8845,15 +8906,15 @@
         <v>380</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="71" t="s">
+      <c r="D14" s="68" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="72"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="70"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="70"/>
+      <c r="G14" s="71"/>
       <c r="H14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>11</v>
       </c>
@@ -8863,15 +8924,15 @@
       <c r="C15" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="73" t="s">
+      <c r="D15" s="64" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="74"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="76"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="66"/>
+      <c r="G15" s="67"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:8" ht="53" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>12</v>
       </c>
@@ -8881,15 +8942,15 @@
       <c r="C16" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D16" s="71" t="s">
+      <c r="D16" s="68" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="72"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="70"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="70"/>
+      <c r="G16" s="71"/>
       <c r="H16" s="5"/>
     </row>
-    <row r="17" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:8" ht="53" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>13</v>
       </c>
@@ -8899,15 +8960,15 @@
       <c r="C17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D17" s="73" t="s">
+      <c r="D17" s="64" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="74"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="76"/>
+      <c r="E17" s="65"/>
+      <c r="F17" s="66"/>
+      <c r="G17" s="67"/>
       <c r="H17" s="3"/>
     </row>
-    <row r="18" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>14</v>
       </c>
@@ -8917,15 +8978,15 @@
       <c r="C18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D18" s="71" t="s">
+      <c r="D18" s="68" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="72"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="70"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="70"/>
+      <c r="G18" s="71"/>
       <c r="H18" s="5"/>
     </row>
-    <row r="19" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>15</v>
       </c>
@@ -8935,15 +8996,15 @@
       <c r="C19" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="D19" s="73" t="s">
+      <c r="D19" s="64" t="s">
         <v>378</v>
       </c>
-      <c r="E19" s="74"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="76"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="66"/>
+      <c r="G19" s="67"/>
       <c r="H19" s="3"/>
     </row>
-    <row r="20" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>16</v>
       </c>
@@ -8953,15 +9014,15 @@
       <c r="C20" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="68" t="s">
         <v>378</v>
       </c>
-      <c r="E20" s="72"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="70"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="70"/>
+      <c r="G20" s="71"/>
       <c r="H20" s="5"/>
     </row>
-    <row r="21" spans="1:8" ht="117.3" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:8" ht="131" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>17</v>
       </c>
@@ -8971,17 +9032,17 @@
       <c r="C21" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="73" t="s">
+      <c r="D21" s="64" t="s">
         <v>378</v>
       </c>
-      <c r="E21" s="74"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="76"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="67"/>
       <c r="H21" s="6" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>18</v>
       </c>
@@ -8991,15 +9052,15 @@
       <c r="C22" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="71" t="s">
+      <c r="D22" s="68" t="s">
         <v>378</v>
       </c>
-      <c r="E22" s="72"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="70"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="71"/>
       <c r="H22" s="5"/>
     </row>
-    <row r="23" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>209</v>
       </c>
@@ -9019,17 +9080,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:8" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="80" t="s">
+      <c r="B24" s="72" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="81"/>
-      <c r="D24" s="81"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="82"/>
-    </row>
-    <row r="25" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="74"/>
+    </row>
+    <row r="25" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
         <v>18</v>
       </c>
@@ -9045,7 +9106,7 @@
       </c>
       <c r="F25" s="3"/>
     </row>
-    <row r="26" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>19</v>
       </c>
@@ -9061,7 +9122,7 @@
       </c>
       <c r="F26" s="5"/>
     </row>
-    <row r="27" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="27" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>20</v>
       </c>
@@ -9077,7 +9138,7 @@
       </c>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="28" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>21</v>
       </c>
@@ -9093,17 +9154,17 @@
       </c>
       <c r="F28" s="5"/>
     </row>
-    <row r="29" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="29" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="66" t="s">
+      <c r="B29" s="61" t="s">
         <v>396</v>
       </c>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="68"/>
-    </row>
-    <row r="30" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="62"/>
+      <c r="F29" s="63"/>
+    </row>
+    <row r="30" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>22</v>
       </c>
@@ -9117,7 +9178,7 @@
       </c>
       <c r="F30" s="5"/>
     </row>
-    <row r="31" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="31" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="6">
         <v>23</v>
       </c>
@@ -9131,7 +9192,7 @@
       </c>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="32" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>24</v>
       </c>
@@ -9145,7 +9206,7 @@
       </c>
       <c r="F32" s="5"/>
     </row>
-    <row r="33" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="33" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>25</v>
       </c>
@@ -9159,7 +9220,7 @@
       </c>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="34" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>26</v>
       </c>
@@ -9173,7 +9234,7 @@
       </c>
       <c r="F34" s="5"/>
     </row>
-    <row r="35" spans="1:6" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="35" spans="1:6" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>27</v>
       </c>
@@ -9187,7 +9248,7 @@
       </c>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="36" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>28</v>
       </c>
@@ -9201,7 +9262,7 @@
       </c>
       <c r="F36" s="5"/>
     </row>
-    <row r="37" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="37" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>29</v>
       </c>
@@ -9215,7 +9276,7 @@
       </c>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="38" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>30</v>
       </c>
@@ -9229,7 +9290,7 @@
       </c>
       <c r="F38" s="5"/>
     </row>
-    <row r="39" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="39" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>31</v>
       </c>
@@ -9243,7 +9304,7 @@
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="40" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>32</v>
       </c>
@@ -9257,17 +9318,17 @@
       </c>
       <c r="F40" s="5"/>
     </row>
-    <row r="41" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="66" t="s">
+      <c r="B41" s="61" t="s">
         <v>408</v>
       </c>
-      <c r="C41" s="67"/>
-      <c r="D41" s="67"/>
-      <c r="E41" s="67"/>
-      <c r="F41" s="68"/>
-    </row>
-    <row r="42" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="C41" s="62"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="62"/>
+      <c r="F41" s="63"/>
+    </row>
+    <row r="42" spans="1:6" ht="79" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>33</v>
       </c>
@@ -9285,7 +9346,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="43" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="43" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>34</v>
       </c>
@@ -9301,7 +9362,7 @@
       </c>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" ht="105.6" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="44" spans="1:6" ht="118" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>35</v>
       </c>
@@ -9319,7 +9380,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
+    <row r="45" spans="1:6" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>36</v>
       </c>
@@ -9339,31 +9400,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="D5:E5"/>
@@ -9377,12 +9419,31 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -9401,19 +9462,19 @@
       <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.84765625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="34.1484375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="10.34765625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="22.6484375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="8.84765625" style="8" customWidth="1"/>
-    <col min="6" max="8" width="8.84765625" style="8"/>
-    <col min="9" max="9" width="41.1484375" style="8" customWidth="1"/>
-    <col min="10" max="16384" width="8.84765625" style="8"/>
+    <col min="1" max="1" width="12.83203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="34.1640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="8" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" style="8" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="8" customWidth="1"/>
+    <col min="6" max="8" width="8.83203125" style="8"/>
+    <col min="9" max="9" width="41.1640625" style="8" customWidth="1"/>
+    <col min="10" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="13" spans="1:1" ht="46.8" x14ac:dyDescent="0.6">
+    <row r="13" spans="1:1" ht="51" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>321</v>
       </c>
@@ -9436,25 +9497,25 @@
       <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="35.1484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.34765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="22.84765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="2" spans="3:9" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="3" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="3" spans="3:9" x14ac:dyDescent="0.2">
       <c r="I3" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="4" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D4" t="s">
         <v>416</v>
       </c>
@@ -9474,7 +9535,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="5" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D5" t="s">
         <v>422</v>
       </c>
@@ -9485,7 +9546,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.2">
       <c r="D6" t="s">
         <v>422</v>
       </c>
@@ -9496,7 +9557,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="7" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E7" t="s">
         <v>425</v>
       </c>
@@ -9504,7 +9565,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="8" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E8" t="s">
         <v>426</v>
       </c>
@@ -9512,7 +9573,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="9" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E9" t="s">
         <v>427</v>
       </c>
@@ -9520,7 +9581,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="10" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E10" t="s">
         <v>428</v>
       </c>
@@ -9528,12 +9589,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="11" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E11" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="12" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E12" t="s">
         <v>430</v>
       </c>
@@ -9541,17 +9602,17 @@
         <v>84</v>
       </c>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="13" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E13" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="14" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E14" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="15" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E15" t="s">
         <v>433</v>
       </c>
@@ -9559,7 +9620,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.6">
+    <row r="16" spans="3:9" x14ac:dyDescent="0.2">
       <c r="E16" t="s">
         <v>434</v>
       </c>
@@ -9567,12 +9628,12 @@
         <v>435</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.6">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E17" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.6">
+    <row r="18" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E18" t="s">
         <v>437</v>
       </c>
@@ -9580,7 +9641,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.6">
+    <row r="19" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E19" t="s">
         <v>438</v>
       </c>
@@ -9588,7 +9649,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.6">
+    <row r="20" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E20" t="s">
         <v>440</v>
       </c>
@@ -9596,7 +9657,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.6">
+    <row r="21" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E21" t="s">
         <v>441</v>
       </c>
@@ -9619,15 +9680,15 @@
       <selection sqref="A1:H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.84765625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="14.6484375" style="8" customWidth="1"/>
-    <col min="3" max="5" width="8.84765625" style="8"/>
-    <col min="6" max="6" width="10.6484375" style="8" customWidth="1"/>
-    <col min="7" max="7" width="36.1484375" style="8" customWidth="1"/>
-    <col min="8" max="8" width="27.34765625" style="8" customWidth="1"/>
-    <col min="9" max="16384" width="8.84765625" style="8"/>
+    <col min="1" max="1" width="13.83203125" style="8" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="8" customWidth="1"/>
+    <col min="3" max="5" width="8.83203125" style="8"/>
+    <col min="6" max="6" width="10.6640625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="27.33203125" style="8" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="8"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -9647,16 +9708,16 @@
       <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.34765625" customWidth="1"/>
-    <col min="2" max="2" width="11.1484375" customWidth="1"/>
-    <col min="3" max="3" width="13.1484375" customWidth="1"/>
-    <col min="4" max="4" width="20.1484375" customWidth="1"/>
-    <col min="5" max="5" width="19.6484375" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -9674,6 +9735,31 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
+    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EEDE7DDB808AF47B14A37A2563255CF" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="17d65d9f425ad811f92dcb994434cebd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8efcafe-ecab-455b-a9ec-2441266f5451" xmlns:ns3="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35cb6db38e7d3d9001b7e6afffee4001" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
@@ -9984,32 +10070,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
-    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3366D879-DBBC-469C-98D7-600868252265}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10027,24 +10108,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
temperature read tests completed
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjkim/Documents/KeckLFC-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12486D21-60BE-9748-81D8-96D2A6A8367E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930FFA16-13F5-CF4C-B78F-91610E2610AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -60,6 +60,7 @@
     <author>tc={6FBD4EDE-C92B-7942-BB7E-96FEA8EF0D1C}</author>
     <author>tc={9270FBFE-6EFE-1048-9F63-76932967FCB6}</author>
     <author>tc={430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}</author>
+    <author>tc={69B9F1A5-B3CA-CD45-A219-E30415369758}</author>
     <author>tc={897DD710-C2AF-F348-9BE6-70FC899ABE2C}</author>
     <author>tc={D3AE0575-FA6E-1242-8525-02B45DC7B747}</author>
     <author>tc={EF222E0F-25E5-D547-9265-DB5E371F9AC7}</author>
@@ -188,7 +189,15 @@
     Keep them and change names</t>
       </text>
     </comment>
-    <comment ref="F35" authorId="12" shapeId="0" xr:uid="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
+    <comment ref="R33" authorId="12" shapeId="0" xr:uid="{69B9F1A5-B3CA-CD45-A219-E30415369758}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Seems not working now? “Timeout expired before operation completed”</t>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="13" shapeId="0" xr:uid="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -196,7 +205,7 @@
     Implementing as float</t>
       </text>
     </comment>
-    <comment ref="B36" authorId="13" shapeId="0" xr:uid="{D3AE0575-FA6E-1242-8525-02B45DC7B747}">
+    <comment ref="B36" authorId="14" shapeId="0" xr:uid="{D3AE0575-FA6E-1242-8525-02B45DC7B747}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -206,7 +215,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="F36" authorId="14" shapeId="0" xr:uid="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
+    <comment ref="F36" authorId="15" shapeId="0" xr:uid="{EF222E0F-25E5-D547-9265-DB5E371F9AC7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -214,7 +223,7 @@
     Not sure what type it’s supposed to be</t>
       </text>
     </comment>
-    <comment ref="B38" authorId="15" shapeId="0" xr:uid="{91A521E9-8C58-AA4E-9DB6-3B7C40324E9D}">
+    <comment ref="B38" authorId="16" shapeId="0" xr:uid="{91A521E9-8C58-AA4E-9DB6-3B7C40324E9D}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -222,7 +231,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="F38" authorId="16" shapeId="0" xr:uid="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
+    <comment ref="F38" authorId="17" shapeId="0" xr:uid="{E8CBB725-766B-9540-AD26-3D88E8136C7F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -230,7 +239,7 @@
     Not sure what type it’s supposed to be</t>
       </text>
     </comment>
-    <comment ref="B42" authorId="17" shapeId="0" xr:uid="{3A13DE3F-FDB4-D54D-8D34-92EEE889D658}">
+    <comment ref="B42" authorId="18" shapeId="0" xr:uid="{3A13DE3F-FDB4-D54D-8D34-92EEE889D658}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -238,7 +247,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B44" authorId="18" shapeId="0" xr:uid="{A2C7FC53-1505-8A45-99CE-70D3C4FD5518}">
+    <comment ref="B44" authorId="19" shapeId="0" xr:uid="{A2C7FC53-1505-8A45-99CE-70D3C4FD5518}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -246,7 +255,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B47" authorId="19" shapeId="0" xr:uid="{3FE72732-F7D7-6A44-A781-0E38E560C217}">
+    <comment ref="B47" authorId="20" shapeId="0" xr:uid="{3FE72732-F7D7-6A44-A781-0E38E560C217}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -254,7 +263,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B48" authorId="20" shapeId="0" xr:uid="{0D3903E9-918D-E349-9E45-0D2B69F31A28}">
+    <comment ref="B48" authorId="21" shapeId="0" xr:uid="{0D3903E9-918D-E349-9E45-0D2B69F31A28}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -262,7 +271,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B51" authorId="21" shapeId="0" xr:uid="{0490C4F1-599B-AB44-B1CC-7E63E4E8065B}">
+    <comment ref="B51" authorId="22" shapeId="0" xr:uid="{0490C4F1-599B-AB44-B1CC-7E63E4E8065B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -270,7 +279,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B52" authorId="22" shapeId="0" xr:uid="{0228CFF7-2A46-824A-BD7E-D1163401FED7}">
+    <comment ref="B52" authorId="23" shapeId="0" xr:uid="{0228CFF7-2A46-824A-BD7E-D1163401FED7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -278,7 +287,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="F55" authorId="23" shapeId="0" xr:uid="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
+    <comment ref="F55" authorId="24" shapeId="0" xr:uid="{C82D50AC-F6ED-B841-AC03-1967E28B201E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -286,7 +295,7 @@
     Only 1-dimensional array allowed</t>
       </text>
     </comment>
-    <comment ref="F57" authorId="24" shapeId="0" xr:uid="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
+    <comment ref="F57" authorId="25" shapeId="0" xr:uid="{C7739DC9-A5B2-EF49-9CE8-416CEC34862C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -294,7 +303,7 @@
     Implemented as float</t>
       </text>
     </comment>
-    <comment ref="B58" authorId="25" shapeId="0" xr:uid="{3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}">
+    <comment ref="B58" authorId="26" shapeId="0" xr:uid="{3EEF165C-090A-3B4C-84BC-79F7D0EB0E3B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -302,7 +311,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B61" authorId="26" shapeId="0" xr:uid="{B06CDA75-3D09-3A4C-9CA2-5DAFC7D0A49C}">
+    <comment ref="B61" authorId="27" shapeId="0" xr:uid="{B06CDA75-3D09-3A4C-9CA2-5DAFC7D0A49C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -310,7 +319,7 @@
     Not needed</t>
       </text>
     </comment>
-    <comment ref="B69" authorId="27" shapeId="0" xr:uid="{6ED25ED1-E5D3-0547-B2AE-B068D8D2FCAB}">
+    <comment ref="B69" authorId="28" shapeId="0" xr:uid="{6ED25ED1-E5D3-0547-B2AE-B068D8D2FCAB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -318,7 +327,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B71" authorId="28" shapeId="0" xr:uid="{766C4F7D-809F-8546-936F-F77DAB106C65}">
+    <comment ref="B71" authorId="29" shapeId="0" xr:uid="{766C4F7D-809F-8546-936F-F77DAB106C65}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -326,7 +335,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B72" authorId="29" shapeId="0" xr:uid="{BF9BF349-FB0E-2A49-BEAB-473752D32B3F}">
+    <comment ref="B72" authorId="30" shapeId="0" xr:uid="{BF9BF349-FB0E-2A49-BEAB-473752D32B3F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -334,7 +343,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B73" authorId="30" shapeId="0" xr:uid="{506BB1FA-65AC-2844-8BBF-2A90D38F6707}">
+    <comment ref="B73" authorId="31" shapeId="0" xr:uid="{506BB1FA-65AC-2844-8BBF-2A90D38F6707}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -342,7 +351,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B74" authorId="31" shapeId="0" xr:uid="{1DDB399D-F138-F04F-99C1-98F0475A5FB6}">
+    <comment ref="B74" authorId="32" shapeId="0" xr:uid="{1DDB399D-F138-F04F-99C1-98F0475A5FB6}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -350,7 +359,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="B75" authorId="32" shapeId="0" xr:uid="{30C5F121-C7F3-DF45-95C8-DA0E6762ECA7}">
+    <comment ref="B75" authorId="33" shapeId="0" xr:uid="{30C5F121-C7F3-DF45-95C8-DA0E6762ECA7}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -358,7 +367,7 @@
     Duplicate</t>
       </text>
     </comment>
-    <comment ref="H75" authorId="33" shapeId="0" xr:uid="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
+    <comment ref="H75" authorId="34" shapeId="0" xr:uid="{E0A4D72A-0143-6945-8315-0EBFC4A9749A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -3133,6 +3142,9 @@
   <threadedComment ref="B23" dT="2024-06-03T18:43:05.98" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{5296AF8B-E0AA-1846-89CA-ED67E861F12F}" parentId="{430161F5-9D6E-7D48-ABD0-E55BECFA1EC4}">
     <text>Keep them and change names</text>
   </threadedComment>
+  <threadedComment ref="R33" dT="2024-06-04T04:32:52.96" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{69B9F1A5-B3CA-CD45-A219-E30415369758}">
+    <text>Seems not working now? “Timeout expired before operation completed”</text>
+  </threadedComment>
   <threadedComment ref="F35" dT="2024-05-25T16:23:38.53" personId="{AB0A5CF8-0FEB-1C4D-8B82-5ADD7D5C6AAD}" id="{897DD710-C2AF-F348-9BE6-70FC899ABE2C}">
     <text>Implementing as float</text>
   </threadedComment>
@@ -6309,8 +6321,8 @@
   <dimension ref="A1:V79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6953,8 +6965,8 @@
       <c r="Q25" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R25" t="s">
-        <v>545</v>
+      <c r="R25" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
@@ -6973,8 +6985,8 @@
       <c r="Q26" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R26" t="s">
-        <v>545</v>
+      <c r="R26" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
@@ -6993,8 +7005,8 @@
       <c r="Q27" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R27" t="s">
-        <v>545</v>
+      <c r="R27" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
@@ -7013,8 +7025,8 @@
       <c r="Q28" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R28" t="s">
-        <v>545</v>
+      <c r="R28" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.2">
@@ -7033,8 +7045,8 @@
       <c r="Q29" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R29" t="s">
-        <v>545</v>
+      <c r="R29" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.2">
@@ -7053,8 +7065,8 @@
       <c r="Q30" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R30" t="s">
-        <v>545</v>
+      <c r="R30" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
@@ -7067,11 +7079,14 @@
       <c r="F31" t="s">
         <v>533</v>
       </c>
+      <c r="N31">
+        <v>20</v>
+      </c>
       <c r="Q31" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R31" t="s">
-        <v>545</v>
+      <c r="R31" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="33" spans="2:19" ht="34" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated keyword list after tests
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yjkim/Documents/KeckLFC-deploy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930FFA16-13F5-CF4C-B78F-91610E2610AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3445B23C-C5D0-6449-B417-75A91270D097}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17780" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17760" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HSF EO Comb" sheetId="1" r:id="rId1"/>
@@ -398,7 +398,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="563">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1450" uniqueCount="560">
   <si>
     <t>Keyword</t>
   </si>
@@ -2055,9 +2055,6 @@
     <t>can test</t>
   </si>
   <si>
-    <t>test after comb on</t>
-  </si>
-  <si>
     <t>float array(%.2f)</t>
   </si>
   <si>
@@ -2074,12 +2071,6 @@
   </si>
   <si>
     <t>Y (lockout)</t>
-  </si>
-  <si>
-    <t>can test (+/- 0.5 degrees)</t>
-  </si>
-  <si>
-    <t>can test (+/- 0.5 degrees from where it is)</t>
   </si>
   <si>
     <t>LFC_TEMP_TEST1</t>
@@ -2110,7 +2101,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2256,12 +2247,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -2645,18 +2630,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="25" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="25" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2665,6 +2639,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2678,59 +2658,14 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2747,7 +2682,57 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="25" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3251,68 +3236,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56"/>
-      <c r="B1" s="57" t="s">
+      <c r="A1" s="55"/>
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="51" t="s">
+      <c r="K1" s="51"/>
+      <c r="L1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="51" t="s">
+      <c r="N1" s="51"/>
+      <c r="O1" s="53" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="52"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="54"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
@@ -3465,10 +3450,10 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="50" t="s">
+      <c r="J7" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="50"/>
+      <c r="K7" s="59"/>
       <c r="M7">
         <v>0</v>
       </c>
@@ -3495,10 +3480,10 @@
       <c r="H8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="50" t="s">
+      <c r="J8" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="50"/>
+      <c r="K8" s="59"/>
       <c r="M8">
         <v>0</v>
       </c>
@@ -3562,7 +3547,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="60" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
@@ -3586,13 +3571,13 @@
       <c r="H11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="50" t="s">
+      <c r="J11" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="50"/>
+      <c r="K11" s="59"/>
     </row>
     <row r="12" spans="1:19" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="49"/>
+      <c r="A12" s="60"/>
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -3614,10 +3599,10 @@
       <c r="H12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="50" t="s">
+      <c r="J12" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="50"/>
+      <c r="K12" s="59"/>
     </row>
     <row r="13" spans="1:19" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="31"/>
@@ -4482,7 +4467,7 @@
       <c r="H54" s="11"/>
     </row>
     <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="53" t="s">
+      <c r="A55" s="50" t="s">
         <v>153</v>
       </c>
       <c r="B55" t="s">
@@ -4492,7 +4477,7 @@
       <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A56" s="53"/>
+      <c r="A56" s="50"/>
       <c r="B56" t="s">
         <v>155</v>
       </c>
@@ -4500,7 +4485,7 @@
       <c r="H56" s="11"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="53"/>
+      <c r="A57" s="50"/>
       <c r="B57" t="s">
         <v>156</v>
       </c>
@@ -4508,7 +4493,7 @@
       <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="53"/>
+      <c r="A58" s="50"/>
       <c r="B58" t="s">
         <v>157</v>
       </c>
@@ -4516,7 +4501,7 @@
       <c r="H58" s="11"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="53"/>
+      <c r="A59" s="50"/>
       <c r="B59" t="s">
         <v>158</v>
       </c>
@@ -4524,7 +4509,7 @@
       <c r="H59" s="11"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="53"/>
+      <c r="A60" s="50"/>
       <c r="B60" t="s">
         <v>159</v>
       </c>
@@ -4532,7 +4517,7 @@
       <c r="H60" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="53"/>
+      <c r="A61" s="50"/>
       <c r="B61" t="s">
         <v>160</v>
       </c>
@@ -4545,7 +4530,7 @@
       <c r="H62" s="11"/>
     </row>
     <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="53" t="s">
+      <c r="A63" s="50" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
@@ -4555,7 +4540,7 @@
       <c r="H63" s="11"/>
     </row>
     <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="53"/>
+      <c r="A64" s="50"/>
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -4563,7 +4548,7 @@
       <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="53"/>
+      <c r="A65" s="50"/>
       <c r="B65" t="s">
         <v>164</v>
       </c>
@@ -4571,7 +4556,7 @@
       <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="53"/>
+      <c r="A66" s="50"/>
       <c r="B66" t="s">
         <v>165</v>
       </c>
@@ -4579,7 +4564,7 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="53"/>
+      <c r="A67" s="50"/>
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -4587,7 +4572,7 @@
       <c r="H67" s="11"/>
     </row>
     <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="53"/>
+      <c r="A68" s="50"/>
       <c r="B68" t="s">
         <v>167</v>
       </c>
@@ -4595,7 +4580,7 @@
       <c r="H68" s="11"/>
     </row>
     <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="53"/>
+      <c r="A69" s="50"/>
       <c r="B69" t="s">
         <v>168</v>
       </c>
@@ -6284,6 +6269,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A55:A61"/>
     <mergeCell ref="A63:A69"/>
     <mergeCell ref="M1:M2"/>
@@ -6300,11 +6290,6 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6322,7 +6307,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N32" sqref="N32"/>
+      <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6335,11 +6320,12 @@
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="7" max="7" width="35.33203125" customWidth="1"/>
     <col min="8" max="8" width="28.83203125" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" customWidth="1"/>
+    <col min="9" max="9" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7" customWidth="1"/>
     <col min="11" max="11" width="8.5" customWidth="1"/>
-    <col min="13" max="13" width="26.5" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" customWidth="1"/>
     <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="16" max="16" width="3.83203125" customWidth="1"/>
     <col min="17" max="17" width="11" customWidth="1"/>
     <col min="18" max="18" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
@@ -6348,77 +6334,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56"/>
-      <c r="B1" s="57" t="s">
+      <c r="A1" s="55"/>
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="51" t="s">
+      <c r="K1" s="51"/>
+      <c r="L1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="54" t="s">
+      <c r="N1" s="51" t="s">
         <v>520</v>
       </c>
-      <c r="O1" s="51" t="s">
+      <c r="O1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="Q1" s="55" t="s">
         <v>521</v>
       </c>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="U1" s="56" t="s">
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="U1" s="55" t="s">
         <v>526</v>
       </c>
-      <c r="V1" s="56"/>
+      <c r="V1" s="55"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="52"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="54"/>
       <c r="Q2" s="1" t="s">
         <v>522</v>
       </c>
@@ -6639,11 +6625,11 @@
       <c r="Q10" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R10" t="s">
-        <v>545</v>
-      </c>
-      <c r="S10" t="s">
-        <v>545</v>
+      <c r="R10" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S10" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.2">
@@ -6715,11 +6701,11 @@
       <c r="Q12" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R12" s="34" t="s">
-        <v>545</v>
-      </c>
-      <c r="S12" t="s">
-        <v>545</v>
+      <c r="R12" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S12" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.2">
@@ -6785,16 +6771,16 @@
       <c r="Q14" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R14" s="34" t="s">
-        <v>545</v>
-      </c>
-      <c r="S14" t="s">
-        <v>546</v>
+      <c r="R14" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S14" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B15" s="39" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C15" t="s">
         <v>451</v>
@@ -6803,7 +6789,7 @@
         <v>59</v>
       </c>
       <c r="G15" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="N15">
         <v>120</v>
@@ -6811,7 +6797,7 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.2">
       <c r="B16" s="39" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="C16" t="s">
         <v>451</v>
@@ -6820,7 +6806,7 @@
         <v>59</v>
       </c>
       <c r="G16" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="N16">
         <v>120</v>
@@ -6831,7 +6817,7 @@
     </row>
     <row r="18" spans="2:18" ht="34" x14ac:dyDescent="0.2">
       <c r="B18" s="39" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C18" t="s">
         <v>539</v>
@@ -6840,7 +6826,7 @@
         <v>132</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="51" x14ac:dyDescent="0.2">
@@ -6865,8 +6851,8 @@
       <c r="Q19" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R19" s="34" t="s">
-        <v>545</v>
+      <c r="R19" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
@@ -6899,13 +6885,13 @@
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="E23" t="s">
         <v>59</v>
       </c>
       <c r="F23" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G23" t="s">
         <v>470</v>
@@ -6925,13 +6911,13 @@
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="E24" t="s">
         <v>59</v>
       </c>
       <c r="F24" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="G24" t="s">
         <v>472</v>
@@ -7097,7 +7083,7 @@
         <v>50</v>
       </c>
       <c r="D33" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="E33" t="s">
         <v>17</v>
@@ -7130,7 +7116,7 @@
         <v>525</v>
       </c>
       <c r="S33" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="34" spans="2:19" ht="34" x14ac:dyDescent="0.2">
@@ -7174,7 +7160,7 @@
         <v>545</v>
       </c>
       <c r="S34" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="35" spans="2:19" ht="68" x14ac:dyDescent="0.2">
@@ -7217,8 +7203,8 @@
       <c r="Q35" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R35" t="s">
-        <v>545</v>
+      <c r="R35" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="36" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -7270,8 +7256,8 @@
       <c r="Q37" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R37" t="s">
-        <v>545</v>
+      <c r="R37" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="38" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -7408,8 +7394,8 @@
       <c r="Q41" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R41" t="s">
-        <v>545</v>
+      <c r="R41" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="42" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -7516,11 +7502,11 @@
       <c r="Q45" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R45" t="s">
-        <v>545</v>
+      <c r="R45" s="40" t="s">
+        <v>525</v>
       </c>
       <c r="S45" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="46" spans="2:19" ht="68" x14ac:dyDescent="0.2">
@@ -7564,7 +7550,7 @@
         <v>545</v>
       </c>
       <c r="S46" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="47" spans="2:19" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -7649,7 +7635,7 @@
         <v>545</v>
       </c>
       <c r="S49" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="50" spans="2:19" ht="17" x14ac:dyDescent="0.2">
@@ -7693,7 +7679,7 @@
         <v>545</v>
       </c>
       <c r="S50" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="51" spans="2:19" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -7856,7 +7842,7 @@
       <c r="N55">
         <v>120</v>
       </c>
-      <c r="Q55" s="83" t="s">
+      <c r="Q55" s="49" t="s">
         <v>26</v>
       </c>
       <c r="R55" t="s">
@@ -7884,7 +7870,7 @@
       <c r="N56">
         <v>120</v>
       </c>
-      <c r="Q56" s="83" t="s">
+      <c r="Q56" s="49" t="s">
         <v>26</v>
       </c>
       <c r="R56" t="s">
@@ -8122,11 +8108,11 @@
       <c r="Q66" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R66" t="s">
-        <v>545</v>
-      </c>
-      <c r="S66" t="s">
-        <v>553</v>
+      <c r="R66" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S66" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="67" spans="2:19" ht="17" x14ac:dyDescent="0.2">
@@ -8158,11 +8144,11 @@
       <c r="Q67" s="40" t="s">
         <v>525</v>
       </c>
-      <c r="R67" t="s">
-        <v>545</v>
-      </c>
-      <c r="S67" t="s">
-        <v>554</v>
+      <c r="R67" s="40" t="s">
+        <v>525</v>
+      </c>
+      <c r="S67" s="40" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="69" spans="2:19" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -8301,10 +8287,10 @@
       <c r="H72" s="45" t="s">
         <v>494</v>
       </c>
-      <c r="J72" s="60" t="s">
+      <c r="J72" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="K72" s="60"/>
+      <c r="K72" s="61"/>
       <c r="M72" s="44">
         <v>0</v>
       </c>
@@ -8331,10 +8317,10 @@
       <c r="H73" s="45" t="s">
         <v>495</v>
       </c>
-      <c r="J73" s="60" t="s">
+      <c r="J73" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="K73" s="60"/>
+      <c r="K73" s="61"/>
       <c r="M73" s="44">
         <v>0</v>
       </c>
@@ -8429,17 +8415,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="J72:K72"/>
     <mergeCell ref="J73:K73"/>
@@ -8447,6 +8422,17 @@
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8718,38 +8704,38 @@
       <c r="D1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="62" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="78" t="s">
+      <c r="F1" s="63"/>
+      <c r="G1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="79"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="64" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="82"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
     </row>
     <row r="3" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="67" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="69"/>
     </row>
     <row r="4" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
@@ -8761,10 +8747,10 @@
       <c r="C4" s="5"/>
       <c r="D4" s="70"/>
       <c r="E4" s="71"/>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="72" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="69"/>
+      <c r="G4" s="73"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -8775,12 +8761,12 @@
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="64" t="s">
+      <c r="D5" s="76"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="65"/>
+      <c r="G5" s="75"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
@@ -8793,10 +8779,10 @@
       <c r="C6" s="5"/>
       <c r="D6" s="70"/>
       <c r="E6" s="71"/>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="72" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="69"/>
+      <c r="G6" s="73"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
@@ -8807,12 +8793,12 @@
         <v>373</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="64" t="s">
+      <c r="D7" s="76"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="65"/>
+      <c r="G7" s="75"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
@@ -8825,10 +8811,10 @@
       <c r="C8" s="5"/>
       <c r="D8" s="70"/>
       <c r="E8" s="71"/>
-      <c r="F8" s="68" t="s">
+      <c r="F8" s="72" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="69"/>
+      <c r="G8" s="73"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="66" thickBot="1" x14ac:dyDescent="0.25">
@@ -8839,25 +8825,25 @@
         <v>374</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="67"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="77"/>
       <c r="H9" s="6" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="78" t="s">
         <v>376</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="77"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="80"/>
     </row>
     <row r="11" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
@@ -8869,12 +8855,12 @@
       <c r="C11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="67"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="77"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="27" thickBot="1" x14ac:dyDescent="0.25">
@@ -8887,10 +8873,10 @@
       <c r="C12" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E12" s="69"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="70"/>
       <c r="G12" s="71"/>
       <c r="H12" s="5"/>
@@ -8905,12 +8891,12 @@
       <c r="C13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="77"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -8921,10 +8907,10 @@
         <v>380</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="68" t="s">
+      <c r="D14" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="69"/>
+      <c r="E14" s="73"/>
       <c r="F14" s="70"/>
       <c r="G14" s="71"/>
       <c r="H14" s="5"/>
@@ -8939,12 +8925,12 @@
       <c r="C15" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="77"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="53" thickBot="1" x14ac:dyDescent="0.25">
@@ -8957,10 +8943,10 @@
       <c r="C16" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D16" s="68" t="s">
+      <c r="D16" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="69"/>
+      <c r="E16" s="73"/>
       <c r="F16" s="70"/>
       <c r="G16" s="71"/>
       <c r="H16" s="5"/>
@@ -8975,12 +8961,12 @@
       <c r="C17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D17" s="64" t="s">
+      <c r="D17" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="65"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="67"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="77"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -8993,10 +8979,10 @@
       <c r="C18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="D18" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="69"/>
+      <c r="E18" s="73"/>
       <c r="F18" s="70"/>
       <c r="G18" s="71"/>
       <c r="H18" s="5"/>
@@ -9011,12 +8997,12 @@
       <c r="C19" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E19" s="65"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="67"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="77"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="40" thickBot="1" x14ac:dyDescent="0.25">
@@ -9029,10 +9015,10 @@
       <c r="C20" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="68" t="s">
+      <c r="D20" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E20" s="69"/>
+      <c r="E20" s="73"/>
       <c r="F20" s="70"/>
       <c r="G20" s="71"/>
       <c r="H20" s="5"/>
@@ -9047,12 +9033,12 @@
       <c r="C21" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="64" t="s">
+      <c r="D21" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E21" s="65"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="67"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="77"/>
       <c r="H21" s="6" t="s">
         <v>389</v>
       </c>
@@ -9067,10 +9053,10 @@
       <c r="C22" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="68" t="s">
+      <c r="D22" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E22" s="69"/>
+      <c r="E22" s="73"/>
       <c r="F22" s="70"/>
       <c r="G22" s="71"/>
       <c r="H22" s="5"/>
@@ -9097,13 +9083,13 @@
     </row>
     <row r="24" spans="1:8" ht="25" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="81" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="74"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="83"/>
     </row>
     <row r="25" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6">
@@ -9171,13 +9157,13 @@
     </row>
     <row r="29" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="67" t="s">
         <v>396</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="69"/>
     </row>
     <row r="30" spans="1:8" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
@@ -9335,13 +9321,13 @@
     </row>
     <row r="41" spans="1:6" ht="24" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3"/>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="63"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="69"/>
     </row>
     <row r="42" spans="1:6" ht="79" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
@@ -9415,12 +9401,31 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="D5:E5"/>
@@ -9434,31 +9439,12 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -9750,31 +9736,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
-    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EEDE7DDB808AF47B14A37A2563255CF" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="17d65d9f425ad811f92dcb994434cebd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8efcafe-ecab-455b-a9ec-2441266f5451" xmlns:ns3="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35cb6db38e7d3d9001b7e6afffee4001" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
@@ -10085,27 +10046,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
+    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3366D879-DBBC-469C-98D7-600868252265}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10123,4 +10089,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
lab HIGHSPEC TEST , dispersion fiber length set in HNLF
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\astrocomb\KeckLFC-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCCD9BD9-E3C9-4A45-BA79-9D995998CC0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1042A58-3383-4741-849B-8C86A1310031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2645,18 +2645,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="25" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2665,6 +2654,12 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2678,59 +2673,14 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2747,7 +2697,57 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="26">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -3251,68 +3251,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="56"/>
-      <c r="B1" s="57" t="s">
+      <c r="A1" s="55"/>
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="51" t="s">
+      <c r="K1" s="51"/>
+      <c r="L1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="54"/>
-      <c r="O1" s="51" t="s">
+      <c r="N1" s="51"/>
+      <c r="O1" s="53" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="52"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="54"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
@@ -3465,10 +3465,10 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="50" t="s">
+      <c r="J7" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="50"/>
+      <c r="K7" s="59"/>
       <c r="M7">
         <v>0</v>
       </c>
@@ -3495,10 +3495,10 @@
       <c r="H8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="50" t="s">
+      <c r="J8" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="50"/>
+      <c r="K8" s="59"/>
       <c r="M8">
         <v>0</v>
       </c>
@@ -3562,7 +3562,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="49" t="s">
+      <c r="A11" s="60" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
@@ -3586,13 +3586,13 @@
       <c r="H11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="50" t="s">
+      <c r="J11" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="50"/>
+      <c r="K11" s="59"/>
     </row>
     <row r="12" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A12" s="49"/>
+      <c r="A12" s="60"/>
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -3614,10 +3614,10 @@
       <c r="H12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="50" t="s">
+      <c r="J12" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="50"/>
+      <c r="K12" s="59"/>
     </row>
     <row r="13" spans="1:19" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A13" s="31"/>
@@ -4482,7 +4482,7 @@
       <c r="H54" s="11"/>
     </row>
     <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A55" s="53" t="s">
+      <c r="A55" s="50" t="s">
         <v>153</v>
       </c>
       <c r="B55" t="s">
@@ -4492,7 +4492,7 @@
       <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A56" s="53"/>
+      <c r="A56" s="50"/>
       <c r="B56" t="s">
         <v>155</v>
       </c>
@@ -4500,7 +4500,7 @@
       <c r="H56" s="11"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A57" s="53"/>
+      <c r="A57" s="50"/>
       <c r="B57" t="s">
         <v>156</v>
       </c>
@@ -4508,7 +4508,7 @@
       <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A58" s="53"/>
+      <c r="A58" s="50"/>
       <c r="B58" t="s">
         <v>157</v>
       </c>
@@ -4516,7 +4516,7 @@
       <c r="H58" s="11"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A59" s="53"/>
+      <c r="A59" s="50"/>
       <c r="B59" t="s">
         <v>158</v>
       </c>
@@ -4524,7 +4524,7 @@
       <c r="H59" s="11"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A60" s="53"/>
+      <c r="A60" s="50"/>
       <c r="B60" t="s">
         <v>159</v>
       </c>
@@ -4532,7 +4532,7 @@
       <c r="H60" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A61" s="53"/>
+      <c r="A61" s="50"/>
       <c r="B61" t="s">
         <v>160</v>
       </c>
@@ -4545,7 +4545,7 @@
       <c r="H62" s="11"/>
     </row>
     <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="53" t="s">
+      <c r="A63" s="50" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
@@ -4555,7 +4555,7 @@
       <c r="H63" s="11"/>
     </row>
     <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A64" s="53"/>
+      <c r="A64" s="50"/>
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -4563,7 +4563,7 @@
       <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A65" s="53"/>
+      <c r="A65" s="50"/>
       <c r="B65" t="s">
         <v>164</v>
       </c>
@@ -4571,7 +4571,7 @@
       <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A66" s="53"/>
+      <c r="A66" s="50"/>
       <c r="B66" t="s">
         <v>165</v>
       </c>
@@ -4579,7 +4579,7 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A67" s="53"/>
+      <c r="A67" s="50"/>
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -4587,7 +4587,7 @@
       <c r="H67" s="11"/>
     </row>
     <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A68" s="53"/>
+      <c r="A68" s="50"/>
       <c r="B68" t="s">
         <v>167</v>
       </c>
@@ -4595,7 +4595,7 @@
       <c r="H68" s="11"/>
     </row>
     <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A69" s="53"/>
+      <c r="A69" s="50"/>
       <c r="B69" t="s">
         <v>168</v>
       </c>
@@ -6284,6 +6284,11 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A55:A61"/>
     <mergeCell ref="A63:A69"/>
     <mergeCell ref="M1:M2"/>
@@ -6300,11 +6305,6 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6322,7 +6322,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="K17"/>
+      <selection pane="bottomLeft" activeCell="Q17" sqref="Q17:S17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
@@ -6350,77 +6350,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="56"/>
-      <c r="B1" s="57" t="s">
+      <c r="A1" s="55"/>
+      <c r="B1" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="58" t="s">
+      <c r="D1" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="58" t="s">
+      <c r="G1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="58" t="s">
+      <c r="H1" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="I1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="54" t="s">
+      <c r="J1" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="51" t="s">
+      <c r="K1" s="51"/>
+      <c r="L1" s="53" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="54" t="s">
+      <c r="M1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="54" t="s">
+      <c r="N1" s="51" t="s">
         <v>518</v>
       </c>
-      <c r="O1" s="51" t="s">
+      <c r="O1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="56" t="s">
+      <c r="Q1" s="55" t="s">
         <v>519</v>
       </c>
-      <c r="R1" s="56"/>
-      <c r="S1" s="56"/>
-      <c r="U1" s="56" t="s">
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="U1" s="55" t="s">
         <v>524</v>
       </c>
-      <c r="V1" s="56"/>
+      <c r="V1" s="55"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.6">
-      <c r="A2" s="57"/>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="58"/>
-      <c r="I2" s="59"/>
+      <c r="A2" s="56"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="58"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="52"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
-      <c r="O2" s="52"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="52"/>
+      <c r="N2" s="52"/>
+      <c r="O2" s="54"/>
       <c r="Q2" s="1" t="s">
         <v>520</v>
       </c>
@@ -6862,11 +6862,11 @@
       <c r="Q17" s="40" t="s">
         <v>523</v>
       </c>
-      <c r="R17" s="39" t="s">
-        <v>564</v>
-      </c>
-      <c r="S17" s="39" t="s">
-        <v>564</v>
+      <c r="R17" s="40" t="s">
+        <v>523</v>
+      </c>
+      <c r="S17" s="40" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="18" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
@@ -7833,7 +7833,7 @@
       <c r="R57" s="40" t="s">
         <v>523</v>
       </c>
-      <c r="S57" s="83" t="s">
+      <c r="S57" s="49" t="s">
         <v>26</v>
       </c>
     </row>
@@ -8434,10 +8434,10 @@
       <c r="H77" s="45" t="s">
         <v>492</v>
       </c>
-      <c r="J77" s="60" t="s">
+      <c r="J77" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="K77" s="60"/>
+      <c r="K77" s="61"/>
       <c r="M77" s="44">
         <v>0</v>
       </c>
@@ -8464,10 +8464,10 @@
       <c r="H78" s="45" t="s">
         <v>493</v>
       </c>
-      <c r="J78" s="60" t="s">
+      <c r="J78" s="61" t="s">
         <v>36</v>
       </c>
-      <c r="K78" s="60"/>
+      <c r="K78" s="61"/>
       <c r="M78" s="44">
         <v>0</v>
       </c>
@@ -8562,17 +8562,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:L2"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="J77:K77"/>
     <mergeCell ref="J78:K78"/>
@@ -8580,6 +8569,17 @@
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="Q1:S1"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8851,38 +8851,38 @@
       <c r="D1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="78" t="s">
+      <c r="E1" s="62" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="79"/>
-      <c r="G1" s="78" t="s">
+      <c r="F1" s="63"/>
+      <c r="G1" s="62" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="79"/>
+      <c r="H1" s="63"/>
     </row>
     <row r="2" spans="1:8" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="64" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="82"/>
+      <c r="B2" s="65"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="3"/>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="67" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="63"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="69"/>
     </row>
     <row r="4" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="4">
@@ -8894,10 +8894,10 @@
       <c r="C4" s="5"/>
       <c r="D4" s="70"/>
       <c r="E4" s="71"/>
-      <c r="F4" s="68" t="s">
+      <c r="F4" s="72" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="69"/>
+      <c r="G4" s="73"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -8908,12 +8908,12 @@
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="67"/>
-      <c r="F5" s="64" t="s">
+      <c r="D5" s="76"/>
+      <c r="E5" s="77"/>
+      <c r="F5" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="65"/>
+      <c r="G5" s="75"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -8926,10 +8926,10 @@
       <c r="C6" s="5"/>
       <c r="D6" s="70"/>
       <c r="E6" s="71"/>
-      <c r="F6" s="68" t="s">
+      <c r="F6" s="72" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="69"/>
+      <c r="G6" s="73"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -8940,12 +8940,12 @@
         <v>373</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="64" t="s">
+      <c r="D7" s="76"/>
+      <c r="E7" s="77"/>
+      <c r="F7" s="74" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="65"/>
+      <c r="G7" s="75"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -8958,10 +8958,10 @@
       <c r="C8" s="5"/>
       <c r="D8" s="70"/>
       <c r="E8" s="71"/>
-      <c r="F8" s="68" t="s">
+      <c r="F8" s="72" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="69"/>
+      <c r="G8" s="73"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -8972,25 +8972,25 @@
         <v>374</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="67"/>
-      <c r="F9" s="66"/>
-      <c r="G9" s="67"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="77"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="77"/>
       <c r="H9" s="6" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="5"/>
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="78" t="s">
         <v>376</v>
       </c>
-      <c r="C10" s="76"/>
-      <c r="D10" s="76"/>
-      <c r="E10" s="76"/>
-      <c r="F10" s="76"/>
-      <c r="G10" s="76"/>
-      <c r="H10" s="77"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="80"/>
     </row>
     <row r="11" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A11" s="6">
@@ -9002,12 +9002,12 @@
       <c r="C11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E11" s="65"/>
-      <c r="F11" s="66"/>
-      <c r="G11" s="67"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="77"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -9020,10 +9020,10 @@
       <c r="C12" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D12" s="68" t="s">
+      <c r="D12" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E12" s="69"/>
+      <c r="E12" s="73"/>
       <c r="F12" s="70"/>
       <c r="G12" s="71"/>
       <c r="H12" s="5"/>
@@ -9038,12 +9038,12 @@
       <c r="C13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="64" t="s">
+      <c r="D13" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="65"/>
-      <c r="F13" s="66"/>
-      <c r="G13" s="67"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="76"/>
+      <c r="G13" s="77"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -9054,10 +9054,10 @@
         <v>380</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="68" t="s">
+      <c r="D14" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="69"/>
+      <c r="E14" s="73"/>
       <c r="F14" s="70"/>
       <c r="G14" s="71"/>
       <c r="H14" s="5"/>
@@ -9072,12 +9072,12 @@
       <c r="C15" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="65"/>
-      <c r="F15" s="66"/>
-      <c r="G15" s="67"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="76"/>
+      <c r="G15" s="77"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -9090,10 +9090,10 @@
       <c r="C16" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D16" s="68" t="s">
+      <c r="D16" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="69"/>
+      <c r="E16" s="73"/>
       <c r="F16" s="70"/>
       <c r="G16" s="71"/>
       <c r="H16" s="5"/>
@@ -9108,12 +9108,12 @@
       <c r="C17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D17" s="64" t="s">
+      <c r="D17" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="65"/>
-      <c r="F17" s="66"/>
-      <c r="G17" s="67"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="77"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -9126,10 +9126,10 @@
       <c r="C18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D18" s="68" t="s">
+      <c r="D18" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="69"/>
+      <c r="E18" s="73"/>
       <c r="F18" s="70"/>
       <c r="G18" s="71"/>
       <c r="H18" s="5"/>
@@ -9144,12 +9144,12 @@
       <c r="C19" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="D19" s="64" t="s">
+      <c r="D19" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E19" s="65"/>
-      <c r="F19" s="66"/>
-      <c r="G19" s="67"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="77"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -9162,10 +9162,10 @@
       <c r="C20" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="68" t="s">
+      <c r="D20" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E20" s="69"/>
+      <c r="E20" s="73"/>
       <c r="F20" s="70"/>
       <c r="G20" s="71"/>
       <c r="H20" s="5"/>
@@ -9180,12 +9180,12 @@
       <c r="C21" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="64" t="s">
+      <c r="D21" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="E21" s="65"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="67"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="76"/>
+      <c r="G21" s="77"/>
       <c r="H21" s="6" t="s">
         <v>389</v>
       </c>
@@ -9200,10 +9200,10 @@
       <c r="C22" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="68" t="s">
+      <c r="D22" s="72" t="s">
         <v>378</v>
       </c>
-      <c r="E22" s="69"/>
+      <c r="E22" s="73"/>
       <c r="F22" s="70"/>
       <c r="G22" s="71"/>
       <c r="H22" s="5"/>
@@ -9230,13 +9230,13 @@
     </row>
     <row r="24" spans="1:8" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A24" s="7"/>
-      <c r="B24" s="72" t="s">
+      <c r="B24" s="81" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="74"/>
+      <c r="C24" s="82"/>
+      <c r="D24" s="82"/>
+      <c r="E24" s="82"/>
+      <c r="F24" s="83"/>
     </row>
     <row r="25" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A25" s="6">
@@ -9304,13 +9304,13 @@
     </row>
     <row r="29" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A29" s="3"/>
-      <c r="B29" s="61" t="s">
+      <c r="B29" s="67" t="s">
         <v>396</v>
       </c>
-      <c r="C29" s="62"/>
-      <c r="D29" s="62"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="63"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="69"/>
     </row>
     <row r="30" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A30" s="4">
@@ -9468,13 +9468,13 @@
     </row>
     <row r="41" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A41" s="3"/>
-      <c r="B41" s="61" t="s">
+      <c r="B41" s="67" t="s">
         <v>408</v>
       </c>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="63"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="68"/>
+      <c r="E41" s="68"/>
+      <c r="F41" s="69"/>
     </row>
     <row r="42" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A42" s="4">
@@ -9548,12 +9548,31 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="D5:E5"/>
@@ -9567,31 +9586,12 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -9883,31 +9883,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
-    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
-    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EEDE7DDB808AF47B14A37A2563255CF" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="17d65d9f425ad811f92dcb994434cebd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8efcafe-ecab-455b-a9ec-2441266f5451" xmlns:ns3="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35cb6db38e7d3d9001b7e6afffee4001" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
@@ -10218,27 +10193,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
-    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Doc_x0020_Number xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <_DCDateModified xmlns="http://schemas.microsoft.com/sharepoint/v3/fields" xsi:nil="true"/>
+    <Number xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451" xsi:nil="true"/>
+    <Description1 xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <COO_x0020_Doc_x0020_Type xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f8efcafe-ecab-455b-a9ec-2441266f5451">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3366D879-DBBC-469C-98D7-600868252265}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10256,4 +10236,24 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7bdbfaba-addc-4ef5-a19e-1af729a4b030"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/fields"/>
+    <ds:schemaRef ds:uri="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
update monitor function in xlsx
</commit_message>
<xml_diff>
--- a/HSF Comb KTL Keywords.xlsx
+++ b/HSF Comb KTL Keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\astrocomb\KeckLFC-deploy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBD93BA9-1BC0-4740-ABE9-87CFE7E511DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D5C74B3-18D3-42AE-BF4E-23BCBACD25DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -398,7 +398,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1491" uniqueCount="566">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1503" uniqueCount="576">
   <si>
     <t>Keyword</t>
   </si>
@@ -2070,18 +2070,6 @@
     <t>LFC_TEMP_TEST2</t>
   </si>
   <si>
-    <t>LFC_EDFA27_INPUT_POWER</t>
-  </si>
-  <si>
-    <t>get input power of edfa27</t>
-  </si>
-  <si>
-    <t>LFC_EDFA23_INPUT_POWER</t>
-  </si>
-  <si>
-    <t>get input power of edfa23</t>
-  </si>
-  <si>
     <t>LFC_MINICOMB_AUTO_SETUP</t>
   </si>
   <si>
@@ -2106,13 +2094,55 @@
     <t>1:pass light/0:shut light //value==none, get YJ status</t>
   </si>
   <si>
-    <t>LFC_PENDULEM_FREQ</t>
-  </si>
-  <si>
     <t>get RF frequency</t>
   </si>
   <si>
     <t>1 :pass light/0 :shut light//none:get status</t>
+  </si>
+  <si>
+    <t>LFC_RFOSCI_MONITOR</t>
+  </si>
+  <si>
+    <t>0 or`1</t>
+  </si>
+  <si>
+    <t>auto rfosci monitor</t>
+  </si>
+  <si>
+    <t>0:normal//1:fault</t>
+  </si>
+  <si>
+    <t>LFC_RFAMP_MONITOR</t>
+  </si>
+  <si>
+    <t>1 or`1</t>
+  </si>
+  <si>
+    <t>auto rfamp monitor</t>
+  </si>
+  <si>
+    <t>LFC_PENDULEM_FREQ_MONITOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 or 1 </t>
+  </si>
+  <si>
+    <t>LFC_EDFA27_INPUT_POWER_MONITOR</t>
+  </si>
+  <si>
+    <t>LFC_EDFA23_INPUT_POWER_MONITOR</t>
+  </si>
+  <si>
+    <t>0 or 1</t>
+  </si>
+  <si>
+    <t>1 or 1</t>
+  </si>
+  <si>
+    <t>monitor input power of edfa27</t>
+  </si>
+  <si>
+    <t>monitor input power of edfa23</t>
   </si>
 </sst>
 </file>
@@ -2657,6 +2687,18 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="25" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2665,12 +2707,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2684,14 +2720,59 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -2706,57 +2787,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -3262,68 +3292,68 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="57"/>
-      <c r="B1" s="58" t="s">
+      <c r="A1" s="59"/>
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="55" t="s">
+      <c r="K1" s="57"/>
+      <c r="L1" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="53"/>
-      <c r="O1" s="55" t="s">
+      <c r="N1" s="57"/>
+      <c r="O1" s="54" t="s">
         <v>11</v>
       </c>
       <c r="P1" s="22"/>
       <c r="Q1" s="22"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="53.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="60"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="56"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="56"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="55"/>
       <c r="P2" s="22"/>
       <c r="Q2" s="22"/>
     </row>
@@ -3476,10 +3506,10 @@
       <c r="H7" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="J7" s="61" t="s">
+      <c r="J7" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="K7" s="61"/>
+      <c r="K7" s="53"/>
       <c r="M7">
         <v>0</v>
       </c>
@@ -3506,10 +3536,10 @@
       <c r="H8" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="J8" s="61" t="s">
+      <c r="J8" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="K8" s="61"/>
+      <c r="K8" s="53"/>
       <c r="M8">
         <v>0</v>
       </c>
@@ -3573,7 +3603,7 @@
       </c>
     </row>
     <row r="11" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A11" s="62" t="s">
+      <c r="A11" s="52" t="s">
         <v>48</v>
       </c>
       <c r="B11" t="s">
@@ -3597,13 +3627,13 @@
       <c r="H11" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="J11" s="61" t="s">
+      <c r="J11" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="61"/>
+      <c r="K11" s="53"/>
     </row>
     <row r="12" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
-      <c r="A12" s="62"/>
+      <c r="A12" s="52"/>
       <c r="B12" t="s">
         <v>55</v>
       </c>
@@ -3625,10 +3655,10 @@
       <c r="H12" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="61" t="s">
+      <c r="J12" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="61"/>
+      <c r="K12" s="53"/>
     </row>
     <row r="13" spans="1:19" ht="62.4" x14ac:dyDescent="0.6">
       <c r="A13" s="31"/>
@@ -4493,7 +4523,7 @@
       <c r="H54" s="11"/>
     </row>
     <row r="55" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A55" s="52" t="s">
+      <c r="A55" s="56" t="s">
         <v>153</v>
       </c>
       <c r="B55" t="s">
@@ -4503,7 +4533,7 @@
       <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A56" s="52"/>
+      <c r="A56" s="56"/>
       <c r="B56" t="s">
         <v>155</v>
       </c>
@@ -4511,7 +4541,7 @@
       <c r="H56" s="11"/>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A57" s="52"/>
+      <c r="A57" s="56"/>
       <c r="B57" t="s">
         <v>156</v>
       </c>
@@ -4519,7 +4549,7 @@
       <c r="H57" s="11"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A58" s="52"/>
+      <c r="A58" s="56"/>
       <c r="B58" t="s">
         <v>157</v>
       </c>
@@ -4527,7 +4557,7 @@
       <c r="H58" s="11"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A59" s="52"/>
+      <c r="A59" s="56"/>
       <c r="B59" t="s">
         <v>158</v>
       </c>
@@ -4535,7 +4565,7 @@
       <c r="H59" s="11"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A60" s="52"/>
+      <c r="A60" s="56"/>
       <c r="B60" t="s">
         <v>159</v>
       </c>
@@ -4543,7 +4573,7 @@
       <c r="H60" s="11"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.6">
-      <c r="A61" s="52"/>
+      <c r="A61" s="56"/>
       <c r="B61" t="s">
         <v>160</v>
       </c>
@@ -4556,7 +4586,7 @@
       <c r="H62" s="11"/>
     </row>
     <row r="63" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A63" s="52" t="s">
+      <c r="A63" s="56" t="s">
         <v>161</v>
       </c>
       <c r="B63" t="s">
@@ -4566,7 +4596,7 @@
       <c r="H63" s="11"/>
     </row>
     <row r="64" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A64" s="52"/>
+      <c r="A64" s="56"/>
       <c r="B64" t="s">
         <v>163</v>
       </c>
@@ -4574,7 +4604,7 @@
       <c r="H64" s="11"/>
     </row>
     <row r="65" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A65" s="52"/>
+      <c r="A65" s="56"/>
       <c r="B65" t="s">
         <v>164</v>
       </c>
@@ -4582,7 +4612,7 @@
       <c r="H65" s="11"/>
     </row>
     <row r="66" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A66" s="52"/>
+      <c r="A66" s="56"/>
       <c r="B66" t="s">
         <v>165</v>
       </c>
@@ -4590,7 +4620,7 @@
       <c r="H66" s="11"/>
     </row>
     <row r="67" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A67" s="52"/>
+      <c r="A67" s="56"/>
       <c r="B67" t="s">
         <v>166</v>
       </c>
@@ -4598,7 +4628,7 @@
       <c r="H67" s="11"/>
     </row>
     <row r="68" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A68" s="52"/>
+      <c r="A68" s="56"/>
       <c r="B68" t="s">
         <v>167</v>
       </c>
@@ -4606,7 +4636,7 @@
       <c r="H68" s="11"/>
     </row>
     <row r="69" spans="1:8" ht="16" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A69" s="52"/>
+      <c r="A69" s="56"/>
       <c r="B69" t="s">
         <v>168</v>
       </c>
@@ -6295,11 +6325,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="J7:K7"/>
     <mergeCell ref="A55:A61"/>
     <mergeCell ref="A63:A69"/>
     <mergeCell ref="M1:M2"/>
@@ -6316,6 +6341,11 @@
     <mergeCell ref="H1:H2"/>
     <mergeCell ref="I1:I2"/>
     <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="J7:K7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6331,15 +6361,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60079DE2-3043-422E-90F3-3EEEEA14A1EF}">
   <dimension ref="A1:V84"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="76" zoomScaleNormal="76" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G14" sqref="G14"/>
+      <selection pane="bottomLeft" activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
   <cols>
     <col min="1" max="1" width="4.34765625" customWidth="1"/>
-    <col min="2" max="2" width="28.046875" customWidth="1"/>
+    <col min="2" max="2" width="31.44921875" customWidth="1"/>
     <col min="3" max="3" width="15.1484375" customWidth="1"/>
     <col min="4" max="4" width="3.34765625" customWidth="1"/>
     <col min="5" max="5" width="10.34765625" customWidth="1"/>
@@ -6361,77 +6391,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15.55" customHeight="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="57"/>
-      <c r="B1" s="58" t="s">
+      <c r="A1" s="59"/>
+      <c r="B1" s="60" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="59" t="s">
+      <c r="G1" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="59" t="s">
+      <c r="H1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="60" t="s">
+      <c r="I1" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="53"/>
-      <c r="L1" s="55" t="s">
+      <c r="K1" s="57"/>
+      <c r="L1" s="54" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="53" t="s">
+      <c r="M1" s="57" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="53" t="s">
+      <c r="N1" s="57" t="s">
         <v>517</v>
       </c>
-      <c r="O1" s="55" t="s">
+      <c r="O1" s="54" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="57" t="s">
+      <c r="Q1" s="59" t="s">
         <v>518</v>
       </c>
-      <c r="R1" s="57"/>
-      <c r="S1" s="57"/>
-      <c r="U1" s="57" t="s">
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="U1" s="59" t="s">
         <v>523</v>
       </c>
-      <c r="V1" s="57"/>
+      <c r="V1" s="59"/>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.6">
-      <c r="A2" s="58"/>
-      <c r="B2" s="58"/>
-      <c r="C2" s="58"/>
-      <c r="D2" s="59"/>
-      <c r="E2" s="58"/>
-      <c r="F2" s="58"/>
-      <c r="G2" s="59"/>
-      <c r="H2" s="59"/>
-      <c r="I2" s="60"/>
+      <c r="A2" s="60"/>
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="61"/>
+      <c r="I2" s="62"/>
       <c r="J2" s="23" t="s">
         <v>12</v>
       </c>
       <c r="K2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="L2" s="56"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="56"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="55"/>
       <c r="Q2" s="1" t="s">
         <v>519</v>
       </c>
@@ -6551,10 +6581,10 @@
         <v>522</v>
       </c>
       <c r="R7" s="39" t="s">
-        <v>26</v>
+        <v>522</v>
       </c>
       <c r="S7" s="39" t="s">
-        <v>26</v>
+        <v>522</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="31.2" x14ac:dyDescent="0.6">
@@ -6571,10 +6601,10 @@
         <v>377</v>
       </c>
       <c r="G8" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="N8">
         <v>120</v>
@@ -6644,7 +6674,7 @@
         <v>459</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>565</v>
+        <v>560</v>
       </c>
       <c r="N10">
         <v>120</v>
@@ -6807,16 +6837,16 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.6">
       <c r="B15" s="51" t="s">
-        <v>551</v>
+        <v>570</v>
       </c>
       <c r="C15" t="s">
-        <v>451</v>
+        <v>572</v>
       </c>
       <c r="E15" t="s">
         <v>59</v>
       </c>
       <c r="G15" t="s">
-        <v>552</v>
+        <v>574</v>
       </c>
       <c r="N15">
         <v>120</v>
@@ -6830,16 +6860,16 @@
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.6">
       <c r="B16" s="51" t="s">
-        <v>553</v>
+        <v>571</v>
       </c>
       <c r="C16" t="s">
-        <v>451</v>
+        <v>573</v>
       </c>
       <c r="E16" t="s">
         <v>59</v>
       </c>
       <c r="G16" t="s">
-        <v>554</v>
+        <v>575</v>
       </c>
       <c r="N16">
         <v>120</v>
@@ -6853,19 +6883,19 @@
     </row>
     <row r="17" spans="2:19" ht="46.8" x14ac:dyDescent="0.6">
       <c r="B17" s="51" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="C17" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="E17" t="s">
         <v>17</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="H17" s="8" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="N17">
         <v>120</v>
@@ -6882,7 +6912,7 @@
     </row>
     <row r="18" spans="2:19" ht="31.2" x14ac:dyDescent="0.6">
       <c r="B18" s="51" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="C18" t="s">
         <v>536</v>
@@ -6891,7 +6921,7 @@
         <v>132</v>
       </c>
       <c r="G18" s="8" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="Q18" s="39" t="s">
         <v>26</v>
@@ -6899,16 +6929,16 @@
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.6">
       <c r="B19" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="C19" t="s">
-        <v>451</v>
+        <v>569</v>
       </c>
       <c r="E19" t="s">
         <v>59</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>564</v>
+        <v>559</v>
       </c>
       <c r="Q19" s="50" t="s">
         <v>26</v>
@@ -6944,12 +6974,52 @@
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.6">
-      <c r="H21" s="8"/>
+      <c r="B21" t="s">
+        <v>561</v>
+      </c>
+      <c r="C21" t="s">
+        <v>562</v>
+      </c>
+      <c r="E21" t="s">
+        <v>59</v>
+      </c>
+      <c r="F21" t="s">
+        <v>377</v>
+      </c>
+      <c r="G21" s="8" t="s">
+        <v>563</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="N21">
+        <v>20</v>
+      </c>
       <c r="Q21" s="40"/>
       <c r="R21" s="40"/>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.6">
-      <c r="H22" s="8"/>
+      <c r="B22" t="s">
+        <v>565</v>
+      </c>
+      <c r="C22" t="s">
+        <v>566</v>
+      </c>
+      <c r="E22" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" t="s">
+        <v>377</v>
+      </c>
+      <c r="G22" s="8" t="s">
+        <v>567</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>564</v>
+      </c>
+      <c r="N22">
+        <v>20</v>
+      </c>
       <c r="Q22" s="40"/>
       <c r="R22" s="40"/>
     </row>
@@ -8589,6 +8659,17 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:L2"/>
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="J77:K77"/>
     <mergeCell ref="J78:K78"/>
@@ -8596,17 +8677,6 @@
     <mergeCell ref="O1:O2"/>
     <mergeCell ref="M1:M2"/>
     <mergeCell ref="Q1:S1"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="H1:H2"/>
-    <mergeCell ref="I1:I2"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
-    <mergeCell ref="E1:E2"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -8878,38 +8948,38 @@
       <c r="D1" s="2" t="s">
         <v>366</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="81" t="s">
         <v>367</v>
       </c>
-      <c r="F1" s="65"/>
-      <c r="G1" s="64" t="s">
+      <c r="F1" s="82"/>
+      <c r="G1" s="81" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="65"/>
+      <c r="H1" s="82"/>
     </row>
     <row r="2" spans="1:8" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="83" t="s">
         <v>368</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="68"/>
+      <c r="B2" s="84"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
+      <c r="H2" s="85"/>
     </row>
     <row r="3" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A3" s="3"/>
-      <c r="B3" s="69" t="s">
+      <c r="B3" s="64" t="s">
         <v>369</v>
       </c>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="71"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
+      <c r="H3" s="66"/>
     </row>
     <row r="4" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A4" s="4">
@@ -8919,12 +8989,12 @@
         <v>370</v>
       </c>
       <c r="C4" s="5"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="74" t="s">
+      <c r="D4" s="73"/>
+      <c r="E4" s="74"/>
+      <c r="F4" s="71" t="s">
         <v>371</v>
       </c>
-      <c r="G4" s="75"/>
+      <c r="G4" s="72"/>
       <c r="H4" s="5"/>
     </row>
     <row r="5" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -8935,12 +9005,12 @@
         <v>28</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="78"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="76" t="s">
+      <c r="D5" s="69"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="67" t="s">
         <v>371</v>
       </c>
-      <c r="G5" s="77"/>
+      <c r="G5" s="68"/>
       <c r="H5" s="3"/>
     </row>
     <row r="6" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -8951,12 +9021,12 @@
         <v>372</v>
       </c>
       <c r="C6" s="5"/>
-      <c r="D6" s="72"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="74" t="s">
+      <c r="D6" s="73"/>
+      <c r="E6" s="74"/>
+      <c r="F6" s="71" t="s">
         <v>371</v>
       </c>
-      <c r="G6" s="75"/>
+      <c r="G6" s="72"/>
       <c r="H6" s="5"/>
     </row>
     <row r="7" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -8967,12 +9037,12 @@
         <v>373</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="78"/>
-      <c r="E7" s="79"/>
-      <c r="F7" s="76" t="s">
+      <c r="D7" s="69"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="67" t="s">
         <v>371</v>
       </c>
-      <c r="G7" s="77"/>
+      <c r="G7" s="68"/>
       <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -8983,12 +9053,12 @@
         <v>53</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="72"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="74" t="s">
+      <c r="D8" s="73"/>
+      <c r="E8" s="74"/>
+      <c r="F8" s="71" t="s">
         <v>371</v>
       </c>
-      <c r="G8" s="75"/>
+      <c r="G8" s="72"/>
       <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -8999,25 +9069,25 @@
         <v>374</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="78"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="79"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="70"/>
       <c r="H9" s="6" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A10" s="5"/>
-      <c r="B10" s="80" t="s">
+      <c r="B10" s="78" t="s">
         <v>376</v>
       </c>
-      <c r="C10" s="81"/>
-      <c r="D10" s="81"/>
-      <c r="E10" s="81"/>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="82"/>
+      <c r="C10" s="79"/>
+      <c r="D10" s="79"/>
+      <c r="E10" s="79"/>
+      <c r="F10" s="79"/>
+      <c r="G10" s="79"/>
+      <c r="H10" s="80"/>
     </row>
     <row r="11" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A11" s="6">
@@ -9029,12 +9099,12 @@
       <c r="C11" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D11" s="76" t="s">
+      <c r="D11" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E11" s="77"/>
-      <c r="F11" s="78"/>
-      <c r="G11" s="79"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="70"/>
       <c r="H11" s="3"/>
     </row>
     <row r="12" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -9047,12 +9117,12 @@
       <c r="C12" s="4" t="s">
         <v>379</v>
       </c>
-      <c r="D12" s="74" t="s">
+      <c r="D12" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E12" s="75"/>
-      <c r="F12" s="72"/>
-      <c r="G12" s="73"/>
+      <c r="E12" s="72"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="74"/>
       <c r="H12" s="5"/>
     </row>
     <row r="13" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -9065,12 +9135,12 @@
       <c r="C13" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D13" s="76" t="s">
+      <c r="D13" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E13" s="77"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="79"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="70"/>
       <c r="H13" s="3"/>
     </row>
     <row r="14" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -9081,12 +9151,12 @@
         <v>380</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="74" t="s">
+      <c r="D14" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E14" s="75"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="73"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="74"/>
       <c r="H14" s="5"/>
     </row>
     <row r="15" spans="1:8" ht="23.7" thickBot="1" x14ac:dyDescent="0.65">
@@ -9099,12 +9169,12 @@
       <c r="C15" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D15" s="76" t="s">
+      <c r="D15" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="77"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="79"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="70"/>
       <c r="H15" s="3"/>
     </row>
     <row r="16" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -9117,12 +9187,12 @@
       <c r="C16" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D16" s="74" t="s">
+      <c r="D16" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E16" s="75"/>
-      <c r="F16" s="72"/>
-      <c r="G16" s="73"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="74"/>
       <c r="H16" s="5"/>
     </row>
     <row r="17" spans="1:8" ht="47.1" thickBot="1" x14ac:dyDescent="0.65">
@@ -9135,12 +9205,12 @@
       <c r="C17" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="D17" s="76" t="s">
+      <c r="D17" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E17" s="77"/>
-      <c r="F17" s="78"/>
-      <c r="G17" s="79"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="70"/>
       <c r="H17" s="3"/>
     </row>
     <row r="18" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -9153,12 +9223,12 @@
       <c r="C18" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E18" s="75"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="73"/>
+      <c r="E18" s="72"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="74"/>
       <c r="H18" s="5"/>
     </row>
     <row r="19" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
@@ -9171,12 +9241,12 @@
       <c r="C19" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="D19" s="76" t="s">
+      <c r="D19" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E19" s="77"/>
-      <c r="F19" s="78"/>
-      <c r="G19" s="79"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="70"/>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" ht="35.4" thickBot="1" x14ac:dyDescent="0.65">
@@ -9189,12 +9259,12 @@
       <c r="C20" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D20" s="74" t="s">
+      <c r="D20" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E20" s="75"/>
-      <c r="F20" s="72"/>
-      <c r="G20" s="73"/>
+      <c r="E20" s="72"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="74"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="117.3" thickBot="1" x14ac:dyDescent="0.65">
@@ -9207,12 +9277,12 @@
       <c r="C21" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="D21" s="76" t="s">
+      <c r="D21" s="67" t="s">
         <v>378</v>
       </c>
-      <c r="E21" s="77"/>
-      <c r="F21" s="78"/>
-      <c r="G21" s="79"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="70"/>
       <c r="H21" s="6" t="s">
         <v>389</v>
       </c>
@@ -9227,12 +9297,12 @@
       <c r="C22" s="4" t="s">
         <v>377</v>
       </c>
-      <c r="D22" s="74" t="s">
+      <c r="D22" s="71" t="s">
         <v>378</v>
       </c>
-      <c r="E22" s="75"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="73"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="74"/>
       <c r="H22" s="5"/>
     </row>
     <row r="23" spans="1:8" ht="15.9" thickBot="1" x14ac:dyDescent="0.65">
@@ -9257,13 +9327,13 @@
     </row>
     <row r="24" spans="1:8" ht="22.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A24" s="7"/>
-      <c r="B24" s="83" t="s">
+      <c r="B24" s="75" t="s">
         <v>391</v>
       </c>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="85"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="77"/>
     </row>
     <row r="25" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A25" s="6">
@@ -9331,13 +9401,13 @@
     </row>
     <row r="29" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A29" s="3"/>
-      <c r="B29" s="69" t="s">
+      <c r="B29" s="64" t="s">
         <v>396</v>
       </c>
-      <c r="C29" s="70"/>
-      <c r="D29" s="70"/>
-      <c r="E29" s="70"/>
-      <c r="F29" s="71"/>
+      <c r="C29" s="65"/>
+      <c r="D29" s="65"/>
+      <c r="E29" s="65"/>
+      <c r="F29" s="66"/>
     </row>
     <row r="30" spans="1:8" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A30" s="4">
@@ -9495,13 +9565,13 @@
     </row>
     <row r="41" spans="1:6" ht="22.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A41" s="3"/>
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="64" t="s">
         <v>408</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="70"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="71"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="66"/>
     </row>
     <row r="42" spans="1:6" ht="70.5" thickBot="1" x14ac:dyDescent="0.65">
       <c r="A42" s="4">
@@ -9575,31 +9645,12 @@
     </row>
   </sheetData>
   <mergeCells count="44">
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="D11:E11"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="D5:E5"/>
@@ -9613,12 +9664,31 @@
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="B10:H10"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="B41:F41"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B29:F29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -9910,6 +9980,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002EEDE7DDB808AF47B14A37A2563255CF" ma:contentTypeVersion="23" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="17d65d9f425ad811f92dcb994434cebd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f8efcafe-ecab-455b-a9ec-2441266f5451" xmlns:ns3="7bdbfaba-addc-4ef5-a19e-1af729a4b030" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="35cb6db38e7d3d9001b7e6afffee4001" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="f8efcafe-ecab-455b-a9ec-2441266f5451"/>
@@ -10220,15 +10299,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -10246,6 +10316,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3366D879-DBBC-469C-98D7-600868252265}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10265,14 +10343,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F24EE04-5C0B-4706-AA51-68EB5D169D0E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{10BB1E28-C1E7-4565-8443-1973DEA3002B}">
   <ds:schemaRefs>

</xml_diff>